<commit_message>
Committing new member test Scripts
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\Dynamic_cloud\Dynamics-CRM-Cloud\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\Dynamics-CRM-Cloud\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E80DCB8-A81C-47DC-8EC3-14C56FF7E3BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266414F1-5DE8-4108-A3E7-10989D460945}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" activeTab="2" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="4" r:id="rId1"/>
@@ -20,11 +20,11 @@
     <sheet name="Contact" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Driver!$A$1:$K$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Driver!$A$1:$K$94</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2738" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3634" uniqueCount="623">
   <si>
     <t>Premier1a</t>
   </si>
@@ -1326,9 +1326,6 @@
     <t>TFS ID_8749:Cloud : Verify if primary account of a contact has been changed then other associated Contact account association should not get end dated</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>TFS ID_8923:Cloud: Verify AG and AG effective date on Account termination when AG populated for NONGPO account</t>
   </si>
   <si>
@@ -1638,18 +1635,9 @@
     <t>2000461295</t>
   </si>
   <si>
-    <t>832157</t>
-  </si>
-  <si>
     <t>TFS ID_9068:Cloud : Bulk Import Create Supplier Template</t>
   </si>
   <si>
-    <t>BulkImport</t>
-  </si>
-  <si>
-    <t>smoke</t>
-  </si>
-  <si>
     <t>FileType</t>
   </si>
   <si>
@@ -1749,15 +1737,6 @@
     <t>https://premierstage.crm.dynamics.com/main.aspx?appid=661f146b-8f54-ec11-8f8e-00224806d209</t>
   </si>
   <si>
-    <t>2000510677</t>
-  </si>
-  <si>
-    <t>2000510678</t>
-  </si>
-  <si>
-    <t>2000510679</t>
-  </si>
-  <si>
     <t>2000510682</t>
   </si>
   <si>
@@ -1797,64 +1776,139 @@
     <t>2000510697</t>
   </si>
   <si>
-    <t>7000567058</t>
-  </si>
-  <si>
-    <t>7000567059</t>
-  </si>
-  <si>
-    <t>7000567060</t>
-  </si>
-  <si>
-    <t>7000567061</t>
-  </si>
-  <si>
-    <t>7000567062</t>
-  </si>
-  <si>
-    <t>7000567063</t>
-  </si>
-  <si>
-    <t>7000567064</t>
-  </si>
-  <si>
-    <t>2000510739</t>
-  </si>
-  <si>
-    <t>2000510740</t>
-  </si>
-  <si>
-    <t>2000510741</t>
-  </si>
-  <si>
-    <t>2000510743</t>
-  </si>
-  <si>
-    <t>2000510744</t>
-  </si>
-  <si>
-    <t>2000510745</t>
-  </si>
-  <si>
-    <t>2000510752</t>
-  </si>
-  <si>
-    <t>2000510762</t>
+    <t>2000511074</t>
+  </si>
+  <si>
+    <t>2000511075</t>
+  </si>
+  <si>
+    <t>2000511076</t>
+  </si>
+  <si>
+    <t>2000511078</t>
+  </si>
+  <si>
+    <t>2000511079</t>
+  </si>
+  <si>
+    <t>2000511080</t>
+  </si>
+  <si>
+    <t>2000511082</t>
+  </si>
+  <si>
+    <t>2000511083</t>
+  </si>
+  <si>
+    <t>7000567442</t>
+  </si>
+  <si>
+    <t>7000567443</t>
+  </si>
+  <si>
+    <t>7000567444</t>
+  </si>
+  <si>
+    <t>7000567445</t>
+  </si>
+  <si>
+    <t>7000567446</t>
+  </si>
+  <si>
+    <t>7000567447</t>
+  </si>
+  <si>
+    <t>7000567450</t>
+  </si>
+  <si>
+    <t>North Oaks Health System</t>
+  </si>
+  <si>
+    <t>693374</t>
+  </si>
+  <si>
+    <t>North Oaks Cardiology Clinic</t>
+  </si>
+  <si>
+    <t>2000511323</t>
+  </si>
+  <si>
+    <t>2000511324</t>
+  </si>
+  <si>
+    <t>2000511325</t>
+  </si>
+  <si>
+    <t>2000511727</t>
+  </si>
+  <si>
+    <t>8816_TerminatedAccountStatus</t>
+  </si>
+  <si>
+    <t>8806_CheckDPExceptionReason</t>
+  </si>
+  <si>
+    <t>TFS ID_8816:Cloud: Verify user is NOT able to create accounts directly with Terminated status</t>
+  </si>
+  <si>
+    <t>TFS ID_8806:Cloud: Verify whether DP Exception Reason should not be required, while creating new account from sub account entity</t>
+  </si>
+  <si>
+    <t>TFS ID_8780:Cloud : Verify corresponding LOB is getting deactivated when end dated membership is deactivated</t>
+  </si>
+  <si>
+    <t>8770_Check LOB End Date</t>
+  </si>
+  <si>
+    <t>TFS ID_8819:Cloud : Verify a GPO member can not be child of NON GPO member</t>
+  </si>
+  <si>
+    <t>8819_VerifyGPOUnderNonGPO</t>
+  </si>
+  <si>
+    <t>TFS ID_8798:Cloud : Verify DP Relation Date is cleared if Is Top Parent Is Set to Yes</t>
+  </si>
+  <si>
+    <t>1000174081</t>
+  </si>
+  <si>
+    <t>2000000037</t>
+  </si>
+  <si>
+    <t>You cannot publish the GPO Member since Direct Parent is NonGPO Member</t>
+  </si>
+  <si>
+    <t>2000511792</t>
+  </si>
+  <si>
+    <t>2000511799</t>
+  </si>
+  <si>
+    <t>TFS ID_8789:Cloud -Verify AG calculated correctly after prospect become a member</t>
+  </si>
+  <si>
+    <t>8789_AG and AG effective date on Account creation as Prospects</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>2022_02_02_09_51_17</t>
+  </si>
+  <si>
+    <t>2022_02_02_10_08_28</t>
+  </si>
+  <si>
+    <t>2022_02_02_10_31_23</t>
+  </si>
+  <si>
+    <t>2022_02_02_12_30_41</t>
   </si>
   <si>
     <t>PASSED</t>
   </si>
   <si>
-    <t>2000510768</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>2022_01_20_03_29_01</t>
-  </si>
-  <si>
-    <t>2022_01_20_03_36_13</t>
+    <t>2022_02_02_12_45_50</t>
   </si>
 </sst>
 </file>
@@ -2015,7 +2069,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2052,8 +2106,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2091,15 +2151,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -2112,7 +2163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2241,17 +2292,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2573,24 +2625,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
-  <dimension ref="A1:P90"/>
+  <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="C52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="132.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="46" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="132.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="9" max="10" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="46.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -2619,10 +2671,10 @@
         <v>30</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>521</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>522</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>59</v>
@@ -2645,21 +2697,21 @@
         <v>40</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>602</v>
+        <v>265</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>603</v>
+        <v>266</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
-      <c r="K2" s="84" t="s">
-        <v>568</v>
+      <c r="K2" s="81" t="s">
+        <v>564</v>
       </c>
       <c r="L2" s="67" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2685,13 +2737,13 @@
         <v>266</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>569</v>
+        <v>599</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="26"/>
-      <c r="L3" s="84" t="s">
-        <v>568</v>
+      <c r="L3" s="81" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -2717,7 +2769,7 @@
         <v>266</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>570</v>
+        <v>597</v>
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
@@ -2746,7 +2798,7 @@
         <v>266</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>571</v>
+        <v>598</v>
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -2811,7 +2863,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>35</v>
@@ -2829,7 +2881,7 @@
         <v>266</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
@@ -2867,7 +2919,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>35</v>
@@ -2885,7 +2937,7 @@
         <v>266</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
@@ -2914,7 +2966,7 @@
         <v>266</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
@@ -2925,7 +2977,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>35</v>
@@ -2943,7 +2995,7 @@
         <v>266</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
@@ -3027,7 +3079,7 @@
         <v>266</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
@@ -3038,7 +3090,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>35</v>
@@ -3056,7 +3108,7 @@
         <v>266</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
@@ -3067,7 +3119,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>35</v>
@@ -3094,7 +3146,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>35</v>
@@ -3148,7 +3200,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>35</v>
@@ -3193,7 +3245,7 @@
         <v>266</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
@@ -3204,7 +3256,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>35</v>
@@ -3223,10 +3275,10 @@
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="K22" s="26"/>
     </row>
@@ -3253,7 +3305,7 @@
         <v>266</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
@@ -3282,7 +3334,7 @@
         <v>266</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
@@ -3311,7 +3363,7 @@
         <v>266</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
@@ -3340,7 +3392,7 @@
         <v>266</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
@@ -3369,7 +3421,7 @@
         <v>266</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
@@ -3398,7 +3450,7 @@
         <v>266</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
@@ -3427,7 +3479,7 @@
         <v>266</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
@@ -3483,7 +3535,7 @@
         <v>266</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25"/>
@@ -3512,7 +3564,7 @@
         <v>266</v>
       </c>
       <c r="H32" s="25" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25"/>
@@ -3633,7 +3685,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>35</v>
@@ -3660,7 +3712,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>35</v>
@@ -3687,7 +3739,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>35</v>
@@ -3714,7 +3766,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>35</v>
@@ -3741,7 +3793,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>35</v>
@@ -3768,7 +3820,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>35</v>
@@ -3795,7 +3847,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>35</v>
@@ -3822,7 +3874,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>35</v>
@@ -3849,7 +3901,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>35</v>
@@ -3876,7 +3928,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>35</v>
@@ -3903,7 +3955,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>35</v>
@@ -3930,7 +3982,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>35</v>
@@ -3957,7 +4009,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>35</v>
@@ -3984,7 +4036,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>35</v>
@@ -4011,7 +4063,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>35</v>
@@ -4038,7 +4090,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>35</v>
@@ -4065,7 +4117,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>35</v>
@@ -4092,7 +4144,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>35</v>
@@ -4119,7 +4171,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>35</v>
@@ -4146,7 +4198,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>35</v>
@@ -4169,186 +4221,182 @@
       <c r="K56" s="25"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="22">
+      <c r="A57" s="7">
         <v>55</v>
       </c>
-      <c r="B57" s="22" t="s">
-        <v>29</v>
+      <c r="B57" s="25" t="s">
+        <v>602</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E57" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F57" s="22" t="s">
+      <c r="F57" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G57" s="22" t="s">
+      <c r="G57" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H57" s="22" t="s">
-        <v>592</v>
-      </c>
-      <c r="I57" s="22"/>
-      <c r="J57" s="22"/>
-      <c r="K57" s="23"/>
+      <c r="H57" s="25"/>
+      <c r="I57" s="25"/>
+      <c r="J57" s="25"/>
+      <c r="K57" s="25"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="22">
+      <c r="A58" s="7">
         <v>56</v>
       </c>
-      <c r="B58" s="22" t="s">
-        <v>468</v>
+      <c r="B58" s="25" t="s">
+        <v>603</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E58" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F58" s="22" t="s">
+      <c r="F58" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G58" s="22" t="s">
+      <c r="G58" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H58" s="22" t="s">
-        <v>593</v>
-      </c>
-      <c r="I58" s="22"/>
-      <c r="J58" s="22"/>
-      <c r="K58" s="23"/>
+      <c r="H58" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="I58" s="25"/>
+      <c r="J58" s="25"/>
+      <c r="K58" s="25"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="22">
+      <c r="A59" s="7">
         <v>57</v>
       </c>
-      <c r="B59" s="22" t="s">
-        <v>472</v>
+      <c r="B59" s="25" t="s">
+        <v>604</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E59" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F59" s="22" t="s">
+      <c r="F59" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G59" s="22" t="s">
+      <c r="G59" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H59" s="22" t="s">
-        <v>594</v>
-      </c>
-      <c r="I59" s="22"/>
-      <c r="J59" s="22"/>
-      <c r="K59" s="23"/>
+      <c r="H59" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="I59" s="25"/>
+      <c r="J59" s="25"/>
+      <c r="K59" s="25"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="22">
+      <c r="A60" s="7">
         <v>58</v>
       </c>
-      <c r="B60" s="22" t="s">
-        <v>455</v>
+      <c r="B60" s="25" t="s">
+        <v>606</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D60" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E60" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F60" s="22" t="s">
+      <c r="F60" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G60" s="22" t="s">
+      <c r="G60" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H60" s="22"/>
-      <c r="I60" s="22"/>
-      <c r="J60" s="22"/>
-      <c r="K60" s="23"/>
+      <c r="H60" s="25" t="s">
+        <v>613</v>
+      </c>
+      <c r="I60" s="25"/>
+      <c r="J60" s="25"/>
+      <c r="K60" s="25"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="22">
+      <c r="A61" s="7">
         <v>59</v>
       </c>
-      <c r="B61" s="22" t="s">
-        <v>92</v>
+      <c r="B61" s="2" t="s">
+        <v>608</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D61" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E61" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E61" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F61" s="22" t="s">
+      <c r="F61" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G61" s="22" t="s">
+      <c r="G61" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H61" s="22" t="s">
-        <v>595</v>
-      </c>
-      <c r="I61" s="22"/>
-      <c r="J61" s="22"/>
-      <c r="K61" s="23"/>
+      <c r="H61" s="25"/>
+      <c r="I61" s="25"/>
+      <c r="J61" s="25"/>
+      <c r="K61" s="25"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="22">
+      <c r="A62" s="7">
         <v>60</v>
       </c>
-      <c r="B62" s="22" t="s">
-        <v>97</v>
+      <c r="B62" s="2" t="s">
+        <v>614</v>
       </c>
       <c r="C62" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E62" s="22" t="s">
+      <c r="D62" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F62" s="22" t="s">
-        <v>265</v>
-      </c>
-      <c r="G62" s="22" t="s">
-        <v>266</v>
-      </c>
-      <c r="H62" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="I62" s="22"/>
-      <c r="J62" s="22"/>
-      <c r="K62" s="23"/>
+      <c r="F62" s="25" t="s">
+        <v>621</v>
+      </c>
+      <c r="G62" s="25" t="s">
+        <v>622</v>
+      </c>
+      <c r="H62" s="25"/>
+      <c r="I62" s="25"/>
+      <c r="J62" s="25"/>
+      <c r="K62" s="25"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="22">
-        <v>61</v>
+      <c r="A63" s="7">
+        <v>57</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D63" s="22" t="s">
         <v>26</v>
@@ -4363,21 +4411,21 @@
         <v>266</v>
       </c>
       <c r="H63" s="22" t="s">
-        <v>104</v>
+        <v>578</v>
       </c>
       <c r="I63" s="22"/>
       <c r="J63" s="22"/>
       <c r="K63" s="23"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="22">
-        <v>62</v>
+      <c r="A64" s="7">
+        <v>58</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>106</v>
+        <v>467</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D64" s="22" t="s">
         <v>26</v>
@@ -4392,21 +4440,21 @@
         <v>266</v>
       </c>
       <c r="H64" s="22" t="s">
-        <v>597</v>
+        <v>579</v>
       </c>
       <c r="I64" s="22"/>
       <c r="J64" s="22"/>
       <c r="K64" s="23"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="22">
-        <v>63</v>
+      <c r="A65" s="7">
+        <v>59</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>109</v>
+        <v>471</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D65" s="22" t="s">
         <v>26</v>
@@ -4421,21 +4469,21 @@
         <v>266</v>
       </c>
       <c r="H65" s="22" t="s">
-        <v>114</v>
+        <v>580</v>
       </c>
       <c r="I65" s="22"/>
       <c r="J65" s="22"/>
       <c r="K65" s="23"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="22">
-        <v>64</v>
+      <c r="A66" s="7">
+        <v>60</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>112</v>
+        <v>454</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D66" s="22" t="s">
         <v>26</v>
@@ -4449,22 +4497,20 @@
       <c r="G66" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H66" s="22" t="s">
-        <v>114</v>
-      </c>
+      <c r="H66" s="22"/>
       <c r="I66" s="22"/>
       <c r="J66" s="22"/>
       <c r="K66" s="23"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="22">
-        <v>65</v>
+      <c r="A67" s="7">
+        <v>61</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D67" s="22" t="s">
         <v>26</v>
@@ -4479,21 +4525,21 @@
         <v>266</v>
       </c>
       <c r="H67" s="22" t="s">
-        <v>119</v>
+        <v>581</v>
       </c>
       <c r="I67" s="22"/>
       <c r="J67" s="22"/>
       <c r="K67" s="23"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="22">
-        <v>66</v>
+      <c r="A68" s="7">
+        <v>62</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D68" s="22" t="s">
         <v>26</v>
@@ -4502,27 +4548,27 @@
         <v>40</v>
       </c>
       <c r="F68" s="22" t="s">
-        <v>600</v>
+        <v>265</v>
       </c>
       <c r="G68" s="22" t="s">
-        <v>604</v>
+        <v>266</v>
       </c>
       <c r="H68" s="22" t="s">
-        <v>543</v>
+        <v>582</v>
       </c>
       <c r="I68" s="22"/>
       <c r="J68" s="22"/>
       <c r="K68" s="23"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="22">
-        <v>67</v>
+      <c r="A69" s="7">
+        <v>63</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D69" s="22" t="s">
         <v>26</v>
@@ -4537,21 +4583,21 @@
         <v>266</v>
       </c>
       <c r="H69" s="22" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="I69" s="22"/>
       <c r="J69" s="22"/>
       <c r="K69" s="23"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="22">
-        <v>68</v>
+      <c r="A70" s="7">
+        <v>64</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>257</v>
+        <v>106</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D70" s="22" t="s">
         <v>26</v>
@@ -4565,20 +4611,22 @@
       <c r="G70" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H70" s="22"/>
+      <c r="H70" s="22" t="s">
+        <v>583</v>
+      </c>
       <c r="I70" s="22"/>
       <c r="J70" s="22"/>
       <c r="K70" s="23"/>
     </row>
-    <row r="71" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="22">
-        <v>69</v>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
+        <v>65</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>186</v>
+        <v>109</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D71" s="22" t="s">
         <v>26</v>
@@ -4593,21 +4641,21 @@
         <v>266</v>
       </c>
       <c r="H71" s="22" t="s">
-        <v>599</v>
+        <v>114</v>
       </c>
       <c r="I71" s="22"/>
       <c r="J71" s="22"/>
       <c r="K71" s="23"/>
     </row>
-    <row r="72" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="22">
-        <v>70</v>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
+        <v>66</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>419</v>
+        <v>112</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D72" s="22" t="s">
         <v>26</v>
@@ -4622,21 +4670,21 @@
         <v>266</v>
       </c>
       <c r="H72" s="22" t="s">
-        <v>598</v>
+        <v>114</v>
       </c>
       <c r="I72" s="22"/>
       <c r="J72" s="22"/>
       <c r="K72" s="23"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="22">
-        <v>71</v>
+      <c r="A73" s="7">
+        <v>67</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>457</v>
+        <v>115</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D73" s="22" t="s">
         <v>26</v>
@@ -4647,23 +4695,25 @@
       <c r="F73" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G73" s="25" t="s">
+      <c r="G73" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H73" s="25"/>
-      <c r="I73" s="25"/>
-      <c r="J73" s="25"/>
-      <c r="K73" s="25"/>
+      <c r="H73" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="I73" s="22"/>
+      <c r="J73" s="22"/>
+      <c r="K73" s="23"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="22">
-        <v>72</v>
+      <c r="A74" s="7">
+        <v>68</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>464</v>
+        <v>122</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D74" s="22" t="s">
         <v>26</v>
@@ -4674,23 +4724,25 @@
       <c r="F74" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G74" s="25" t="s">
+      <c r="G74" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H74" s="25"/>
-      <c r="I74" s="25"/>
-      <c r="J74" s="25"/>
-      <c r="K74" s="25"/>
+      <c r="H74" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="I74" s="22"/>
+      <c r="J74" s="22"/>
+      <c r="K74" s="23"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="22">
-        <v>73</v>
+      <c r="A75" s="7">
+        <v>69</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>469</v>
+        <v>129</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D75" s="22" t="s">
         <v>26</v>
@@ -4701,23 +4753,25 @@
       <c r="F75" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G75" s="25" t="s">
+      <c r="G75" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H75" s="25"/>
-      <c r="I75" s="25"/>
-      <c r="J75" s="25"/>
-      <c r="K75" s="25"/>
+      <c r="H75" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="I75" s="22"/>
+      <c r="J75" s="22"/>
+      <c r="K75" s="23"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="22">
-        <v>74</v>
+      <c r="A76" s="7">
+        <v>70</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>474</v>
+        <v>257</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D76" s="22" t="s">
         <v>26</v>
@@ -4728,23 +4782,23 @@
       <c r="F76" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G76" s="25" t="s">
+      <c r="G76" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H76" s="25"/>
-      <c r="I76" s="25"/>
-      <c r="J76" s="25"/>
-      <c r="K76" s="25"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="22">
-        <v>75</v>
+      <c r="H76" s="22"/>
+      <c r="I76" s="22"/>
+      <c r="J76" s="22"/>
+      <c r="K76" s="23"/>
+    </row>
+    <row r="77" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="7">
+        <v>71</v>
       </c>
       <c r="B77" s="22" t="s">
-        <v>477</v>
+        <v>186</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D77" s="22" t="s">
         <v>26</v>
@@ -4755,23 +4809,25 @@
       <c r="F77" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G77" s="25" t="s">
+      <c r="G77" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H77" s="25"/>
-      <c r="I77" s="25"/>
-      <c r="J77" s="25"/>
-      <c r="K77" s="25"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="22">
-        <v>76</v>
-      </c>
-      <c r="B78" s="22" t="s">
-        <v>480</v>
+      <c r="H77" s="22" t="s">
+        <v>584</v>
+      </c>
+      <c r="I77" s="22"/>
+      <c r="J77" s="22"/>
+      <c r="K77" s="23"/>
+    </row>
+    <row r="78" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
+        <v>72</v>
+      </c>
+      <c r="B78" s="82" t="s">
+        <v>419</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D78" s="22" t="s">
         <v>26</v>
@@ -4782,23 +4838,25 @@
       <c r="F78" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G78" s="25" t="s">
+      <c r="G78" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H78" s="25"/>
-      <c r="I78" s="25"/>
-      <c r="J78" s="25"/>
-      <c r="K78" s="25"/>
+      <c r="H78" s="22" t="s">
+        <v>585</v>
+      </c>
+      <c r="I78" s="22"/>
+      <c r="J78" s="22"/>
+      <c r="K78" s="23"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="22">
-        <v>77</v>
+      <c r="A79" s="7">
+        <v>73</v>
       </c>
       <c r="B79" s="22" t="s">
-        <v>475</v>
+        <v>456</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D79" s="22" t="s">
         <v>26</v>
@@ -4818,311 +4876,427 @@
       <c r="K79" s="25"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="30">
-        <v>78</v>
-      </c>
-      <c r="B80" s="30" t="s">
-        <v>221</v>
+      <c r="A80" s="7">
+        <v>74</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>463</v>
       </c>
       <c r="C80" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D80" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="E80" s="31" t="s">
+      <c r="D80" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E80" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F80" s="31" t="s">
+      <c r="F80" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G80" s="28" t="s">
+      <c r="G80" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H80" s="28" t="s">
-        <v>585</v>
-      </c>
-      <c r="I80" s="28"/>
-      <c r="J80" s="28"/>
-      <c r="K80" s="28"/>
+      <c r="H80" s="25"/>
+      <c r="I80" s="25"/>
+      <c r="J80" s="25"/>
+      <c r="K80" s="25"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="30">
-        <v>79</v>
-      </c>
-      <c r="B81" s="30" t="s">
-        <v>421</v>
+      <c r="A81" s="7">
+        <v>75</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>468</v>
       </c>
       <c r="C81" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D81" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="E81" s="31" t="s">
+      <c r="D81" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E81" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F81" s="31" t="s">
+      <c r="F81" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G81" s="28" t="s">
+      <c r="G81" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H81" s="28" t="s">
-        <v>586</v>
-      </c>
-      <c r="I81" s="28"/>
-      <c r="J81" s="28"/>
-      <c r="K81" s="28"/>
+      <c r="H81" s="25"/>
+      <c r="I81" s="25"/>
+      <c r="J81" s="25"/>
+      <c r="K81" s="25"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="30">
-        <v>80</v>
-      </c>
-      <c r="B82" s="30" t="s">
-        <v>422</v>
+      <c r="A82" s="7">
+        <v>76</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>473</v>
       </c>
       <c r="C82" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D82" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="E82" s="31" t="s">
+      <c r="D82" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E82" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F82" s="31" t="s">
+      <c r="F82" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G82" s="28" t="s">
+      <c r="G82" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H82" s="28" t="s">
-        <v>587</v>
-      </c>
-      <c r="I82" s="28"/>
-      <c r="J82" s="28"/>
-      <c r="K82" s="28"/>
+      <c r="H82" s="25"/>
+      <c r="I82" s="25"/>
+      <c r="J82" s="25"/>
+      <c r="K82" s="25"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="30">
-        <v>81</v>
-      </c>
-      <c r="B83" s="30" t="s">
-        <v>423</v>
+      <c r="A83" s="7">
+        <v>77</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>476</v>
       </c>
       <c r="C83" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D83" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="E83" s="31" t="s">
+      <c r="D83" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E83" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F83" s="30" t="s">
+      <c r="F83" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G83" s="29" t="s">
+      <c r="G83" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H83" s="29" t="s">
-        <v>588</v>
-      </c>
-      <c r="I83" s="29"/>
-      <c r="J83" s="29"/>
-      <c r="K83" s="29"/>
+      <c r="H83" s="25"/>
+      <c r="I83" s="25"/>
+      <c r="J83" s="25"/>
+      <c r="K83" s="25"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="30">
-        <v>82</v>
-      </c>
-      <c r="B84" s="30" t="s">
-        <v>424</v>
+      <c r="A84" s="7">
+        <v>78</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>479</v>
       </c>
       <c r="C84" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D84" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="E84" s="31" t="s">
+      <c r="D84" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E84" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F84" s="30" t="s">
+      <c r="F84" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G84" s="29" t="s">
+      <c r="G84" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H84" s="29" t="s">
-        <v>589</v>
-      </c>
-      <c r="I84" s="29"/>
-      <c r="J84" s="29"/>
-      <c r="K84" s="29"/>
+      <c r="H84" s="25"/>
+      <c r="I84" s="25"/>
+      <c r="J84" s="25"/>
+      <c r="K84" s="25"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="30">
-        <v>83</v>
-      </c>
-      <c r="B85" s="30" t="s">
-        <v>420</v>
+      <c r="A85" s="7">
+        <v>79</v>
+      </c>
+      <c r="B85" s="22" t="s">
+        <v>474</v>
       </c>
       <c r="C85" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D85" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="E85" s="31" t="s">
+      <c r="D85" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E85" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F85" s="30" t="s">
+      <c r="F85" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G85" s="29" t="s">
+      <c r="G85" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H85" s="29"/>
-      <c r="I85" s="29"/>
-      <c r="J85" s="29"/>
-      <c r="K85" s="29"/>
+      <c r="H85" s="25"/>
+      <c r="I85" s="25"/>
+      <c r="J85" s="25"/>
+      <c r="K85" s="25"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" s="30">
-        <v>84</v>
+      <c r="A86" s="7">
+        <v>80</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>425</v>
+        <v>221</v>
       </c>
       <c r="C86" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D86" s="30" t="s">
+      <c r="D86" s="31" t="s">
         <v>220</v>
       </c>
       <c r="E86" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="F86" s="30" t="s">
+      <c r="F86" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="G86" s="29" t="s">
+      <c r="G86" s="28" t="s">
         <v>266</v>
       </c>
-      <c r="H86" s="29"/>
-      <c r="I86" s="29"/>
-      <c r="J86" s="29"/>
-      <c r="K86" s="29"/>
+      <c r="H86" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="I86" s="28"/>
+      <c r="J86" s="28"/>
+      <c r="K86" s="28"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="30">
-        <v>85</v>
+      <c r="A87" s="7">
+        <v>81</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="C87" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D87" s="30" t="s">
+      <c r="D87" s="31" t="s">
         <v>220</v>
       </c>
       <c r="E87" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="F87" s="30" t="s">
+      <c r="F87" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="G87" s="29" t="s">
+      <c r="G87" s="28" t="s">
         <v>266</v>
       </c>
-      <c r="H87" s="29" t="s">
-        <v>590</v>
-      </c>
-      <c r="I87" s="29"/>
-      <c r="J87" s="29"/>
-      <c r="K87" s="29"/>
-    </row>
-    <row r="88" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="30">
-        <v>86</v>
-      </c>
-      <c r="B88" s="31" t="s">
-        <v>427</v>
+      <c r="H87" s="28" t="s">
+        <v>586</v>
+      </c>
+      <c r="I87" s="28"/>
+      <c r="J87" s="28"/>
+      <c r="K87" s="28"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="7">
+        <v>82</v>
+      </c>
+      <c r="B88" s="30" t="s">
+        <v>422</v>
       </c>
       <c r="C88" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D88" s="30" t="s">
+      <c r="D88" s="31" t="s">
         <v>220</v>
       </c>
       <c r="E88" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="F88" s="30" t="s">
+      <c r="F88" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="G88" s="29" t="s">
+      <c r="G88" s="28" t="s">
         <v>266</v>
       </c>
-      <c r="H88" s="29" t="s">
-        <v>591</v>
-      </c>
-      <c r="I88" s="29"/>
-      <c r="J88" s="29"/>
-      <c r="K88" s="29"/>
-    </row>
-    <row r="89" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="78">
-        <v>87</v>
-      </c>
-      <c r="B89" s="78" t="s">
-        <v>533</v>
+      <c r="H88" s="28" t="s">
+        <v>587</v>
+      </c>
+      <c r="I88" s="28"/>
+      <c r="J88" s="28"/>
+      <c r="K88" s="28"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="7">
+        <v>83</v>
+      </c>
+      <c r="B89" s="30" t="s">
+        <v>423</v>
       </c>
       <c r="C89" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D89" s="79" t="s">
-        <v>534</v>
-      </c>
-      <c r="E89" s="78" t="s">
-        <v>535</v>
-      </c>
-      <c r="F89" s="78" t="s">
+      <c r="D89" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E89" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F89" s="30" t="s">
         <v>265</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G89" s="29" t="s">
         <v>266</v>
       </c>
+      <c r="H89" s="29" t="s">
+        <v>588</v>
+      </c>
+      <c r="I89" s="29"/>
+      <c r="J89" s="29"/>
+      <c r="K89" s="29"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A90" s="81">
-        <v>88</v>
-      </c>
-      <c r="B90" s="82" t="s">
-        <v>540</v>
+      <c r="A90" s="7">
+        <v>84</v>
+      </c>
+      <c r="B90" s="30" t="s">
+        <v>424</v>
       </c>
       <c r="C90" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D90" s="79" t="s">
-        <v>534</v>
-      </c>
-      <c r="E90" s="78" t="s">
-        <v>535</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="D90" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E90" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F90" s="30" t="s">
         <v>265</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G90" s="29" t="s">
         <v>266</v>
       </c>
+      <c r="H90" s="29" t="s">
+        <v>589</v>
+      </c>
+      <c r="I90" s="29"/>
+      <c r="J90" s="29"/>
+      <c r="K90" s="29"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="7">
+        <v>85</v>
+      </c>
+      <c r="B91" s="30" t="s">
+        <v>420</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D91" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E91" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F91" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G91" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H91" s="29"/>
+      <c r="I91" s="29"/>
+      <c r="J91" s="29"/>
+      <c r="K91" s="29"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="7">
+        <v>86</v>
+      </c>
+      <c r="B92" s="30" t="s">
+        <v>425</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D92" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E92" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F92" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G92" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H92" s="29"/>
+      <c r="I92" s="29"/>
+      <c r="J92" s="29"/>
+      <c r="K92" s="29"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="7">
+        <v>87</v>
+      </c>
+      <c r="B93" s="30" t="s">
+        <v>426</v>
+      </c>
+      <c r="C93" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D93" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E93" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F93" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G93" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H93" s="29" t="s">
+        <v>590</v>
+      </c>
+      <c r="I93" s="29"/>
+      <c r="J93" s="29"/>
+      <c r="K93" s="29"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" s="7">
+        <v>88</v>
+      </c>
+      <c r="B94" s="31" t="s">
+        <v>427</v>
+      </c>
+      <c r="C94" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D94" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E94" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F94" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G94" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H94" s="29" t="s">
+        <v>591</v>
+      </c>
+      <c r="I94" s="29"/>
+      <c r="J94" s="29"/>
+      <c r="K94" s="29"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C90" xr:uid="{C9334235-52FB-4F10-8331-5687DC05318C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C94" xr:uid="{C9334235-52FB-4F10-8331-5687DC05318C}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5160,10 +5334,10 @@
         <v>286</v>
       </c>
       <c r="E1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="F1" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -5171,7 +5345,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>322</v>
@@ -5179,19 +5353,19 @@
       <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="80" t="s">
-        <v>538</v>
-      </c>
-      <c r="F2" s="80" t="s">
-        <v>539</v>
+      <c r="E2" s="78" t="s">
+        <v>534</v>
+      </c>
+      <c r="F2" s="78" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="82" t="s">
-        <v>540</v>
+      <c r="B3" s="79" t="s">
+        <v>536</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>322</v>
@@ -5199,11 +5373,11 @@
       <c r="D3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="80" t="s">
-        <v>538</v>
-      </c>
-      <c r="F3" s="80" t="s">
-        <v>539</v>
+      <c r="E3" s="78" t="s">
+        <v>534</v>
+      </c>
+      <c r="F3" s="78" t="s">
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -5218,96 +5392,96 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
-  <dimension ref="A1:DY56"/>
+  <dimension ref="A1:DY62"/>
   <sheetViews>
-    <sheetView topLeftCell="AO1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AW2" sqref="AW2"/>
+    <sheetView tabSelected="1" topLeftCell="AQ43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AX62" sqref="AX62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="121" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="69.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="36.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="73.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="20.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="21.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="27.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="18.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="4.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="8.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="24.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="9.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="9.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="22.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="24.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="16.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="10.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="20.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="20.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="26.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="25" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="15.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="15.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="17.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="26.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="30.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="23.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="66" width="23.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="26.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="18.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="18.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="71" max="77" width="26.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="78" max="78" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="79" max="79" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="80" max="80" width="22.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="81" max="81" width="18.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="82" max="82" width="9.140625" style="2" collapsed="1"/>
-    <col min="83" max="83" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="84" max="84" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="85" max="85" width="17.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="86" max="86" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="87" max="87" width="15.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="88" max="88" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="89" max="89" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="90" max="90" width="14.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="91" max="91" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="92" max="92" width="10.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="93" max="93" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="94" max="94" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="95" max="95" width="9.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="96" max="96" width="14.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="97" max="97" width="32" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="98" max="98" width="16.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="99" max="105" width="9.140625" style="2" collapsed="1"/>
-    <col min="106" max="106" width="10" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="107" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="5.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="121.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="29.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="11.28515625" collapsed="true"/>
+    <col min="6" max="8" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="69.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="2" width="36.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="73.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="20.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="15.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="2" width="21.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="2" width="4.42578125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="8.28515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="2" width="24.140625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="2" width="24.140625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="9.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="2" width="9.5703125" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="2" width="22.28515625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" style="2" width="24.5703125" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="2" width="20.5703125" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="2" width="26.42578125" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" style="2" width="15.140625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" style="2" width="15.7109375" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
+    <col min="51" max="51" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" style="2" width="30.42578125" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
+    <col min="55" max="66" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
+    <col min="67" max="67" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="68" max="68" bestFit="true" customWidth="true" style="2" width="26.140625" collapsed="true"/>
+    <col min="69" max="69" bestFit="true" customWidth="true" style="2" width="18.140625" collapsed="true"/>
+    <col min="70" max="70" customWidth="true" style="2" width="18.140625" collapsed="true"/>
+    <col min="71" max="77" customWidth="true" style="2" width="26.140625" collapsed="true"/>
+    <col min="78" max="78" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="79" max="79" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="80" max="80" bestFit="true" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
+    <col min="81" max="81" bestFit="true" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
+    <col min="82" max="82" style="2" width="9.140625" collapsed="true"/>
+    <col min="83" max="83" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
+    <col min="84" max="84" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="85" max="85" bestFit="true" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
+    <col min="86" max="86" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="87" max="87" bestFit="true" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
+    <col min="88" max="88" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
+    <col min="89" max="89" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
+    <col min="90" max="90" bestFit="true" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
+    <col min="91" max="91" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
+    <col min="92" max="92" bestFit="true" customWidth="true" style="2" width="10.7109375" collapsed="true"/>
+    <col min="93" max="93" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
+    <col min="94" max="94" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
+    <col min="95" max="95" bestFit="true" customWidth="true" style="2" width="9.28515625" collapsed="true"/>
+    <col min="96" max="96" bestFit="true" customWidth="true" style="2" width="14.140625" collapsed="true"/>
+    <col min="97" max="97" bestFit="true" customWidth="true" style="2" width="32.0" collapsed="true"/>
+    <col min="98" max="98" bestFit="true" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
+    <col min="99" max="105" style="2" width="9.140625" collapsed="true"/>
+    <col min="106" max="106" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
+    <col min="107" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:118" s="60" customFormat="1" x14ac:dyDescent="0.25">
@@ -5725,7 +5899,7 @@
         <v>7</v>
       </c>
       <c r="AB2" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC2" s="16"/>
       <c r="AD2" s="35" t="s">
@@ -5736,7 +5910,7 @@
       </c>
       <c r="AF2" s="16"/>
       <c r="AG2" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AH2" s="35" t="s">
         <v>240</v>
@@ -5763,9 +5937,11 @@
         <v>35</v>
       </c>
       <c r="AV2" s="16"/>
-      <c r="AW2" s="16"/>
+      <c r="AW2" s="16" t="s">
+        <v>593</v>
+      </c>
       <c r="AX2" s="16" t="s">
-        <v>244</v>
+        <v>595</v>
       </c>
       <c r="AY2" s="16"/>
       <c r="AZ2" s="16" t="s">
@@ -5907,7 +6083,7 @@
         <v>7</v>
       </c>
       <c r="AB3" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC3" s="16"/>
       <c r="AD3" s="35" t="s">
@@ -5950,10 +6126,10 @@
       </c>
       <c r="AV3" s="16"/>
       <c r="AW3" s="16" t="s">
-        <v>557</v>
+        <v>593</v>
       </c>
       <c r="AX3" s="16" t="s">
-        <v>244</v>
+        <v>595</v>
       </c>
       <c r="AY3" s="16"/>
       <c r="AZ3" s="16" t="s">
@@ -6095,7 +6271,7 @@
         <v>7</v>
       </c>
       <c r="AB4" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC4" s="16"/>
       <c r="AD4" s="35" t="s">
@@ -6138,10 +6314,10 @@
       </c>
       <c r="AV4" s="16"/>
       <c r="AW4" s="16" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="AX4" s="16" t="s">
-        <v>244</v>
+        <v>595</v>
       </c>
       <c r="AY4" s="16"/>
       <c r="AZ4" s="16" t="s">
@@ -6281,7 +6457,7 @@
         <v>7</v>
       </c>
       <c r="AB5" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC5" s="16"/>
       <c r="AD5" s="35" t="s">
@@ -6292,7 +6468,7 @@
       </c>
       <c r="AF5" s="16"/>
       <c r="AG5" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AH5" s="35" t="s">
         <v>240</v>
@@ -6321,7 +6497,7 @@
       <c r="AV5" s="16"/>
       <c r="AW5" s="16"/>
       <c r="AX5" s="16" t="s">
-        <v>244</v>
+        <v>595</v>
       </c>
       <c r="AY5" s="16"/>
       <c r="AZ5" s="16" t="s">
@@ -6463,7 +6639,7 @@
         <v>7</v>
       </c>
       <c r="AB6" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC6" s="15"/>
       <c r="AD6" s="38" t="s">
@@ -6474,7 +6650,7 @@
       </c>
       <c r="AF6" s="15"/>
       <c r="AG6" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AH6" s="38" t="s">
         <v>240</v>
@@ -6502,8 +6678,8 @@
       </c>
       <c r="AV6" s="15"/>
       <c r="AW6" s="15"/>
-      <c r="AX6" s="15" t="s">
-        <v>244</v>
+      <c r="AX6" s="16" t="s">
+        <v>595</v>
       </c>
       <c r="AY6" s="15"/>
       <c r="AZ6" s="15" t="s">
@@ -6643,7 +6819,7 @@
         <v>7</v>
       </c>
       <c r="AB7" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC7" s="15"/>
       <c r="AD7" s="38" t="s">
@@ -6654,7 +6830,7 @@
       </c>
       <c r="AF7" s="15"/>
       <c r="AG7" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AH7" s="38" t="s">
         <v>240</v>
@@ -6682,8 +6858,8 @@
       </c>
       <c r="AV7" s="15"/>
       <c r="AW7" s="15"/>
-      <c r="AX7" s="15" t="s">
-        <v>244</v>
+      <c r="AX7" s="16" t="s">
+        <v>595</v>
       </c>
       <c r="AY7" s="15"/>
       <c r="AZ7" s="15" t="s">
@@ -6771,7 +6947,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C8" s="33" t="s">
         <v>299</v>
@@ -6784,7 +6960,7 @@
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
@@ -6844,7 +7020,7 @@
         <v>47</v>
       </c>
       <c r="AK8" s="16" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="AL8" s="35" t="s">
         <v>240</v>
@@ -6875,7 +7051,7 @@
       </c>
       <c r="AW8" s="16"/>
       <c r="AX8" s="16" t="s">
-        <v>244</v>
+        <v>595</v>
       </c>
       <c r="AY8" s="16"/>
       <c r="AZ8" s="16" t="s">
@@ -7036,7 +7212,7 @@
         <v>47</v>
       </c>
       <c r="AK9" s="16" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="AL9" s="35" t="s">
         <v>240</v>
@@ -7071,7 +7247,7 @@
       </c>
       <c r="AW9" s="16"/>
       <c r="AX9" s="16" t="s">
-        <v>244</v>
+        <v>595</v>
       </c>
       <c r="AY9" s="16"/>
       <c r="AZ9" s="16" t="s">
@@ -7159,7 +7335,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C10" s="33" t="s">
         <v>321</v>
@@ -7172,7 +7348,7 @@
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
@@ -7215,7 +7391,7 @@
         <v>7</v>
       </c>
       <c r="AB10" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC10" s="16" t="s">
         <v>11</v>
@@ -7256,10 +7432,10 @@
       </c>
       <c r="AV10" s="16"/>
       <c r="AW10" s="16" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="AX10" s="16" t="s">
-        <v>244</v>
+        <v>595</v>
       </c>
       <c r="AY10" s="16"/>
       <c r="AZ10" s="16" t="s">
@@ -7403,7 +7579,7 @@
         <v>7</v>
       </c>
       <c r="AB11" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC11" s="16" t="s">
         <v>11</v>
@@ -7448,10 +7624,10 @@
       </c>
       <c r="AV11" s="16"/>
       <c r="AW11" s="16" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="AX11" s="16" t="s">
-        <v>244</v>
+        <v>595</v>
       </c>
       <c r="AY11" s="16"/>
       <c r="AZ11" s="16" t="s">
@@ -7539,7 +7715,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C12" s="33" t="s">
         <v>321</v>
@@ -7552,7 +7728,7 @@
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
@@ -7595,7 +7771,7 @@
         <v>7</v>
       </c>
       <c r="AB12" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC12" s="16" t="s">
         <v>11</v>
@@ -7637,7 +7813,7 @@
       <c r="AV12" s="16"/>
       <c r="AW12" s="16"/>
       <c r="AX12" s="16" t="s">
-        <v>244</v>
+        <v>595</v>
       </c>
       <c r="AY12" s="16"/>
       <c r="AZ12" s="16" t="s">
@@ -7781,7 +7957,7 @@
         <v>7</v>
       </c>
       <c r="AB13" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC13" s="16" t="s">
         <v>11</v>
@@ -7823,7 +7999,7 @@
       <c r="AV13" s="16"/>
       <c r="AW13" s="16"/>
       <c r="AX13" s="16" t="s">
-        <v>244</v>
+        <v>595</v>
       </c>
       <c r="AY13" s="16"/>
       <c r="AZ13" s="16" t="s">
@@ -7967,7 +8143,7 @@
         <v>7</v>
       </c>
       <c r="AB14" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC14" s="16" t="s">
         <v>11</v>
@@ -8009,7 +8185,7 @@
       <c r="AV14" s="16"/>
       <c r="AW14" s="16"/>
       <c r="AX14" s="16" t="s">
-        <v>244</v>
+        <v>595</v>
       </c>
       <c r="AY14" s="16"/>
       <c r="AZ14" s="16" t="s">
@@ -8153,7 +8329,7 @@
         <v>7</v>
       </c>
       <c r="AB15" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC15" s="16" t="s">
         <v>11</v>
@@ -8194,10 +8370,10 @@
       </c>
       <c r="AV15" s="16"/>
       <c r="AW15" s="16" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="AX15" s="16" t="s">
-        <v>244</v>
+        <v>595</v>
       </c>
       <c r="AY15" s="16"/>
       <c r="AZ15" s="16" t="s">
@@ -8285,7 +8461,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C16" s="33" t="s">
         <v>321</v>
@@ -8298,7 +8474,7 @@
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
       <c r="I16" s="16" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
@@ -8341,7 +8517,7 @@
         <v>7</v>
       </c>
       <c r="AB16" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC16" s="16" t="s">
         <v>11</v>
@@ -8382,7 +8558,7 @@
       </c>
       <c r="AV16" s="16"/>
       <c r="AW16" s="16" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="AX16" s="16" t="s">
         <v>244</v>
@@ -8473,7 +8649,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C17" s="33" t="s">
         <v>321</v>
@@ -8482,10 +8658,10 @@
         <v>0</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="F17" s="42" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="G17" s="42" t="s">
         <v>215</v>
@@ -8494,7 +8670,7 @@
         <v>210</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J17" s="43" t="s">
         <v>216</v>
@@ -8627,7 +8803,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C18" s="33" t="s">
         <v>321</v>
@@ -8640,7 +8816,7 @@
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
@@ -8689,7 +8865,7 @@
         <v>7</v>
       </c>
       <c r="AB18" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC18" s="16" t="s">
         <v>11</v>
@@ -8953,7 +9129,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C20" s="33" t="s">
         <v>321</v>
@@ -8966,7 +9142,7 @@
       <c r="G20" s="45"/>
       <c r="H20" s="45"/>
       <c r="I20" s="45" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J20" s="45"/>
       <c r="K20" s="45"/>
@@ -9007,7 +9183,7 @@
         <v>7</v>
       </c>
       <c r="AB20" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC20" s="16"/>
       <c r="AD20" s="35" t="s">
@@ -9104,7 +9280,7 @@
       </c>
       <c r="CB20" s="45"/>
       <c r="CC20" s="35" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="CD20" s="45" t="s">
         <v>253</v>
@@ -9211,7 +9387,7 @@
         <v>7</v>
       </c>
       <c r="AB21" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC21" s="16" t="s">
         <v>51</v>
@@ -9270,7 +9446,7 @@
         <v>51</v>
       </c>
       <c r="AW21" s="16" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="AX21" s="16" t="s">
         <v>244</v>
@@ -9416,10 +9592,10 @@
         <v>35</v>
       </c>
       <c r="DK21" s="14" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="DL21" s="14" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="DM21" s="45" t="s">
         <v>35</v>
@@ -9433,7 +9609,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C22" s="33" t="s">
         <v>321</v>
@@ -9446,7 +9622,7 @@
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
@@ -9487,7 +9663,7 @@
         <v>7</v>
       </c>
       <c r="AB22" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC22" s="16"/>
       <c r="AD22" s="35" t="s">
@@ -9530,7 +9706,7 @@
       </c>
       <c r="AV22" s="16"/>
       <c r="AW22" s="16" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="AX22" s="16" t="s">
         <v>244</v>
@@ -9624,13 +9800,13 @@
         <v>178</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E23" s="50" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F23" s="45"/>
       <c r="G23" s="45"/>
@@ -9764,13 +9940,13 @@
         <v>177</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E24" s="50" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F24" s="45"/>
       <c r="G24" s="45"/>
@@ -9904,13 +10080,13 @@
         <v>169</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E25" s="50" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="F25" s="45"/>
       <c r="G25" s="45"/>
@@ -10044,13 +10220,13 @@
         <v>179</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E26" s="50" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="F26" s="45"/>
       <c r="G26" s="45"/>
@@ -10184,13 +10360,13 @@
         <v>180</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E27" s="50" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="F27" s="45"/>
       <c r="G27" s="45"/>
@@ -10326,13 +10502,13 @@
         <v>181</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E28" s="50" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="F28" s="45"/>
       <c r="G28" s="45"/>
@@ -10511,7 +10687,7 @@
         <v>7</v>
       </c>
       <c r="AB29" s="50" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="AC29" s="45"/>
       <c r="AD29" s="35" t="s">
@@ -10622,7 +10798,7 @@
         <v>211</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>0</v>
@@ -10839,7 +11015,7 @@
         <v>7</v>
       </c>
       <c r="AB31" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC31" s="16"/>
       <c r="AD31" s="35" t="s">
@@ -11015,7 +11191,7 @@
         <v>7</v>
       </c>
       <c r="AB32" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC32" s="16"/>
       <c r="AD32" s="35" t="s">
@@ -11193,7 +11369,7 @@
         <v>7</v>
       </c>
       <c r="AB33" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC33" s="16"/>
       <c r="AD33" s="35" t="s">
@@ -11343,8 +11519,8 @@
       <c r="I34" s="45" t="s">
         <v>364</v>
       </c>
-      <c r="J34" s="83" t="s">
-        <v>547</v>
+      <c r="J34" s="80" t="s">
+        <v>543</v>
       </c>
       <c r="K34" s="45"/>
       <c r="L34" s="45"/>
@@ -11522,7 +11698,7 @@
         <v>7</v>
       </c>
       <c r="AB35" s="37" t="s">
-        <v>532</v>
+        <v>594</v>
       </c>
       <c r="AC35" s="16"/>
       <c r="AD35" s="35" t="s">
@@ -11694,7 +11870,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="50" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="F36" s="45"/>
       <c r="G36" s="45"/>
@@ -11765,14 +11941,14 @@
         <v>235</v>
       </c>
       <c r="BP36" s="35" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="BQ36" s="16" t="s">
         <v>236</v>
       </c>
       <c r="BR36" s="45"/>
       <c r="BS36" s="35" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="BT36" s="45"/>
       <c r="BU36" s="45"/>
@@ -11831,7 +12007,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C37" s="33" t="s">
         <v>299</v>
@@ -11844,7 +12020,7 @@
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
@@ -12005,7 +12181,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>299</v>
@@ -12018,7 +12194,7 @@
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
@@ -12179,7 +12355,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C39" s="33" t="s">
         <v>299</v>
@@ -12192,7 +12368,7 @@
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
       <c r="I39" s="15" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
@@ -12353,7 +12529,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C40" s="33" t="s">
         <v>299</v>
@@ -12366,7 +12542,7 @@
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
       <c r="I40" s="15" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J40" s="15"/>
       <c r="K40" s="15"/>
@@ -12527,7 +12703,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>299</v>
@@ -12540,7 +12716,7 @@
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
       <c r="I41" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J41" s="15"/>
       <c r="K41" s="15"/>
@@ -12701,7 +12877,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="55" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C42" s="33" t="s">
         <v>299</v>
@@ -12714,7 +12890,7 @@
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
       <c r="I42" s="15" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J42" s="15"/>
       <c r="K42" s="15"/>
@@ -12875,7 +13051,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="55" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C43" s="33" t="s">
         <v>299</v>
@@ -12888,7 +13064,7 @@
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
       <c r="I43" s="15" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J43" s="15"/>
       <c r="K43" s="15"/>
@@ -13051,7 +13227,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="55" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>299</v>
@@ -13064,7 +13240,7 @@
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
       <c r="I44" s="15" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
@@ -13227,7 +13403,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="55" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C45" s="33" t="s">
         <v>299</v>
@@ -13240,7 +13416,7 @@
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
       <c r="I45" s="15" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
@@ -13403,7 +13579,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="55" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C46" s="33" t="s">
         <v>299</v>
@@ -13416,7 +13592,7 @@
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
       <c r="I46" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
@@ -13583,7 +13759,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="55" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C47" s="33" t="s">
         <v>299</v>
@@ -13596,7 +13772,7 @@
       <c r="G47" s="15"/>
       <c r="H47" s="15"/>
       <c r="I47" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
@@ -13763,7 +13939,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="55" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C48" s="33" t="s">
         <v>299</v>
@@ -13776,7 +13952,7 @@
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
       <c r="I48" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
@@ -13943,7 +14119,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="55" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C49" s="33" t="s">
         <v>299</v>
@@ -13951,14 +14127,12 @@
       <c r="D49" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E49" s="15" t="s">
-        <v>428</v>
-      </c>
+      <c r="E49" s="15"/>
       <c r="F49" s="15"/>
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
       <c r="I49" s="15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
@@ -14125,7 +14299,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="55" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C50" s="33" t="s">
         <v>299</v>
@@ -14138,7 +14312,7 @@
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
       <c r="I50" s="15" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
@@ -14305,7 +14479,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C51" s="33" t="s">
         <v>299</v>
@@ -14318,7 +14492,7 @@
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
       <c r="I51" s="15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
@@ -14485,7 +14659,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="55" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C52" s="33" t="s">
         <v>299</v>
@@ -14498,7 +14672,7 @@
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
       <c r="I52" s="15" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
@@ -14667,7 +14841,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="55" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C53" s="33" t="s">
         <v>299</v>
@@ -14680,7 +14854,7 @@
       <c r="G53" s="15"/>
       <c r="H53" s="15"/>
       <c r="I53" s="15" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
@@ -14849,7 +15023,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="55" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C54" s="33" t="s">
         <v>299</v>
@@ -14862,7 +15036,7 @@
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
       <c r="I54" s="45" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J54" s="15"/>
       <c r="K54" s="15"/>
@@ -15031,7 +15205,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C55" s="33" t="s">
         <v>299</v>
@@ -15044,7 +15218,7 @@
       <c r="G55" s="15"/>
       <c r="H55" s="15"/>
       <c r="I55" s="15" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J55" s="15"/>
       <c r="K55" s="15"/>
@@ -15205,7 +15379,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="55" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C56" s="33" t="s">
         <v>299</v>
@@ -15218,7 +15392,7 @@
       <c r="G56" s="45"/>
       <c r="H56" s="45"/>
       <c r="I56" s="45" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J56" s="45"/>
       <c r="K56" s="45"/>
@@ -15380,6 +15554,517 @@
       <c r="DM56" s="45"/>
       <c r="DN56" s="45"/>
     </row>
+    <row r="57" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>55</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>602</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="AB57" s="37" t="s">
+        <v>594</v>
+      </c>
+      <c r="AD57" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AG57" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH57" s="38" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="58" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>56</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>603</v>
+      </c>
+      <c r="C58" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="L58" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="M58" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="N58" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="O58" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="P58" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="V58" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="W58" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="X58" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y58" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z58" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA58" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB58" s="37" t="s">
+        <v>594</v>
+      </c>
+      <c r="AC58" s="15"/>
+      <c r="AD58" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE58" s="38"/>
+      <c r="AF58" s="15"/>
+      <c r="AG58" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH58" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="AI58" s="15"/>
+      <c r="AJ58" s="15"/>
+      <c r="AK58" s="15"/>
+      <c r="AP58" s="54" t="s">
+        <v>418</v>
+      </c>
+      <c r="AZ58" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA58" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB58" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="BO58" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="BP58" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ58" s="54" t="s">
+        <v>418</v>
+      </c>
+      <c r="BR58" s="45"/>
+      <c r="BS58" s="45"/>
+      <c r="BT58" s="45"/>
+      <c r="BU58" s="45"/>
+      <c r="BV58" s="45"/>
+      <c r="BW58" s="45"/>
+      <c r="BX58" s="45"/>
+      <c r="BY58" s="45"/>
+    </row>
+    <row r="59" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>57</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>604</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="L59" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="M59" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="N59" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="O59" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="P59" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="V59" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="W59" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="X59" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y59" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z59" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA59" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB59" s="37" t="s">
+        <v>594</v>
+      </c>
+      <c r="AD59" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AG59" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH59" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="AI59" s="15"/>
+      <c r="AZ59" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA59" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB59" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="BC59" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="BD59" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="BE59" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="BO59" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="BP59" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ59" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="BR59" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="BS59" s="35" t="s">
+        <v>355</v>
+      </c>
+      <c r="CC59" s="35" t="s">
+        <v>415</v>
+      </c>
+      <c r="CD59" s="45" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="60" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>58</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>606</v>
+      </c>
+      <c r="C60" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="L60" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="M60" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="N60" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="O60" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="P60" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="V60" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="W60" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="X60" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y60" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z60" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA60" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB60" s="40" t="s">
+        <v>417</v>
+      </c>
+      <c r="AD60" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF60" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG60" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="AH60" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="AI60" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ60" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA60" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB60" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="BO60" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="BP60" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ60" s="16" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="61" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="83" t="s">
+        <v>609</v>
+      </c>
+      <c r="F61" s="83" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="62" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="C62" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15" t="s">
+        <v>615</v>
+      </c>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="M62" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="N62" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="O62" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="P62" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q62" s="15"/>
+      <c r="R62" s="15"/>
+      <c r="S62" s="15"/>
+      <c r="T62" s="15"/>
+      <c r="U62" s="15"/>
+      <c r="V62" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="W62" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="X62" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y62" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z62" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA62" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB62" s="54" t="s">
+        <v>410</v>
+      </c>
+      <c r="AC62" s="15"/>
+      <c r="AD62" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE62" s="38"/>
+      <c r="AF62" s="15"/>
+      <c r="AG62" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH62" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="AI62" s="15"/>
+      <c r="AJ62" s="15"/>
+      <c r="AK62" s="15"/>
+      <c r="AL62" s="15"/>
+      <c r="AM62" s="15"/>
+      <c r="AN62" s="15"/>
+      <c r="AO62" s="45"/>
+      <c r="AP62" s="46" t="s">
+        <v>414</v>
+      </c>
+      <c r="AQ62" s="45"/>
+      <c r="AR62" s="45"/>
+      <c r="AS62" s="45"/>
+      <c r="AT62" s="45"/>
+      <c r="AU62" s="45"/>
+      <c r="AV62" s="45"/>
+      <c r="AW62" s="45"/>
+      <c r="AX62" s="45"/>
+      <c r="AY62" s="45"/>
+      <c r="AZ62" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA62" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB62" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="BC62" s="38"/>
+      <c r="BD62" s="38"/>
+      <c r="BE62" s="38"/>
+      <c r="BF62" s="38"/>
+      <c r="BG62" s="38"/>
+      <c r="BH62" s="38"/>
+      <c r="BI62" s="38"/>
+      <c r="BJ62" s="38"/>
+      <c r="BK62" s="38"/>
+      <c r="BL62" s="38"/>
+      <c r="BM62" s="38"/>
+      <c r="BN62" s="38"/>
+      <c r="BO62" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="BP62" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ62" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="BR62" s="45"/>
+      <c r="BS62" s="45"/>
+      <c r="BT62" s="45"/>
+      <c r="BU62" s="45"/>
+      <c r="BV62" s="45"/>
+      <c r="BW62" s="45"/>
+      <c r="BX62" s="45"/>
+      <c r="BY62" s="45"/>
+      <c r="BZ62" s="45"/>
+      <c r="CA62" s="45"/>
+      <c r="CB62" s="45"/>
+      <c r="CC62" s="45"/>
+      <c r="CD62" s="45"/>
+      <c r="CE62" s="45"/>
+      <c r="CF62" s="45"/>
+      <c r="CG62" s="45"/>
+      <c r="CH62" s="45"/>
+      <c r="CI62" s="45"/>
+      <c r="CJ62" s="45"/>
+      <c r="CK62" s="45"/>
+      <c r="CL62" s="45"/>
+      <c r="CM62" s="45"/>
+      <c r="CN62" s="45"/>
+      <c r="CO62" s="45"/>
+      <c r="CP62" s="45"/>
+      <c r="CQ62" s="45"/>
+      <c r="CR62" s="45"/>
+      <c r="CS62" s="45"/>
+      <c r="CT62" s="45"/>
+      <c r="CU62" s="45"/>
+      <c r="CV62" s="45"/>
+      <c r="CW62" s="45"/>
+      <c r="CX62" s="45"/>
+      <c r="CY62" s="45"/>
+      <c r="CZ62" s="45"/>
+      <c r="DA62" s="45"/>
+      <c r="DB62" s="45"/>
+      <c r="DC62" s="45"/>
+      <c r="DD62" s="45"/>
+      <c r="DE62" s="45"/>
+      <c r="DF62" s="45"/>
+      <c r="DG62" s="45"/>
+      <c r="DH62" s="45"/>
+      <c r="DI62" s="45"/>
+      <c r="DJ62" s="45"/>
+      <c r="DK62" s="45"/>
+      <c r="DL62" s="45"/>
+      <c r="DM62" s="45"/>
+      <c r="DN62" s="45"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -15412,60 +16097,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="114" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="82.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="34.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="29" width="29" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="38" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="114.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="82.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="28" max="29" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="37" max="38" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:57" x14ac:dyDescent="0.25">
@@ -15479,7 +16164,7 @@
         <v>285</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="E1" s="32" t="s">
         <v>286</v>
@@ -15551,10 +16236,10 @@
         <v>76</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>462</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>77</v>
@@ -15728,7 +16413,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>322</v>
@@ -15814,7 +16499,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>322</v>
@@ -15902,7 +16587,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C5" s="33" t="s">
         <v>323</v>
@@ -16384,12 +17069,12 @@
         <v>114</v>
       </c>
       <c r="V10" s="73" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="W10" s="72"/>
       <c r="X10" s="72"/>
       <c r="Y10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="Z10" s="14"/>
       <c r="AA10" s="14"/>
@@ -16466,12 +17151,12 @@
         <v>114</v>
       </c>
       <c r="V11" s="73" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="W11" s="73"/>
       <c r="X11" s="73"/>
       <c r="Y11" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="Z11" s="14"/>
       <c r="AA11" s="14"/>
@@ -16847,7 +17532,7 @@
         <v>96</v>
       </c>
       <c r="AE15" s="25" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="AF15" s="25"/>
       <c r="AG15" s="25"/>
@@ -16957,7 +17642,7 @@
         <v>267</v>
       </c>
       <c r="O16" s="48" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="P16" s="51" t="s">
         <v>267</v>
@@ -17043,7 +17728,7 @@
       </c>
       <c r="J17" s="14"/>
       <c r="K17" s="14" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L17" s="35" t="s">
         <v>240</v>
@@ -17116,7 +17801,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C18" s="33" t="s">
         <v>322</v>
@@ -17131,10 +17816,10 @@
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="L18" s="51" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="M18" s="14"/>
       <c r="N18" s="63"/>
@@ -17145,7 +17830,7 @@
       <c r="S18" s="62"/>
       <c r="T18" s="14"/>
       <c r="U18" s="48" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="V18" s="14"/>
       <c r="W18" s="14"/>
@@ -17153,25 +17838,25 @@
       <c r="Y18" s="14"/>
       <c r="Z18" s="14"/>
       <c r="AA18" s="14" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="AB18" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="AC18" s="14" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AD18" s="14"/>
       <c r="AE18" s="14"/>
       <c r="AF18" s="35" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="AG18" s="14"/>
       <c r="AH18" s="69" t="s">
         <v>236</v>
       </c>
       <c r="AI18" s="51" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AJ18" s="69" t="s">
         <v>260</v>
@@ -17202,7 +17887,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C19" s="33" t="s">
         <v>322</v>
@@ -17221,7 +17906,7 @@
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="L19" s="35" t="s">
         <v>111</v>
@@ -17235,7 +17920,7 @@
       <c r="S19" s="62"/>
       <c r="T19" s="14"/>
       <c r="U19" s="48" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="V19" s="14"/>
       <c r="W19" s="14"/>
@@ -17243,16 +17928,16 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
       <c r="AA19" s="14" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="AB19" s="14" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AC19" s="14"/>
       <c r="AD19" s="14"/>
       <c r="AE19" s="14"/>
       <c r="AF19" s="35" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="AG19" s="69" t="s">
         <v>235</v>
@@ -17292,7 +17977,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C20" s="33" t="s">
         <v>322</v>
@@ -17311,10 +17996,10 @@
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
       <c r="K20" s="14" t="s">
+        <v>469</v>
+      </c>
+      <c r="L20" s="35" t="s">
         <v>470</v>
-      </c>
-      <c r="L20" s="35" t="s">
-        <v>471</v>
       </c>
       <c r="M20" s="14"/>
       <c r="N20" s="63"/>
@@ -17325,7 +18010,7 @@
       <c r="S20" s="62"/>
       <c r="T20" s="14"/>
       <c r="U20" s="48" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="V20" s="14"/>
       <c r="W20" s="14"/>
@@ -17333,16 +18018,16 @@
       <c r="Y20" s="14"/>
       <c r="Z20" s="14"/>
       <c r="AA20" s="14" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="AB20" s="14" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="AC20" s="14"/>
       <c r="AD20" s="14"/>
       <c r="AE20" s="14"/>
       <c r="AF20" s="35" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="AG20" s="69" t="s">
         <v>235</v>
@@ -17351,7 +18036,7 @@
         <v>236</v>
       </c>
       <c r="AI20" s="35" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="AJ20" s="69" t="s">
         <v>260</v>
@@ -17382,7 +18067,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C21" s="33" t="s">
         <v>323</v>
@@ -17403,7 +18088,7 @@
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="70" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L21" s="51" t="s">
         <v>84</v>
@@ -17472,7 +18157,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C22" s="33" t="s">
         <v>322</v>
@@ -17495,7 +18180,7 @@
         <v>116</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L22" s="35" t="s">
         <v>240</v>
@@ -17507,7 +18192,7 @@
         <v>267</v>
       </c>
       <c r="O22" s="48" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P22" s="51" t="s">
         <v>267</v>
@@ -17568,7 +18253,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C23" s="33" t="s">
         <v>322</v>
@@ -17591,7 +18276,7 @@
         <v>116</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L23" s="14"/>
       <c r="M23" s="14"/>
@@ -17648,7 +18333,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C24" s="33" t="s">
         <v>322</v>
@@ -17671,7 +18356,7 @@
         <v>116</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="L24" s="51" t="s">
         <v>240</v>
@@ -17683,7 +18368,7 @@
         <v>267</v>
       </c>
       <c r="O24" s="48" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P24" s="51" t="s">
         <v>267</v>
@@ -17782,26 +18467,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="108" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="65.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="73.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="108.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="65.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="73.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -17884,7 +18569,7 @@
         <v>224</v>
       </c>
       <c r="H2" s="74" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I2" s="24"/>
       <c r="J2" s="16" t="s">
@@ -17935,10 +18620,10 @@
         <v>220</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H3" s="74" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I3" s="24"/>
       <c r="J3" s="16" t="s">
@@ -17951,7 +18636,7 @@
         <v>231</v>
       </c>
       <c r="M3" s="75" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N3" s="24" t="s">
         <v>25</v>
@@ -17963,7 +18648,7 @@
       <c r="Q3" s="24"/>
       <c r="R3" s="24"/>
       <c r="S3" s="75" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="T3" s="12"/>
       <c r="U3" s="9"/>
@@ -17997,10 +18682,10 @@
         <v>220</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H4" s="74" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I4" s="24"/>
       <c r="J4" s="16" t="s">
@@ -18013,7 +18698,7 @@
         <v>231</v>
       </c>
       <c r="M4" s="75" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N4" s="24" t="s">
         <v>25</v>
@@ -18053,16 +18738,16 @@
         <v>0</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>220</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I5" s="24"/>
       <c r="J5" s="16" t="s">
@@ -18113,10 +18798,10 @@
         <v>220</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H6" s="74" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I6" s="24"/>
       <c r="J6" s="16" t="s">
@@ -18163,7 +18848,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
@@ -18209,7 +18894,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F8" s="24"/>
       <c r="G8" s="24"/>
@@ -18259,10 +18944,10 @@
         <v>220</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H9" s="74" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I9" s="24"/>
       <c r="J9" s="16" t="s">
@@ -18317,13 +19002,13 @@
         <v>220</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H10" s="74" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I10" s="74" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J10" s="16" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Committing new Member Test cases
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\Dynamics-CRM-Cloud\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266414F1-5DE8-4108-A3E7-10989D460945}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E823294F-4680-426B-B715-4955C62A1294}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" activeTab="2" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Contact" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Driver!$A$1:$K$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Driver!$A$1:$K$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3634" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3452" uniqueCount="649">
   <si>
     <t>Premier1a</t>
   </si>
@@ -1788,15 +1788,9 @@
     <t>2000511078</t>
   </si>
   <si>
-    <t>2000511079</t>
-  </si>
-  <si>
     <t>2000511080</t>
   </si>
   <si>
-    <t>2000511082</t>
-  </si>
-  <si>
     <t>2000511083</t>
   </si>
   <si>
@@ -1818,9 +1812,6 @@
     <t>7000567447</t>
   </si>
   <si>
-    <t>7000567450</t>
-  </si>
-  <si>
     <t>North Oaks Health System</t>
   </si>
   <si>
@@ -1839,9 +1830,6 @@
     <t>2000511325</t>
   </si>
   <si>
-    <t>2000511727</t>
-  </si>
-  <si>
     <t>8816_TerminatedAccountStatus</t>
   </si>
   <si>
@@ -1878,37 +1866,127 @@
     <t>You cannot publish the GPO Member since Direct Parent is NonGPO Member</t>
   </si>
   <si>
-    <t>2000511792</t>
-  </si>
-  <si>
-    <t>2000511799</t>
-  </si>
-  <si>
     <t>TFS ID_8789:Cloud -Verify AG calculated correctly after prospect become a member</t>
   </si>
   <si>
     <t>8789_AG and AG effective date on Account creation as Prospects</t>
   </si>
   <si>
+    <t>TFS ID_8790:Cloud - Verify FBO calculated correctly after prospect become a member</t>
+  </si>
+  <si>
+    <t>2000511811</t>
+  </si>
+  <si>
+    <t>2000511812</t>
+  </si>
+  <si>
+    <t>8790_VerifyFBOCreated</t>
+  </si>
+  <si>
+    <t>TFS ID_4505:Verify TP can be created without providing DP relation date - Manual</t>
+  </si>
+  <si>
+    <t>TFS ID_8781:Cloud : Verify CP, FSP, FBORD, AG dates are recalculated when reactivating an account</t>
+  </si>
+  <si>
+    <t>8781_Chk_Terminated_member</t>
+  </si>
+  <si>
+    <t>North Oaks NonAcute</t>
+  </si>
+  <si>
+    <t>TFS ID_9287:Cloud-Member Accounts with Entity code should not be able to Deactivate</t>
+  </si>
+  <si>
+    <t>9287_CreateMemberDeactivate</t>
+  </si>
+  <si>
+    <t>TFS ID_8803:Cloud : Verify whether child Account cannot be published if DP does not have entity code</t>
+  </si>
+  <si>
+    <t>8803_VerifyChildofDraftAccount</t>
+  </si>
+  <si>
+    <t>2000511850</t>
+  </si>
+  <si>
+    <t>TFS ID_8794:Cloud - Verify TP exception reason should not be mandatory when creating new member with DP is same as TP</t>
+  </si>
+  <si>
+    <t>8794_Member</t>
+  </si>
+  <si>
+    <t>TFS ID_8820:Cloud: Verify a non gpo account can be created under a GPO member</t>
+  </si>
+  <si>
+    <t>8820_VerifyNonGPOUnderGPO</t>
+  </si>
+  <si>
+    <t>TFS ID_8821:Cloud: Verify member can not be terminated if its child account is active</t>
+  </si>
+  <si>
+    <t>608827</t>
+  </si>
+  <si>
+    <t>2000511878</t>
+  </si>
+  <si>
+    <t>2000511879</t>
+  </si>
+  <si>
+    <t>2000511881</t>
+  </si>
+  <si>
+    <t>2000511882</t>
+  </si>
+  <si>
+    <t>2000511884</t>
+  </si>
+  <si>
+    <t>2000511886</t>
+  </si>
+  <si>
+    <t>2000511888</t>
+  </si>
+  <si>
+    <t>2000511889</t>
+  </si>
+  <si>
+    <t>TFS ID_8785:Cloud - Validate Active Member requires one active LOB</t>
+  </si>
+  <si>
+    <t>7000567873</t>
+  </si>
+  <si>
+    <t>8785_CreateMemberWithoutLOB</t>
+  </si>
+  <si>
     <t>Failed</t>
   </si>
   <si>
-    <t>2022_02_02_09_51_17</t>
-  </si>
-  <si>
-    <t>2022_02_02_10_08_28</t>
-  </si>
-  <si>
-    <t>2022_02_02_10_31_23</t>
-  </si>
-  <si>
-    <t>2022_02_02_12_30_41</t>
+    <t>LOB is required for the below Premier Membership</t>
+  </si>
+  <si>
+    <t>TFS ID_9642:Cloud : Verify whether "Save &amp; New Button" is not displayed in the form</t>
+  </si>
+  <si>
+    <t>2000511907</t>
+  </si>
+  <si>
+    <t>2022_02_16_01_32_12</t>
+  </si>
+  <si>
+    <t>LOB is required for the below Premier Membership Provider</t>
+  </si>
+  <si>
+    <t>2000511908</t>
   </si>
   <si>
     <t>PASSED</t>
   </si>
   <si>
-    <t>2022_02_02_12_45_50</t>
+    <t>2022_02_16_01_52_12</t>
   </si>
 </sst>
 </file>
@@ -2163,7 +2241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2304,6 +2382,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2625,10 +2705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
-  <dimension ref="A1:P94"/>
+  <dimension ref="A1:P104"/>
   <sheetViews>
-    <sheetView topLeftCell="C52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView topLeftCell="C65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2703,7 +2783,7 @@
         <v>266</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
@@ -2737,7 +2817,7 @@
         <v>266</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>599</v>
+        <v>622</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
@@ -2769,7 +2849,7 @@
         <v>266</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
@@ -2798,7 +2878,7 @@
         <v>266</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -4225,7 +4305,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C57" s="18" t="s">
         <v>35</v>
@@ -4252,7 +4332,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C58" s="18" t="s">
         <v>35</v>
@@ -4281,7 +4361,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C59" s="18" t="s">
         <v>35</v>
@@ -4299,7 +4379,7 @@
         <v>266</v>
       </c>
       <c r="H59" s="25" t="s">
-        <v>612</v>
+        <v>629</v>
       </c>
       <c r="I59" s="25"/>
       <c r="J59" s="25"/>
@@ -4310,7 +4390,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C60" s="18" t="s">
         <v>35</v>
@@ -4328,7 +4408,7 @@
         <v>266</v>
       </c>
       <c r="H60" s="25" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
       <c r="I60" s="25"/>
       <c r="J60" s="25"/>
@@ -4339,7 +4419,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C61" s="18" t="s">
         <v>35</v>
@@ -4366,10 +4446,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>2</v>
@@ -4378,10 +4458,10 @@
         <v>40</v>
       </c>
       <c r="F62" s="25" t="s">
-        <v>621</v>
+        <v>265</v>
       </c>
       <c r="G62" s="25" t="s">
-        <v>622</v>
+        <v>266</v>
       </c>
       <c r="H62" s="25"/>
       <c r="I62" s="25"/>
@@ -4390,298 +4470,294 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
-        <v>57</v>
-      </c>
-      <c r="B63" s="22" t="s">
-        <v>29</v>
+        <v>61</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>610</v>
       </c>
       <c r="C63" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D63" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E63" s="22" t="s">
+      <c r="D63" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F63" s="22" t="s">
+      <c r="F63" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G63" s="22" t="s">
+      <c r="G63" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H63" s="22" t="s">
-        <v>578</v>
-      </c>
-      <c r="I63" s="22"/>
-      <c r="J63" s="22"/>
-      <c r="K63" s="23"/>
+      <c r="H63" s="25" t="s">
+        <v>631</v>
+      </c>
+      <c r="I63" s="25"/>
+      <c r="J63" s="25"/>
+      <c r="K63" s="25"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>58</v>
-      </c>
-      <c r="B64" s="22" t="s">
-        <v>467</v>
+        <v>62</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>614</v>
       </c>
       <c r="C64" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D64" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E64" s="22" t="s">
+      <c r="D64" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E64" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F64" s="22" t="s">
+      <c r="F64" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G64" s="22" t="s">
+      <c r="G64" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H64" s="22" t="s">
-        <v>579</v>
-      </c>
-      <c r="I64" s="22"/>
-      <c r="J64" s="22"/>
-      <c r="K64" s="23"/>
+      <c r="H64" s="25" t="s">
+        <v>632</v>
+      </c>
+      <c r="I64" s="25"/>
+      <c r="J64" s="25"/>
+      <c r="K64" s="25"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
-        <v>59</v>
-      </c>
-      <c r="B65" s="22" t="s">
-        <v>471</v>
+        <v>63</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>615</v>
       </c>
       <c r="C65" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D65" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E65" s="22" t="s">
+      <c r="D65" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E65" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F65" s="22" t="s">
+      <c r="F65" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G65" s="22" t="s">
+      <c r="G65" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H65" s="22" t="s">
-        <v>580</v>
-      </c>
-      <c r="I65" s="22"/>
-      <c r="J65" s="22"/>
-      <c r="K65" s="23"/>
+      <c r="H65" s="25"/>
+      <c r="I65" s="25"/>
+      <c r="J65" s="25"/>
+      <c r="K65" s="25"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
-        <v>60</v>
-      </c>
-      <c r="B66" s="22" t="s">
-        <v>454</v>
+        <v>64</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>618</v>
       </c>
       <c r="C66" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D66" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E66" s="22" t="s">
+      <c r="D66" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F66" s="22" t="s">
+      <c r="F66" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G66" s="22" t="s">
+      <c r="G66" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H66" s="22"/>
-      <c r="I66" s="22"/>
-      <c r="J66" s="22"/>
-      <c r="K66" s="23"/>
+      <c r="H66" s="25" t="s">
+        <v>633</v>
+      </c>
+      <c r="I66" s="25"/>
+      <c r="J66" s="25"/>
+      <c r="K66" s="25"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
-        <v>61</v>
-      </c>
-      <c r="B67" s="22" t="s">
-        <v>92</v>
+        <v>65</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>620</v>
       </c>
       <c r="C67" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D67" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E67" s="22" t="s">
+      <c r="D67" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F67" s="22" t="s">
+      <c r="F67" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G67" s="22" t="s">
+      <c r="G67" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H67" s="22" t="s">
-        <v>581</v>
-      </c>
-      <c r="I67" s="22"/>
-      <c r="J67" s="22"/>
-      <c r="K67" s="23"/>
+      <c r="H67" s="25" t="s">
+        <v>634</v>
+      </c>
+      <c r="I67" s="25"/>
+      <c r="J67" s="25"/>
+      <c r="K67" s="25"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
-        <v>62</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>97</v>
+        <v>66</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>623</v>
       </c>
       <c r="C68" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D68" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E68" s="22" t="s">
+      <c r="D68" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F68" s="22" t="s">
+      <c r="F68" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G68" s="22" t="s">
+      <c r="G68" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H68" s="22" t="s">
-        <v>582</v>
-      </c>
-      <c r="I68" s="22"/>
-      <c r="J68" s="22"/>
-      <c r="K68" s="23"/>
+      <c r="H68" s="25" t="s">
+        <v>635</v>
+      </c>
+      <c r="I68" s="25"/>
+      <c r="J68" s="25"/>
+      <c r="K68" s="25"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
-        <v>63</v>
-      </c>
-      <c r="B69" s="22" t="s">
-        <v>101</v>
+        <v>67</v>
+      </c>
+      <c r="B69" s="25" t="s">
+        <v>625</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D69" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E69" s="22" t="s">
+      <c r="D69" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E69" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F69" s="22" t="s">
+      <c r="F69" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G69" s="22" t="s">
+      <c r="G69" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H69" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="I69" s="22"/>
-      <c r="J69" s="22"/>
-      <c r="K69" s="23"/>
+      <c r="H69" s="25" t="s">
+        <v>636</v>
+      </c>
+      <c r="I69" s="25"/>
+      <c r="J69" s="25"/>
+      <c r="K69" s="25"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
-        <v>64</v>
-      </c>
-      <c r="B70" s="22" t="s">
-        <v>106</v>
+        <v>68</v>
+      </c>
+      <c r="B70" s="25" t="s">
+        <v>627</v>
       </c>
       <c r="C70" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D70" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E70" s="22" t="s">
+      <c r="D70" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F70" s="22" t="s">
+      <c r="F70" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G70" s="22" t="s">
+      <c r="G70" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H70" s="22" t="s">
-        <v>583</v>
-      </c>
-      <c r="I70" s="22"/>
-      <c r="J70" s="22"/>
-      <c r="K70" s="23"/>
+      <c r="H70" s="25"/>
+      <c r="I70" s="25"/>
+      <c r="J70" s="25"/>
+      <c r="K70" s="25"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
-        <v>65</v>
-      </c>
-      <c r="B71" s="22" t="s">
-        <v>109</v>
+        <v>69</v>
+      </c>
+      <c r="B71" s="25" t="s">
+        <v>637</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D71" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E71" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F71" s="22" t="s">
-        <v>265</v>
-      </c>
-      <c r="G71" s="22" t="s">
-        <v>266</v>
-      </c>
-      <c r="H71" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="I71" s="22"/>
-      <c r="J71" s="22"/>
-      <c r="K71" s="23"/>
+      <c r="F71" s="25" t="s">
+        <v>647</v>
+      </c>
+      <c r="G71" s="25" t="s">
+        <v>648</v>
+      </c>
+      <c r="H71" s="25" t="s">
+        <v>646</v>
+      </c>
+      <c r="I71" s="25"/>
+      <c r="J71" s="25"/>
+      <c r="K71" s="25"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
-        <v>66</v>
-      </c>
-      <c r="B72" s="22" t="s">
-        <v>112</v>
+        <v>70</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>642</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D72" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E72" s="22" t="s">
+      <c r="D72" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E72" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F72" s="22" t="s">
+      <c r="F72" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="G72" s="22" t="s">
+      <c r="G72" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H72" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="I72" s="22"/>
-      <c r="J72" s="22"/>
-      <c r="K72" s="23"/>
+      <c r="H72" s="25"/>
+      <c r="I72" s="25"/>
+      <c r="J72" s="25"/>
+      <c r="K72" s="25"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="C73" s="18" t="s">
         <v>35</v>
@@ -4699,7 +4775,7 @@
         <v>266</v>
       </c>
       <c r="H73" s="22" t="s">
-        <v>119</v>
+        <v>578</v>
       </c>
       <c r="I73" s="22"/>
       <c r="J73" s="22"/>
@@ -4707,10 +4783,10 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>122</v>
+        <v>467</v>
       </c>
       <c r="C74" s="18" t="s">
         <v>35</v>
@@ -4728,7 +4804,7 @@
         <v>266</v>
       </c>
       <c r="H74" s="22" t="s">
-        <v>539</v>
+        <v>579</v>
       </c>
       <c r="I74" s="22"/>
       <c r="J74" s="22"/>
@@ -4736,10 +4812,10 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>129</v>
+        <v>471</v>
       </c>
       <c r="C75" s="18" t="s">
         <v>35</v>
@@ -4757,7 +4833,7 @@
         <v>266</v>
       </c>
       <c r="H75" s="22" t="s">
-        <v>131</v>
+        <v>580</v>
       </c>
       <c r="I75" s="22"/>
       <c r="J75" s="22"/>
@@ -4765,10 +4841,10 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>257</v>
+        <v>454</v>
       </c>
       <c r="C76" s="18" t="s">
         <v>35</v>
@@ -4790,12 +4866,12 @@
       <c r="J76" s="22"/>
       <c r="K76" s="23"/>
     </row>
-    <row r="77" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B77" s="22" t="s">
-        <v>186</v>
+        <v>92</v>
       </c>
       <c r="C77" s="18" t="s">
         <v>35</v>
@@ -4813,18 +4889,18 @@
         <v>266</v>
       </c>
       <c r="H77" s="22" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="I77" s="22"/>
       <c r="J77" s="22"/>
       <c r="K77" s="23"/>
     </row>
-    <row r="78" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
-        <v>72</v>
-      </c>
-      <c r="B78" s="82" t="s">
-        <v>419</v>
+        <v>76</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="C78" s="18" t="s">
         <v>35</v>
@@ -4842,7 +4918,7 @@
         <v>266</v>
       </c>
       <c r="H78" s="22" t="s">
-        <v>585</v>
+        <v>612</v>
       </c>
       <c r="I78" s="22"/>
       <c r="J78" s="22"/>
@@ -4850,10 +4926,10 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B79" s="22" t="s">
-        <v>456</v>
+        <v>101</v>
       </c>
       <c r="C79" s="18" t="s">
         <v>35</v>
@@ -4867,20 +4943,22 @@
       <c r="F79" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G79" s="25" t="s">
+      <c r="G79" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H79" s="25"/>
-      <c r="I79" s="25"/>
-      <c r="J79" s="25"/>
-      <c r="K79" s="25"/>
+      <c r="H79" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="I79" s="22"/>
+      <c r="J79" s="22"/>
+      <c r="K79" s="23"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B80" s="22" t="s">
-        <v>463</v>
+        <v>106</v>
       </c>
       <c r="C80" s="18" t="s">
         <v>35</v>
@@ -4894,20 +4972,22 @@
       <c r="F80" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G80" s="25" t="s">
+      <c r="G80" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H80" s="25"/>
-      <c r="I80" s="25"/>
-      <c r="J80" s="25"/>
-      <c r="K80" s="25"/>
+      <c r="H80" s="22" t="s">
+        <v>582</v>
+      </c>
+      <c r="I80" s="22"/>
+      <c r="J80" s="22"/>
+      <c r="K80" s="23"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B81" s="22" t="s">
-        <v>468</v>
+        <v>109</v>
       </c>
       <c r="C81" s="18" t="s">
         <v>35</v>
@@ -4921,20 +5001,22 @@
       <c r="F81" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G81" s="25" t="s">
+      <c r="G81" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H81" s="25"/>
-      <c r="I81" s="25"/>
-      <c r="J81" s="25"/>
-      <c r="K81" s="25"/>
+      <c r="H81" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="I81" s="22"/>
+      <c r="J81" s="22"/>
+      <c r="K81" s="23"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>473</v>
+        <v>112</v>
       </c>
       <c r="C82" s="18" t="s">
         <v>35</v>
@@ -4948,20 +5030,22 @@
       <c r="F82" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G82" s="25" t="s">
+      <c r="G82" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H82" s="25"/>
-      <c r="I82" s="25"/>
-      <c r="J82" s="25"/>
-      <c r="K82" s="25"/>
+      <c r="H82" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="I82" s="22"/>
+      <c r="J82" s="22"/>
+      <c r="K82" s="23"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>476</v>
+        <v>115</v>
       </c>
       <c r="C83" s="18" t="s">
         <v>35</v>
@@ -4975,20 +5059,22 @@
       <c r="F83" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G83" s="25" t="s">
+      <c r="G83" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H83" s="25"/>
-      <c r="I83" s="25"/>
-      <c r="J83" s="25"/>
-      <c r="K83" s="25"/>
+      <c r="H83" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="I83" s="22"/>
+      <c r="J83" s="22"/>
+      <c r="K83" s="23"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B84" s="22" t="s">
-        <v>479</v>
+        <v>122</v>
       </c>
       <c r="C84" s="18" t="s">
         <v>35</v>
@@ -5002,20 +5088,22 @@
       <c r="F84" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G84" s="25" t="s">
+      <c r="G84" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H84" s="25"/>
-      <c r="I84" s="25"/>
-      <c r="J84" s="25"/>
-      <c r="K84" s="25"/>
+      <c r="H84" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="I84" s="22"/>
+      <c r="J84" s="22"/>
+      <c r="K84" s="23"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>474</v>
+        <v>129</v>
       </c>
       <c r="C85" s="18" t="s">
         <v>35</v>
@@ -5029,274 +5117,550 @@
       <c r="F85" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G85" s="25" t="s">
+      <c r="G85" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H85" s="25"/>
-      <c r="I85" s="25"/>
-      <c r="J85" s="25"/>
-      <c r="K85" s="25"/>
+      <c r="H85" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="I85" s="22"/>
+      <c r="J85" s="22"/>
+      <c r="K85" s="23"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
-        <v>80</v>
-      </c>
-      <c r="B86" s="30" t="s">
-        <v>221</v>
+        <v>84</v>
+      </c>
+      <c r="B86" s="22" t="s">
+        <v>257</v>
       </c>
       <c r="C86" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D86" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="E86" s="31" t="s">
+      <c r="D86" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E86" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F86" s="31" t="s">
+      <c r="F86" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G86" s="28" t="s">
+      <c r="G86" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H86" s="28" t="s">
-        <v>592</v>
-      </c>
-      <c r="I86" s="28"/>
-      <c r="J86" s="28"/>
-      <c r="K86" s="28"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H86" s="22"/>
+      <c r="I86" s="22"/>
+      <c r="J86" s="22"/>
+      <c r="K86" s="23"/>
+    </row>
+    <row r="87" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
-        <v>81</v>
-      </c>
-      <c r="B87" s="30" t="s">
-        <v>421</v>
+        <v>85</v>
+      </c>
+      <c r="B87" s="22" t="s">
+        <v>186</v>
       </c>
       <c r="C87" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D87" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="E87" s="31" t="s">
+      <c r="D87" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E87" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F87" s="31" t="s">
+      <c r="F87" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G87" s="28" t="s">
+      <c r="G87" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H87" s="28" t="s">
-        <v>586</v>
-      </c>
-      <c r="I87" s="28"/>
-      <c r="J87" s="28"/>
-      <c r="K87" s="28"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H87" s="22" t="s">
+        <v>611</v>
+      </c>
+      <c r="I87" s="22"/>
+      <c r="J87" s="22"/>
+      <c r="K87" s="23"/>
+    </row>
+    <row r="88" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
-        <v>82</v>
-      </c>
-      <c r="B88" s="30" t="s">
-        <v>422</v>
+        <v>86</v>
+      </c>
+      <c r="B88" s="82" t="s">
+        <v>419</v>
       </c>
       <c r="C88" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D88" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="E88" s="31" t="s">
+      <c r="D88" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E88" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F88" s="31" t="s">
+      <c r="F88" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G88" s="28" t="s">
+      <c r="G88" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="H88" s="28" t="s">
-        <v>587</v>
-      </c>
-      <c r="I88" s="28"/>
-      <c r="J88" s="28"/>
-      <c r="K88" s="28"/>
+      <c r="H88" s="22" t="s">
+        <v>583</v>
+      </c>
+      <c r="I88" s="22"/>
+      <c r="J88" s="22"/>
+      <c r="K88" s="23"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
-        <v>83</v>
-      </c>
-      <c r="B89" s="30" t="s">
-        <v>423</v>
+        <v>87</v>
+      </c>
+      <c r="B89" s="22" t="s">
+        <v>456</v>
       </c>
       <c r="C89" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D89" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="E89" s="31" t="s">
+      <c r="D89" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E89" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F89" s="30" t="s">
+      <c r="F89" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G89" s="29" t="s">
+      <c r="G89" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H89" s="29" t="s">
-        <v>588</v>
-      </c>
-      <c r="I89" s="29"/>
-      <c r="J89" s="29"/>
-      <c r="K89" s="29"/>
+      <c r="H89" s="25"/>
+      <c r="I89" s="25"/>
+      <c r="J89" s="25"/>
+      <c r="K89" s="25"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
-        <v>84</v>
-      </c>
-      <c r="B90" s="30" t="s">
-        <v>424</v>
+        <v>88</v>
+      </c>
+      <c r="B90" s="22" t="s">
+        <v>463</v>
       </c>
       <c r="C90" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D90" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="E90" s="31" t="s">
+      <c r="D90" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E90" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F90" s="30" t="s">
+      <c r="F90" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G90" s="29" t="s">
+      <c r="G90" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H90" s="29" t="s">
-        <v>589</v>
-      </c>
-      <c r="I90" s="29"/>
-      <c r="J90" s="29"/>
-      <c r="K90" s="29"/>
+      <c r="H90" s="25"/>
+      <c r="I90" s="25"/>
+      <c r="J90" s="25"/>
+      <c r="K90" s="25"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
-        <v>85</v>
-      </c>
-      <c r="B91" s="30" t="s">
-        <v>420</v>
+        <v>89</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>468</v>
       </c>
       <c r="C91" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D91" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="E91" s="31" t="s">
+      <c r="D91" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E91" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F91" s="30" t="s">
+      <c r="F91" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G91" s="29" t="s">
+      <c r="G91" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H91" s="29"/>
-      <c r="I91" s="29"/>
-      <c r="J91" s="29"/>
-      <c r="K91" s="29"/>
+      <c r="H91" s="25"/>
+      <c r="I91" s="25"/>
+      <c r="J91" s="25"/>
+      <c r="K91" s="25"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
-        <v>86</v>
-      </c>
-      <c r="B92" s="30" t="s">
-        <v>425</v>
+        <v>90</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>473</v>
       </c>
       <c r="C92" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D92" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="E92" s="31" t="s">
+      <c r="D92" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E92" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F92" s="30" t="s">
+      <c r="F92" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G92" s="29" t="s">
+      <c r="G92" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H92" s="29"/>
-      <c r="I92" s="29"/>
-      <c r="J92" s="29"/>
-      <c r="K92" s="29"/>
+      <c r="H92" s="25"/>
+      <c r="I92" s="25"/>
+      <c r="J92" s="25"/>
+      <c r="K92" s="25"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
-        <v>87</v>
-      </c>
-      <c r="B93" s="30" t="s">
-        <v>426</v>
+        <v>91</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>476</v>
       </c>
       <c r="C93" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D93" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="E93" s="31" t="s">
+      <c r="D93" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E93" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F93" s="30" t="s">
+      <c r="F93" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="G93" s="29" t="s">
+      <c r="G93" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="H93" s="29" t="s">
-        <v>590</v>
-      </c>
-      <c r="I93" s="29"/>
-      <c r="J93" s="29"/>
-      <c r="K93" s="29"/>
+      <c r="H93" s="25"/>
+      <c r="I93" s="25"/>
+      <c r="J93" s="25"/>
+      <c r="K93" s="25"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
-        <v>88</v>
-      </c>
-      <c r="B94" s="31" t="s">
-        <v>427</v>
+        <v>92</v>
+      </c>
+      <c r="B94" s="22" t="s">
+        <v>479</v>
       </c>
       <c r="C94" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D94" s="30" t="s">
+      <c r="D94" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E94" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F94" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="G94" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="H94" s="25"/>
+      <c r="I94" s="25"/>
+      <c r="J94" s="25"/>
+      <c r="K94" s="25"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="7">
+        <v>93</v>
+      </c>
+      <c r="B95" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D95" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E95" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F95" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="G95" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="H95" s="25"/>
+      <c r="I95" s="25"/>
+      <c r="J95" s="25"/>
+      <c r="K95" s="25"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="7">
+        <v>94</v>
+      </c>
+      <c r="B96" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D96" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="E94" s="31" t="s">
+      <c r="E96" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="F94" s="30" t="s">
+      <c r="F96" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="G94" s="29" t="s">
+      <c r="G96" s="28" t="s">
         <v>266</v>
       </c>
-      <c r="H94" s="29" t="s">
-        <v>591</v>
-      </c>
-      <c r="I94" s="29"/>
-      <c r="J94" s="29"/>
-      <c r="K94" s="29"/>
+      <c r="H96" s="28" t="s">
+        <v>638</v>
+      </c>
+      <c r="I96" s="28"/>
+      <c r="J96" s="28"/>
+      <c r="K96" s="28"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="7">
+        <v>95</v>
+      </c>
+      <c r="B97" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D97" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="E97" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F97" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="G97" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="H97" s="28" t="s">
+        <v>584</v>
+      </c>
+      <c r="I97" s="28"/>
+      <c r="J97" s="28"/>
+      <c r="K97" s="28"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
+        <v>96</v>
+      </c>
+      <c r="B98" s="30" t="s">
+        <v>422</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D98" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="E98" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F98" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="G98" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="H98" s="28" t="s">
+        <v>585</v>
+      </c>
+      <c r="I98" s="28"/>
+      <c r="J98" s="28"/>
+      <c r="K98" s="28"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="7">
+        <v>97</v>
+      </c>
+      <c r="B99" s="30" t="s">
+        <v>423</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E99" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F99" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G99" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H99" s="29" t="s">
+        <v>586</v>
+      </c>
+      <c r="I99" s="29"/>
+      <c r="J99" s="29"/>
+      <c r="K99" s="29"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="7">
+        <v>98</v>
+      </c>
+      <c r="B100" s="30" t="s">
+        <v>424</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D100" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E100" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F100" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G100" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H100" s="29" t="s">
+        <v>587</v>
+      </c>
+      <c r="I100" s="29"/>
+      <c r="J100" s="29"/>
+      <c r="K100" s="29"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="7">
+        <v>99</v>
+      </c>
+      <c r="B101" s="30" t="s">
+        <v>420</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D101" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E101" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F101" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G101" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H101" s="29"/>
+      <c r="I101" s="29"/>
+      <c r="J101" s="29"/>
+      <c r="K101" s="29"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="7">
+        <v>100</v>
+      </c>
+      <c r="B102" s="30" t="s">
+        <v>425</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D102" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E102" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F102" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G102" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H102" s="29"/>
+      <c r="I102" s="29"/>
+      <c r="J102" s="29"/>
+      <c r="K102" s="29"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="7">
+        <v>101</v>
+      </c>
+      <c r="B103" s="30" t="s">
+        <v>426</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D103" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E103" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F103" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G103" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H103" s="29" t="s">
+        <v>588</v>
+      </c>
+      <c r="I103" s="29"/>
+      <c r="J103" s="29"/>
+      <c r="K103" s="29"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="7">
+        <v>102</v>
+      </c>
+      <c r="B104" s="31" t="s">
+        <v>427</v>
+      </c>
+      <c r="C104" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D104" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E104" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F104" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G104" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H104" s="29" t="s">
+        <v>589</v>
+      </c>
+      <c r="I104" s="29"/>
+      <c r="J104" s="29"/>
+      <c r="K104" s="29"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C94" xr:uid="{C9334235-52FB-4F10-8331-5687DC05318C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C104" xr:uid="{C9334235-52FB-4F10-8331-5687DC05318C}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5392,10 +5756,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
-  <dimension ref="A1:DY62"/>
+  <dimension ref="A1:DY72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AX62" sqref="AX62"/>
+    <sheetView tabSelected="1" topLeftCell="J55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K71" sqref="K71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5899,7 +6263,7 @@
         <v>7</v>
       </c>
       <c r="AB2" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC2" s="16"/>
       <c r="AD2" s="35" t="s">
@@ -5938,10 +6302,10 @@
       </c>
       <c r="AV2" s="16"/>
       <c r="AW2" s="16" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="AX2" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY2" s="16"/>
       <c r="AZ2" s="16" t="s">
@@ -6026,7 +6390,7 @@
     </row>
     <row r="3" spans="1:118" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>37</v>
@@ -6083,7 +6447,7 @@
         <v>7</v>
       </c>
       <c r="AB3" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC3" s="16"/>
       <c r="AD3" s="35" t="s">
@@ -6126,10 +6490,10 @@
       </c>
       <c r="AV3" s="16"/>
       <c r="AW3" s="16" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="AX3" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY3" s="16"/>
       <c r="AZ3" s="16" t="s">
@@ -6271,7 +6635,7 @@
         <v>7</v>
       </c>
       <c r="AB4" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC4" s="16"/>
       <c r="AD4" s="35" t="s">
@@ -6317,7 +6681,7 @@
         <v>553</v>
       </c>
       <c r="AX4" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY4" s="16"/>
       <c r="AZ4" s="16" t="s">
@@ -6457,7 +6821,7 @@
         <v>7</v>
       </c>
       <c r="AB5" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC5" s="16"/>
       <c r="AD5" s="35" t="s">
@@ -6497,7 +6861,7 @@
       <c r="AV5" s="16"/>
       <c r="AW5" s="16"/>
       <c r="AX5" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY5" s="16"/>
       <c r="AZ5" s="16" t="s">
@@ -6639,7 +7003,7 @@
         <v>7</v>
       </c>
       <c r="AB6" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC6" s="15"/>
       <c r="AD6" s="38" t="s">
@@ -6679,7 +7043,7 @@
       <c r="AV6" s="15"/>
       <c r="AW6" s="15"/>
       <c r="AX6" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY6" s="15"/>
       <c r="AZ6" s="15" t="s">
@@ -6819,7 +7183,7 @@
         <v>7</v>
       </c>
       <c r="AB7" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC7" s="15"/>
       <c r="AD7" s="38" t="s">
@@ -6859,7 +7223,7 @@
       <c r="AV7" s="15"/>
       <c r="AW7" s="15"/>
       <c r="AX7" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY7" s="15"/>
       <c r="AZ7" s="15" t="s">
@@ -7051,7 +7415,7 @@
       </c>
       <c r="AW8" s="16"/>
       <c r="AX8" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY8" s="16"/>
       <c r="AZ8" s="16" t="s">
@@ -7247,7 +7611,7 @@
       </c>
       <c r="AW9" s="16"/>
       <c r="AX9" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY9" s="16"/>
       <c r="AZ9" s="16" t="s">
@@ -7391,7 +7755,7 @@
         <v>7</v>
       </c>
       <c r="AB10" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC10" s="16" t="s">
         <v>11</v>
@@ -7435,7 +7799,7 @@
         <v>553</v>
       </c>
       <c r="AX10" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY10" s="16"/>
       <c r="AZ10" s="16" t="s">
@@ -7579,7 +7943,7 @@
         <v>7</v>
       </c>
       <c r="AB11" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC11" s="16" t="s">
         <v>11</v>
@@ -7627,7 +7991,7 @@
         <v>553</v>
       </c>
       <c r="AX11" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY11" s="16"/>
       <c r="AZ11" s="16" t="s">
@@ -7771,7 +8135,7 @@
         <v>7</v>
       </c>
       <c r="AB12" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC12" s="16" t="s">
         <v>11</v>
@@ -7813,7 +8177,7 @@
       <c r="AV12" s="16"/>
       <c r="AW12" s="16"/>
       <c r="AX12" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY12" s="16"/>
       <c r="AZ12" s="16" t="s">
@@ -7957,7 +8321,7 @@
         <v>7</v>
       </c>
       <c r="AB13" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC13" s="16" t="s">
         <v>11</v>
@@ -7999,7 +8363,7 @@
       <c r="AV13" s="16"/>
       <c r="AW13" s="16"/>
       <c r="AX13" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY13" s="16"/>
       <c r="AZ13" s="16" t="s">
@@ -8143,7 +8507,7 @@
         <v>7</v>
       </c>
       <c r="AB14" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC14" s="16" t="s">
         <v>11</v>
@@ -8185,7 +8549,7 @@
       <c r="AV14" s="16"/>
       <c r="AW14" s="16"/>
       <c r="AX14" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY14" s="16"/>
       <c r="AZ14" s="16" t="s">
@@ -8329,7 +8693,7 @@
         <v>7</v>
       </c>
       <c r="AB15" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC15" s="16" t="s">
         <v>11</v>
@@ -8373,7 +8737,7 @@
         <v>553</v>
       </c>
       <c r="AX15" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AY15" s="16"/>
       <c r="AZ15" s="16" t="s">
@@ -8517,7 +8881,7 @@
         <v>7</v>
       </c>
       <c r="AB16" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC16" s="16" t="s">
         <v>11</v>
@@ -8865,7 +9229,7 @@
         <v>7</v>
       </c>
       <c r="AB18" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC18" s="16" t="s">
         <v>11</v>
@@ -9183,7 +9547,7 @@
         <v>7</v>
       </c>
       <c r="AB20" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC20" s="16"/>
       <c r="AD20" s="35" t="s">
@@ -9387,7 +9751,7 @@
         <v>7</v>
       </c>
       <c r="AB21" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC21" s="16" t="s">
         <v>51</v>
@@ -9663,7 +10027,7 @@
         <v>7</v>
       </c>
       <c r="AB22" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC22" s="16"/>
       <c r="AD22" s="35" t="s">
@@ -11015,7 +11379,7 @@
         <v>7</v>
       </c>
       <c r="AB31" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC31" s="16"/>
       <c r="AD31" s="35" t="s">
@@ -11191,7 +11555,7 @@
         <v>7</v>
       </c>
       <c r="AB32" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC32" s="16"/>
       <c r="AD32" s="35" t="s">
@@ -11369,7 +11733,7 @@
         <v>7</v>
       </c>
       <c r="AB33" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC33" s="16"/>
       <c r="AD33" s="35" t="s">
@@ -11698,7 +12062,7 @@
         <v>7</v>
       </c>
       <c r="AB35" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC35" s="16"/>
       <c r="AD35" s="35" t="s">
@@ -14114,7 +14478,7 @@
       <c r="DM48" s="45"/>
       <c r="DN48" s="45"/>
     </row>
-    <row r="49" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
         <v>47</v>
       </c>
@@ -14294,7 +14658,7 @@
       <c r="DM49" s="45"/>
       <c r="DN49" s="45"/>
     </row>
-    <row r="50" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>48</v>
       </c>
@@ -14474,7 +14838,7 @@
       <c r="DM50" s="45"/>
       <c r="DN50" s="45"/>
     </row>
-    <row r="51" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>49</v>
       </c>
@@ -14654,7 +15018,7 @@
       <c r="DM51" s="45"/>
       <c r="DN51" s="45"/>
     </row>
-    <row r="52" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>50</v>
       </c>
@@ -14836,7 +15200,7 @@
       <c r="DM52" s="45"/>
       <c r="DN52" s="45"/>
     </row>
-    <row r="53" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>51</v>
       </c>
@@ -15018,7 +15382,7 @@
       <c r="DM53" s="45"/>
       <c r="DN53" s="45"/>
     </row>
-    <row r="54" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>52</v>
       </c>
@@ -15200,7 +15564,7 @@
       <c r="DM54" s="45"/>
       <c r="DN54" s="45"/>
     </row>
-    <row r="55" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
         <v>53</v>
       </c>
@@ -15374,7 +15738,7 @@
       <c r="DM55" s="45"/>
       <c r="DN55" s="45"/>
     </row>
-    <row r="56" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
         <v>54</v>
       </c>
@@ -15554,12 +15918,12 @@
       <c r="DM56" s="45"/>
       <c r="DN56" s="45"/>
     </row>
-    <row r="57" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>55</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C57" s="33" t="s">
         <v>299</v>
@@ -15568,10 +15932,10 @@
         <v>0</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="AB57" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AD57" s="38" t="s">
         <v>240</v>
@@ -15583,12 +15947,12 @@
         <v>355</v>
       </c>
     </row>
-    <row r="58" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>56</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C58" s="33" t="s">
         <v>299</v>
@@ -15597,7 +15961,7 @@
         <v>0</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="L58" s="34" t="s">
         <v>154</v>
@@ -15633,7 +15997,7 @@
         <v>7</v>
       </c>
       <c r="AB58" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AC58" s="15"/>
       <c r="AD58" s="38" t="s">
@@ -15680,12 +16044,12 @@
       <c r="BX58" s="45"/>
       <c r="BY58" s="45"/>
     </row>
-    <row r="59" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>57</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C59" s="33" t="s">
         <v>299</v>
@@ -15694,7 +16058,7 @@
         <v>0</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="L59" s="34" t="s">
         <v>154</v>
@@ -15730,7 +16094,7 @@
         <v>7</v>
       </c>
       <c r="AB59" s="37" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AD59" s="38" t="s">
         <v>240</v>
@@ -15782,12 +16146,12 @@
         <v>253</v>
       </c>
     </row>
-    <row r="60" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>58</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C60" s="33" t="s">
         <v>299</v>
@@ -15796,10 +16160,10 @@
         <v>0</v>
       </c>
       <c r="I60" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="J60" s="2" t="s">
         <v>607</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>611</v>
       </c>
       <c r="L60" s="34" t="s">
         <v>154</v>
@@ -15871,12 +16235,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="61" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C61" s="33" t="s">
         <v>299</v>
@@ -15885,18 +16249,18 @@
         <v>0</v>
       </c>
       <c r="E61" s="83" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="F61" s="83" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="62" spans="1:118" x14ac:dyDescent="0.25">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="62" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="C62" s="33" t="s">
         <v>299</v>
@@ -15909,7 +16273,7 @@
       <c r="G62" s="15"/>
       <c r="H62" s="15"/>
       <c r="I62" s="15" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="J62" s="15"/>
       <c r="K62" s="15"/>
@@ -16065,6 +16429,1461 @@
       <c r="DM62" s="45"/>
       <c r="DN62" s="45"/>
     </row>
+    <row r="63" spans="1:124" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>61</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="C63" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="L63" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="M63" s="34"/>
+      <c r="N63" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O63" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="P63" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q63" s="16"/>
+      <c r="R63" s="16"/>
+      <c r="S63" s="16"/>
+      <c r="T63" s="16"/>
+      <c r="U63" s="16"/>
+      <c r="V63" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="W63" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="X63" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y63" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z63" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA63" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB63" s="37" t="s">
+        <v>591</v>
+      </c>
+      <c r="AC63" s="16"/>
+      <c r="AD63" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE63" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF63" s="16"/>
+      <c r="AG63" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH63" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI63" s="16"/>
+      <c r="AJ63" s="16"/>
+      <c r="AK63" s="16"/>
+      <c r="AL63" s="16"/>
+      <c r="AM63" s="16"/>
+      <c r="AN63" s="16"/>
+      <c r="AO63" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP63" s="16"/>
+      <c r="AQ63" s="16"/>
+      <c r="AR63" s="16"/>
+      <c r="AS63" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AT63" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AU63" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV63" s="16"/>
+      <c r="AW63" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="AX63" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="AY63" s="16"/>
+      <c r="AZ63" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA63" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB63" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BC63" s="35"/>
+      <c r="BD63" s="35"/>
+      <c r="BE63" s="35"/>
+      <c r="BF63" s="35"/>
+      <c r="BG63" s="35"/>
+      <c r="BH63" s="35"/>
+      <c r="BI63" s="35"/>
+      <c r="BJ63" s="35"/>
+      <c r="BK63" s="35"/>
+      <c r="BL63" s="35"/>
+      <c r="BM63" s="35"/>
+      <c r="BN63" s="35"/>
+      <c r="BO63" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="BP63" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ63" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="BR63" s="16"/>
+      <c r="BS63" s="35"/>
+      <c r="BT63" s="35"/>
+      <c r="BU63" s="35"/>
+      <c r="BV63" s="35"/>
+      <c r="BW63" s="35"/>
+      <c r="BX63" s="35"/>
+      <c r="BY63" s="35"/>
+      <c r="BZ63" s="16"/>
+      <c r="CA63" s="16"/>
+      <c r="CB63" s="16"/>
+      <c r="CC63" s="16"/>
+      <c r="CD63" s="16"/>
+      <c r="CE63" s="16"/>
+      <c r="CF63" s="16"/>
+      <c r="CG63" s="16"/>
+      <c r="CH63" s="16"/>
+      <c r="CI63" s="16"/>
+      <c r="CJ63" s="16"/>
+      <c r="CK63" s="16"/>
+      <c r="CL63" s="16"/>
+      <c r="CM63" s="16"/>
+      <c r="CN63" s="16"/>
+      <c r="CO63" s="16"/>
+      <c r="CP63" s="16"/>
+      <c r="CQ63" s="16"/>
+      <c r="CR63" s="16"/>
+      <c r="CS63" s="16"/>
+      <c r="CT63" s="16"/>
+      <c r="CU63" s="16"/>
+      <c r="CV63" s="16"/>
+      <c r="CW63" s="16"/>
+      <c r="CX63" s="16"/>
+      <c r="CY63" s="16"/>
+      <c r="CZ63" s="16"/>
+      <c r="DA63" s="16"/>
+      <c r="DB63" s="16"/>
+      <c r="DC63" s="16"/>
+      <c r="DD63" s="16"/>
+      <c r="DE63" s="16"/>
+      <c r="DF63" s="16"/>
+      <c r="DG63" s="16"/>
+      <c r="DH63" s="16"/>
+      <c r="DI63" s="16"/>
+      <c r="DJ63" s="16"/>
+      <c r="DK63" s="16"/>
+      <c r="DL63" s="16"/>
+    </row>
+    <row r="64" spans="1:124" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>62</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="C64" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+      <c r="I64" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
+      <c r="L64" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="M64" s="34"/>
+      <c r="N64" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O64" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="P64" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q64" s="16"/>
+      <c r="R64" s="16"/>
+      <c r="S64" s="16"/>
+      <c r="T64" s="16"/>
+      <c r="U64" s="16"/>
+      <c r="V64" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="W64" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="X64" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y64" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z64" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA64" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB64" s="37"/>
+      <c r="AC64" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD64" s="16"/>
+      <c r="AE64" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF64" s="16"/>
+      <c r="AG64" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH64" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI64" s="16"/>
+      <c r="AJ64" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK64" s="16" t="s">
+        <v>538</v>
+      </c>
+      <c r="AL64" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AM64" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN64" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AO64" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP64" s="16"/>
+      <c r="AQ64" s="16"/>
+      <c r="AR64" s="16"/>
+      <c r="AS64" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AT64" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU64" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AV64" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AW64" s="16"/>
+      <c r="AX64" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="AY64" s="16"/>
+      <c r="AZ64" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA64" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB64" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BC64" s="35"/>
+      <c r="BD64" s="35"/>
+      <c r="BE64" s="35"/>
+      <c r="BF64" s="35"/>
+      <c r="BG64" s="35"/>
+      <c r="BH64" s="35"/>
+      <c r="BI64" s="35"/>
+      <c r="BJ64" s="35"/>
+      <c r="BK64" s="35"/>
+      <c r="BL64" s="35"/>
+      <c r="BM64" s="35"/>
+      <c r="BN64" s="35"/>
+      <c r="BO64" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="BP64" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ64" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="BR64" s="16"/>
+      <c r="BS64" s="35"/>
+      <c r="BT64" s="35"/>
+      <c r="BU64" s="35"/>
+      <c r="BV64" s="35"/>
+      <c r="BW64" s="35"/>
+      <c r="BX64" s="35"/>
+      <c r="BY64" s="35"/>
+      <c r="BZ64" s="16"/>
+      <c r="CA64" s="16"/>
+      <c r="CB64" s="16"/>
+      <c r="CC64" s="16"/>
+      <c r="CD64" s="16"/>
+      <c r="CE64" s="16"/>
+      <c r="CF64" s="16"/>
+      <c r="CG64" s="16"/>
+      <c r="CH64" s="16"/>
+      <c r="CI64" s="16"/>
+      <c r="CJ64" s="16"/>
+      <c r="CK64" s="16"/>
+      <c r="CL64" s="16"/>
+      <c r="CM64" s="16"/>
+      <c r="CN64" s="16"/>
+      <c r="CO64" s="16"/>
+      <c r="CP64" s="16"/>
+      <c r="CQ64" s="16"/>
+      <c r="CR64" s="16"/>
+      <c r="CS64" s="16"/>
+      <c r="CT64" s="16"/>
+      <c r="CU64" s="16"/>
+      <c r="CV64" s="16"/>
+      <c r="CW64" s="16"/>
+      <c r="CX64" s="16"/>
+      <c r="CY64" s="16"/>
+      <c r="CZ64" s="16"/>
+      <c r="DA64" s="16"/>
+      <c r="DB64" s="16"/>
+      <c r="DC64" s="16"/>
+      <c r="DD64" s="16"/>
+      <c r="DE64" s="16"/>
+      <c r="DF64" s="16"/>
+      <c r="DG64" s="16"/>
+      <c r="DH64" s="16"/>
+      <c r="DI64" s="16"/>
+      <c r="DJ64" s="16"/>
+      <c r="DK64" s="16"/>
+      <c r="DL64" s="16"/>
+      <c r="DM64" s="16"/>
+      <c r="DN64" s="16"/>
+      <c r="DO64" s="4"/>
+      <c r="DP64" s="4"/>
+      <c r="DQ64" s="4"/>
+      <c r="DR64" s="4"/>
+      <c r="DS64" s="4"/>
+      <c r="DT64" s="4"/>
+    </row>
+    <row r="65" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>63</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="C65" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="J65" s="45"/>
+      <c r="K65" s="45"/>
+      <c r="L65" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="M65" s="34"/>
+      <c r="N65" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O65" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="P65" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q65" s="45"/>
+      <c r="R65" s="45"/>
+      <c r="S65" s="45"/>
+      <c r="T65" s="45"/>
+      <c r="U65" s="45"/>
+      <c r="V65" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="W65" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="X65" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y65" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z65" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA65" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB65" s="37" t="s">
+        <v>591</v>
+      </c>
+      <c r="AC65" s="16"/>
+      <c r="AD65" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="AE65" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="AF65" s="45"/>
+      <c r="AG65" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH65" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="AI65" s="45"/>
+      <c r="AJ65" s="45"/>
+      <c r="AK65" s="45"/>
+      <c r="AL65" s="45"/>
+      <c r="AM65" s="45"/>
+      <c r="AN65" s="45"/>
+      <c r="AO65" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP65" s="46" t="s">
+        <v>617</v>
+      </c>
+      <c r="AQ65" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="AR65" s="45"/>
+      <c r="AS65" s="45"/>
+      <c r="AT65" s="45"/>
+      <c r="AU65" s="45"/>
+      <c r="AV65" s="45"/>
+      <c r="AW65" s="45"/>
+      <c r="AX65" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="AY65" s="45"/>
+      <c r="AZ65" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA65" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB65" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="BC65" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="BD65" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="BE65" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="BF65" s="35"/>
+      <c r="BG65" s="35"/>
+      <c r="BH65" s="35"/>
+      <c r="BI65" s="35"/>
+      <c r="BJ65" s="35"/>
+      <c r="BK65" s="35"/>
+      <c r="BL65" s="35"/>
+      <c r="BM65" s="35"/>
+      <c r="BN65" s="35"/>
+      <c r="BO65" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="BP65" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="BQ65" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="BR65" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="BS65" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="BT65" s="35"/>
+      <c r="BU65" s="35"/>
+      <c r="BV65" s="35"/>
+      <c r="BW65" s="35"/>
+      <c r="BX65" s="35"/>
+      <c r="BY65" s="35"/>
+      <c r="BZ65" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="CA65" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="CB65" s="45"/>
+      <c r="CC65" s="35" t="s">
+        <v>544</v>
+      </c>
+      <c r="CD65" s="45" t="s">
+        <v>253</v>
+      </c>
+      <c r="CE65" s="45"/>
+      <c r="CF65" s="45"/>
+      <c r="CG65" s="45"/>
+      <c r="CH65" s="45"/>
+      <c r="CI65" s="45"/>
+      <c r="CJ65" s="45"/>
+      <c r="CK65" s="45"/>
+      <c r="CL65" s="45"/>
+      <c r="CM65" s="45"/>
+      <c r="CN65" s="45"/>
+      <c r="CO65" s="45"/>
+      <c r="CP65" s="45"/>
+      <c r="CQ65" s="45"/>
+      <c r="CR65" s="45"/>
+      <c r="CS65" s="45"/>
+      <c r="CT65" s="45"/>
+      <c r="CU65" s="45"/>
+      <c r="CV65" s="45"/>
+      <c r="CW65" s="45"/>
+      <c r="CX65" s="45"/>
+      <c r="CY65" s="45"/>
+      <c r="CZ65" s="45"/>
+      <c r="DA65" s="45"/>
+      <c r="DB65" s="45"/>
+      <c r="DC65" s="45"/>
+      <c r="DD65" s="45"/>
+      <c r="DE65" s="45"/>
+      <c r="DF65" s="45"/>
+      <c r="DG65" s="45"/>
+      <c r="DH65" s="45"/>
+      <c r="DI65" s="45"/>
+      <c r="DJ65" s="45"/>
+      <c r="DK65" s="45"/>
+      <c r="DL65" s="45"/>
+      <c r="DM65" s="45"/>
+      <c r="DN65" s="45"/>
+    </row>
+    <row r="66" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>64</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="C66" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I66" s="16" t="s">
+        <v>619</v>
+      </c>
+      <c r="J66" s="16"/>
+      <c r="K66" s="16"/>
+      <c r="L66" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="M66" s="34"/>
+      <c r="N66" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O66" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="P66" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q66" s="16"/>
+      <c r="R66" s="16"/>
+      <c r="S66" s="16"/>
+      <c r="T66" s="16"/>
+      <c r="U66" s="16"/>
+      <c r="V66" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="W66" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="X66" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y66" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z66" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA66" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB66" s="37" t="s">
+        <v>591</v>
+      </c>
+      <c r="AC66" s="16"/>
+      <c r="AD66" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE66" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF66" s="16"/>
+      <c r="AG66" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH66" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI66" s="16"/>
+      <c r="AJ66" s="16"/>
+      <c r="AK66" s="16"/>
+      <c r="AL66" s="16"/>
+      <c r="AM66" s="16"/>
+      <c r="AN66" s="16"/>
+      <c r="AO66" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP66" s="16"/>
+      <c r="AQ66" s="16"/>
+      <c r="AR66" s="16"/>
+      <c r="AS66" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AT66" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AU66" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV66" s="16"/>
+      <c r="AW66" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="AX66" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="AY66" s="16"/>
+      <c r="AZ66" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA66" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB66" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BC66" s="35"/>
+      <c r="BD66" s="35"/>
+      <c r="BE66" s="35"/>
+      <c r="BF66" s="35"/>
+      <c r="BG66" s="35"/>
+      <c r="BH66" s="35"/>
+      <c r="BI66" s="35"/>
+      <c r="BJ66" s="35"/>
+      <c r="BK66" s="35"/>
+      <c r="BL66" s="35"/>
+      <c r="BM66" s="35"/>
+      <c r="BN66" s="35"/>
+      <c r="BO66" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="BP66" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ66" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="BR66" s="16"/>
+      <c r="BS66" s="35"/>
+      <c r="BT66" s="35"/>
+      <c r="BU66" s="35"/>
+      <c r="BV66" s="35"/>
+      <c r="BW66" s="35"/>
+      <c r="BX66" s="35"/>
+      <c r="BY66" s="35"/>
+      <c r="BZ66" s="16"/>
+      <c r="CA66" s="16"/>
+      <c r="CB66" s="16"/>
+      <c r="CC66" s="16"/>
+      <c r="CD66" s="16"/>
+      <c r="CE66" s="16"/>
+      <c r="CF66" s="16"/>
+      <c r="CG66" s="16"/>
+      <c r="CH66" s="16"/>
+      <c r="CI66" s="16"/>
+      <c r="CJ66" s="16"/>
+      <c r="CK66" s="16"/>
+      <c r="CL66" s="16"/>
+      <c r="CM66" s="16"/>
+      <c r="CN66" s="16"/>
+      <c r="CO66" s="16"/>
+      <c r="CP66" s="16"/>
+      <c r="CQ66" s="16"/>
+      <c r="CR66" s="16"/>
+      <c r="CS66" s="16"/>
+      <c r="CT66" s="16"/>
+      <c r="CU66" s="16"/>
+      <c r="CV66" s="16"/>
+      <c r="CW66" s="16"/>
+      <c r="CX66" s="16"/>
+      <c r="CY66" s="16"/>
+    </row>
+    <row r="67" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="C67" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="L67" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="M67" s="34"/>
+      <c r="N67" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O67" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="P67" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q67" s="16"/>
+      <c r="R67" s="16"/>
+      <c r="S67" s="16"/>
+      <c r="T67" s="16"/>
+      <c r="U67" s="16"/>
+      <c r="V67" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="W67" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="X67" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y67" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z67" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA67" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB67" s="37" t="s">
+        <v>591</v>
+      </c>
+      <c r="AC67" s="16"/>
+      <c r="AD67" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE67" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF67" s="16"/>
+      <c r="AG67" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH67" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI67" s="16"/>
+      <c r="AJ67" s="16"/>
+      <c r="AK67" s="16"/>
+      <c r="AL67" s="16"/>
+      <c r="AM67" s="16"/>
+      <c r="AN67" s="16"/>
+      <c r="AO67" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP67" s="16"/>
+      <c r="AQ67" s="16"/>
+      <c r="AR67" s="16"/>
+      <c r="AS67" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AT67" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AU67" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV67" s="16"/>
+      <c r="AW67" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="AX67" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="AY67" s="16"/>
+      <c r="AZ67" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA67" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB67" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BC67" s="35"/>
+      <c r="BD67" s="35"/>
+      <c r="BE67" s="35"/>
+      <c r="BF67" s="35"/>
+      <c r="BG67" s="35"/>
+      <c r="BH67" s="35"/>
+      <c r="BI67" s="35"/>
+      <c r="BJ67" s="35"/>
+      <c r="BK67" s="35"/>
+      <c r="BL67" s="35"/>
+      <c r="BM67" s="35"/>
+      <c r="BN67" s="35"/>
+      <c r="BO67" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="BP67" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ67" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="BR67" s="16"/>
+      <c r="BS67" s="35"/>
+      <c r="BT67" s="35"/>
+      <c r="BU67" s="35"/>
+      <c r="BV67" s="35"/>
+      <c r="BW67" s="35"/>
+      <c r="BX67" s="35"/>
+      <c r="BY67" s="35"/>
+      <c r="BZ67" s="16"/>
+      <c r="CA67" s="16"/>
+      <c r="CB67" s="16"/>
+      <c r="CC67" s="35" t="s">
+        <v>544</v>
+      </c>
+      <c r="CD67" s="45" t="s">
+        <v>253</v>
+      </c>
+      <c r="CE67" s="16"/>
+      <c r="CF67" s="16"/>
+      <c r="CG67" s="16"/>
+      <c r="CH67" s="16"/>
+      <c r="CI67" s="16"/>
+      <c r="CJ67" s="16"/>
+      <c r="CK67" s="16"/>
+      <c r="CL67" s="16"/>
+      <c r="CM67" s="16"/>
+      <c r="CN67" s="16"/>
+      <c r="CO67" s="16"/>
+      <c r="CP67" s="16"/>
+      <c r="CQ67" s="16"/>
+      <c r="CR67" s="16"/>
+      <c r="CS67" s="16"/>
+      <c r="CT67" s="16"/>
+      <c r="CU67" s="16"/>
+      <c r="CV67" s="16"/>
+      <c r="CW67" s="16"/>
+      <c r="CX67" s="16"/>
+      <c r="CY67" s="16"/>
+    </row>
+    <row r="68" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>66</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="C68" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+      <c r="I68" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="L68" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="M68" s="34"/>
+      <c r="N68" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O68" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="P68" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q68" s="16"/>
+      <c r="R68" s="16"/>
+      <c r="S68" s="16"/>
+      <c r="T68" s="16"/>
+      <c r="U68" s="16"/>
+      <c r="V68" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="W68" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="X68" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y68" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z68" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA68" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB68" s="37"/>
+      <c r="AC68" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD68" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE68" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF68" s="16"/>
+      <c r="AG68" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH68" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI68" s="16"/>
+      <c r="AJ68" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK68" s="16" t="s">
+        <v>538</v>
+      </c>
+      <c r="AL68" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AM68" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN68" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AO68" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP68" s="16"/>
+      <c r="AQ68" s="16"/>
+      <c r="AR68" s="16"/>
+      <c r="AS68" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AT68" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU68" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AV68" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AW68" s="16"/>
+      <c r="AX68" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="AY68" s="16"/>
+      <c r="AZ68" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA68" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB68" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BC68" s="35"/>
+      <c r="BD68" s="35"/>
+      <c r="BE68" s="35"/>
+      <c r="BF68" s="35"/>
+      <c r="BG68" s="35"/>
+      <c r="BH68" s="35"/>
+      <c r="BI68" s="35"/>
+      <c r="BJ68" s="35"/>
+      <c r="BK68" s="35"/>
+      <c r="BL68" s="35"/>
+      <c r="BM68" s="35"/>
+      <c r="BN68" s="35"/>
+      <c r="BO68" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="BP68" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ68" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="BR68" s="16"/>
+      <c r="BS68" s="35"/>
+      <c r="BT68" s="35"/>
+      <c r="BU68" s="35"/>
+      <c r="BV68" s="35"/>
+      <c r="BW68" s="35"/>
+      <c r="BX68" s="35"/>
+      <c r="BY68" s="35"/>
+      <c r="BZ68" s="16"/>
+      <c r="CA68" s="16"/>
+      <c r="CB68" s="16"/>
+      <c r="CC68" s="16"/>
+      <c r="CD68" s="16"/>
+      <c r="CE68" s="16"/>
+      <c r="CF68" s="16"/>
+      <c r="CG68" s="16"/>
+      <c r="CH68" s="16"/>
+      <c r="CI68" s="16"/>
+      <c r="CJ68" s="16"/>
+      <c r="CK68" s="16"/>
+      <c r="CL68" s="16"/>
+      <c r="CM68" s="16"/>
+      <c r="CN68" s="16"/>
+      <c r="CO68" s="16"/>
+      <c r="CP68" s="16"/>
+      <c r="CQ68" s="16"/>
+      <c r="CR68" s="16"/>
+      <c r="CS68" s="16"/>
+      <c r="CT68" s="16"/>
+      <c r="CU68" s="16"/>
+      <c r="CV68" s="16"/>
+      <c r="CW68" s="16"/>
+      <c r="CX68" s="16"/>
+      <c r="CY68" s="16"/>
+      <c r="CZ68" s="16"/>
+      <c r="DA68" s="16"/>
+      <c r="DB68" s="16"/>
+      <c r="DC68" s="16"/>
+      <c r="DD68" s="16"/>
+      <c r="DE68" s="16"/>
+      <c r="DF68" s="16"/>
+      <c r="DG68" s="16"/>
+      <c r="DH68" s="16"/>
+      <c r="DI68" s="16"/>
+      <c r="DJ68" s="16"/>
+      <c r="DK68" s="16"/>
+      <c r="DL68" s="16"/>
+      <c r="DM68" s="16"/>
+      <c r="DN68" s="16"/>
+    </row>
+    <row r="69" spans="1:118" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="10">
+        <v>67</v>
+      </c>
+      <c r="B69" s="25" t="s">
+        <v>625</v>
+      </c>
+      <c r="C69" s="67" t="s">
+        <v>299</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I69" s="10" t="s">
+        <v>626</v>
+      </c>
+      <c r="L69" s="84" t="s">
+        <v>154</v>
+      </c>
+      <c r="M69" s="84"/>
+      <c r="N69" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="O69" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="P69" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q69" s="15"/>
+      <c r="R69" s="15"/>
+      <c r="S69" s="15"/>
+      <c r="T69" s="15"/>
+      <c r="U69" s="15"/>
+      <c r="V69" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="W69" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="X69" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y69" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z69" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA69" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB69" s="40" t="s">
+        <v>591</v>
+      </c>
+      <c r="AC69" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD69" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE69" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF69" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG69" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH69" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI69" s="15"/>
+      <c r="AJ69" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK69" s="15" t="s">
+        <v>538</v>
+      </c>
+      <c r="AL69" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AM69" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN69" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AO69" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AS69" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AT69" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU69" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AV69" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AZ69" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA69" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB69" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="BC69" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="BD69" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="BE69" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="BO69" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="BP69" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ69" s="85" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="70" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>68</v>
+      </c>
+      <c r="B70" s="25" t="s">
+        <v>627</v>
+      </c>
+      <c r="C70" s="67" t="s">
+        <v>299</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB70" s="83" t="s">
+        <v>628</v>
+      </c>
+      <c r="BO70" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="BQ70" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="CC70" s="35" t="s">
+        <v>544</v>
+      </c>
+      <c r="CD70" s="45" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="71" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>69</v>
+      </c>
+      <c r="B71" s="25" t="s">
+        <v>637</v>
+      </c>
+      <c r="C71" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16" t="s">
+        <v>639</v>
+      </c>
+      <c r="J71" s="16" t="s">
+        <v>645</v>
+      </c>
+      <c r="K71" s="16" t="s">
+        <v>641</v>
+      </c>
+      <c r="L71" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="M71" s="34"/>
+      <c r="N71" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O71" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="P71" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q71" s="16"/>
+      <c r="R71" s="16"/>
+      <c r="S71" s="16"/>
+      <c r="T71" s="16"/>
+      <c r="U71" s="16"/>
+      <c r="V71" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="W71" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="X71" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y71" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z71" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA71" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB71" s="37" t="s">
+        <v>591</v>
+      </c>
+      <c r="AC71" s="16"/>
+      <c r="AD71" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE71" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF71" s="16"/>
+      <c r="AG71" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH71" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI71" s="16"/>
+      <c r="AJ71" s="16"/>
+      <c r="AK71" s="16"/>
+      <c r="AL71" s="16"/>
+      <c r="AM71" s="16"/>
+      <c r="AN71" s="16"/>
+      <c r="AO71" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP71" s="16"/>
+      <c r="AQ71" s="16"/>
+      <c r="AR71" s="16"/>
+      <c r="AS71" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AT71" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AU71" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV71" s="16"/>
+      <c r="AW71" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="AX71" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="AY71" s="16"/>
+      <c r="AZ71" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA71" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="BB71" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BC71" s="35"/>
+      <c r="BD71" s="35"/>
+      <c r="BE71" s="35"/>
+      <c r="BF71" s="35"/>
+      <c r="BG71" s="35"/>
+      <c r="BH71" s="35"/>
+      <c r="BI71" s="35"/>
+      <c r="BJ71" s="35"/>
+      <c r="BK71" s="35"/>
+      <c r="BL71" s="35"/>
+      <c r="BM71" s="35"/>
+      <c r="BN71" s="35"/>
+      <c r="BO71" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="BP71" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ71" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="BR71" s="16"/>
+      <c r="BS71" s="35"/>
+      <c r="BT71" s="35"/>
+      <c r="BU71" s="35"/>
+      <c r="BV71" s="35"/>
+      <c r="BW71" s="35"/>
+      <c r="BX71" s="35"/>
+      <c r="BY71" s="35"/>
+      <c r="BZ71" s="16"/>
+      <c r="CA71" s="16"/>
+      <c r="CB71" s="16"/>
+      <c r="CC71" s="16"/>
+      <c r="CD71" s="16"/>
+      <c r="CE71" s="16"/>
+      <c r="CF71" s="16"/>
+      <c r="CG71" s="16"/>
+      <c r="CH71" s="16"/>
+      <c r="CI71" s="16"/>
+      <c r="CJ71" s="16"/>
+      <c r="CK71" s="16"/>
+      <c r="CL71" s="16"/>
+      <c r="CM71" s="16"/>
+      <c r="CN71" s="16"/>
+      <c r="CO71" s="16"/>
+      <c r="CP71" s="16"/>
+      <c r="CQ71" s="16"/>
+      <c r="CR71" s="16"/>
+      <c r="CS71" s="16"/>
+      <c r="CT71" s="16"/>
+      <c r="CU71" s="16"/>
+      <c r="CV71" s="16"/>
+      <c r="CW71" s="16"/>
+      <c r="CX71" s="16"/>
+      <c r="CY71" s="16"/>
+      <c r="CZ71" s="16"/>
+      <c r="DA71" s="16"/>
+      <c r="DB71" s="16"/>
+      <c r="DC71" s="16"/>
+      <c r="DD71" s="16"/>
+      <c r="DE71" s="16"/>
+      <c r="DF71" s="16"/>
+      <c r="DG71" s="16"/>
+      <c r="DH71" s="16"/>
+      <c r="DI71" s="16"/>
+      <c r="DJ71" s="16"/>
+      <c r="DK71" s="16"/>
+      <c r="DL71" s="16"/>
+      <c r="DM71" s="16"/>
+      <c r="DN71" s="16"/>
+    </row>
+    <row r="72" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>70</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="C72" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -16081,9 +17900,11 @@
     <hyperlink ref="C22" r:id="rId11" xr:uid="{A4C270D7-E880-46D0-87DA-E14CE53E534C}"/>
     <hyperlink ref="C23" r:id="rId12" xr:uid="{CE425BFD-B123-481D-BDFD-CFF64FCDF6EB}"/>
     <hyperlink ref="C24:C28" r:id="rId13" display="CRMTest06@corp.premierinc.com" xr:uid="{CBABE6F4-EF70-4915-BC24-AEC98C9D0AE2}"/>
+    <hyperlink ref="C71" r:id="rId14" xr:uid="{2241BBF0-2CE3-4F5C-A3AF-E58F7FA5B364}"/>
+    <hyperlink ref="C72" r:id="rId15" xr:uid="{109D2082-96EF-42F1-A1B2-D5A928B5933C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
@@ -16091,8 +17912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D073B921-24DF-4F78-BD1E-1984D65F897D}">
   <dimension ref="A1:BE24"/>
   <sheetViews>
-    <sheetView topLeftCell="L8" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18461,8 +20282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51C67A-098B-49A1-9024-B5BC951889FA}">
   <dimension ref="A1:AF10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Committing Test Case 8906
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\Dynamics-CRM-Cloud\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD963C69-5CA8-457F-9482-18E71E016B66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB671648-B230-4DAA-8FCB-517BA2451431}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4366" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4369" uniqueCount="924">
   <si>
     <t>Premier1a</t>
   </si>
@@ -2688,9 +2688,6 @@
     <t>TFS ID_10752:Cloud:Verify on end dating HIN, user should not allow to enter End date which is today's date /Future date</t>
   </si>
   <si>
-    <t>PASSED</t>
-  </si>
-  <si>
     <t>TFS ID_10753:Cloud:Verify on End dating active HIN ,should get removed from Member form</t>
   </si>
   <si>
@@ -2799,13 +2796,22 @@
     <t>2000512119</t>
   </si>
   <si>
-    <t>2022_04_19_11_23_02</t>
-  </si>
-  <si>
     <t>TFS ID_ 8906:Cloud: Verify if the DEA expiration date is displayed</t>
   </si>
   <si>
     <t>DEAExpiryDate</t>
+  </si>
+  <si>
+    <t>A94143361</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>2000512128</t>
+  </si>
+  <si>
+    <t>2022_04_19_08_33_26</t>
   </si>
 </sst>
 </file>
@@ -3125,7 +3131,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3314,20 +3320,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3338,8 +3330,8 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3663,9 +3655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
   <dimension ref="A1:P171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A165" sqref="A165"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3682,7 +3672,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="107" t="s">
@@ -3720,7 +3710,7 @@
       <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -3733,20 +3723,20 @@
         <v>40</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>882</v>
+        <v>265</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>919</v>
+        <v>742</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
-      <c r="K2" s="80" t="s">
+      <c r="K2" s="48" t="s">
         <v>555</v>
       </c>
-      <c r="L2" s="66" t="s">
+      <c r="L2" s="114" t="s">
         <v>536</v>
       </c>
     </row>
@@ -3754,7 +3744,7 @@
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -3786,7 +3776,7 @@
       <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -3815,7 +3805,7 @@
       <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="17" t="s">
@@ -3834,7 +3824,7 @@
         <v>742</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
@@ -3844,7 +3834,7 @@
       <c r="A6" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="12" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -3871,7 +3861,7 @@
       <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="17" t="s">
@@ -3898,7 +3888,7 @@
       <c r="A8" s="17">
         <v>7</v>
       </c>
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="12" t="s">
         <v>452</v>
       </c>
       <c r="C8" s="17" t="s">
@@ -3917,7 +3907,7 @@
         <v>742</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
@@ -3927,7 +3917,7 @@
       <c r="A9" s="17">
         <v>8</v>
       </c>
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="12" t="s">
         <v>46</v>
       </c>
       <c r="C9" s="17" t="s">
@@ -3954,7 +3944,7 @@
       <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="12" t="s">
         <v>451</v>
       </c>
       <c r="C10" s="17" t="s">
@@ -3973,7 +3963,7 @@
         <v>742</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
@@ -3983,7 +3973,7 @@
       <c r="A11" s="17">
         <v>10</v>
       </c>
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="17" t="s">
@@ -4002,7 +3992,7 @@
         <v>742</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
@@ -4012,7 +4002,7 @@
       <c r="A12" s="17">
         <v>11</v>
       </c>
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="12" t="s">
         <v>450</v>
       </c>
       <c r="C12" s="17" t="s">
@@ -4031,7 +4021,7 @@
         <v>742</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
@@ -4042,7 +4032,7 @@
       <c r="A13" s="17">
         <v>12</v>
       </c>
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C13" s="17" t="s">
@@ -4069,7 +4059,7 @@
       <c r="A14" s="17">
         <v>13</v>
       </c>
-      <c r="B14" s="108" t="s">
+      <c r="B14" s="12" t="s">
         <v>252</v>
       </c>
       <c r="C14" s="17" t="s">
@@ -4096,7 +4086,7 @@
       <c r="A15" s="17">
         <v>14</v>
       </c>
-      <c r="B15" s="108" t="s">
+      <c r="B15" s="12" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -4115,7 +4105,7 @@
         <v>742</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
@@ -4125,7 +4115,7 @@
       <c r="A16" s="17">
         <v>15</v>
       </c>
-      <c r="B16" s="108" t="s">
+      <c r="B16" s="12" t="s">
         <v>449</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -4144,7 +4134,7 @@
         <v>742</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
@@ -4154,7 +4144,7 @@
       <c r="A17" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="108" t="s">
+      <c r="B17" s="12" t="s">
         <v>448</v>
       </c>
       <c r="C17" s="17" t="s">
@@ -4181,7 +4171,7 @@
       <c r="A18" s="17">
         <v>17</v>
       </c>
-      <c r="B18" s="108" t="s">
+      <c r="B18" s="12" t="s">
         <v>447</v>
       </c>
       <c r="C18" s="17" t="s">
@@ -4208,7 +4198,7 @@
       <c r="A19" s="17">
         <v>18</v>
       </c>
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="12" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -4235,7 +4225,7 @@
       <c r="A20" s="17">
         <v>19</v>
       </c>
-      <c r="B20" s="108" t="s">
+      <c r="B20" s="12" t="s">
         <v>446</v>
       </c>
       <c r="C20" s="17" t="s">
@@ -4262,7 +4252,7 @@
       <c r="A21" s="17">
         <v>20</v>
       </c>
-      <c r="B21" s="108" t="s">
+      <c r="B21" s="12" t="s">
         <v>241</v>
       </c>
       <c r="C21" s="17" t="s">
@@ -4281,7 +4271,7 @@
         <v>742</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
@@ -4291,7 +4281,7 @@
       <c r="A22" s="17">
         <v>21</v>
       </c>
-      <c r="B22" s="108" t="s">
+      <c r="B22" s="12" t="s">
         <v>491</v>
       </c>
       <c r="C22" s="17" t="s">
@@ -4311,7 +4301,7 @@
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="17" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="J22" s="17"/>
       <c r="K22" s="25"/>
@@ -4320,7 +4310,7 @@
       <c r="A23" s="17">
         <v>22</v>
       </c>
-      <c r="B23" s="108" t="s">
+      <c r="B23" s="12" t="s">
         <v>178</v>
       </c>
       <c r="C23" s="17" t="s">
@@ -4347,7 +4337,7 @@
       <c r="A24" s="17">
         <v>23</v>
       </c>
-      <c r="B24" s="108" t="s">
+      <c r="B24" s="12" t="s">
         <v>177</v>
       </c>
       <c r="C24" s="17" t="s">
@@ -4374,7 +4364,7 @@
       <c r="A25" s="17">
         <v>24</v>
       </c>
-      <c r="B25" s="108" t="s">
+      <c r="B25" s="12" t="s">
         <v>169</v>
       </c>
       <c r="C25" s="17" t="s">
@@ -4401,7 +4391,7 @@
       <c r="A26" s="17">
         <v>25</v>
       </c>
-      <c r="B26" s="108" t="s">
+      <c r="B26" s="12" t="s">
         <v>179</v>
       </c>
       <c r="C26" s="17" t="s">
@@ -4428,7 +4418,7 @@
       <c r="A27" s="17">
         <v>26</v>
       </c>
-      <c r="B27" s="108" t="s">
+      <c r="B27" s="12" t="s">
         <v>180</v>
       </c>
       <c r="C27" s="17" t="s">
@@ -4455,7 +4445,7 @@
       <c r="A28" s="17">
         <v>27</v>
       </c>
-      <c r="B28" s="108" t="s">
+      <c r="B28" s="12" t="s">
         <v>181</v>
       </c>
       <c r="C28" s="17" t="s">
@@ -4482,7 +4472,7 @@
       <c r="A29" s="17">
         <v>28</v>
       </c>
-      <c r="B29" s="108" t="s">
+      <c r="B29" s="12" t="s">
         <v>184</v>
       </c>
       <c r="C29" s="17" t="s">
@@ -4509,7 +4499,7 @@
       <c r="A30" s="17">
         <v>29</v>
       </c>
-      <c r="B30" s="108" t="s">
+      <c r="B30" s="12" t="s">
         <v>211</v>
       </c>
       <c r="C30" s="17" t="s">
@@ -4536,7 +4526,7 @@
       <c r="A31" s="17">
         <v>30</v>
       </c>
-      <c r="B31" s="109" t="s">
+      <c r="B31" s="24" t="s">
         <v>347</v>
       </c>
       <c r="C31" s="17" t="s">
@@ -4563,7 +4553,7 @@
       <c r="A32" s="17">
         <v>31</v>
       </c>
-      <c r="B32" s="109" t="s">
+      <c r="B32" s="24" t="s">
         <v>348</v>
       </c>
       <c r="C32" s="17" t="s">
@@ -4590,7 +4580,7 @@
       <c r="A33" s="17">
         <v>32</v>
       </c>
-      <c r="B33" s="109" t="s">
+      <c r="B33" s="24" t="s">
         <v>359</v>
       </c>
       <c r="C33" s="17" t="s">
@@ -4617,7 +4607,7 @@
       <c r="A34" s="17">
         <v>33</v>
       </c>
-      <c r="B34" s="109" t="s">
+      <c r="B34" s="24" t="s">
         <v>362</v>
       </c>
       <c r="C34" s="17" t="s">
@@ -4644,7 +4634,7 @@
       <c r="A35" s="17">
         <v>34</v>
       </c>
-      <c r="B35" s="109" t="s">
+      <c r="B35" s="24" t="s">
         <v>364</v>
       </c>
       <c r="C35" s="17" t="s">
@@ -4671,7 +4661,7 @@
       <c r="A36" s="17">
         <v>35</v>
       </c>
-      <c r="B36" s="109" t="s">
+      <c r="B36" s="24" t="s">
         <v>381</v>
       </c>
       <c r="C36" s="17" t="s">
@@ -4698,7 +4688,7 @@
       <c r="A37" s="17">
         <v>36</v>
       </c>
-      <c r="B37" s="109" t="s">
+      <c r="B37" s="24" t="s">
         <v>445</v>
       </c>
       <c r="C37" s="17" t="s">
@@ -4725,7 +4715,7 @@
       <c r="A38" s="17">
         <v>37</v>
       </c>
-      <c r="B38" s="109" t="s">
+      <c r="B38" s="24" t="s">
         <v>454</v>
       </c>
       <c r="C38" s="17" t="s">
@@ -4752,7 +4742,7 @@
       <c r="A39" s="17">
         <v>38</v>
       </c>
-      <c r="B39" s="109" t="s">
+      <c r="B39" s="24" t="s">
         <v>444</v>
       </c>
       <c r="C39" s="17" t="s">
@@ -4779,7 +4769,7 @@
       <c r="A40" s="17">
         <v>39</v>
       </c>
-      <c r="B40" s="109" t="s">
+      <c r="B40" s="24" t="s">
         <v>443</v>
       </c>
       <c r="C40" s="17" t="s">
@@ -4806,7 +4796,7 @@
       <c r="A41" s="17">
         <v>40</v>
       </c>
-      <c r="B41" s="109" t="s">
+      <c r="B41" s="24" t="s">
         <v>442</v>
       </c>
       <c r="C41" s="17" t="s">
@@ -4833,7 +4823,7 @@
       <c r="A42" s="17">
         <v>41</v>
       </c>
-      <c r="B42" s="109" t="s">
+      <c r="B42" s="24" t="s">
         <v>441</v>
       </c>
       <c r="C42" s="17" t="s">
@@ -4860,7 +4850,7 @@
       <c r="A43" s="17">
         <v>42</v>
       </c>
-      <c r="B43" s="109" t="s">
+      <c r="B43" s="24" t="s">
         <v>440</v>
       </c>
       <c r="C43" s="17" t="s">
@@ -4887,7 +4877,7 @@
       <c r="A44" s="17">
         <v>43</v>
       </c>
-      <c r="B44" s="109" t="s">
+      <c r="B44" s="24" t="s">
         <v>439</v>
       </c>
       <c r="C44" s="17" t="s">
@@ -4914,7 +4904,7 @@
       <c r="A45" s="17">
         <v>44</v>
       </c>
-      <c r="B45" s="109" t="s">
+      <c r="B45" s="24" t="s">
         <v>438</v>
       </c>
       <c r="C45" s="17" t="s">
@@ -4941,7 +4931,7 @@
       <c r="A46" s="17">
         <v>45</v>
       </c>
-      <c r="B46" s="109" t="s">
+      <c r="B46" s="24" t="s">
         <v>437</v>
       </c>
       <c r="C46" s="17" t="s">
@@ -4968,7 +4958,7 @@
       <c r="A47" s="17">
         <v>46</v>
       </c>
-      <c r="B47" s="109" t="s">
+      <c r="B47" s="24" t="s">
         <v>436</v>
       </c>
       <c r="C47" s="17" t="s">
@@ -4995,7 +4985,7 @@
       <c r="A48" s="17">
         <v>47</v>
       </c>
-      <c r="B48" s="109" t="s">
+      <c r="B48" s="24" t="s">
         <v>435</v>
       </c>
       <c r="C48" s="17" t="s">
@@ -5022,7 +5012,7 @@
       <c r="A49" s="17">
         <v>48</v>
       </c>
-      <c r="B49" s="109" t="s">
+      <c r="B49" s="24" t="s">
         <v>434</v>
       </c>
       <c r="C49" s="17" t="s">
@@ -5049,7 +5039,7 @@
       <c r="A50" s="17">
         <v>49</v>
       </c>
-      <c r="B50" s="109" t="s">
+      <c r="B50" s="24" t="s">
         <v>433</v>
       </c>
       <c r="C50" s="17" t="s">
@@ -5076,7 +5066,7 @@
       <c r="A51" s="17">
         <v>50</v>
       </c>
-      <c r="B51" s="109" t="s">
+      <c r="B51" s="24" t="s">
         <v>432</v>
       </c>
       <c r="C51" s="17" t="s">
@@ -5103,7 +5093,7 @@
       <c r="A52" s="17">
         <v>51</v>
       </c>
-      <c r="B52" s="109" t="s">
+      <c r="B52" s="24" t="s">
         <v>431</v>
       </c>
       <c r="C52" s="17" t="s">
@@ -5130,7 +5120,7 @@
       <c r="A53" s="17">
         <v>52</v>
       </c>
-      <c r="B53" s="109" t="s">
+      <c r="B53" s="24" t="s">
         <v>430</v>
       </c>
       <c r="C53" s="17" t="s">
@@ -5157,7 +5147,7 @@
       <c r="A54" s="17">
         <v>53</v>
       </c>
-      <c r="B54" s="109" t="s">
+      <c r="B54" s="24" t="s">
         <v>429</v>
       </c>
       <c r="C54" s="17" t="s">
@@ -5184,7 +5174,7 @@
       <c r="A55" s="17">
         <v>54</v>
       </c>
-      <c r="B55" s="109" t="s">
+      <c r="B55" s="24" t="s">
         <v>428</v>
       </c>
       <c r="C55" s="17" t="s">
@@ -5211,7 +5201,7 @@
       <c r="A56" s="17">
         <v>55</v>
       </c>
-      <c r="B56" s="109" t="s">
+      <c r="B56" s="24" t="s">
         <v>427</v>
       </c>
       <c r="C56" s="17" t="s">
@@ -5238,7 +5228,7 @@
       <c r="A57" s="17">
         <v>56</v>
       </c>
-      <c r="B57" s="109" t="s">
+      <c r="B57" s="24" t="s">
         <v>563</v>
       </c>
       <c r="C57" s="17" t="s">
@@ -5265,7 +5255,7 @@
       <c r="A58" s="17">
         <v>57</v>
       </c>
-      <c r="B58" s="109" t="s">
+      <c r="B58" s="24" t="s">
         <v>564</v>
       </c>
       <c r="C58" s="17" t="s">
@@ -5292,7 +5282,7 @@
       <c r="A59" s="17">
         <v>58</v>
       </c>
-      <c r="B59" s="109" t="s">
+      <c r="B59" s="24" t="s">
         <v>565</v>
       </c>
       <c r="C59" s="17" t="s">
@@ -5319,7 +5309,7 @@
       <c r="A60" s="17">
         <v>59</v>
       </c>
-      <c r="B60" s="109" t="s">
+      <c r="B60" s="24" t="s">
         <v>567</v>
       </c>
       <c r="C60" s="17" t="s">
@@ -5346,7 +5336,7 @@
       <c r="A61" s="17">
         <v>60</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="44" t="s">
         <v>569</v>
       </c>
       <c r="C61" s="17" t="s">
@@ -5373,7 +5363,7 @@
       <c r="A62" s="17">
         <v>61</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="44" t="s">
         <v>573</v>
       </c>
       <c r="C62" s="17" t="s">
@@ -5400,7 +5390,7 @@
       <c r="A63" s="17">
         <v>62</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="44" t="s">
         <v>575</v>
       </c>
       <c r="C63" s="17" t="s">
@@ -5427,7 +5417,7 @@
       <c r="A64" s="17">
         <v>63</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="44" t="s">
         <v>577</v>
       </c>
       <c r="C64" s="17" t="s">
@@ -5454,7 +5444,7 @@
       <c r="A65" s="17">
         <v>64</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="44" t="s">
         <v>578</v>
       </c>
       <c r="C65" s="17" t="s">
@@ -5481,7 +5471,7 @@
       <c r="A66" s="17">
         <v>65</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="44" t="s">
         <v>581</v>
       </c>
       <c r="C66" s="17" t="s">
@@ -5508,7 +5498,7 @@
       <c r="A67" s="17">
         <v>66</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="44" t="s">
         <v>583</v>
       </c>
       <c r="C67" s="17" t="s">
@@ -5535,7 +5525,7 @@
       <c r="A68" s="17">
         <v>67</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="44" t="s">
         <v>585</v>
       </c>
       <c r="C68" s="17" t="s">
@@ -5562,7 +5552,7 @@
       <c r="A69" s="17">
         <v>68</v>
       </c>
-      <c r="B69" s="109" t="s">
+      <c r="B69" s="24" t="s">
         <v>587</v>
       </c>
       <c r="C69" s="17" t="s">
@@ -5589,7 +5579,7 @@
       <c r="A70" s="17">
         <v>69</v>
       </c>
-      <c r="B70" s="109" t="s">
+      <c r="B70" s="24" t="s">
         <v>589</v>
       </c>
       <c r="C70" s="17" t="s">
@@ -5616,7 +5606,7 @@
       <c r="A71" s="17">
         <v>70</v>
       </c>
-      <c r="B71" s="109" t="s">
+      <c r="B71" s="24" t="s">
         <v>591</v>
       </c>
       <c r="C71" s="17" t="s">
@@ -5643,7 +5633,7 @@
       <c r="A72" s="17">
         <v>71</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="44" t="s">
         <v>594</v>
       </c>
       <c r="C72" s="17" t="s">
@@ -5670,7 +5660,7 @@
       <c r="A73" s="17">
         <v>72</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="44" t="s">
         <v>596</v>
       </c>
       <c r="C73" s="17" t="s">
@@ -5697,7 +5687,7 @@
       <c r="A74" s="17">
         <v>73</v>
       </c>
-      <c r="B74" s="110" t="s">
+      <c r="B74" s="15" t="s">
         <v>598</v>
       </c>
       <c r="C74" s="17" t="s">
@@ -5724,7 +5714,7 @@
       <c r="A75" s="17">
         <v>74</v>
       </c>
-      <c r="B75" s="109" t="s">
+      <c r="B75" s="24" t="s">
         <v>600</v>
       </c>
       <c r="C75" s="17" t="s">
@@ -5751,7 +5741,7 @@
       <c r="A76" s="17">
         <v>75</v>
       </c>
-      <c r="B76" s="109" t="s">
+      <c r="B76" s="24" t="s">
         <v>602</v>
       </c>
       <c r="C76" s="17" t="s">
@@ -5778,7 +5768,7 @@
       <c r="A77" s="17">
         <v>76</v>
       </c>
-      <c r="B77" s="109" t="s">
+      <c r="B77" s="24" t="s">
         <v>605</v>
       </c>
       <c r="C77" s="17" t="s">
@@ -5805,7 +5795,7 @@
       <c r="A78" s="17">
         <v>77</v>
       </c>
-      <c r="B78" s="111" t="s">
+      <c r="B78" s="14" t="s">
         <v>606</v>
       </c>
       <c r="C78" s="17" t="s">
@@ -5832,7 +5822,7 @@
       <c r="A79" s="17">
         <v>78</v>
       </c>
-      <c r="B79" s="111" t="s">
+      <c r="B79" s="14" t="s">
         <v>607</v>
       </c>
       <c r="C79" s="17" t="s">
@@ -5859,7 +5849,7 @@
       <c r="A80" s="17">
         <v>79</v>
       </c>
-      <c r="B80" s="111" t="s">
+      <c r="B80" s="14" t="s">
         <v>608</v>
       </c>
       <c r="C80" s="17" t="s">
@@ -5886,7 +5876,7 @@
       <c r="A81" s="17">
         <v>80</v>
       </c>
-      <c r="B81" s="111" t="s">
+      <c r="B81" s="14" t="s">
         <v>686</v>
       </c>
       <c r="C81" s="17" t="s">
@@ -5913,7 +5903,7 @@
       <c r="A82" s="17">
         <v>81</v>
       </c>
-      <c r="B82" s="112" t="s">
+      <c r="B82" s="40" t="s">
         <v>609</v>
       </c>
       <c r="C82" s="17" t="s">
@@ -5940,7 +5930,7 @@
       <c r="A83" s="17">
         <v>82</v>
       </c>
-      <c r="B83" s="111" t="s">
+      <c r="B83" s="14" t="s">
         <v>729</v>
       </c>
       <c r="C83" s="17" t="s">
@@ -5967,7 +5957,7 @@
       <c r="A84" s="17">
         <v>83</v>
       </c>
-      <c r="B84" s="112" t="s">
+      <c r="B84" s="40" t="s">
         <v>731</v>
       </c>
       <c r="C84" s="17" t="s">
@@ -5995,7 +5985,7 @@
       <c r="A85" s="17">
         <v>84</v>
       </c>
-      <c r="B85" s="112" t="s">
+      <c r="B85" s="40" t="s">
         <v>732</v>
       </c>
       <c r="C85" s="17" t="s">
@@ -6023,7 +6013,7 @@
       <c r="A86" s="17">
         <v>85</v>
       </c>
-      <c r="B86" s="112" t="s">
+      <c r="B86" s="40" t="s">
         <v>735</v>
       </c>
       <c r="C86" s="17" t="s">
@@ -6303,7 +6293,7 @@
       <c r="A96" s="17">
         <v>95</v>
       </c>
-      <c r="B96" s="112" t="s">
+      <c r="B96" s="40" t="s">
         <v>782</v>
       </c>
       <c r="C96" s="17" t="s">
@@ -7006,7 +6996,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="40" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C122" s="17" t="s">
         <v>35</v>
@@ -7033,7 +7023,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C123" s="17" t="s">
         <v>35</v>
@@ -7060,7 +7050,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="40" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C124" s="17" t="s">
         <v>35</v>
@@ -7087,7 +7077,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="40" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C125" s="17" t="s">
         <v>35</v>
@@ -7114,7 +7104,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C126" s="17" t="s">
         <v>35</v>
@@ -7136,38 +7126,38 @@
       <c r="J126" s="17"/>
       <c r="K126" s="17"/>
     </row>
-    <row r="127" spans="1:11" s="123" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="17">
         <v>126</v>
       </c>
-      <c r="B127" s="121" t="s">
-        <v>902</v>
+      <c r="B127" s="111" t="s">
+        <v>901</v>
       </c>
       <c r="C127" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D127" s="121" t="s">
+      <c r="D127" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="E127" s="121" t="s">
+      <c r="E127" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="F127" s="122" t="s">
+      <c r="F127" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="G127" s="121" t="s">
+      <c r="G127" s="111" t="s">
         <v>742</v>
       </c>
-      <c r="H127" s="121"/>
-      <c r="I127" s="121"/>
-      <c r="J127" s="121"/>
-      <c r="K127" s="121"/>
+      <c r="H127" s="111"/>
+      <c r="I127" s="111"/>
+      <c r="J127" s="111"/>
+      <c r="K127" s="111"/>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="17">
         <v>127</v>
       </c>
-      <c r="B128" s="113" t="s">
+      <c r="B128" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C128" s="17" t="s">
@@ -7194,7 +7184,7 @@
       <c r="A129" s="17">
         <v>128</v>
       </c>
-      <c r="B129" s="113" t="s">
+      <c r="B129" s="21" t="s">
         <v>466</v>
       </c>
       <c r="C129" s="17" t="s">
@@ -7221,7 +7211,7 @@
       <c r="A130" s="17">
         <v>129</v>
       </c>
-      <c r="B130" s="113" t="s">
+      <c r="B130" s="21" t="s">
         <v>470</v>
       </c>
       <c r="C130" s="17" t="s">
@@ -7248,7 +7238,7 @@
       <c r="A131" s="17">
         <v>130</v>
       </c>
-      <c r="B131" s="113" t="s">
+      <c r="B131" s="21" t="s">
         <v>453</v>
       </c>
       <c r="C131" s="17" t="s">
@@ -7275,7 +7265,7 @@
       <c r="A132" s="17">
         <v>131</v>
       </c>
-      <c r="B132" s="113" t="s">
+      <c r="B132" s="21" t="s">
         <v>92</v>
       </c>
       <c r="C132" s="17" t="s">
@@ -7302,7 +7292,7 @@
       <c r="A133" s="17">
         <v>132</v>
       </c>
-      <c r="B133" s="113" t="s">
+      <c r="B133" s="21" t="s">
         <v>97</v>
       </c>
       <c r="C133" s="17" t="s">
@@ -7329,7 +7319,7 @@
       <c r="A134" s="17">
         <v>133</v>
       </c>
-      <c r="B134" s="113" t="s">
+      <c r="B134" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C134" s="17" t="s">
@@ -7356,7 +7346,7 @@
       <c r="A135" s="17">
         <v>134</v>
       </c>
-      <c r="B135" s="113" t="s">
+      <c r="B135" s="21" t="s">
         <v>106</v>
       </c>
       <c r="C135" s="17" t="s">
@@ -7383,7 +7373,7 @@
       <c r="A136" s="17">
         <v>135</v>
       </c>
-      <c r="B136" s="113" t="s">
+      <c r="B136" s="21" t="s">
         <v>109</v>
       </c>
       <c r="C136" s="17" t="s">
@@ -7410,7 +7400,7 @@
       <c r="A137" s="17">
         <v>136</v>
       </c>
-      <c r="B137" s="113" t="s">
+      <c r="B137" s="21" t="s">
         <v>112</v>
       </c>
       <c r="C137" s="17" t="s">
@@ -7437,7 +7427,7 @@
       <c r="A138" s="17">
         <v>137</v>
       </c>
-      <c r="B138" s="113" t="s">
+      <c r="B138" s="21" t="s">
         <v>115</v>
       </c>
       <c r="C138" s="17" t="s">
@@ -7464,7 +7454,7 @@
       <c r="A139" s="17">
         <v>138</v>
       </c>
-      <c r="B139" s="113" t="s">
+      <c r="B139" s="21" t="s">
         <v>122</v>
       </c>
       <c r="C139" s="17" t="s">
@@ -7491,7 +7481,7 @@
       <c r="A140" s="17">
         <v>139</v>
       </c>
-      <c r="B140" s="113" t="s">
+      <c r="B140" s="21" t="s">
         <v>129</v>
       </c>
       <c r="C140" s="17" t="s">
@@ -7518,7 +7508,7 @@
       <c r="A141" s="17">
         <v>140</v>
       </c>
-      <c r="B141" s="113" t="s">
+      <c r="B141" s="21" t="s">
         <v>257</v>
       </c>
       <c r="C141" s="17" t="s">
@@ -7545,7 +7535,7 @@
       <c r="A142" s="17">
         <v>141</v>
       </c>
-      <c r="B142" s="113" t="s">
+      <c r="B142" s="21" t="s">
         <v>186</v>
       </c>
       <c r="C142" s="17" t="s">
@@ -7572,7 +7562,7 @@
       <c r="A143" s="17">
         <v>142</v>
       </c>
-      <c r="B143" s="114" t="s">
+      <c r="B143" s="115" t="s">
         <v>418</v>
       </c>
       <c r="C143" s="17" t="s">
@@ -7599,7 +7589,7 @@
       <c r="A144" s="17">
         <v>143</v>
       </c>
-      <c r="B144" s="113" t="s">
+      <c r="B144" s="21" t="s">
         <v>455</v>
       </c>
       <c r="C144" s="17" t="s">
@@ -7626,7 +7616,7 @@
       <c r="A145" s="17">
         <v>144</v>
       </c>
-      <c r="B145" s="113" t="s">
+      <c r="B145" s="21" t="s">
         <v>462</v>
       </c>
       <c r="C145" s="17" t="s">
@@ -7653,7 +7643,7 @@
       <c r="A146" s="17">
         <v>145</v>
       </c>
-      <c r="B146" s="113" t="s">
+      <c r="B146" s="21" t="s">
         <v>467</v>
       </c>
       <c r="C146" s="17" t="s">
@@ -7680,7 +7670,7 @@
       <c r="A147" s="17">
         <v>146</v>
       </c>
-      <c r="B147" s="113" t="s">
+      <c r="B147" s="21" t="s">
         <v>472</v>
       </c>
       <c r="C147" s="17" t="s">
@@ -7707,7 +7697,7 @@
       <c r="A148" s="17">
         <v>147</v>
       </c>
-      <c r="B148" s="113" t="s">
+      <c r="B148" s="21" t="s">
         <v>475</v>
       </c>
       <c r="C148" s="17" t="s">
@@ -7734,7 +7724,7 @@
       <c r="A149" s="17">
         <v>148</v>
       </c>
-      <c r="B149" s="113" t="s">
+      <c r="B149" s="21" t="s">
         <v>478</v>
       </c>
       <c r="C149" s="17" t="s">
@@ -7761,7 +7751,7 @@
       <c r="A150" s="17">
         <v>149</v>
       </c>
-      <c r="B150" s="113" t="s">
+      <c r="B150" s="21" t="s">
         <v>473</v>
       </c>
       <c r="C150" s="17" t="s">
@@ -7788,7 +7778,7 @@
       <c r="A151" s="17">
         <v>150</v>
       </c>
-      <c r="B151" s="113" t="s">
+      <c r="B151" s="21" t="s">
         <v>605</v>
       </c>
       <c r="C151" s="17" t="s">
@@ -7803,12 +7793,17 @@
       <c r="F151" s="24" t="s">
         <v>265</v>
       </c>
+      <c r="G151" s="13"/>
+      <c r="H151" s="13"/>
+      <c r="I151" s="13"/>
+      <c r="J151" s="13"/>
+      <c r="K151" s="13"/>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="17">
         <v>151</v>
       </c>
-      <c r="B152" s="113" t="s">
+      <c r="B152" s="21" t="s">
         <v>610</v>
       </c>
       <c r="C152" s="17" t="s">
@@ -7835,7 +7830,7 @@
       <c r="A153" s="17">
         <v>152</v>
       </c>
-      <c r="B153" s="113" t="s">
+      <c r="B153" s="21" t="s">
         <v>611</v>
       </c>
       <c r="C153" s="17" t="s">
@@ -7862,7 +7857,7 @@
       <c r="A154" s="17">
         <v>153</v>
       </c>
-      <c r="B154" s="113" t="s">
+      <c r="B154" s="21" t="s">
         <v>612</v>
       </c>
       <c r="C154" s="17" t="s">
@@ -7889,7 +7884,7 @@
       <c r="A155" s="17">
         <v>154</v>
       </c>
-      <c r="B155" s="113" t="s">
+      <c r="B155" s="21" t="s">
         <v>613</v>
       </c>
       <c r="C155" s="17" t="s">
@@ -7916,7 +7911,7 @@
       <c r="A156" s="17">
         <v>155</v>
       </c>
-      <c r="B156" s="113" t="s">
+      <c r="B156" s="21" t="s">
         <v>614</v>
       </c>
       <c r="C156" s="17" t="s">
@@ -7943,7 +7938,7 @@
       <c r="A157" s="17">
         <v>156</v>
       </c>
-      <c r="B157" s="113" t="s">
+      <c r="B157" s="21" t="s">
         <v>615</v>
       </c>
       <c r="C157" s="17" t="s">
@@ -7970,7 +7965,7 @@
       <c r="A158" s="17">
         <v>157</v>
       </c>
-      <c r="B158" s="113" t="s">
+      <c r="B158" s="21" t="s">
         <v>616</v>
       </c>
       <c r="C158" s="17" t="s">
@@ -7997,7 +7992,7 @@
       <c r="A159" s="17">
         <v>158</v>
       </c>
-      <c r="B159" s="113" t="s">
+      <c r="B159" s="21" t="s">
         <v>617</v>
       </c>
       <c r="C159" s="17" t="s">
@@ -8024,7 +8019,7 @@
       <c r="A160" s="17">
         <v>159</v>
       </c>
-      <c r="B160" s="113" t="s">
+      <c r="B160" s="21" t="s">
         <v>618</v>
       </c>
       <c r="C160" s="17" t="s">
@@ -8078,7 +8073,7 @@
       <c r="A162" s="17">
         <v>161</v>
       </c>
-      <c r="B162" s="115" t="s">
+      <c r="B162" s="29" t="s">
         <v>221</v>
       </c>
       <c r="C162" s="17" t="s">
@@ -8105,7 +8100,7 @@
       <c r="A163" s="17">
         <v>162</v>
       </c>
-      <c r="B163" s="115" t="s">
+      <c r="B163" s="29" t="s">
         <v>420</v>
       </c>
       <c r="C163" s="17" t="s">
@@ -8132,7 +8127,7 @@
       <c r="A164" s="17">
         <v>163</v>
       </c>
-      <c r="B164" s="115" t="s">
+      <c r="B164" s="29" t="s">
         <v>421</v>
       </c>
       <c r="C164" s="17" t="s">
@@ -8159,7 +8154,7 @@
       <c r="A165" s="17">
         <v>164</v>
       </c>
-      <c r="B165" s="115" t="s">
+      <c r="B165" s="29" t="s">
         <v>422</v>
       </c>
       <c r="C165" s="17" t="s">
@@ -8186,7 +8181,7 @@
       <c r="A166" s="17">
         <v>165</v>
       </c>
-      <c r="B166" s="115" t="s">
+      <c r="B166" s="29" t="s">
         <v>423</v>
       </c>
       <c r="C166" s="17" t="s">
@@ -8213,7 +8208,7 @@
       <c r="A167" s="17">
         <v>166</v>
       </c>
-      <c r="B167" s="115" t="s">
+      <c r="B167" s="29" t="s">
         <v>419</v>
       </c>
       <c r="C167" s="17" t="s">
@@ -8240,7 +8235,7 @@
       <c r="A168" s="17">
         <v>167</v>
       </c>
-      <c r="B168" s="115" t="s">
+      <c r="B168" s="29" t="s">
         <v>424</v>
       </c>
       <c r="C168" s="17" t="s">
@@ -8267,7 +8262,7 @@
       <c r="A169" s="17">
         <v>168</v>
       </c>
-      <c r="B169" s="115" t="s">
+      <c r="B169" s="29" t="s">
         <v>425</v>
       </c>
       <c r="C169" s="17" t="s">
@@ -8294,7 +8289,7 @@
       <c r="A170" s="17">
         <v>169</v>
       </c>
-      <c r="B170" s="116" t="s">
+      <c r="B170" s="30" t="s">
         <v>426</v>
       </c>
       <c r="C170" s="17" t="s">
@@ -8318,24 +8313,33 @@
       <c r="K170" s="28"/>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A171" s="124">
+      <c r="A171" s="17">
         <v>170</v>
       </c>
-      <c r="B171" s="78" t="s">
-        <v>920</v>
-      </c>
-      <c r="C171" s="124" t="s">
+      <c r="B171" s="29" t="s">
+        <v>918</v>
+      </c>
+      <c r="C171" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D171" s="125" t="s">
+      <c r="D171" s="29" t="s">
         <v>2</v>
       </c>
       <c r="E171" s="30" t="s">
         <v>40</v>
       </c>
       <c r="F171" s="24" t="s">
-        <v>265</v>
-      </c>
+        <v>921</v>
+      </c>
+      <c r="G171" s="13" t="s">
+        <v>923</v>
+      </c>
+      <c r="H171" s="13" t="s">
+        <v>922</v>
+      </c>
+      <c r="I171" s="13"/>
+      <c r="J171" s="13"/>
+      <c r="K171" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -8435,8 +8439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
   <dimension ref="A1:EP128"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127:XFD128"/>
+    <sheetView topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13152,12 +13156,12 @@
         <v>35</v>
       </c>
       <c r="EA21" s="13" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="EB21" s="13"/>
       <c r="EC21" s="13"/>
       <c r="ED21" s="13" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="EE21" s="44" t="s">
         <v>35</v>
@@ -19899,10 +19903,10 @@
       </c>
       <c r="M57" s="44"/>
       <c r="T57" s="44"/>
-      <c r="U57" s="118"/>
-      <c r="V57" s="118"/>
-      <c r="W57" s="118"/>
-      <c r="X57" s="118"/>
+      <c r="U57" s="108"/>
+      <c r="V57" s="108"/>
+      <c r="W57" s="108"/>
+      <c r="X57" s="108"/>
       <c r="AI57" s="36" t="s">
         <v>559</v>
       </c>
@@ -20108,10 +20112,10 @@
         <v>205</v>
       </c>
       <c r="T59" s="44"/>
-      <c r="U59" s="118"/>
-      <c r="V59" s="118"/>
-      <c r="W59" s="118"/>
-      <c r="X59" s="118"/>
+      <c r="U59" s="108"/>
+      <c r="V59" s="108"/>
+      <c r="W59" s="108"/>
+      <c r="X59" s="108"/>
       <c r="AC59" s="14" t="s">
         <v>2</v>
       </c>
@@ -20239,10 +20243,10 @@
         <v>205</v>
       </c>
       <c r="T60" s="44"/>
-      <c r="U60" s="118"/>
-      <c r="V60" s="118"/>
-      <c r="W60" s="118"/>
-      <c r="X60" s="118"/>
+      <c r="U60" s="108"/>
+      <c r="V60" s="108"/>
+      <c r="W60" s="108"/>
+      <c r="X60" s="108"/>
       <c r="AC60" s="14" t="s">
         <v>2</v>
       </c>
@@ -20337,10 +20341,10 @@
         <v>620</v>
       </c>
       <c r="T61" s="44"/>
-      <c r="U61" s="118"/>
-      <c r="V61" s="118"/>
-      <c r="W61" s="118"/>
-      <c r="X61" s="118"/>
+      <c r="U61" s="108"/>
+      <c r="V61" s="108"/>
+      <c r="W61" s="108"/>
+      <c r="X61" s="108"/>
       <c r="AM61" s="34"/>
       <c r="AX61" s="15"/>
       <c r="BB61" s="44"/>
@@ -25024,7 +25028,7 @@
       <c r="D91" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E91" s="119" t="s">
+      <c r="E91" s="109" t="s">
         <v>757</v>
       </c>
       <c r="F91" s="36"/>
@@ -25184,7 +25188,7 @@
       <c r="D92" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E92" s="119"/>
+      <c r="E92" s="109"/>
       <c r="F92" s="36"/>
       <c r="G92" s="15"/>
       <c r="H92" s="15"/>
@@ -25336,7 +25340,7 @@
       <c r="D93" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E93" s="119"/>
+      <c r="E93" s="109"/>
       <c r="F93" s="36"/>
       <c r="G93" s="15"/>
       <c r="H93" s="15"/>
@@ -25488,7 +25492,7 @@
       <c r="D94" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E94" s="119"/>
+      <c r="E94" s="109"/>
       <c r="F94" s="36"/>
       <c r="G94" s="15"/>
       <c r="H94" s="15"/>
@@ -25640,7 +25644,7 @@
       <c r="D95" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E95" s="119"/>
+      <c r="E95" s="109"/>
       <c r="F95" s="36"/>
       <c r="G95" s="15"/>
       <c r="H95" s="15"/>
@@ -25950,7 +25954,7 @@
       <c r="D97" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="119" t="s">
+      <c r="E97" s="109" t="s">
         <v>757</v>
       </c>
       <c r="F97" s="36"/>
@@ -26272,7 +26276,7 @@
       <c r="D99" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E99" s="119"/>
+      <c r="E99" s="109"/>
       <c r="F99" s="36"/>
       <c r="G99" s="15"/>
       <c r="H99" s="15"/>
@@ -26424,7 +26428,7 @@
       <c r="D100" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E100" s="119"/>
+      <c r="E100" s="109"/>
       <c r="F100" s="36"/>
       <c r="G100" s="15"/>
       <c r="H100" s="15"/>
@@ -26576,7 +26580,7 @@
       <c r="D101" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E101" s="119"/>
+      <c r="E101" s="109"/>
       <c r="F101" s="36"/>
       <c r="G101" s="15"/>
       <c r="H101" s="15"/>
@@ -26728,7 +26732,7 @@
       <c r="D102" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E102" s="119"/>
+      <c r="E102" s="109"/>
       <c r="F102" s="36"/>
       <c r="G102" s="15"/>
       <c r="H102" s="15"/>
@@ -27302,7 +27306,7 @@
       <c r="D105" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E105" s="119" t="s">
+      <c r="E105" s="109" t="s">
         <v>808</v>
       </c>
       <c r="F105" s="36"/>
@@ -27468,7 +27472,7 @@
       <c r="D106" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E106" s="119" t="s">
+      <c r="E106" s="109" t="s">
         <v>817</v>
       </c>
       <c r="F106" s="36"/>
@@ -28868,7 +28872,7 @@
         <v>852</v>
       </c>
       <c r="EB114" s="36"/>
-      <c r="EC114" s="120" t="s">
+      <c r="EC114" s="110" t="s">
         <v>851</v>
       </c>
       <c r="ED114" s="15"/>
@@ -29026,7 +29030,7 @@
         <v>856</v>
       </c>
       <c r="EB115" s="36"/>
-      <c r="EC115" s="120"/>
+      <c r="EC115" s="110"/>
       <c r="ED115" s="15"/>
       <c r="EE115" s="15"/>
       <c r="EF115" s="92"/>
@@ -29182,7 +29186,7 @@
         <v>860</v>
       </c>
       <c r="EB116" s="36"/>
-      <c r="EC116" s="120"/>
+      <c r="EC116" s="110"/>
       <c r="ED116" s="15"/>
       <c r="EE116" s="15"/>
       <c r="EF116" s="92"/>
@@ -29984,7 +29988,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="40" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C122" s="32" t="s">
         <v>320</v>
@@ -29994,13 +29998,13 @@
       </c>
       <c r="E122" s="13"/>
       <c r="F122" s="36" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="G122" s="15"/>
       <c r="H122" s="15"/>
       <c r="I122" s="15"/>
       <c r="J122" s="40" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="K122" s="15"/>
       <c r="L122" s="15"/>
@@ -30124,9 +30128,9 @@
       <c r="DZ122" s="15"/>
       <c r="EA122" s="36"/>
       <c r="EB122" s="36"/>
-      <c r="EC122" s="120"/>
+      <c r="EC122" s="110"/>
       <c r="ED122" s="36" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="EE122" s="15"/>
       <c r="EF122" s="92"/>
@@ -30140,7 +30144,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C123" s="32" t="s">
         <v>320</v>
@@ -30150,13 +30154,13 @@
       </c>
       <c r="E123" s="13"/>
       <c r="F123" s="36" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="G123" s="15"/>
       <c r="H123" s="15"/>
       <c r="I123" s="15"/>
       <c r="J123" s="40" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="K123" s="15"/>
       <c r="L123" s="15"/>
@@ -30280,9 +30284,9 @@
       <c r="DZ123" s="15"/>
       <c r="EA123" s="36"/>
       <c r="EB123" s="36"/>
-      <c r="EC123" s="120"/>
+      <c r="EC123" s="110"/>
       <c r="ED123" s="15" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="EE123" s="15"/>
       <c r="EF123" s="92"/>
@@ -30296,7 +30300,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="40" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C124" s="32" t="s">
         <v>320</v>
@@ -30306,13 +30310,13 @@
       </c>
       <c r="E124" s="13"/>
       <c r="F124" s="36" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="G124" s="15"/>
       <c r="H124" s="15"/>
       <c r="I124" s="15"/>
       <c r="J124" s="40" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="K124" s="15"/>
       <c r="L124" s="15"/>
@@ -30436,9 +30440,9 @@
       <c r="DZ124" s="15"/>
       <c r="EA124" s="36"/>
       <c r="EB124" s="36"/>
-      <c r="EC124" s="120"/>
+      <c r="EC124" s="110"/>
       <c r="ED124" s="15" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="EE124" s="15"/>
       <c r="EF124" s="92"/>
@@ -30452,7 +30456,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="40" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C125" s="32" t="s">
         <v>320</v>
@@ -30468,7 +30472,7 @@
       <c r="H125" s="15"/>
       <c r="I125" s="15"/>
       <c r="J125" s="40" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="K125" s="15" t="s">
         <v>877</v>
@@ -30596,7 +30600,7 @@
       <c r="EB125" s="36"/>
       <c r="EC125" s="36"/>
       <c r="ED125" s="36" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="EE125" s="15"/>
       <c r="EF125" s="92"/>
@@ -30610,7 +30614,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C126" s="32" t="s">
         <v>320</v>
@@ -30626,10 +30630,10 @@
       <c r="H126" s="15"/>
       <c r="I126" s="15"/>
       <c r="J126" s="40" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="K126" s="15" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="L126" s="15"/>
       <c r="M126" s="15"/>
@@ -30754,7 +30758,7 @@
       <c r="EB126" s="36"/>
       <c r="EC126" s="36"/>
       <c r="ED126" s="36" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="EE126" s="15"/>
       <c r="EF126" s="92"/>
@@ -30768,7 +30772,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="40" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C127" s="32" t="s">
         <v>320</v>
@@ -30782,10 +30786,10 @@
       <c r="H127" s="15"/>
       <c r="I127" s="15"/>
       <c r="J127" s="40" t="s">
+        <v>902</v>
+      </c>
+      <c r="K127" s="15" t="s">
         <v>903</v>
-      </c>
-      <c r="K127" s="15" t="s">
-        <v>904</v>
       </c>
       <c r="L127" s="15"/>
       <c r="M127" s="15"/>
@@ -30810,7 +30814,7 @@
       <c r="AF127" s="15"/>
       <c r="AG127" s="15"/>
       <c r="AH127" s="15" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AI127" s="36"/>
       <c r="AJ127" s="15"/>
@@ -30824,13 +30828,13 @@
         <v>48</v>
       </c>
       <c r="AR127" s="15" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AS127" s="15" t="s">
         <v>35</v>
       </c>
       <c r="AT127" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="AU127" s="15"/>
       <c r="AV127" s="15"/>
@@ -30936,7 +30940,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="40" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C128" s="32" t="s">
         <v>298</v>
@@ -30950,7 +30954,7 @@
       <c r="H128" s="15"/>
       <c r="I128" s="15"/>
       <c r="J128" s="40" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="K128" s="15"/>
       <c r="L128" s="15"/>
@@ -31126,7 +31130,9 @@
       <c r="DX128" s="15"/>
       <c r="DY128" s="15"/>
       <c r="DZ128" s="15"/>
-      <c r="EA128" s="36"/>
+      <c r="EA128" s="36" t="s">
+        <v>920</v>
+      </c>
       <c r="EB128" s="36"/>
       <c r="EC128" s="36"/>
       <c r="ED128" s="36"/>
@@ -35597,24 +35603,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -35848,25 +35836,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC0974DE-324A-423C-B9D7-F4F768EFCB0A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35884,4 +35872,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Committing the Account number test cases
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fahmed2\git\Dynamics-CRM-Cloud Apr18\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\Dynamics-CRM-Cloud\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396A47D9-2DA5-421E-9107-CB5F5AC35612}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4057BA-C65D-4F2D-BC3F-7D993DEE3DD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4424" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4624" uniqueCount="972">
   <si>
     <t>Premier1a</t>
   </si>
@@ -2881,6 +2881,81 @@
   </si>
   <si>
     <t>2022_04_21_06_51_09</t>
+  </si>
+  <si>
+    <t>TFS ID_8905:Cloud: Verify DEA expiration date is displayed in the search result screen</t>
+  </si>
+  <si>
+    <t>TFS ID_8910_Cloud: Validate Check Digit on Account Number</t>
+  </si>
+  <si>
+    <t>TFS ID_8903_Cloud: Verify a new field "Calculated Name" in Account Number Entity</t>
+  </si>
+  <si>
+    <t>TFS ID_8909_Cloud: Verify if HIN accepts Characters, Numbers, Alphanumeric values but it should be 9 char in length</t>
+  </si>
+  <si>
+    <t>TFS ID_8907_Cloud: Verify if DEA and HIN numbers are displayed in the member form</t>
+  </si>
+  <si>
+    <t>TFS ID_8908_Cloud: Verify DEA and HIN number field are available in the Accounts view</t>
+  </si>
+  <si>
+    <t>TFS ID_8978_Cloud: Verify all type of Account Rep types</t>
+  </si>
+  <si>
+    <t>TFS ID_8997_Automation_Cloud: Verify user should not be allowed to change the account status to Active manually when Premier End date is present</t>
+  </si>
+  <si>
+    <t>AI3630</t>
+  </si>
+  <si>
+    <t>CheckDigitonAccountNumber</t>
+  </si>
+  <si>
+    <t>2000004929</t>
+  </si>
+  <si>
+    <t>CheckCalculatedName</t>
+  </si>
+  <si>
+    <t>CheckHIN</t>
+  </si>
+  <si>
+    <t>VerifyDEAinMemberForm</t>
+  </si>
+  <si>
+    <t>1000172270</t>
+  </si>
+  <si>
+    <t>FD1950092</t>
+  </si>
+  <si>
+    <t>AB2276990</t>
+  </si>
+  <si>
+    <t>6HK7P3603</t>
+  </si>
+  <si>
+    <t>AB26769989876</t>
+  </si>
+  <si>
+    <t>AB3456</t>
+  </si>
+  <si>
+    <t>816440160</t>
+  </si>
+  <si>
+    <t>vf7672442</t>
+  </si>
+  <si>
+    <t>837295004</t>
+  </si>
+  <si>
+    <t>MP2448555</t>
+  </si>
+  <si>
+    <t>8089Q8N00</t>
   </si>
 </sst>
 </file>
@@ -3200,7 +3275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3401,6 +3476,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3722,10 +3799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
-  <dimension ref="A1:P175"/>
+  <dimension ref="A1:P183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B134" sqref="B134"/>
+    <sheetView tabSelected="1" topLeftCell="A168" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8522,9 +8599,193 @@
       <c r="J175" s="13"/>
       <c r="K175" s="13"/>
     </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A176" s="117">
+        <v>174</v>
+      </c>
+      <c r="B176" s="116" t="s">
+        <v>947</v>
+      </c>
+      <c r="C176" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D176" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E176" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F176" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="G176" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="17">
+        <v>175</v>
+      </c>
+      <c r="B177" s="116" t="s">
+        <v>948</v>
+      </c>
+      <c r="C177" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D177" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E177" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F177" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="G177" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="17">
+        <v>176</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="C178" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D178" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E178" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F178" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="G178" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="117">
+        <v>177</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="C179" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D179" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E179" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F179" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="G179" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="17">
+        <v>178</v>
+      </c>
+      <c r="B180" s="116" t="s">
+        <v>951</v>
+      </c>
+      <c r="C180" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D180" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E180" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F180" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="G180" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" s="17">
+        <v>179</v>
+      </c>
+      <c r="B181" s="116" t="s">
+        <v>952</v>
+      </c>
+      <c r="C181" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D181" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E181" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F181" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="G181" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" s="117">
+        <v>180</v>
+      </c>
+      <c r="B182" s="116" t="s">
+        <v>953</v>
+      </c>
+      <c r="C182" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D182" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E182" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F182" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="G182" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="17">
+        <v>181</v>
+      </c>
+      <c r="B183" s="116" t="s">
+        <v>954</v>
+      </c>
+      <c r="C183" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D183" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E183" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F183" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="G183" t="s">
+        <v>742</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C175" xr:uid="{C9334235-52FB-4F10-8331-5687DC05318C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C183" xr:uid="{C9334235-52FB-4F10-8331-5687DC05318C}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8618,10 +8879,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
-  <dimension ref="A1:EQ130"/>
+  <dimension ref="A1:EQ138"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+    <sheetView topLeftCell="A120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31444,7 +31705,7 @@
       <c r="EJ128" s="15"/>
       <c r="EK128" s="90"/>
     </row>
-    <row r="129" spans="1:141" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:143" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <v>128</v>
       </c>
@@ -31607,7 +31868,7 @@
       <c r="EJ129" s="15"/>
       <c r="EK129" s="15"/>
     </row>
-    <row r="130" spans="1:141" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:143" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <v>129</v>
       </c>
@@ -31768,6 +32029,854 @@
       <c r="EJ130" s="15"/>
       <c r="EK130" s="15"/>
     </row>
+    <row r="131" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>130</v>
+      </c>
+      <c r="B131" s="116" t="s">
+        <v>947</v>
+      </c>
+      <c r="C131" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="D131" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI131" s="81" t="s">
+        <v>955</v>
+      </c>
+      <c r="EA131" s="81" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="132" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="A132" s="15">
+        <v>131</v>
+      </c>
+      <c r="B132" s="116" t="s">
+        <v>948</v>
+      </c>
+      <c r="C132" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="D132" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J132" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="N132" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="O132" s="33"/>
+      <c r="P132" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q132" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="R132" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="S132" s="15"/>
+      <c r="T132" s="15"/>
+      <c r="U132" s="15"/>
+      <c r="V132" s="15"/>
+      <c r="W132" s="15"/>
+      <c r="X132" s="15"/>
+      <c r="Y132" s="15"/>
+      <c r="Z132" s="15"/>
+      <c r="AA132" s="15"/>
+      <c r="AB132" s="15"/>
+      <c r="AC132" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD132" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE132" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF132" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG132" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH132" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI132" s="36" t="s">
+        <v>957</v>
+      </c>
+      <c r="AJ132" s="15"/>
+      <c r="AK132" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AL132" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AM132" s="34"/>
+      <c r="AN132" s="15"/>
+      <c r="AO132" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="AP132" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AQ132" s="15"/>
+      <c r="AR132" s="15"/>
+      <c r="AS132" s="15"/>
+      <c r="AT132" s="15"/>
+      <c r="AU132" s="15"/>
+      <c r="AV132" s="15"/>
+      <c r="AW132" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX132" s="15"/>
+      <c r="AY132" s="15"/>
+      <c r="AZ132" s="15"/>
+      <c r="BA132" s="15"/>
+      <c r="BB132" s="15"/>
+      <c r="BC132" s="15"/>
+      <c r="BD132" s="15"/>
+      <c r="BE132" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF132" s="15"/>
+      <c r="BG132" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BH132" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BI132" s="15"/>
+      <c r="BJ132" s="15"/>
+      <c r="BK132" s="15" t="s">
+        <v>558</v>
+      </c>
+      <c r="BL132" s="15" t="s">
+        <v>560</v>
+      </c>
+      <c r="BM132" s="15"/>
+      <c r="BN132" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BO132" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BP132" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ132" s="34"/>
+      <c r="BR132" s="34"/>
+      <c r="BS132" s="34"/>
+      <c r="BT132" s="34"/>
+      <c r="BU132" s="34"/>
+      <c r="BV132" s="34"/>
+      <c r="BW132" s="34"/>
+      <c r="BX132" s="34"/>
+      <c r="BY132" s="34"/>
+      <c r="BZ132" s="34"/>
+      <c r="CA132" s="34"/>
+      <c r="CB132" s="34"/>
+      <c r="CC132" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="CD132" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="CE132" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="CF132" s="15"/>
+      <c r="CG132" s="34"/>
+      <c r="CH132" s="34"/>
+      <c r="CI132" s="34"/>
+      <c r="CJ132" s="34"/>
+      <c r="CK132" s="34"/>
+      <c r="CL132" s="34"/>
+      <c r="CM132" s="34"/>
+      <c r="CN132" s="15"/>
+      <c r="CO132" s="15"/>
+      <c r="CP132" s="15"/>
+      <c r="CQ132" s="15"/>
+      <c r="CR132" s="15"/>
+      <c r="CS132" s="15"/>
+      <c r="CT132" s="15"/>
+      <c r="CU132" s="15"/>
+      <c r="CV132" s="15"/>
+      <c r="CW132" s="15"/>
+      <c r="CX132" s="15"/>
+      <c r="CY132" s="15"/>
+      <c r="CZ132" s="15"/>
+      <c r="DA132" s="15"/>
+      <c r="DB132" s="15"/>
+      <c r="DC132" s="15"/>
+      <c r="DD132" s="15"/>
+      <c r="DE132" s="15"/>
+      <c r="DF132" s="15"/>
+      <c r="DG132" s="15"/>
+      <c r="DH132" s="15"/>
+      <c r="DI132" s="15"/>
+      <c r="DJ132" s="15"/>
+      <c r="DK132" s="15"/>
+      <c r="DL132" s="15"/>
+      <c r="DM132" s="15"/>
+      <c r="DN132" s="15"/>
+      <c r="DO132" s="15"/>
+      <c r="DP132" s="15"/>
+      <c r="DQ132" s="15"/>
+      <c r="DR132" s="15"/>
+      <c r="DS132" s="15"/>
+      <c r="DT132" s="15"/>
+      <c r="DU132" s="15"/>
+      <c r="DV132" s="15"/>
+      <c r="DW132" s="15"/>
+      <c r="DX132" s="15"/>
+      <c r="EA132" s="81" t="s">
+        <v>963</v>
+      </c>
+      <c r="ED132" s="36" t="s">
+        <v>964</v>
+      </c>
+      <c r="EK132" s="81" t="s">
+        <v>965</v>
+      </c>
+      <c r="EL132" s="81" t="s">
+        <v>965</v>
+      </c>
+      <c r="EM132" s="81" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="133" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="A133" s="15">
+        <v>132</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="C133" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="D133" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J133" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="N133" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="O133" s="33"/>
+      <c r="P133" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q133" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="R133" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="S133" s="15"/>
+      <c r="T133" s="15"/>
+      <c r="U133" s="15"/>
+      <c r="V133" s="15"/>
+      <c r="W133" s="15"/>
+      <c r="X133" s="15"/>
+      <c r="Y133" s="15"/>
+      <c r="Z133" s="15"/>
+      <c r="AA133" s="15"/>
+      <c r="AB133" s="15"/>
+      <c r="AC133" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD133" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE133" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF133" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG133" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH133" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI133" s="36" t="s">
+        <v>957</v>
+      </c>
+      <c r="AJ133" s="15"/>
+      <c r="AK133" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AL133" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AM133" s="34"/>
+      <c r="AN133" s="15"/>
+      <c r="AO133" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="AP133" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AQ133" s="15"/>
+      <c r="AR133" s="15"/>
+      <c r="AS133" s="15"/>
+      <c r="AT133" s="15"/>
+      <c r="AU133" s="15"/>
+      <c r="AV133" s="15"/>
+      <c r="AW133" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX133" s="15"/>
+      <c r="AY133" s="15"/>
+      <c r="AZ133" s="15"/>
+      <c r="BA133" s="15"/>
+      <c r="BB133" s="15"/>
+      <c r="BC133" s="15"/>
+      <c r="BD133" s="15"/>
+      <c r="BE133" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF133" s="15"/>
+      <c r="BG133" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BH133" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BI133" s="15"/>
+      <c r="BJ133" s="15"/>
+      <c r="BK133" s="15" t="s">
+        <v>558</v>
+      </c>
+      <c r="BL133" s="15" t="s">
+        <v>560</v>
+      </c>
+      <c r="BM133" s="15"/>
+      <c r="BN133" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BO133" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BP133" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ133" s="34"/>
+      <c r="BR133" s="34"/>
+      <c r="BS133" s="34"/>
+      <c r="BT133" s="34"/>
+      <c r="BU133" s="34"/>
+      <c r="BV133" s="34"/>
+      <c r="BW133" s="34"/>
+      <c r="BX133" s="34"/>
+      <c r="BY133" s="34"/>
+      <c r="BZ133" s="34"/>
+      <c r="CA133" s="34"/>
+      <c r="CB133" s="34"/>
+      <c r="CC133" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="CD133" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="CE133" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="CF133" s="15"/>
+      <c r="CG133" s="34"/>
+      <c r="CH133" s="34"/>
+      <c r="CI133" s="34"/>
+      <c r="CJ133" s="34"/>
+      <c r="CK133" s="34"/>
+      <c r="CL133" s="34"/>
+      <c r="CM133" s="34"/>
+      <c r="CN133" s="15"/>
+      <c r="CO133" s="15"/>
+      <c r="CP133" s="15"/>
+      <c r="CQ133" s="15"/>
+      <c r="CR133" s="15"/>
+      <c r="CS133" s="15"/>
+      <c r="CT133" s="15"/>
+      <c r="CU133" s="15"/>
+      <c r="CV133" s="15"/>
+      <c r="CW133" s="15"/>
+      <c r="CX133" s="15"/>
+      <c r="CY133" s="15"/>
+      <c r="CZ133" s="15"/>
+      <c r="DA133" s="15"/>
+      <c r="DB133" s="15"/>
+      <c r="DC133" s="15"/>
+      <c r="DD133" s="15"/>
+      <c r="DE133" s="15"/>
+      <c r="DF133" s="15"/>
+      <c r="DG133" s="15"/>
+      <c r="DH133" s="15"/>
+      <c r="DI133" s="15"/>
+      <c r="DJ133" s="15"/>
+      <c r="DK133" s="15"/>
+      <c r="DL133" s="15"/>
+      <c r="DM133" s="15"/>
+      <c r="DN133" s="15"/>
+      <c r="DO133" s="15"/>
+      <c r="DP133" s="15"/>
+      <c r="DQ133" s="15"/>
+      <c r="DR133" s="15"/>
+      <c r="DS133" s="15"/>
+      <c r="DT133" s="15"/>
+      <c r="DU133" s="15"/>
+      <c r="DV133" s="15"/>
+      <c r="DW133" s="15"/>
+      <c r="DX133" s="15"/>
+      <c r="EL133" s="2" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="134" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>133</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="C134" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="D134" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J134" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="N134" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="O134" s="33"/>
+      <c r="P134" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q134" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="R134" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="S134" s="15"/>
+      <c r="T134" s="15"/>
+      <c r="U134" s="15"/>
+      <c r="V134" s="15"/>
+      <c r="W134" s="15"/>
+      <c r="X134" s="15"/>
+      <c r="Y134" s="15"/>
+      <c r="Z134" s="15"/>
+      <c r="AA134" s="15"/>
+      <c r="AB134" s="15"/>
+      <c r="AC134" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD134" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE134" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF134" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG134" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH134" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI134" s="36" t="s">
+        <v>957</v>
+      </c>
+      <c r="AJ134" s="15"/>
+      <c r="AK134" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AL134" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AM134" s="34"/>
+      <c r="AN134" s="15"/>
+      <c r="AO134" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="AP134" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AQ134" s="15"/>
+      <c r="AR134" s="15"/>
+      <c r="AS134" s="15"/>
+      <c r="AT134" s="15"/>
+      <c r="AU134" s="15"/>
+      <c r="AV134" s="15"/>
+      <c r="AW134" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX134" s="15"/>
+      <c r="AY134" s="15"/>
+      <c r="AZ134" s="15"/>
+      <c r="BA134" s="15"/>
+      <c r="BB134" s="15"/>
+      <c r="BC134" s="15"/>
+      <c r="BD134" s="15"/>
+      <c r="BE134" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF134" s="15"/>
+      <c r="BG134" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BH134" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BI134" s="15"/>
+      <c r="BJ134" s="15"/>
+      <c r="BK134" s="15" t="s">
+        <v>558</v>
+      </c>
+      <c r="BL134" s="15" t="s">
+        <v>560</v>
+      </c>
+      <c r="BM134" s="15"/>
+      <c r="BN134" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BO134" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BP134" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ134" s="34"/>
+      <c r="BR134" s="34"/>
+      <c r="BS134" s="34"/>
+      <c r="BT134" s="34"/>
+      <c r="BU134" s="34"/>
+      <c r="BV134" s="34"/>
+      <c r="BW134" s="34"/>
+      <c r="BX134" s="34"/>
+      <c r="BY134" s="34"/>
+      <c r="BZ134" s="34"/>
+      <c r="CA134" s="34"/>
+      <c r="CB134" s="34"/>
+      <c r="CC134" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="CD134" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="CE134" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="CF134" s="15"/>
+      <c r="CG134" s="34"/>
+      <c r="CH134" s="34"/>
+      <c r="CI134" s="34"/>
+      <c r="CJ134" s="34"/>
+      <c r="CK134" s="34"/>
+      <c r="CL134" s="34"/>
+      <c r="CM134" s="34"/>
+      <c r="CN134" s="15"/>
+      <c r="CO134" s="15"/>
+      <c r="CP134" s="15"/>
+      <c r="CQ134" s="15"/>
+      <c r="CR134" s="15"/>
+      <c r="CS134" s="15"/>
+      <c r="CT134" s="15"/>
+      <c r="CU134" s="15"/>
+      <c r="CV134" s="15"/>
+      <c r="CW134" s="15"/>
+      <c r="CX134" s="15"/>
+      <c r="CY134" s="15"/>
+      <c r="CZ134" s="15"/>
+      <c r="DA134" s="15"/>
+      <c r="DB134" s="15"/>
+      <c r="DC134" s="15"/>
+      <c r="DD134" s="15"/>
+      <c r="DE134" s="15"/>
+      <c r="DF134" s="15"/>
+      <c r="DG134" s="15"/>
+      <c r="DH134" s="15"/>
+      <c r="DI134" s="15"/>
+      <c r="DJ134" s="15"/>
+      <c r="DK134" s="15"/>
+      <c r="DL134" s="15"/>
+      <c r="DM134" s="15"/>
+      <c r="DN134" s="15"/>
+      <c r="DO134" s="15"/>
+      <c r="DP134" s="15"/>
+      <c r="DQ134" s="15"/>
+      <c r="DR134" s="15"/>
+      <c r="DS134" s="15"/>
+      <c r="DT134" s="15"/>
+      <c r="DU134" s="15"/>
+      <c r="DV134" s="15"/>
+      <c r="DW134" s="15"/>
+      <c r="DX134" s="15"/>
+      <c r="ED134" t="s">
+        <v>967</v>
+      </c>
+      <c r="EL134" s="2" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="135" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="A135" s="15">
+        <v>134</v>
+      </c>
+      <c r="B135" s="116" t="s">
+        <v>951</v>
+      </c>
+      <c r="C135" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="D135" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J135" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="N135" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="O135" s="33"/>
+      <c r="P135" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q135" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="R135" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="S135" s="15"/>
+      <c r="T135" s="15"/>
+      <c r="U135" s="15"/>
+      <c r="V135" s="15"/>
+      <c r="W135" s="15"/>
+      <c r="X135" s="15"/>
+      <c r="Y135" s="15"/>
+      <c r="Z135" s="15"/>
+      <c r="AA135" s="15"/>
+      <c r="AB135" s="15"/>
+      <c r="AC135" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD135" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE135" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF135" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG135" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH135" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI135" s="36" t="s">
+        <v>957</v>
+      </c>
+      <c r="AJ135" s="15"/>
+      <c r="AK135" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AL135" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AM135" s="34"/>
+      <c r="AN135" s="15"/>
+      <c r="AO135" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="AP135" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AQ135" s="15"/>
+      <c r="AR135" s="15"/>
+      <c r="AS135" s="15"/>
+      <c r="AT135" s="15"/>
+      <c r="AU135" s="15"/>
+      <c r="AV135" s="15"/>
+      <c r="AW135" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX135" s="15"/>
+      <c r="AY135" s="15"/>
+      <c r="AZ135" s="15"/>
+      <c r="BA135" s="15"/>
+      <c r="BB135" s="15"/>
+      <c r="BC135" s="15"/>
+      <c r="BD135" s="15"/>
+      <c r="BE135" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF135" s="15"/>
+      <c r="BG135" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BH135" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BI135" s="15"/>
+      <c r="BJ135" s="15"/>
+      <c r="BK135" s="15" t="s">
+        <v>558</v>
+      </c>
+      <c r="BL135" s="15" t="s">
+        <v>560</v>
+      </c>
+      <c r="BM135" s="15"/>
+      <c r="BN135" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BO135" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BP135" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ135" s="34"/>
+      <c r="BR135" s="34"/>
+      <c r="BS135" s="34"/>
+      <c r="BT135" s="34"/>
+      <c r="BU135" s="34"/>
+      <c r="BV135" s="34"/>
+      <c r="BW135" s="34"/>
+      <c r="BX135" s="34"/>
+      <c r="BY135" s="34"/>
+      <c r="BZ135" s="34"/>
+      <c r="CA135" s="34"/>
+      <c r="CB135" s="34"/>
+      <c r="CC135" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="CD135" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="CE135" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="CF135" s="15"/>
+      <c r="CG135" s="34"/>
+      <c r="CH135" s="34"/>
+      <c r="CI135" s="34"/>
+      <c r="CJ135" s="34"/>
+      <c r="CK135" s="34"/>
+      <c r="CL135" s="34"/>
+      <c r="CM135" s="34"/>
+      <c r="CN135" s="15"/>
+      <c r="CO135" s="15"/>
+      <c r="CP135" s="15"/>
+      <c r="CQ135" s="15"/>
+      <c r="CR135" s="15"/>
+      <c r="CS135" s="15"/>
+      <c r="CT135" s="15"/>
+      <c r="CU135" s="15"/>
+      <c r="CV135" s="15"/>
+      <c r="CW135" s="15"/>
+      <c r="CX135" s="15"/>
+      <c r="CY135" s="15"/>
+      <c r="CZ135" s="15"/>
+      <c r="DA135" s="15"/>
+      <c r="DB135" s="15"/>
+      <c r="DC135" s="15"/>
+      <c r="DD135" s="15"/>
+      <c r="DE135" s="15"/>
+      <c r="DF135" s="15"/>
+      <c r="DG135" s="15"/>
+      <c r="DH135" s="15"/>
+      <c r="DI135" s="15"/>
+      <c r="DJ135" s="15"/>
+      <c r="DK135" s="15"/>
+      <c r="DL135" s="15"/>
+      <c r="DM135" s="15"/>
+      <c r="DN135" s="15"/>
+      <c r="DO135" s="15"/>
+      <c r="DP135" s="15"/>
+      <c r="DQ135" s="15"/>
+      <c r="DR135" s="15"/>
+      <c r="DS135" s="15"/>
+      <c r="DT135" s="15"/>
+      <c r="DU135" s="15"/>
+      <c r="DV135" s="15"/>
+      <c r="DW135" s="15"/>
+      <c r="DX135" s="15"/>
+      <c r="EA135" t="s">
+        <v>968</v>
+      </c>
+      <c r="ED135" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="136" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="A136" s="15">
+        <v>135</v>
+      </c>
+      <c r="B136" s="116" t="s">
+        <v>952</v>
+      </c>
+      <c r="C136" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="D136" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="EA136" s="81" t="s">
+        <v>970</v>
+      </c>
+      <c r="ED136" s="81" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="137" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <v>136</v>
+      </c>
+      <c r="B137" s="116" t="s">
+        <v>953</v>
+      </c>
+      <c r="C137" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="D137" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI137" s="36" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="138" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="A138" s="15">
+        <v>137</v>
+      </c>
+      <c r="B138" s="116" t="s">
+        <v>954</v>
+      </c>
+      <c r="C138" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="D138" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F138" s="81" t="s">
+        <v>961</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -31848,9 +32957,17 @@
     <hyperlink ref="DS21" r:id="rId75" xr:uid="{16A04B90-4C95-42FB-B108-D3A9617D5B2D}"/>
     <hyperlink ref="C128" r:id="rId76" xr:uid="{D5FAB0B7-042C-4705-9759-A05346C53411}"/>
     <hyperlink ref="E129" r:id="rId77" xr:uid="{C7344BEE-CAF7-4A3C-9480-37D7D1C32698}"/>
+    <hyperlink ref="C131" r:id="rId78" xr:uid="{A9A4A3DD-D4F8-4698-A8C7-A99B7402260C}"/>
+    <hyperlink ref="C132" r:id="rId79" xr:uid="{52562B6B-518D-4429-96DE-0623B77C68F7}"/>
+    <hyperlink ref="C133" r:id="rId80" xr:uid="{829EADEC-AD0B-4909-8DEB-DC7FC479F4E2}"/>
+    <hyperlink ref="C134" r:id="rId81" xr:uid="{967D73DA-2441-4C15-814F-1257FA9B4B56}"/>
+    <hyperlink ref="C135" r:id="rId82" xr:uid="{A8767F48-A8F6-4365-9D1B-F2D4D1235C56}"/>
+    <hyperlink ref="C136" r:id="rId83" xr:uid="{8D946F3A-D1F9-4D66-ABC7-AF602F3A9C3E}"/>
+    <hyperlink ref="C137" r:id="rId84" xr:uid="{0432B6A4-F0FA-48FB-B674-2829283EAB86}"/>
+    <hyperlink ref="C138" r:id="rId85" xr:uid="{DDF07B09-3B7C-4DAE-9733-5728B1D719AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId78"/>
+  <pageSetup orientation="portrait" r:id="rId86"/>
 </worksheet>
 </file>
 
@@ -36397,24 +37514,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -36648,25 +37747,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC0974DE-324A-423C-B9D7-F4F768EFCB0A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36684,4 +37783,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Contact Module fixes -Complete
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fahmed2\git\Dynamics_CRM_Cloud_After_Wave1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8D1EA7-E2E2-4F3A-B40B-69231E02FB10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325C8D35-B1EB-41C5-8E20-F1763A065AFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4490" uniqueCount="990">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4490" uniqueCount="995">
   <si>
     <t>Premier1a</t>
   </si>
@@ -2961,55 +2961,70 @@
     <t>2022_05_12_10_04_35</t>
   </si>
   <si>
-    <t>2022_05_12_10_12_16</t>
-  </si>
-  <si>
     <t>2022_05_12_10_15_17</t>
   </si>
   <si>
     <t>2022_05_12_10_57_07</t>
   </si>
   <si>
-    <t>2022_05_12_11_10_13</t>
-  </si>
-  <si>
-    <t>2022_05_12_02_47_37</t>
-  </si>
-  <si>
-    <t>2022_05_12_02_54_17</t>
-  </si>
-  <si>
-    <t>2022_05_12_03_38_13</t>
-  </si>
-  <si>
-    <t>2022_05_12_03_48_12</t>
-  </si>
-  <si>
-    <t>2022_05_12_03_53_27</t>
-  </si>
-  <si>
-    <t>2022_05_12_04_22_16</t>
-  </si>
-  <si>
-    <t>2022_05_12_04_28_16</t>
-  </si>
-  <si>
-    <t>2022_05_12_05_00_10</t>
-  </si>
-  <si>
-    <t>2022_05_12_05_07_03</t>
-  </si>
-  <si>
-    <t>2022_05_12_05_11_16</t>
-  </si>
-  <si>
-    <t>2022_05_12_06_17_29</t>
-  </si>
-  <si>
-    <t>2022_05_12_07_32_07</t>
-  </si>
-  <si>
     <t>2022_05_12_07_36_48</t>
+  </si>
+  <si>
+    <t>7000568142</t>
+  </si>
+  <si>
+    <t>2022_05_19_01_58_56</t>
+  </si>
+  <si>
+    <t>7000568143</t>
+  </si>
+  <si>
+    <t>2022_05_19_02_21_26</t>
+  </si>
+  <si>
+    <t>7000568144</t>
+  </si>
+  <si>
+    <t>2022_05_19_02_29_25</t>
+  </si>
+  <si>
+    <t>7000568145</t>
+  </si>
+  <si>
+    <t>2022_05_19_04_01_26</t>
+  </si>
+  <si>
+    <t>7000568146</t>
+  </si>
+  <si>
+    <t>2022_05_19_04_12_51</t>
+  </si>
+  <si>
+    <t>7000568147</t>
+  </si>
+  <si>
+    <t>2022_05_19_04_23_01</t>
+  </si>
+  <si>
+    <t>7000568148</t>
+  </si>
+  <si>
+    <t>2022_05_19_05_06_15</t>
+  </si>
+  <si>
+    <t>7000568149</t>
+  </si>
+  <si>
+    <t>2022_05_19_05_25_50</t>
+  </si>
+  <si>
+    <t>2022_05_19_05_46_18</t>
+  </si>
+  <si>
+    <t>7000568151</t>
+  </si>
+  <si>
+    <t>2022_05_19_05_59_30</t>
   </si>
 </sst>
 </file>
@@ -3861,8 +3876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
   <dimension ref="A1:P183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7946,7 +7961,7 @@
         <v>955</v>
       </c>
       <c r="G161" s="21" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H161" s="21"/>
       <c r="I161" s="21"/>
@@ -7961,7 +7976,7 @@
         <v>614</v>
       </c>
       <c r="C162" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D162" s="21" t="s">
         <v>26</v>
@@ -7973,7 +7988,7 @@
         <v>955</v>
       </c>
       <c r="G162" s="21" t="s">
-        <v>989</v>
+        <v>975</v>
       </c>
       <c r="H162" s="21"/>
       <c r="I162" s="21"/>
@@ -8000,7 +8015,7 @@
         <v>955</v>
       </c>
       <c r="G163" s="21" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="H163" s="21"/>
       <c r="I163" s="21"/>
@@ -8178,10 +8193,14 @@
         <v>40</v>
       </c>
       <c r="F170" s="17" t="s">
-        <v>264</v>
-      </c>
-      <c r="G170" s="28"/>
-      <c r="H170" s="28"/>
+        <v>955</v>
+      </c>
+      <c r="G170" s="28" t="s">
+        <v>977</v>
+      </c>
+      <c r="H170" s="28" t="s">
+        <v>976</v>
+      </c>
       <c r="I170" s="28"/>
       <c r="J170" s="28"/>
       <c r="K170" s="28"/>
@@ -8269,7 +8288,7 @@
         <v>424</v>
       </c>
       <c r="C174" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D174" s="29" t="s">
         <v>219</v>
@@ -8278,10 +8297,14 @@
         <v>40</v>
       </c>
       <c r="F174" s="17" t="s">
-        <v>264</v>
-      </c>
-      <c r="G174" s="28"/>
-      <c r="H174" s="28"/>
+        <v>955</v>
+      </c>
+      <c r="G174" s="28" t="s">
+        <v>994</v>
+      </c>
+      <c r="H174" s="28" t="s">
+        <v>993</v>
+      </c>
       <c r="I174" s="28"/>
       <c r="J174" s="28"/>
       <c r="K174" s="28"/>
@@ -37325,6 +37348,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -37558,7 +37590,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -37567,16 +37599,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC0974DE-324A-423C-B9D7-F4F768EFCB0A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37596,7 +37627,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -37604,12 +37635,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Committing the Test data sheet
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\Dynamics-CRM-Cloud\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E757496-1734-48AF-AC73-87CA0CABC93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FBF840-02D8-4E0E-BD6A-292841C238FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="4" r:id="rId1"/>
-    <sheet name="BulkImport" sheetId="8" r:id="rId2"/>
-    <sheet name="Member" sheetId="2" r:id="rId3"/>
-    <sheet name="LOBFSC" sheetId="9" r:id="rId4"/>
-    <sheet name="ConvertingAccounts" sheetId="10" r:id="rId5"/>
-    <sheet name="Supplier" sheetId="3" r:id="rId6"/>
-    <sheet name="Contact" sheetId="7" r:id="rId7"/>
+    <sheet name="Pipeline" sheetId="11" r:id="rId2"/>
+    <sheet name="BulkImport" sheetId="8" r:id="rId3"/>
+    <sheet name="Member" sheetId="2" r:id="rId4"/>
+    <sheet name="LOBFSC" sheetId="9" r:id="rId5"/>
+    <sheet name="ConvertingAccounts" sheetId="10" r:id="rId6"/>
+    <sheet name="Supplier" sheetId="3" r:id="rId7"/>
+    <sheet name="Contact" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Driver!$A$1:$K$185</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6073" uniqueCount="1113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6112" uniqueCount="1119">
   <si>
     <t>Premier1a</t>
   </si>
@@ -3365,22 +3366,40 @@
     <t>4533_SubAccShipToAccProspectFirst</t>
   </si>
   <si>
-    <t>2022_06_06_03_10_56</t>
-  </si>
-  <si>
-    <t>2000512727</t>
-  </si>
-  <si>
     <t>TFS ID_4531:Verify cascade works fine when a shipto account gets converted to a main account</t>
   </si>
   <si>
     <t>4531_VerifyAccounttoLocationType</t>
   </si>
   <si>
-    <t>2022_06_06_08_42_47</t>
-  </si>
-  <si>
-    <t>2000512733</t>
+    <t>2000512735</t>
+  </si>
+  <si>
+    <t>2022_06_07_01_09_18</t>
+  </si>
+  <si>
+    <t>4/4/2021</t>
+  </si>
+  <si>
+    <t>5/4/2021</t>
+  </si>
+  <si>
+    <t>2000512736</t>
+  </si>
+  <si>
+    <t>2022_06_07_01_42_29</t>
+  </si>
+  <si>
+    <t>TFS ID_4532:Verify if FBO cascade works fine when ship-to account is converted back to main account</t>
+  </si>
+  <si>
+    <t>4532_VerifyFBOCascade</t>
+  </si>
+  <si>
+    <t>2000512737</t>
+  </si>
+  <si>
+    <t>2022_06_07_03_24_07</t>
   </si>
 </sst>
 </file>
@@ -4271,11 +4290,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
-  <dimension ref="A1:P217"/>
+  <dimension ref="A1:P218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B216" sqref="B216"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10079,7 +10096,7 @@
         <v>1105</v>
       </c>
       <c r="C216" s="123" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D216" s="125" t="s">
         <v>1080</v>
@@ -10091,10 +10108,10 @@
         <v>938</v>
       </c>
       <c r="G216" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
       <c r="H216" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.25">
@@ -10102,10 +10119,10 @@
         <v>216</v>
       </c>
       <c r="B217" s="82" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="C217" s="123" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D217" s="125" t="s">
         <v>1080</v>
@@ -10114,13 +10131,39 @@
         <v>40</v>
       </c>
       <c r="F217" s="123" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="G217" t="s">
-        <v>1111</v>
+        <v>1114</v>
       </c>
       <c r="H217" t="s">
-        <v>1112</v>
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A218" s="109">
+        <v>217</v>
+      </c>
+      <c r="B218" s="82" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C218" s="109" t="s">
+        <v>34</v>
+      </c>
+      <c r="D218" s="125" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E218" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F218" s="123" t="s">
+        <v>937</v>
+      </c>
+      <c r="G218" t="s">
+        <v>1118</v>
+      </c>
+      <c r="H218" t="s">
+        <v>1117</v>
       </c>
     </row>
   </sheetData>
@@ -10140,6 +10183,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EE9E61-0D15-477A-8CFB-C15463A4D1C5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E671484F-6321-49DA-BE73-52BC99C1ECF8}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -10217,7 +10273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
   <dimension ref="A1:EQ138"/>
   <sheetViews>
@@ -34380,7 +34436,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA8C006-EF24-4A27-B0DA-8A03B54F96DC}">
   <dimension ref="A1:EK23"/>
   <sheetViews>
@@ -39020,12 +39076,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8AE2E5-47E0-4BAE-8731-05D8E0293EC0}">
-  <dimension ref="A1:FD10"/>
+  <dimension ref="A1:FD11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40820,7 +40876,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="82" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>294</v>
@@ -40832,7 +40888,7 @@
         <v>935</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="N10" s="33" t="s">
         <v>153</v>
@@ -40882,7 +40938,7 @@
       </c>
       <c r="AJ10" s="15"/>
       <c r="AK10" s="34" t="s">
-        <v>239</v>
+        <v>1111</v>
       </c>
       <c r="AL10" s="34" t="s">
         <v>239</v>
@@ -40893,7 +40949,7 @@
         <v>278</v>
       </c>
       <c r="AP10" s="34" t="s">
-        <v>239</v>
+        <v>1112</v>
       </c>
       <c r="AQ10" s="15"/>
       <c r="AR10" s="15"/>
@@ -40998,6 +41054,186 @@
       <c r="DO10" s="15"/>
       <c r="DP10" s="15"/>
     </row>
+    <row r="11" spans="1:160" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="82" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>1116</v>
+      </c>
+      <c r="N11" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="O11" s="33"/>
+      <c r="P11" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="R11" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="S11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH11" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI11" s="36" t="s">
+        <v>934</v>
+      </c>
+      <c r="AJ11" s="15"/>
+      <c r="AK11" s="34" t="s">
+        <v>1111</v>
+      </c>
+      <c r="AL11" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="AM11" s="34"/>
+      <c r="AN11" s="15"/>
+      <c r="AO11" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="AP11" s="34" t="s">
+        <v>1112</v>
+      </c>
+      <c r="AQ11" s="15"/>
+      <c r="AR11" s="15"/>
+      <c r="AS11" s="15"/>
+      <c r="AT11" s="15"/>
+      <c r="AU11" s="15"/>
+      <c r="AV11" s="15"/>
+      <c r="AW11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX11" s="15"/>
+      <c r="AY11" s="15"/>
+      <c r="AZ11" s="15"/>
+      <c r="BA11" s="15"/>
+      <c r="BB11" s="15"/>
+      <c r="BC11" s="15"/>
+      <c r="BD11" s="15"/>
+      <c r="BE11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF11" s="15"/>
+      <c r="BG11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BH11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BI11" s="15"/>
+      <c r="BJ11" s="15"/>
+      <c r="BK11" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="BL11" s="15" t="s">
+        <v>550</v>
+      </c>
+      <c r="BM11" s="15"/>
+      <c r="BN11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BO11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="BP11" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="BQ11" s="34"/>
+      <c r="BR11" s="34"/>
+      <c r="BS11" s="34"/>
+      <c r="BT11" s="34"/>
+      <c r="BU11" s="34"/>
+      <c r="BV11" s="34"/>
+      <c r="BW11" s="34"/>
+      <c r="BX11" s="34"/>
+      <c r="BY11" s="34"/>
+      <c r="BZ11" s="34"/>
+      <c r="CA11" s="34"/>
+      <c r="CB11" s="34"/>
+      <c r="CC11" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="CD11" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="CE11" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="CF11" s="15"/>
+      <c r="CG11" s="34"/>
+      <c r="CH11" s="34"/>
+      <c r="CI11" s="34"/>
+      <c r="CJ11" s="34"/>
+      <c r="CK11" s="34"/>
+      <c r="CL11" s="34"/>
+      <c r="CM11" s="34"/>
+      <c r="CN11" s="15"/>
+      <c r="CO11" s="15"/>
+      <c r="CP11" s="15"/>
+      <c r="CQ11" s="15"/>
+      <c r="CR11" s="15"/>
+      <c r="CS11" s="15"/>
+      <c r="CT11" s="15"/>
+      <c r="CU11" s="15"/>
+      <c r="CV11" s="15"/>
+      <c r="CW11" s="15"/>
+      <c r="CX11" s="15"/>
+      <c r="CY11" s="15"/>
+      <c r="CZ11" s="15"/>
+      <c r="DA11" s="15"/>
+      <c r="DB11" s="15"/>
+      <c r="DC11" s="15"/>
+      <c r="DD11" s="15"/>
+      <c r="DE11" s="15"/>
+      <c r="DF11" s="15"/>
+      <c r="DG11" s="15"/>
+      <c r="DH11" s="15"/>
+      <c r="DI11" s="15"/>
+      <c r="DJ11" s="15"/>
+      <c r="DK11" s="15"/>
+      <c r="DL11" s="15"/>
+      <c r="DM11" s="15"/>
+      <c r="DN11" s="15"/>
+      <c r="DO11" s="15"/>
+      <c r="DP11" s="15"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{A7B91FD6-6F68-4471-8898-5C914670C339}"/>
@@ -41013,7 +41249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D073B921-24DF-4F78-BD1E-1984D65F897D}">
   <dimension ref="A1:BV37"/>
   <sheetViews>
@@ -45211,7 +45447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51C67A-098B-49A1-9024-B5BC951889FA}">
   <dimension ref="A1:AF11"/>
   <sheetViews>
@@ -45833,12 +46069,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46076,18 +46312,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -46113,11 +46351,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Committing the Latest Changes
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\Dynamics-CRM-Cloud\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1F8E68-628A-400D-ACC7-EAAE45FF2073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57C212E-37B5-42D0-B2B1-260B0940A2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -37,7 +37,7 @@
     <sheet name="Contact" sheetId="7" r:id="rId22"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Driver!$A$1:$L$303</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Driver!$A$1:$L$315</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10484" uniqueCount="1473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10534" uniqueCount="1519">
   <si>
     <t>Premier1a</t>
   </si>
@@ -4109,9 +4109,6 @@
     <t>Dpsearch</t>
   </si>
   <si>
-    <t>2022_08_26_06_53_19</t>
-  </si>
-  <si>
     <t>TFS ID_8811:Cloud - Verify newly added fields in Subaccounts view</t>
   </si>
   <si>
@@ -4139,18 +4136,12 @@
     <t>2000141868</t>
   </si>
   <si>
-    <t>2022_08_30_03_46_28</t>
-  </si>
-  <si>
     <t>TFS ID_9633:Cloud : Verify whether user should not get any script error on add any Supplier Diversity</t>
   </si>
   <si>
     <t>9633:Cloud -Add Diversity information to a supplier</t>
   </si>
   <si>
-    <t>2022_08_30_06_12_41</t>
-  </si>
-  <si>
     <t>TFS ID_9634:Cloud : Verify whether "Account for interactive experience" form layout should not get displayed additionally</t>
   </si>
   <si>
@@ -4277,9 +4268,6 @@
     <t>2000000117</t>
   </si>
   <si>
-    <t>2022_09_06_03_56_59</t>
-  </si>
-  <si>
     <t>2022_09_06_04_01_23</t>
   </si>
   <si>
@@ -4439,27 +4427,12 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>2000513401</t>
-  </si>
-  <si>
-    <t>2022_09_29_01_15_59</t>
-  </si>
-  <si>
-    <t>2000513402</t>
-  </si>
-  <si>
     <t>2022_09_29_01_30_08</t>
   </si>
   <si>
-    <t>2000513403</t>
-  </si>
-  <si>
     <t>Failed</t>
   </si>
   <si>
-    <t>2022_09_29_01_41_22</t>
-  </si>
-  <si>
     <t>2000513404</t>
   </si>
   <si>
@@ -4469,13 +4442,178 @@
     <t>2022_09_29_02_05_18</t>
   </si>
   <si>
-    <t>2000513406</t>
-  </si>
-  <si>
     <t>2022_09_29_02_40_53</t>
   </si>
   <si>
     <t>2000513407</t>
+  </si>
+  <si>
+    <t>2000513415</t>
+  </si>
+  <si>
+    <t>https://premierdev1.crm.dynamics.com/main.aspx?appid=0c73db26-7543-ed11-bba3-000d3a53dec8&amp;pagetype=dashboard&amp;type=system&amp;_canOverride=true</t>
+  </si>
+  <si>
+    <t>2000552581</t>
+  </si>
+  <si>
+    <t>2022_10_06_01_53_17</t>
+  </si>
+  <si>
+    <t>2000552585</t>
+  </si>
+  <si>
+    <t>2022_10_06_02_26_21</t>
+  </si>
+  <si>
+    <t>2000552586</t>
+  </si>
+  <si>
+    <t>2022_10_06_02_33_29</t>
+  </si>
+  <si>
+    <t>2000552587</t>
+  </si>
+  <si>
+    <t>2022_10_06_02_39_28</t>
+  </si>
+  <si>
+    <t>2022_10_06_02_42_52</t>
+  </si>
+  <si>
+    <t>2000552589</t>
+  </si>
+  <si>
+    <t>2022_10_06_02_48_49</t>
+  </si>
+  <si>
+    <t>2000552591</t>
+  </si>
+  <si>
+    <t>2022_10_06_02_54_57</t>
+  </si>
+  <si>
+    <t>2022_10_06_03_00_16</t>
+  </si>
+  <si>
+    <t>2000552592</t>
+  </si>
+  <si>
+    <t>2022_10_06_03_06_16</t>
+  </si>
+  <si>
+    <t>2022_10_06_03_13_07</t>
+  </si>
+  <si>
+    <t>2022_10_06_03_19_58</t>
+  </si>
+  <si>
+    <t>2022_10_06_03_26_19</t>
+  </si>
+  <si>
+    <t>2000141844</t>
+  </si>
+  <si>
+    <t>2022_10_06_03_36_58</t>
+  </si>
+  <si>
+    <t>2022_10_06_03_43_17</t>
+  </si>
+  <si>
+    <t>2022_10_06_03_56_47</t>
+  </si>
+  <si>
+    <t>2000552599</t>
+  </si>
+  <si>
+    <t>2022_10_06_04_05_21</t>
+  </si>
+  <si>
+    <t>2000552604</t>
+  </si>
+  <si>
+    <t>2022_10_06_04_31_31</t>
+  </si>
+  <si>
+    <t>2022_10_06_04_35_19</t>
+  </si>
+  <si>
+    <t>2022_10_06_04_39_18</t>
+  </si>
+  <si>
+    <t>2022_10_06_04_43_17</t>
+  </si>
+  <si>
+    <t>2022_10_06_04_50_48</t>
+  </si>
+  <si>
+    <t>2022_10_06_04_55_08</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_00_16</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_07_46</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_14_19</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_17_48</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_19_59</t>
+  </si>
+  <si>
+    <t>2000552610</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_26_14</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_29_43</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_33_08</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_37_20</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_40_58</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_42_27</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_44_30</t>
+  </si>
+  <si>
+    <t>2022_10_06_05_49_40</t>
+  </si>
+  <si>
+    <t>2022_10_06_06_07_22</t>
+  </si>
+  <si>
+    <t>2022_10_06_06_11_09</t>
+  </si>
+  <si>
+    <t>2022_10_06_06_19_20</t>
+  </si>
+  <si>
+    <t>2022_10_06_06_24_00</t>
+  </si>
+  <si>
+    <t>7000578029</t>
+  </si>
+  <si>
+    <t>2022_10_06_06_47_13</t>
+  </si>
+  <si>
+    <t>7000578030</t>
+  </si>
+  <si>
+    <t>2022_10_06_07_00_19</t>
   </si>
 </sst>
 </file>
@@ -5452,8 +5590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
   <dimension ref="A1:P315"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B169" sqref="B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5523,18 +5661,18 @@
         <v>39</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>1461</v>
+        <v>1466</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>1460</v>
+        <v>1465</v>
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
       <c r="K2" s="48" t="s">
-        <v>544</v>
+        <v>1464</v>
       </c>
       <c r="L2" s="106" t="s">
         <v>530</v>
@@ -5557,13 +5695,13 @@
         <v>39</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>1459</v>
+        <v>1455</v>
       </c>
       <c r="G3" s="17" t="s">
+        <v>1456</v>
+      </c>
+      <c r="H3" s="17" t="s">
         <v>1463</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>1462</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -5580,7 +5718,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="150" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>2</v>
@@ -5589,13 +5727,13 @@
         <v>39</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>1465</v>
+        <v>1457</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>1471</v>
+        <v>1461</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>1472</v>
+        <v>1462</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
@@ -5619,13 +5757,13 @@
         <v>39</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>1465</v>
+        <v>1457</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>1468</v>
+        <v>1459</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>1467</v>
+        <v>1458</v>
       </c>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
@@ -5649,10 +5787,10 @@
         <v>39</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>1459</v>
+        <v>1455</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>1469</v>
+        <v>1460</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
@@ -5680,7 +5818,7 @@
         <v>261</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>1450</v>
+        <v>1446</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
@@ -5708,10 +5846,10 @@
         <v>261</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>1452</v>
+        <v>1448</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>1451</v>
+        <v>1447</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
@@ -5738,7 +5876,7 @@
         <v>261</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
@@ -5766,10 +5904,10 @@
         <v>261</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>1455</v>
+        <v>1451</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>1454</v>
+        <v>1450</v>
       </c>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
@@ -5796,10 +5934,10 @@
         <v>261</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>1456</v>
+        <v>1452</v>
       </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
@@ -7340,9 +7478,11 @@
         <v>39</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G70" s="24"/>
+        <v>1455</v>
+      </c>
+      <c r="G70" s="24" t="s">
+        <v>1499</v>
+      </c>
       <c r="H70" s="24"/>
       <c r="I70" s="24"/>
       <c r="J70" s="24"/>
@@ -8952,10 +9092,14 @@
         <v>39</v>
       </c>
       <c r="F132" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G132" s="21"/>
-      <c r="H132" s="21"/>
+        <v>1455</v>
+      </c>
+      <c r="G132" s="21" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H132" s="21" t="s">
+        <v>1467</v>
+      </c>
       <c r="I132" s="21"/>
       <c r="J132" s="21"/>
       <c r="K132" s="22"/>
@@ -8978,10 +9122,14 @@
         <v>39</v>
       </c>
       <c r="F133" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G133" s="21"/>
-      <c r="H133" s="21"/>
+        <v>1457</v>
+      </c>
+      <c r="G133" s="21" t="s">
+        <v>1470</v>
+      </c>
+      <c r="H133" s="21" t="s">
+        <v>1469</v>
+      </c>
       <c r="I133" s="21"/>
       <c r="J133" s="21"/>
       <c r="K133" s="22"/>
@@ -9004,10 +9152,14 @@
         <v>39</v>
       </c>
       <c r="F134" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G134" s="21"/>
-      <c r="H134" s="21"/>
+        <v>1455</v>
+      </c>
+      <c r="G134" s="21" t="s">
+        <v>1472</v>
+      </c>
+      <c r="H134" s="21" t="s">
+        <v>1471</v>
+      </c>
       <c r="I134" s="21"/>
       <c r="J134" s="21"/>
       <c r="K134" s="22"/>
@@ -9030,9 +9182,11 @@
         <v>39</v>
       </c>
       <c r="F135" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G135" s="21"/>
+        <v>1457</v>
+      </c>
+      <c r="G135" s="21" t="s">
+        <v>1473</v>
+      </c>
       <c r="H135" s="21"/>
       <c r="I135" s="21"/>
       <c r="J135" s="21"/>
@@ -9056,10 +9210,14 @@
         <v>39</v>
       </c>
       <c r="F136" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G136" s="21"/>
-      <c r="H136" s="21"/>
+        <v>1455</v>
+      </c>
+      <c r="G136" s="21" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H136" s="21" t="s">
+        <v>1474</v>
+      </c>
       <c r="I136" s="21"/>
       <c r="J136" s="21"/>
       <c r="K136" s="22"/>
@@ -9082,10 +9240,14 @@
         <v>39</v>
       </c>
       <c r="F137" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G137" s="21"/>
-      <c r="H137" s="21"/>
+        <v>1455</v>
+      </c>
+      <c r="G137" s="21" t="s">
+        <v>1477</v>
+      </c>
+      <c r="H137" s="21" t="s">
+        <v>1476</v>
+      </c>
       <c r="I137" s="21"/>
       <c r="J137" s="21"/>
       <c r="K137" s="22"/>
@@ -9108,10 +9270,14 @@
         <v>39</v>
       </c>
       <c r="F138" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G138" s="21"/>
-      <c r="H138" s="21"/>
+        <v>1457</v>
+      </c>
+      <c r="G138" s="21" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H138" s="21" t="s">
+        <v>102</v>
+      </c>
       <c r="I138" s="21"/>
       <c r="J138" s="21"/>
       <c r="K138" s="22"/>
@@ -9134,10 +9300,14 @@
         <v>39</v>
       </c>
       <c r="F139" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G139" s="21"/>
-      <c r="H139" s="21"/>
+        <v>1455</v>
+      </c>
+      <c r="G139" s="21" t="s">
+        <v>1480</v>
+      </c>
+      <c r="H139" s="21" t="s">
+        <v>1479</v>
+      </c>
       <c r="I139" s="21"/>
       <c r="J139" s="21"/>
       <c r="K139" s="22"/>
@@ -9160,10 +9330,14 @@
         <v>39</v>
       </c>
       <c r="F140" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G140" s="21"/>
-      <c r="H140" s="21"/>
+        <v>1455</v>
+      </c>
+      <c r="G140" s="21" t="s">
+        <v>1481</v>
+      </c>
+      <c r="H140" s="21" t="s">
+        <v>112</v>
+      </c>
       <c r="I140" s="21"/>
       <c r="J140" s="21"/>
       <c r="K140" s="22"/>
@@ -9186,10 +9360,14 @@
         <v>39</v>
       </c>
       <c r="F141" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G141" s="21"/>
-      <c r="H141" s="21"/>
+        <v>1455</v>
+      </c>
+      <c r="G141" s="21" t="s">
+        <v>1482</v>
+      </c>
+      <c r="H141" s="21" t="s">
+        <v>112</v>
+      </c>
       <c r="I141" s="21"/>
       <c r="J141" s="21"/>
       <c r="K141" s="22"/>
@@ -9212,10 +9390,14 @@
         <v>39</v>
       </c>
       <c r="F142" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G142" s="21"/>
-      <c r="H142" s="21"/>
+        <v>1455</v>
+      </c>
+      <c r="G142" s="21" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H142" s="21" t="s">
+        <v>117</v>
+      </c>
       <c r="I142" s="21"/>
       <c r="J142" s="21"/>
       <c r="K142" s="22"/>
@@ -9238,10 +9420,14 @@
         <v>39</v>
       </c>
       <c r="F143" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G143" s="21"/>
-      <c r="H143" s="21"/>
+        <v>1457</v>
+      </c>
+      <c r="G143" s="21" t="s">
+        <v>1485</v>
+      </c>
+      <c r="H143" s="21" t="s">
+        <v>1484</v>
+      </c>
       <c r="I143" s="21"/>
       <c r="J143" s="21"/>
       <c r="K143" s="22"/>
@@ -9264,10 +9450,14 @@
         <v>39</v>
       </c>
       <c r="F144" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G144" s="21"/>
-      <c r="H144" s="21"/>
+        <v>1455</v>
+      </c>
+      <c r="G144" s="21" t="s">
+        <v>1486</v>
+      </c>
+      <c r="H144" s="21" t="s">
+        <v>129</v>
+      </c>
       <c r="I144" s="21"/>
       <c r="J144" s="21"/>
       <c r="K144" s="22"/>
@@ -9290,9 +9480,11 @@
         <v>39</v>
       </c>
       <c r="F145" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G145" s="21"/>
+        <v>1457</v>
+      </c>
+      <c r="G145" s="21" t="s">
+        <v>1487</v>
+      </c>
       <c r="H145" s="21"/>
       <c r="I145" s="21"/>
       <c r="J145" s="21"/>
@@ -9316,10 +9508,14 @@
         <v>39</v>
       </c>
       <c r="F146" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G146" s="21"/>
-      <c r="H146" s="21"/>
+        <v>1457</v>
+      </c>
+      <c r="G146" s="21" t="s">
+        <v>1489</v>
+      </c>
+      <c r="H146" s="21" t="s">
+        <v>1488</v>
+      </c>
       <c r="I146" s="21"/>
       <c r="J146" s="21"/>
       <c r="K146" s="22"/>
@@ -9342,10 +9538,14 @@
         <v>39</v>
       </c>
       <c r="F147" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G147" s="21"/>
-      <c r="H147" s="21"/>
+        <v>1455</v>
+      </c>
+      <c r="G147" s="21" t="s">
+        <v>1491</v>
+      </c>
+      <c r="H147" s="21" t="s">
+        <v>1490</v>
+      </c>
       <c r="I147" s="21"/>
       <c r="J147" s="21"/>
       <c r="K147" s="22"/>
@@ -9368,9 +9568,11 @@
         <v>39</v>
       </c>
       <c r="F148" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G148" s="24"/>
+        <v>1457</v>
+      </c>
+      <c r="G148" s="24" t="s">
+        <v>1492</v>
+      </c>
       <c r="H148" s="24"/>
       <c r="I148" s="24"/>
       <c r="J148" s="24"/>
@@ -9394,9 +9596,11 @@
         <v>39</v>
       </c>
       <c r="F149" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G149" s="24"/>
+        <v>1457</v>
+      </c>
+      <c r="G149" s="24" t="s">
+        <v>1493</v>
+      </c>
       <c r="H149" s="24"/>
       <c r="I149" s="24"/>
       <c r="J149" s="24"/>
@@ -9420,9 +9624,11 @@
         <v>39</v>
       </c>
       <c r="F150" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G150" s="24"/>
+        <v>1457</v>
+      </c>
+      <c r="G150" s="24" t="s">
+        <v>1494</v>
+      </c>
       <c r="H150" s="24"/>
       <c r="I150" s="24"/>
       <c r="J150" s="24"/>
@@ -9446,9 +9652,11 @@
         <v>39</v>
       </c>
       <c r="F151" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G151" s="24"/>
+        <v>1455</v>
+      </c>
+      <c r="G151" s="24" t="s">
+        <v>1495</v>
+      </c>
       <c r="H151" s="24"/>
       <c r="I151" s="24"/>
       <c r="J151" s="24"/>
@@ -9472,9 +9680,11 @@
         <v>39</v>
       </c>
       <c r="F152" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G152" s="24"/>
+        <v>1457</v>
+      </c>
+      <c r="G152" s="24" t="s">
+        <v>1496</v>
+      </c>
       <c r="H152" s="24"/>
       <c r="I152" s="24"/>
       <c r="J152" s="24"/>
@@ -9498,9 +9708,11 @@
         <v>39</v>
       </c>
       <c r="F153" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G153" s="24"/>
+        <v>1455</v>
+      </c>
+      <c r="G153" s="24" t="s">
+        <v>1497</v>
+      </c>
       <c r="H153" s="24"/>
       <c r="I153" s="24"/>
       <c r="J153" s="24"/>
@@ -9524,9 +9736,11 @@
         <v>39</v>
       </c>
       <c r="F154" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G154" s="24"/>
+        <v>1457</v>
+      </c>
+      <c r="G154" s="24" t="s">
+        <v>1498</v>
+      </c>
       <c r="H154" s="24"/>
       <c r="I154" s="24"/>
       <c r="J154" s="24"/>
@@ -9576,9 +9790,11 @@
         <v>39</v>
       </c>
       <c r="F156" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G156" s="24"/>
+        <v>1457</v>
+      </c>
+      <c r="G156" s="24" t="s">
+        <v>1500</v>
+      </c>
       <c r="H156" s="24"/>
       <c r="I156" s="24"/>
       <c r="J156" s="24"/>
@@ -9602,9 +9818,11 @@
         <v>39</v>
       </c>
       <c r="F157" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G157" s="24"/>
+        <v>1455</v>
+      </c>
+      <c r="G157" s="24" t="s">
+        <v>1501</v>
+      </c>
       <c r="H157" s="24"/>
       <c r="I157" s="24"/>
       <c r="J157" s="24"/>
@@ -9628,10 +9846,14 @@
         <v>39</v>
       </c>
       <c r="F158" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G158" s="24"/>
-      <c r="H158" s="24"/>
+        <v>1455</v>
+      </c>
+      <c r="G158" s="24" t="s">
+        <v>1503</v>
+      </c>
+      <c r="H158" s="24" t="s">
+        <v>1502</v>
+      </c>
       <c r="I158" s="24"/>
       <c r="J158" s="24"/>
       <c r="K158" s="24"/>
@@ -9654,9 +9876,11 @@
         <v>39</v>
       </c>
       <c r="F159" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G159" s="21"/>
+        <v>1457</v>
+      </c>
+      <c r="G159" s="21" t="s">
+        <v>1504</v>
+      </c>
       <c r="H159" s="21"/>
       <c r="I159" s="21"/>
       <c r="J159" s="21"/>
@@ -9680,9 +9904,11 @@
         <v>39</v>
       </c>
       <c r="F160" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G160" s="21"/>
+        <v>1457</v>
+      </c>
+      <c r="G160" s="21" t="s">
+        <v>1505</v>
+      </c>
       <c r="H160" s="21"/>
       <c r="I160" s="21"/>
       <c r="J160" s="21"/>
@@ -9706,10 +9932,10 @@
         <v>39</v>
       </c>
       <c r="F161" s="17" t="s">
-        <v>261</v>
+        <v>1455</v>
       </c>
       <c r="G161" s="21" t="s">
-        <v>1360</v>
+        <v>1506</v>
       </c>
       <c r="H161" s="21"/>
       <c r="I161" s="21"/>
@@ -9734,9 +9960,11 @@
         <v>39</v>
       </c>
       <c r="F162" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G162" s="21"/>
+        <v>1457</v>
+      </c>
+      <c r="G162" s="21" t="s">
+        <v>1507</v>
+      </c>
       <c r="H162" s="21"/>
       <c r="I162" s="21"/>
       <c r="J162" s="21"/>
@@ -9760,9 +9988,11 @@
         <v>39</v>
       </c>
       <c r="F163" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G163" s="21"/>
+        <v>1457</v>
+      </c>
+      <c r="G163" s="21" t="s">
+        <v>1508</v>
+      </c>
       <c r="H163" s="21"/>
       <c r="I163" s="21"/>
       <c r="J163" s="21"/>
@@ -9786,9 +10016,11 @@
         <v>39</v>
       </c>
       <c r="F164" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G164" s="21"/>
+        <v>1457</v>
+      </c>
+      <c r="G164" s="21" t="s">
+        <v>1509</v>
+      </c>
       <c r="H164" s="21"/>
       <c r="I164" s="21"/>
       <c r="J164" s="21"/>
@@ -9812,9 +10044,11 @@
         <v>39</v>
       </c>
       <c r="F165" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G165" s="21"/>
+        <v>1457</v>
+      </c>
+      <c r="G165" s="21" t="s">
+        <v>1510</v>
+      </c>
       <c r="H165" s="21"/>
       <c r="I165" s="21"/>
       <c r="J165" s="21"/>
@@ -9838,9 +10072,11 @@
         <v>39</v>
       </c>
       <c r="F166" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G166" s="21"/>
+        <v>1455</v>
+      </c>
+      <c r="G166" s="21" t="s">
+        <v>1511</v>
+      </c>
       <c r="H166" s="21"/>
       <c r="I166" s="21"/>
       <c r="J166" s="21"/>
@@ -9890,10 +10126,10 @@
         <v>39</v>
       </c>
       <c r="F168" s="17" t="s">
-        <v>261</v>
+        <v>1457</v>
       </c>
       <c r="G168" s="21" t="s">
-        <v>1350</v>
+        <v>1512</v>
       </c>
       <c r="H168" s="21"/>
       <c r="I168" s="21"/>
@@ -9909,7 +10145,7 @@
         <v>219</v>
       </c>
       <c r="C169" s="150" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D169" s="30" t="s">
         <v>218</v>
@@ -9918,10 +10154,14 @@
         <v>39</v>
       </c>
       <c r="F169" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G169" s="27"/>
-      <c r="H169" s="27"/>
+        <v>1457</v>
+      </c>
+      <c r="G169" s="27" t="s">
+        <v>1518</v>
+      </c>
+      <c r="H169" s="27" t="s">
+        <v>1517</v>
+      </c>
       <c r="I169" s="27"/>
       <c r="J169" s="27"/>
       <c r="K169" s="27"/>
@@ -12863,7 +13103,7 @@
         <v>285</v>
       </c>
       <c r="B290" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="C290" s="150" t="s">
         <v>34</v>
@@ -12878,7 +13118,7 @@
         <v>261</v>
       </c>
       <c r="G290" t="s">
-        <v>1458</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.25">
@@ -12886,7 +13126,7 @@
         <v>285</v>
       </c>
       <c r="B291" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="C291" s="150" t="s">
         <v>34</v>
@@ -12901,7 +13141,7 @@
         <v>261</v>
       </c>
       <c r="G291" t="s">
-        <v>1448</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="292" spans="1:8" x14ac:dyDescent="0.25">
@@ -12909,7 +13149,7 @@
         <v>285</v>
       </c>
       <c r="B292" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="C292" s="150" t="s">
         <v>34</v>
@@ -12924,7 +13164,7 @@
         <v>261</v>
       </c>
       <c r="G292" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="293" spans="1:8" x14ac:dyDescent="0.25">
@@ -12932,7 +13172,7 @@
         <v>286</v>
       </c>
       <c r="B293" s="150" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="C293" s="150" t="s">
         <v>34</v>
@@ -12947,7 +13187,7 @@
         <v>261</v>
       </c>
       <c r="G293" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="294" spans="1:8" x14ac:dyDescent="0.25">
@@ -12955,7 +13195,7 @@
         <v>287</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="C294" s="150" t="s">
         <v>34</v>
@@ -12970,7 +13210,7 @@
         <v>261</v>
       </c>
       <c r="G294" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="H294" t="s">
         <v>320</v>
@@ -12981,10 +13221,10 @@
         <v>288</v>
       </c>
       <c r="B295" s="162" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="C295" s="150" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D295" s="21" t="s">
         <v>26</v>
@@ -12993,10 +13233,10 @@
         <v>39</v>
       </c>
       <c r="F295" s="17" t="s">
-        <v>261</v>
+        <v>1457</v>
       </c>
       <c r="G295" t="s">
-        <v>1363</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="296" spans="1:8" x14ac:dyDescent="0.25">
@@ -13004,7 +13244,7 @@
         <v>289</v>
       </c>
       <c r="B296" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
       <c r="C296" s="150" t="s">
         <v>34</v>
@@ -13024,7 +13264,7 @@
         <v>289</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="C297" s="150" t="s">
         <v>34</v>
@@ -13039,7 +13279,7 @@
         <v>261</v>
       </c>
       <c r="G297" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="298" spans="1:8" x14ac:dyDescent="0.25">
@@ -13047,7 +13287,7 @@
         <v>290</v>
       </c>
       <c r="B298" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="C298" s="150" t="s">
         <v>34</v>
@@ -13062,7 +13302,7 @@
         <v>261</v>
       </c>
       <c r="G298" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.25">
@@ -13070,7 +13310,7 @@
         <v>291</v>
       </c>
       <c r="B299" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="C299" s="150" t="s">
         <v>34</v>
@@ -13085,7 +13325,7 @@
         <v>261</v>
       </c>
       <c r="G299" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.25">
@@ -13093,7 +13333,7 @@
         <v>292</v>
       </c>
       <c r="B300" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="C300" s="150" t="s">
         <v>34</v>
@@ -13108,7 +13348,7 @@
         <v>261</v>
       </c>
       <c r="G300" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="301" spans="1:8" x14ac:dyDescent="0.25">
@@ -13116,7 +13356,7 @@
         <v>293</v>
       </c>
       <c r="B301" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="C301" s="150" t="s">
         <v>34</v>
@@ -13136,7 +13376,7 @@
         <v>294</v>
       </c>
       <c r="B302" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="C302" s="150" t="s">
         <v>34</v>
@@ -13151,7 +13391,7 @@
         <v>261</v>
       </c>
       <c r="G302" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="303" spans="1:8" x14ac:dyDescent="0.25">
@@ -13159,7 +13399,7 @@
         <v>295</v>
       </c>
       <c r="B303" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="C303" s="150" t="s">
         <v>34</v>
@@ -13171,10 +13411,10 @@
         <v>39</v>
       </c>
       <c r="F303" s="17" t="s">
-        <v>261</v>
+        <v>1457</v>
       </c>
       <c r="G303" t="s">
-        <v>1406</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="304" spans="1:8" x14ac:dyDescent="0.25">
@@ -13182,13 +13422,13 @@
         <v>296</v>
       </c>
       <c r="B304" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="C304" s="150" t="s">
         <v>34</v>
       </c>
       <c r="D304" s="150" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E304" s="17" t="s">
         <v>39</v>
@@ -13197,10 +13437,10 @@
         <v>261</v>
       </c>
       <c r="G304" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="H304" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.25">
@@ -13208,13 +13448,13 @@
         <v>297</v>
       </c>
       <c r="B305" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="C305" s="150" t="s">
         <v>34</v>
       </c>
       <c r="D305" s="150" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E305" s="17" t="s">
         <v>39</v>
@@ -13223,7 +13463,7 @@
         <v>261</v>
       </c>
       <c r="G305" t="s">
-        <v>1407</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.25">
@@ -13231,13 +13471,13 @@
         <v>298</v>
       </c>
       <c r="B306" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="C306" s="150" t="s">
         <v>34</v>
       </c>
       <c r="D306" s="150" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E306" s="17" t="s">
         <v>39</v>
@@ -13246,7 +13486,7 @@
         <v>261</v>
       </c>
       <c r="G306" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.25">
@@ -13254,13 +13494,13 @@
         <v>299</v>
       </c>
       <c r="B307" t="s">
-        <v>1408</v>
+        <v>1404</v>
       </c>
       <c r="C307" s="150" t="s">
         <v>34</v>
       </c>
       <c r="D307" s="150" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E307" s="17" t="s">
         <v>39</v>
@@ -13269,7 +13509,7 @@
         <v>261</v>
       </c>
       <c r="G307" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.25">
@@ -13277,13 +13517,13 @@
         <v>300</v>
       </c>
       <c r="B308" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
       <c r="C308" s="150" t="s">
         <v>34</v>
       </c>
       <c r="D308" s="150" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E308" s="17" t="s">
         <v>39</v>
@@ -13292,10 +13532,10 @@
         <v>261</v>
       </c>
       <c r="G308" t="s">
-        <v>1416</v>
+        <v>1412</v>
       </c>
       <c r="H308" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.25">
@@ -13303,13 +13543,13 @@
         <v>301</v>
       </c>
       <c r="B309" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="C309" s="150" t="s">
         <v>34</v>
       </c>
       <c r="D309" s="150" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E309" s="17" t="s">
         <v>39</v>
@@ -13318,10 +13558,10 @@
         <v>261</v>
       </c>
       <c r="G309" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
       <c r="H309" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.25">
@@ -13329,13 +13569,13 @@
         <v>302</v>
       </c>
       <c r="B310" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
       <c r="C310" s="150" t="s">
         <v>34</v>
       </c>
       <c r="D310" s="150" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E310" s="17" t="s">
         <v>39</v>
@@ -13344,10 +13584,10 @@
         <v>261</v>
       </c>
       <c r="G310" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
       <c r="H310" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.25">
@@ -13355,13 +13595,13 @@
         <v>303</v>
       </c>
       <c r="B311" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
       <c r="C311" s="150" t="s">
         <v>34</v>
       </c>
       <c r="D311" s="150" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E311" s="17" t="s">
         <v>39</v>
@@ -13370,10 +13610,10 @@
         <v>261</v>
       </c>
       <c r="G311" t="s">
-        <v>1431</v>
+        <v>1427</v>
       </c>
       <c r="H311" t="s">
-        <v>1430</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.25">
@@ -13381,13 +13621,13 @@
         <v>304</v>
       </c>
       <c r="B312" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
       <c r="C312" s="150" t="s">
         <v>34</v>
       </c>
       <c r="D312" s="150" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E312" s="17" t="s">
         <v>39</v>
@@ -13396,10 +13636,10 @@
         <v>261</v>
       </c>
       <c r="G312" t="s">
-        <v>1436</v>
+        <v>1432</v>
       </c>
       <c r="H312" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="313" spans="1:8" x14ac:dyDescent="0.25">
@@ -13407,13 +13647,13 @@
         <v>305</v>
       </c>
       <c r="B313" t="s">
-        <v>1434</v>
+        <v>1430</v>
       </c>
       <c r="C313" s="150" t="s">
         <v>34</v>
       </c>
       <c r="D313" s="150" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E313" s="17" t="s">
         <v>39</v>
@@ -13422,10 +13662,10 @@
         <v>261</v>
       </c>
       <c r="G313" t="s">
-        <v>1438</v>
+        <v>1434</v>
       </c>
       <c r="H313" t="s">
-        <v>1437</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.25">
@@ -13433,13 +13673,13 @@
         <v>306</v>
       </c>
       <c r="B314" t="s">
-        <v>1439</v>
+        <v>1435</v>
       </c>
       <c r="C314" s="150" t="s">
         <v>34</v>
       </c>
       <c r="D314" s="150" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E314" s="17" t="s">
         <v>39</v>
@@ -13448,10 +13688,10 @@
         <v>261</v>
       </c>
       <c r="G314" t="s">
-        <v>1442</v>
+        <v>1438</v>
       </c>
       <c r="H314" t="s">
-        <v>1441</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="315" spans="1:8" x14ac:dyDescent="0.25">
@@ -13459,13 +13699,13 @@
         <v>307</v>
       </c>
       <c r="B315" t="s">
-        <v>1443</v>
+        <v>1439</v>
       </c>
       <c r="C315" s="150" t="s">
         <v>34</v>
       </c>
       <c r="D315" s="150" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E315" s="17" t="s">
         <v>39</v>
@@ -13474,14 +13714,13 @@
         <v>261</v>
       </c>
       <c r="G315" t="s">
-        <v>1447</v>
+        <v>1443</v>
       </c>
       <c r="H315" t="s">
-        <v>1446</v>
+        <v>1442</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L303" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}"/>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1" xr:uid="{C4DE44B4-9E86-4104-81E3-C93D60F64BE3}"/>
     <hyperlink ref="L2" r:id="rId2" xr:uid="{A4124D5F-F457-4A70-A072-5DFAF5EA33F8}"/>
@@ -28382,7 +28621,7 @@
         <v>64</v>
       </c>
       <c r="EQ1" s="1" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="ER1" s="1" t="s">
         <v>19</v>
@@ -28406,22 +28645,22 @@
         <v>74</v>
       </c>
       <c r="EY1" s="59" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="EZ1" s="59" t="s">
+        <v>1364</v>
+      </c>
+      <c r="FA1" s="59" t="s">
+        <v>1368</v>
+      </c>
+      <c r="FB1" s="59" t="s">
         <v>1367</v>
       </c>
-      <c r="FA1" s="59" t="s">
-        <v>1371</v>
-      </c>
-      <c r="FB1" s="59" t="s">
-        <v>1370</v>
-      </c>
       <c r="FC1" s="59" t="s">
-        <v>1432</v>
+        <v>1428</v>
       </c>
       <c r="FD1" s="59" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="2" spans="1:181" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -28429,13 +28668,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="C2" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -28443,7 +28682,7 @@
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
@@ -28644,19 +28883,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="C3" s="32" t="s">
         <v>316</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="AI3" s="70" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="AK3" s="34" t="s">
         <v>238</v>
@@ -28670,22 +28909,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="F4" s="70" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="EY4" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="EZ4" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="5" spans="1:181" x14ac:dyDescent="0.25">
@@ -28693,22 +28932,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1408</v>
+        <v>1404</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="F5" s="70" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="EY5" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="EZ5" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="6" spans="1:181" x14ac:dyDescent="0.25">
@@ -28716,20 +28955,20 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="F6" s="36"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
@@ -28776,7 +29015,7 @@
         <v>7</v>
       </c>
       <c r="AI6" s="36" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="AJ6" s="15"/>
       <c r="AK6" s="34" t="s">
@@ -28949,16 +29188,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
@@ -29107,7 +29346,7 @@
       <c r="CO7" s="15"/>
       <c r="CP7" s="15"/>
       <c r="CQ7" s="34" t="s">
-        <v>1414</v>
+        <v>1410</v>
       </c>
       <c r="CR7" s="44" t="s">
         <v>249</v>
@@ -29203,13 +29442,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -29217,7 +29456,7 @@
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15" t="s">
-        <v>1418</v>
+        <v>1414</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
@@ -29413,10 +29652,10 @@
       <c r="EJ8" s="15"/>
       <c r="EK8" s="15"/>
       <c r="EY8" s="4" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
       <c r="EZ8" s="4" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="9" spans="1:181" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -29424,13 +29663,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -29438,7 +29677,7 @@
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
@@ -29634,10 +29873,10 @@
       <c r="EJ9" s="15"/>
       <c r="EK9" s="15"/>
       <c r="EY9" s="4" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
       <c r="EZ9" s="4" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="10" spans="1:181" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -29645,13 +29884,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -29659,7 +29898,7 @@
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
@@ -29855,22 +30094,22 @@
       <c r="EJ10" s="15"/>
       <c r="EK10" s="15"/>
       <c r="EY10" s="4" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="EZ10" s="4" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="FA10" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="FB10" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="FC10" s="4" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="FD10" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="11" spans="1:181" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -29878,13 +30117,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>1434</v>
+        <v>1430</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
@@ -29892,7 +30131,7 @@
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
@@ -30088,22 +30327,22 @@
       <c r="EJ11" s="15"/>
       <c r="EK11" s="15"/>
       <c r="EY11" s="4" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="EZ11" s="4" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="FA11" s="4" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="FB11" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="FC11" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="FD11" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="12" spans="1:181" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -30111,13 +30350,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>1439</v>
+        <v>1435</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -30125,7 +30364,7 @@
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
       <c r="J12" s="15" t="s">
-        <v>1440</v>
+        <v>1436</v>
       </c>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
@@ -30321,22 +30560,22 @@
       <c r="EJ12" s="15"/>
       <c r="EK12" s="15"/>
       <c r="EY12" s="4" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="EZ12" s="4" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="FA12" s="4" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="FB12" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="FC12" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="FD12" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="13" spans="1:181" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -30344,13 +30583,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>1443</v>
+        <v>1439</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -30358,7 +30597,7 @@
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15" t="s">
-        <v>1444</v>
+        <v>1440</v>
       </c>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
@@ -30554,20 +30793,20 @@
       <c r="EJ13" s="15"/>
       <c r="EK13" s="15"/>
       <c r="EY13" s="4" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="EZ13" s="4" t="s">
-        <v>1369</v>
+        <v>1366</v>
       </c>
       <c r="FA13" s="4" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="FB13" s="4" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="FC13"/>
       <c r="FD13" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
     </row>
   </sheetData>
@@ -32739,7 +32978,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>293</v>
@@ -32767,8 +33006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D073B921-24DF-4F78-BD1E-1984D65F897D}">
   <dimension ref="A1:BY39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33083,7 +33322,7 @@
       </c>
       <c r="D2" s="32"/>
       <c r="E2" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>25</v>
@@ -33173,7 +33412,7 @@
       <c r="BV2" s="13"/>
       <c r="BW2" s="13"/>
     </row>
-    <row r="3" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -33185,7 +33424,7 @@
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>25</v>
@@ -33278,7 +33517,7 @@
       <c r="BV3" s="13"/>
       <c r="BW3" s="13"/>
     </row>
-    <row r="4" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -33290,7 +33529,7 @@
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>25</v>
@@ -33385,7 +33624,7 @@
       <c r="BV4" s="13"/>
       <c r="BW4" s="13"/>
     </row>
-    <row r="5" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -33399,7 +33638,7 @@
         <v>316</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>25</v>
@@ -33490,7 +33729,7 @@
       <c r="BV5" s="13"/>
       <c r="BW5" s="13"/>
     </row>
-    <row r="6" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -33502,7 +33741,7 @@
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>25</v>
@@ -33599,7 +33838,7 @@
       <c r="BV6" s="13"/>
       <c r="BW6" s="13"/>
     </row>
-    <row r="7" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -33611,7 +33850,7 @@
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>25</v>
@@ -33708,7 +33947,7 @@
       <c r="BV7" s="13"/>
       <c r="BW7" s="13"/>
     </row>
-    <row r="8" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -33720,7 +33959,7 @@
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>25</v>
@@ -33809,7 +34048,7 @@
       <c r="BV8" s="13"/>
       <c r="BW8" s="13"/>
     </row>
-    <row r="9" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -33821,7 +34060,7 @@
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>25</v>
@@ -33922,7 +34161,7 @@
       <c r="BV9" s="13"/>
       <c r="BW9" s="13"/>
     </row>
-    <row r="10" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -33934,7 +34173,7 @@
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>25</v>
@@ -34023,7 +34262,7 @@
       <c r="BV10" s="13"/>
       <c r="BW10" s="13"/>
     </row>
-    <row r="11" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>10</v>
       </c>
@@ -34035,7 +34274,7 @@
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>25</v>
@@ -34120,7 +34359,7 @@
       <c r="BV11" s="13"/>
       <c r="BW11" s="13"/>
     </row>
-    <row r="12" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>11</v>
       </c>
@@ -34132,7 +34371,7 @@
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>25</v>
@@ -34227,7 +34466,7 @@
       <c r="BV12" s="13"/>
       <c r="BW12" s="13"/>
     </row>
-    <row r="13" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>12</v>
       </c>
@@ -34241,7 +34480,7 @@
         <v>316</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>25</v>
@@ -34338,7 +34577,7 @@
       <c r="BV13" s="13"/>
       <c r="BW13" s="13"/>
     </row>
-    <row r="14" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>13</v>
       </c>
@@ -34350,7 +34589,7 @@
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>25</v>
@@ -34445,7 +34684,7 @@
       <c r="BV14" s="13"/>
       <c r="BW14" s="13"/>
     </row>
-    <row r="15" spans="1:77" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:77" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>14</v>
       </c>
@@ -34456,8 +34695,8 @@
         <v>316</v>
       </c>
       <c r="D15" s="32"/>
-      <c r="E15" s="24" t="s">
-        <v>0</v>
+      <c r="E15" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>25</v>
@@ -34606,7 +34845,7 @@
       </c>
       <c r="BW15" s="24"/>
     </row>
-    <row r="16" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>15</v>
       </c>
@@ -34618,7 +34857,7 @@
       </c>
       <c r="D16" s="32"/>
       <c r="E16" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>25</v>
@@ -34727,7 +34966,7 @@
       <c r="BV16" s="13"/>
       <c r="BW16" s="13"/>
     </row>
-    <row r="17" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>16</v>
       </c>
@@ -34739,7 +34978,7 @@
       </c>
       <c r="D17" s="32"/>
       <c r="E17" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>25</v>
@@ -34840,7 +35079,7 @@
       <c r="BV17" s="13"/>
       <c r="BW17" s="13"/>
     </row>
-    <row r="18" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>17</v>
       </c>
@@ -34852,7 +35091,7 @@
       </c>
       <c r="D18" s="32"/>
       <c r="E18" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
@@ -34945,7 +35184,7 @@
       <c r="BV18" s="13"/>
       <c r="BW18" s="13"/>
     </row>
-    <row r="19" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>18</v>
       </c>
@@ -34957,7 +35196,7 @@
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>25</v>
@@ -35054,7 +35293,7 @@
       <c r="BV19" s="13"/>
       <c r="BW19" s="13"/>
     </row>
-    <row r="20" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>19</v>
       </c>
@@ -35066,7 +35305,7 @@
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>25</v>
@@ -35163,7 +35402,7 @@
       <c r="BV20" s="13"/>
       <c r="BW20" s="13"/>
     </row>
-    <row r="21" spans="1:75" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:75" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>20</v>
       </c>
@@ -35175,7 +35414,7 @@
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>25</v>
@@ -35272,7 +35511,7 @@
       <c r="BV21" s="13"/>
       <c r="BW21" s="13"/>
     </row>
-    <row r="22" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>21</v>
       </c>
@@ -35284,7 +35523,7 @@
       </c>
       <c r="D22" s="32"/>
       <c r="E22" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>25</v>
@@ -35387,7 +35626,7 @@
       <c r="BV22" s="13"/>
       <c r="BW22" s="13"/>
     </row>
-    <row r="23" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>22</v>
       </c>
@@ -35399,7 +35638,7 @@
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>25</v>
@@ -35486,7 +35725,7 @@
       <c r="BV23" s="13"/>
       <c r="BW23" s="13"/>
     </row>
-    <row r="24" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>23</v>
       </c>
@@ -35498,7 +35737,7 @@
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>25</v>
@@ -35601,7 +35840,7 @@
       <c r="BV24" s="13"/>
       <c r="BW24" s="13"/>
     </row>
-    <row r="25" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A25" s="82">
         <v>24</v>
       </c>
@@ -35612,7 +35851,7 @@
         <v>316</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>25</v>
@@ -35713,7 +35952,7 @@
       <c r="BV25" s="13"/>
       <c r="BW25" s="13"/>
     </row>
-    <row r="26" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>24</v>
       </c>
@@ -35725,7 +35964,7 @@
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F26" s="13" t="s">
         <v>25</v>
@@ -35812,7 +36051,7 @@
       <c r="BV26" s="13"/>
       <c r="BW26" s="13"/>
     </row>
-    <row r="27" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>25</v>
       </c>
@@ -35824,7 +36063,7 @@
       </c>
       <c r="D27" s="32"/>
       <c r="E27" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>25</v>
@@ -35903,7 +36142,7 @@
       <c r="BV27" s="13"/>
       <c r="BW27" s="13"/>
     </row>
-    <row r="28" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>26</v>
       </c>
@@ -35915,7 +36154,7 @@
       </c>
       <c r="D28" s="32"/>
       <c r="E28" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>25</v>
@@ -36012,7 +36251,7 @@
       <c r="BV28" s="13"/>
       <c r="BW28" s="13"/>
     </row>
-    <row r="29" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>27</v>
       </c>
@@ -36024,7 +36263,7 @@
       </c>
       <c r="D29" s="32"/>
       <c r="E29" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>25</v>
@@ -36113,7 +36352,7 @@
       <c r="BV29" s="13"/>
       <c r="BW29" s="13"/>
     </row>
-    <row r="30" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>28</v>
       </c>
@@ -36125,7 +36364,7 @@
       </c>
       <c r="D30" s="32"/>
       <c r="E30" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>25</v>
@@ -36206,7 +36445,7 @@
       <c r="BV30" s="13"/>
       <c r="BW30" s="13"/>
     </row>
-    <row r="31" spans="1:75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>29</v>
       </c>
@@ -36218,7 +36457,7 @@
       </c>
       <c r="D31" s="32"/>
       <c r="E31" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F31" s="13" t="s">
         <v>25</v>
@@ -36247,7 +36486,7 @@
       <c r="X31" s="60"/>
       <c r="Y31" s="60"/>
       <c r="Z31" s="60" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="AA31" s="60"/>
       <c r="AB31" s="60" t="s">
@@ -36307,7 +36546,7 @@
       <c r="BV31" s="13"/>
       <c r="BW31" s="13"/>
     </row>
-    <row r="32" spans="1:75" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>30</v>
       </c>
@@ -36319,7 +36558,7 @@
       </c>
       <c r="D32" s="32"/>
       <c r="E32" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>25</v>
@@ -36410,7 +36649,7 @@
       <c r="BV32" s="13"/>
       <c r="BW32" s="13"/>
     </row>
-    <row r="33" spans="1:77" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="96">
         <v>31</v>
       </c>
@@ -36421,8 +36660,8 @@
         <v>316</v>
       </c>
       <c r="D33" s="99"/>
-      <c r="E33" s="96" t="s">
-        <v>0</v>
+      <c r="E33" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="F33" s="96" t="s">
         <v>25</v>
@@ -36503,7 +36742,7 @@
       <c r="BV33" s="96"/>
       <c r="BW33" s="96"/>
     </row>
-    <row r="34" spans="1:77" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>33</v>
       </c>
@@ -36515,7 +36754,7 @@
       </c>
       <c r="D34" s="32"/>
       <c r="E34" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F34" s="13" t="s">
         <v>25</v>
@@ -36612,7 +36851,7 @@
       <c r="BV34" s="13"/>
       <c r="BW34" s="13"/>
     </row>
-    <row r="35" spans="1:77" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>34</v>
       </c>
@@ -36624,7 +36863,7 @@
       </c>
       <c r="D35" s="32"/>
       <c r="E35" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F35" s="13" t="s">
         <v>25</v>
@@ -36709,7 +36948,7 @@
       <c r="BV35" s="13"/>
       <c r="BW35" s="13"/>
     </row>
-    <row r="36" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A36" s="18">
         <v>35</v>
       </c>
@@ -36721,7 +36960,7 @@
       </c>
       <c r="D36" s="13"/>
       <c r="E36" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>25</v>
@@ -36808,7 +37047,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="37" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A37" s="82">
         <v>36</v>
       </c>
@@ -36820,7 +37059,7 @@
       </c>
       <c r="D37" s="32"/>
       <c r="E37" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F37" s="13" t="s">
         <v>25</v>
@@ -36837,19 +37076,19 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="38" spans="1:77" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A38" s="82">
         <v>37</v>
       </c>
       <c r="B38" s="162" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="C38" s="32" t="s">
         <v>316</v>
       </c>
       <c r="D38" s="32"/>
       <c r="E38" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F38" s="13" t="s">
         <v>25</v>
@@ -36862,7 +37101,7 @@
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
       <c r="L38" s="16" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="M38" s="50"/>
       <c r="N38" s="13"/>
@@ -36882,7 +37121,7 @@
       <c r="X38" s="60"/>
       <c r="Y38" s="60"/>
       <c r="Z38" s="60" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="AA38" s="60"/>
       <c r="AB38" s="60" t="s">
@@ -36947,14 +37186,14 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="C39" s="32" t="s">
         <v>316</v>
       </c>
       <c r="D39" s="32"/>
       <c r="E39" s="13" t="s">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="F39" s="13" t="s">
         <v>25</v>
@@ -36969,10 +37208,10 @@
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
       <c r="L39" s="16" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="P39" s="50" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="S39" s="13" t="s">
         <v>6</v>
@@ -36984,7 +37223,7 @@
         <v>44</v>
       </c>
       <c r="BL39" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="BX39" s="34" t="s">
         <v>238</v>
@@ -37034,8 +37273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51C67A-098B-49A1-9024-B5BC951889FA}">
   <dimension ref="A1:AJ12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37141,15 +37380,15 @@
       <c r="B2" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>315</v>
+      <c r="C2" s="32" t="s">
+        <v>293</v>
       </c>
       <c r="D2" s="48"/>
       <c r="E2" s="48"/>
       <c r="F2" s="48"/>
       <c r="G2" s="48"/>
-      <c r="H2" s="23" t="s">
-        <v>0</v>
+      <c r="H2" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="23" t="s">
@@ -37206,8 +37445,8 @@
       <c r="E3" s="48"/>
       <c r="F3" s="48"/>
       <c r="G3" s="48"/>
-      <c r="H3" s="23" t="s">
-        <v>0</v>
+      <c r="H3" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="23" t="s">
@@ -37272,8 +37511,8 @@
       <c r="E4" s="48"/>
       <c r="F4" s="48"/>
       <c r="G4" s="48"/>
-      <c r="H4" s="23" t="s">
-        <v>0</v>
+      <c r="H4" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="23" t="s">
@@ -37336,8 +37575,8 @@
       <c r="E5" s="48"/>
       <c r="F5" s="48"/>
       <c r="G5" s="48"/>
-      <c r="H5" s="23" t="s">
-        <v>0</v>
+      <c r="H5" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="I5" s="36" t="s">
         <v>481</v>
@@ -37396,8 +37635,8 @@
       <c r="E6" s="48"/>
       <c r="F6" s="48"/>
       <c r="G6" s="48"/>
-      <c r="H6" s="23" t="s">
-        <v>0</v>
+      <c r="H6" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="23" t="s">
@@ -37454,8 +37693,8 @@
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
       <c r="G7" s="48"/>
-      <c r="H7" s="23" t="s">
-        <v>0</v>
+      <c r="H7" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="I7" s="36" t="s">
         <v>481</v>
@@ -37504,8 +37743,8 @@
       <c r="E8" s="48"/>
       <c r="F8" s="48"/>
       <c r="G8" s="48"/>
-      <c r="H8" s="23" t="s">
-        <v>0</v>
+      <c r="H8" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="I8" s="36" t="s">
         <v>481</v>
@@ -37554,8 +37793,8 @@
       <c r="E9" s="48"/>
       <c r="F9" s="48"/>
       <c r="G9" s="48"/>
-      <c r="H9" s="23" t="s">
-        <v>0</v>
+      <c r="H9" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="I9" s="23"/>
       <c r="J9" s="23" t="s">
@@ -37616,8 +37855,8 @@
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
       <c r="G10" s="48"/>
-      <c r="H10" s="23" t="s">
-        <v>0</v>
+      <c r="H10" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="I10" s="23"/>
       <c r="J10" s="23" t="s">
@@ -37682,8 +37921,8 @@
       <c r="E11" s="48"/>
       <c r="F11" s="48"/>
       <c r="G11" s="48"/>
-      <c r="H11" s="23" t="s">
-        <v>0</v>
+      <c r="H11" s="13" t="s">
+        <v>1441</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
@@ -37708,8 +37947,8 @@
       <c r="G12" s="32" t="s">
         <v>522</v>
       </c>
-      <c r="H12" s="23" t="s">
-        <v>0</v>
+      <c r="H12" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="I12" s="36" t="s">
         <v>481</v>
@@ -37724,20 +37963,20 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{E516A3F0-4A35-405F-A276-07D78E1B53B1}"/>
-    <hyperlink ref="C2" r:id="rId2" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{DF58F28A-C0AB-416F-8C71-40A2BAEF333C}"/>
-    <hyperlink ref="C3" r:id="rId3" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{DA7CC61C-6AAE-421F-8787-FF3FFEEEC2AC}"/>
-    <hyperlink ref="C4" r:id="rId4" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{329023C2-3A6B-43D7-AEEB-D3EC037D355C}"/>
-    <hyperlink ref="C5" r:id="rId5" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{DCE97C82-55B3-42F0-852B-18BAA6201127}"/>
-    <hyperlink ref="C6" r:id="rId6" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{2BACC580-6FC9-4B29-B946-40E5CB295937}"/>
-    <hyperlink ref="C7" r:id="rId7" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{081E6968-DA19-414F-8046-6015F87ADB15}"/>
-    <hyperlink ref="C8" r:id="rId8" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{DB6266BE-B085-4A20-B316-DD7D632F457B}"/>
-    <hyperlink ref="C9" r:id="rId9" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{752CF1E0-75D6-49E1-923B-BABE42CF60F9}"/>
-    <hyperlink ref="C11" r:id="rId10" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{80498F71-6095-4ADA-A47A-BFFA3EB2D667}"/>
-    <hyperlink ref="D12" r:id="rId11" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{2699F44E-6F32-47AA-A6B0-95ABB089C7F1}"/>
-    <hyperlink ref="F12" r:id="rId12" xr:uid="{34DA70B0-76F3-4D40-8D19-18C69D98D9C6}"/>
-    <hyperlink ref="E12" r:id="rId13" xr:uid="{FBA259BC-2277-4813-85C4-E44904FE86D1}"/>
-    <hyperlink ref="G12" r:id="rId14" xr:uid="{57FCA32A-B722-4BED-956F-DCF5BF0AF473}"/>
-    <hyperlink ref="C12" r:id="rId15" xr:uid="{BE65505C-0B58-48B7-9600-29A56A11F036}"/>
+    <hyperlink ref="C3" r:id="rId2" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{DA7CC61C-6AAE-421F-8787-FF3FFEEEC2AC}"/>
+    <hyperlink ref="C4" r:id="rId3" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{329023C2-3A6B-43D7-AEEB-D3EC037D355C}"/>
+    <hyperlink ref="C5" r:id="rId4" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{DCE97C82-55B3-42F0-852B-18BAA6201127}"/>
+    <hyperlink ref="C6" r:id="rId5" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{2BACC580-6FC9-4B29-B946-40E5CB295937}"/>
+    <hyperlink ref="C7" r:id="rId6" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{081E6968-DA19-414F-8046-6015F87ADB15}"/>
+    <hyperlink ref="C8" r:id="rId7" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{DB6266BE-B085-4A20-B316-DD7D632F457B}"/>
+    <hyperlink ref="C9" r:id="rId8" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{752CF1E0-75D6-49E1-923B-BABE42CF60F9}"/>
+    <hyperlink ref="C11" r:id="rId9" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{80498F71-6095-4ADA-A47A-BFFA3EB2D667}"/>
+    <hyperlink ref="D12" r:id="rId10" display="mailto:CRMTest02@corp.premierinc.com" xr:uid="{2699F44E-6F32-47AA-A6B0-95ABB089C7F1}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{34DA70B0-76F3-4D40-8D19-18C69D98D9C6}"/>
+    <hyperlink ref="E12" r:id="rId12" xr:uid="{FBA259BC-2277-4813-85C4-E44904FE86D1}"/>
+    <hyperlink ref="G12" r:id="rId13" xr:uid="{57FCA32A-B722-4BED-956F-DCF5BF0AF473}"/>
+    <hyperlink ref="C12" r:id="rId14" xr:uid="{BE65505C-0B58-48B7-9600-29A56A11F036}"/>
+    <hyperlink ref="C2" r:id="rId15" xr:uid="{C0150249-B667-42F5-8CE9-5877243C51D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
@@ -37830,7 +38069,7 @@
         <v>315</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E2" s="70" t="s">
         <v>1291</v>
@@ -37865,7 +38104,7 @@
         <v>315</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E3" s="70" t="s">
         <v>1291</v>
@@ -37924,16 +38163,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>315</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E4" s="70" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="F4" s="159" t="s">
         <v>1319</v>
@@ -37959,13 +38198,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>315</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E5" s="70" t="s">
         <v>1291</v>
@@ -38069,7 +38308,7 @@
         <v>315</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E2" s="70" t="s">
         <v>1291</v>
@@ -38086,7 +38325,7 @@
         <v>315</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E3" s="70" t="s">
         <v>1291</v>
@@ -38103,7 +38342,7 @@
         <v>315</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E4" s="70" t="s">
         <v>1291</v>
@@ -41089,8 +41328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
   <dimension ref="A1:FH140"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="BO1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BS2" sqref="BS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41639,7 +41878,7 @@
         <v>64</v>
       </c>
       <c r="EQ1" s="1" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="ER1" s="1" t="s">
         <v>19</v>
@@ -41663,16 +41902,16 @@
         <v>74</v>
       </c>
       <c r="EY1" s="59" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="EZ1" s="59" t="s">
+        <v>1364</v>
+      </c>
+      <c r="FA1" s="59" t="s">
+        <v>1368</v>
+      </c>
+      <c r="FB1" s="59" t="s">
         <v>1367</v>
-      </c>
-      <c r="FA1" s="59" t="s">
-        <v>1371</v>
-      </c>
-      <c r="FB1" s="59" t="s">
-        <v>1370</v>
       </c>
     </row>
     <row r="2" spans="1:158" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -41683,10 +41922,10 @@
         <v>35</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>315</v>
+        <v>293</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="36" t="s">
@@ -41908,7 +42147,7 @@
         <v>315</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="36" t="s">
@@ -42134,7 +42373,7 @@
         <v>315</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="36" t="s">
@@ -42347,7 +42586,7 @@
         <v>315</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="36" t="s">
@@ -42552,7 +42791,7 @@
         <v>315</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="36" t="s">
@@ -42759,7 +42998,7 @@
         <v>315</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="36" t="s">
@@ -42964,7 +43203,7 @@
         <v>293</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -43179,7 +43418,7 @@
         <v>293</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -43398,7 +43637,7 @@
         <v>315</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="36" t="s">
@@ -43611,7 +43850,7 @@
         <v>315</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="36" t="s">
@@ -43828,7 +44067,7 @@
         <v>315</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="36" t="s">
@@ -44039,7 +44278,7 @@
         <v>315</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="36" t="s">
@@ -44250,7 +44489,7 @@
         <v>315</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="36" t="s">
@@ -44461,7 +44700,7 @@
         <v>315</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="36" t="s">
@@ -44674,7 +44913,7 @@
         <v>315</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="36" t="s">
@@ -44887,7 +45126,7 @@
         <v>315</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -45096,7 +45335,7 @@
         <v>315</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="44"/>
@@ -45317,7 +45556,7 @@
         <v>315</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="36" t="s">
@@ -45624,7 +45863,7 @@
         <v>315</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="36" t="s">
@@ -45837,7 +46076,7 @@
         <v>537</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="49" t="s">
@@ -46000,7 +46239,7 @@
         <v>537</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="49" t="s">
@@ -46163,7 +46402,7 @@
         <v>537</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="49" t="s">
@@ -46326,7 +46565,7 @@
         <v>537</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="49" t="s">
@@ -46489,7 +46728,7 @@
         <v>537</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="49" t="s">
@@ -46654,7 +46893,7 @@
         <v>537</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="49" t="s">
@@ -46819,7 +47058,7 @@
         <v>537</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="36" t="s">
@@ -46998,7 +47237,7 @@
         <v>522</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="50"/>
@@ -47187,7 +47426,7 @@
         <v>315</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="15"/>
@@ -47394,7 +47633,7 @@
         <v>293</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="49" t="s">
@@ -47555,7 +47794,7 @@
         <v>293</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
@@ -47752,7 +47991,7 @@
         <v>293</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
@@ -47949,7 +48188,7 @@
         <v>293</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
@@ -48146,7 +48385,7 @@
         <v>293</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
@@ -48343,7 +48582,7 @@
         <v>293</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
@@ -48540,7 +48779,7 @@
         <v>293</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
@@ -48737,7 +48976,7 @@
         <v>293</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
@@ -48936,7 +49175,7 @@
         <v>293</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
@@ -49135,7 +49374,7 @@
         <v>293</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -49334,7 +49573,7 @@
         <v>293</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
@@ -49537,7 +49776,7 @@
         <v>293</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
@@ -49740,7 +49979,7 @@
         <v>293</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
@@ -49943,7 +50182,7 @@
         <v>293</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="14"/>
@@ -50146,7 +50385,7 @@
         <v>293</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
@@ -50349,7 +50588,7 @@
         <v>293</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
@@ -50552,7 +50791,7 @@
         <v>293</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
@@ -50757,7 +50996,7 @@
         <v>293</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
@@ -50962,7 +51201,7 @@
         <v>293</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
@@ -51167,7 +51406,7 @@
         <v>293</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
@@ -51364,7 +51603,7 @@
         <v>293</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="44"/>
@@ -51567,7 +51806,7 @@
         <v>293</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E51" s="7"/>
       <c r="F51" s="36" t="s">
@@ -51707,7 +51946,7 @@
         <v>293</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E52" s="7"/>
       <c r="J52" s="2" t="s">
@@ -51831,7 +52070,7 @@
         <v>293</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E53" s="7"/>
       <c r="J53" s="2" t="s">
@@ -51938,7 +52177,7 @@
         <v>293</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E54" s="7"/>
       <c r="F54" s="79" t="s">
@@ -51976,7 +52215,7 @@
         <v>293</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E55" s="14"/>
       <c r="F55" s="14"/>
@@ -52158,7 +52397,7 @@
         <v>293</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="36" t="s">
@@ -52348,7 +52587,7 @@
         <v>293</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
@@ -52549,7 +52788,7 @@
         <v>293</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E58" s="4"/>
       <c r="J58" s="2" t="s">
@@ -52751,7 +52990,7 @@
         <v>293</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E59" s="4"/>
       <c r="J59" s="15" t="s">
@@ -52921,7 +53160,7 @@
         <v>293</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="79" t="s">
@@ -53115,7 +53354,7 @@
         <v>293</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E61" s="15"/>
       <c r="F61" s="15"/>
@@ -53315,7 +53554,7 @@
         <v>293</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" s="36" t="s">
@@ -53470,7 +53709,7 @@
         <v>293</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E63" s="7"/>
       <c r="AI63" s="79" t="s">
@@ -53504,7 +53743,7 @@
         <v>315</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E64" s="13"/>
       <c r="F64" s="15"/>
@@ -53700,7 +53939,7 @@
         <v>315</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E65"/>
       <c r="EH65" s="44"/>
@@ -53719,7 +53958,7 @@
         <v>315</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E66"/>
       <c r="K66" s="2" t="s">
@@ -53747,7 +53986,7 @@
         <v>293</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E67" s="15"/>
       <c r="F67" s="15"/>
@@ -53966,7 +54205,7 @@
         <v>315</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E68" s="13"/>
       <c r="F68" s="15"/>
@@ -54162,7 +54401,7 @@
         <v>293</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E69" s="4"/>
       <c r="J69" s="15" t="s">
@@ -54350,7 +54589,7 @@
         <v>315</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E70" s="32" t="s">
         <v>316</v>
@@ -54543,7 +54782,7 @@
         <v>537</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E71" s="14"/>
       <c r="F71" s="50" t="s">
@@ -54744,7 +54983,7 @@
         <v>537</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E72" s="14"/>
       <c r="F72" s="50" t="s">
@@ -54955,7 +55194,7 @@
         <v>537</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E73" s="14"/>
       <c r="F73" s="50" t="s">
@@ -55116,7 +55355,7 @@
         <v>537</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E74" s="14"/>
       <c r="F74" s="50" t="s">
@@ -55275,7 +55514,7 @@
         <v>537</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E75" s="14"/>
       <c r="F75" s="50"/>
@@ -55434,7 +55673,7 @@
         <v>537</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E76" s="14"/>
       <c r="F76" s="50" t="s">
@@ -55593,7 +55832,7 @@
         <v>537</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E77" s="13"/>
       <c r="F77" s="15"/>
@@ -55746,7 +55985,7 @@
         <v>537</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E78" s="13"/>
       <c r="F78" s="15"/>
@@ -55899,7 +56138,7 @@
         <v>537</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E79" s="13"/>
       <c r="F79" s="36" t="s">
@@ -56058,7 +56297,7 @@
         <v>537</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E80" s="13"/>
       <c r="F80" s="36"/>
@@ -56211,7 +56450,7 @@
         <v>537</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E81" s="13"/>
       <c r="F81" s="36"/>
@@ -56372,7 +56611,7 @@
         <v>537</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E82" s="13"/>
       <c r="F82" s="36"/>
@@ -56533,7 +56772,7 @@
         <v>537</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E83" s="13"/>
       <c r="F83" s="36"/>
@@ -56686,7 +56925,7 @@
         <v>537</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E84" s="102" t="s">
         <v>745</v>
@@ -56847,7 +57086,7 @@
         <v>537</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E85" s="102"/>
       <c r="F85" s="36"/>
@@ -57000,7 +57239,7 @@
         <v>537</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E86" s="102"/>
       <c r="F86" s="36"/>
@@ -57153,7 +57392,7 @@
         <v>522</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E87" s="102"/>
       <c r="F87" s="36"/>
@@ -57306,7 +57545,7 @@
         <v>522</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E88" s="102"/>
       <c r="F88" s="36"/>
@@ -57459,7 +57698,7 @@
         <v>522</v>
       </c>
       <c r="D89" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E89" s="14"/>
       <c r="F89" s="50"/>
@@ -57618,7 +57857,7 @@
         <v>522</v>
       </c>
       <c r="D90" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E90" s="102" t="s">
         <v>745</v>
@@ -57781,7 +58020,7 @@
         <v>522</v>
       </c>
       <c r="D91" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E91" s="13"/>
       <c r="F91" s="36" t="s">
@@ -57942,7 +58181,7 @@
         <v>522</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E92" s="102"/>
       <c r="F92" s="36"/>
@@ -58095,7 +58334,7 @@
         <v>522</v>
       </c>
       <c r="D93" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E93" s="102"/>
       <c r="F93" s="36"/>
@@ -58248,7 +58487,7 @@
         <v>522</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E94" s="102"/>
       <c r="F94" s="36"/>
@@ -58401,7 +58640,7 @@
         <v>522</v>
       </c>
       <c r="D95" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E95" s="102"/>
       <c r="F95" s="36"/>
@@ -58554,7 +58793,7 @@
         <v>522</v>
       </c>
       <c r="D96" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E96" s="14"/>
       <c r="F96" s="50" t="s">
@@ -58821,7 +59060,7 @@
         <v>522</v>
       </c>
       <c r="D97" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E97" s="44"/>
       <c r="F97" s="50" t="s">
@@ -58978,7 +59217,7 @@
         <v>522</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E98" s="102" t="s">
         <v>796</v>
@@ -59145,7 +59384,7 @@
         <v>522</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E99" s="102" t="s">
         <v>805</v>
@@ -59314,7 +59553,7 @@
         <v>293</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E100" s="32" t="s">
         <v>522</v>
@@ -59483,7 +59722,7 @@
         <v>522</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E101" s="13"/>
       <c r="F101" s="36"/>
@@ -59636,7 +59875,7 @@
         <v>522</v>
       </c>
       <c r="D102" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E102" s="13"/>
       <c r="F102" s="36"/>
@@ -59789,7 +60028,7 @@
         <v>522</v>
       </c>
       <c r="D103" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E103" s="13"/>
       <c r="F103" s="36"/>
@@ -59944,7 +60183,7 @@
         <v>315</v>
       </c>
       <c r="D104" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E104" s="13"/>
       <c r="F104" s="36" t="s">
@@ -60103,7 +60342,7 @@
         <v>315</v>
       </c>
       <c r="D105" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E105" s="13"/>
       <c r="F105" s="36" t="s">
@@ -60262,7 +60501,7 @@
         <v>315</v>
       </c>
       <c r="D106" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E106" s="13"/>
       <c r="F106" s="36" t="s">
@@ -60419,7 +60658,7 @@
         <v>315</v>
       </c>
       <c r="D107" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E107" s="13"/>
       <c r="F107" s="36" t="s">
@@ -60578,7 +60817,7 @@
         <v>315</v>
       </c>
       <c r="D108" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E108" s="13"/>
       <c r="F108" s="36" t="s">
@@ -60735,7 +60974,7 @@
         <v>315</v>
       </c>
       <c r="D109" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E109" s="13"/>
       <c r="F109" s="36" t="s">
@@ -60892,7 +61131,7 @@
         <v>293</v>
       </c>
       <c r="D110" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E110" s="13"/>
       <c r="F110" s="36" t="s">
@@ -61051,7 +61290,7 @@
         <v>293</v>
       </c>
       <c r="D111" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E111" s="13"/>
       <c r="F111" s="36" t="s">
@@ -61210,7 +61449,7 @@
         <v>315</v>
       </c>
       <c r="D112" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E112" s="13"/>
       <c r="F112" s="36" t="s">
@@ -61369,7 +61608,7 @@
         <v>315</v>
       </c>
       <c r="D113" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E113" s="13"/>
       <c r="F113" s="36" t="s">
@@ -61528,7 +61767,7 @@
         <v>315</v>
       </c>
       <c r="D114" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E114" s="13"/>
       <c r="F114" s="36" t="s">
@@ -61685,7 +61924,7 @@
         <v>315</v>
       </c>
       <c r="D115" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E115" s="13"/>
       <c r="F115" s="36" t="s">
@@ -61842,7 +62081,7 @@
         <v>315</v>
       </c>
       <c r="D116" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E116" s="13"/>
       <c r="F116" s="36" t="s">
@@ -61999,7 +62238,7 @@
         <v>315</v>
       </c>
       <c r="D117" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E117" s="13"/>
       <c r="F117" s="36" t="s">
@@ -62156,7 +62395,7 @@
         <v>315</v>
       </c>
       <c r="D118" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E118" s="13"/>
       <c r="F118" s="36" t="s">
@@ -62315,7 +62554,7 @@
         <v>315</v>
       </c>
       <c r="D119" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E119" s="13"/>
       <c r="F119" s="36" t="s">
@@ -62474,7 +62713,7 @@
         <v>315</v>
       </c>
       <c r="D120" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E120" s="13"/>
       <c r="F120" s="36"/>
@@ -62657,7 +62896,7 @@
         <v>293</v>
       </c>
       <c r="D121" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E121" s="13"/>
       <c r="F121" s="36"/>
@@ -62866,7 +63105,7 @@
         <v>293</v>
       </c>
       <c r="D122" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E122" s="32" t="s">
         <v>316</v>
@@ -63029,7 +63268,7 @@
         <v>293</v>
       </c>
       <c r="D123" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E123" s="32"/>
       <c r="F123" s="36" t="s">
@@ -63190,7 +63429,7 @@
         <v>293</v>
       </c>
       <c r="D124" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="AI124" s="79" t="s">
         <v>920</v>
@@ -63210,7 +63449,7 @@
         <v>293</v>
       </c>
       <c r="D125" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="J125" s="2" t="s">
         <v>921</v>
@@ -63411,7 +63650,7 @@
         <v>293</v>
       </c>
       <c r="D126" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="J126" s="2" t="s">
         <v>922</v>
@@ -63600,7 +63839,7 @@
         <v>293</v>
       </c>
       <c r="D127" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="J127" s="2" t="s">
         <v>923</v>
@@ -63792,7 +64031,7 @@
         <v>293</v>
       </c>
       <c r="D128" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="J128" s="2" t="s">
         <v>924</v>
@@ -63984,7 +64223,7 @@
         <v>293</v>
       </c>
       <c r="D129" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="EA129" s="79" t="s">
         <v>930</v>
@@ -64004,7 +64243,7 @@
         <v>293</v>
       </c>
       <c r="D130" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="AI130" s="36" t="s">
         <v>548</v>
@@ -64021,7 +64260,7 @@
         <v>315</v>
       </c>
       <c r="D131" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E131" s="13"/>
       <c r="F131" s="36" t="s">
@@ -64228,7 +64467,7 @@
         <v>315</v>
       </c>
       <c r="D132" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E132" s="13"/>
       <c r="F132" s="36" t="s">
@@ -64429,13 +64668,13 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="C133" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D133" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E133" s="15"/>
       <c r="F133" s="36" t="s">
@@ -64453,13 +64692,13 @@
         <v>132</v>
       </c>
       <c r="B134" s="150" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="C134" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D134" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="E134" s="32" t="s">
         <v>316</v>
@@ -64471,7 +64710,7 @@
       <c r="H134" s="15"/>
       <c r="I134" s="15"/>
       <c r="J134" s="15" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="K134" s="15"/>
       <c r="L134" s="15"/>
@@ -64709,13 +64948,13 @@
         <v>133</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="C135" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D135" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="F135" s="36" t="s">
         <v>934</v>
@@ -64724,7 +64963,7 @@
       <c r="H135" s="15"/>
       <c r="I135" s="15"/>
       <c r="J135" s="15" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="K135" s="15"/>
       <c r="L135" s="15"/>
@@ -64928,13 +65167,13 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
       <c r="C136" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D136" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="137" spans="1:164" x14ac:dyDescent="0.25">
@@ -64942,28 +65181,28 @@
         <v>135</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="C137" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D137" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="F137" s="79" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="EY137" s="2" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="EZ137" s="2" t="s">
+        <v>1366</v>
+      </c>
+      <c r="FA137" s="2" t="s">
         <v>1369</v>
       </c>
-      <c r="FA137" s="2" t="s">
-        <v>1372</v>
-      </c>
       <c r="FB137" s="2" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="138" spans="1:164" x14ac:dyDescent="0.25">
@@ -64971,16 +65210,16 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="C138" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D138" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="F138" s="79" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="139" spans="1:164" x14ac:dyDescent="0.25">
@@ -64988,22 +65227,22 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="C139" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D139" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="J139" s="79" t="s">
+        <v>1379</v>
+      </c>
+      <c r="EA139" t="s">
+        <v>1381</v>
+      </c>
+      <c r="ED139" t="s">
         <v>1382</v>
-      </c>
-      <c r="EA139" t="s">
-        <v>1384</v>
-      </c>
-      <c r="ED139" t="s">
-        <v>1385</v>
       </c>
     </row>
     <row r="140" spans="1:164" x14ac:dyDescent="0.25">
@@ -65011,13 +65250,13 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="C140" s="32" t="s">
         <v>293</v>
       </c>
       <c r="D140" s="13" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="F140" s="79" t="s">
         <v>1242</v>
@@ -65091,41 +65330,40 @@
     <hyperlink ref="C20" r:id="rId63" xr:uid="{88DDF8CF-8656-43EC-8392-604FE39635FB}"/>
     <hyperlink ref="C28" r:id="rId64" xr:uid="{DB18DE21-C3FB-40D0-820B-7F4C01DE84C3}"/>
     <hyperlink ref="C29" r:id="rId65" xr:uid="{3F64DDC4-F553-41F8-8AA4-9089AB98F155}"/>
-    <hyperlink ref="C2:C7" r:id="rId66" display="CRMTest02@corp.premierinc.com" xr:uid="{EFB3EAB7-9048-4382-93C1-EB4FB27A3F75}"/>
-    <hyperlink ref="C10:C17" r:id="rId67" display="CRMTest02@corp.premierinc.com" xr:uid="{5E951E68-F759-4A8B-8D5E-74E1DB8FBEB8}"/>
-    <hyperlink ref="C19" r:id="rId68" xr:uid="{3EBA7228-DE62-438A-8E68-E18EF0323C34}"/>
-    <hyperlink ref="DS19" r:id="rId69" xr:uid="{558F1011-DCFF-438E-96B8-7AA96C164068}"/>
-    <hyperlink ref="C121" r:id="rId70" xr:uid="{746EBFB2-151E-40D3-AE55-79B9BC5DED1F}"/>
-    <hyperlink ref="E122" r:id="rId71" xr:uid="{D6AB8FA4-13F3-4E22-9A66-98C0A0525051}"/>
-    <hyperlink ref="C124" r:id="rId72" xr:uid="{6BF8CAF4-B892-4CE6-8DEC-C7F39D884BD8}"/>
-    <hyperlink ref="C125" r:id="rId73" xr:uid="{EC651A7F-4A6B-4DE6-82F3-7DF9CD169926}"/>
-    <hyperlink ref="C126" r:id="rId74" xr:uid="{FB833FFD-8613-4E39-A26D-7E4ACB703464}"/>
-    <hyperlink ref="C127" r:id="rId75" xr:uid="{C5FB9522-A7BF-4171-8F5F-C89826D19296}"/>
-    <hyperlink ref="C128" r:id="rId76" xr:uid="{5DDE73DC-D5AB-45C0-8623-5068DC3782F5}"/>
-    <hyperlink ref="C129" r:id="rId77" xr:uid="{2C3B9E27-09F0-4E99-8879-178C6E517CFE}"/>
-    <hyperlink ref="C130" r:id="rId78" xr:uid="{E15EF213-4A2E-454C-AEC4-2BB9C4F7BD9E}"/>
-    <hyperlink ref="C21" r:id="rId79" xr:uid="{41BDBFA1-19C7-40CF-BE8E-AE28E7384D20}"/>
-    <hyperlink ref="C22" r:id="rId80" xr:uid="{AE8E882E-CD4E-4A8D-8543-E09F9F2CFBDF}"/>
-    <hyperlink ref="C23" r:id="rId81" xr:uid="{DB4B16BD-1CF1-47E3-80FA-4DED7FA29FBA}"/>
-    <hyperlink ref="C24" r:id="rId82" xr:uid="{B6FB9A83-C9BF-4397-87DB-8D77092B7F0F}"/>
-    <hyperlink ref="C25" r:id="rId83" xr:uid="{217128AA-03A3-4F1B-8F80-A4FFCEC825EF}"/>
-    <hyperlink ref="C26" r:id="rId84" xr:uid="{EC17A159-4F9E-46A6-93B9-3EF1DC2BB1FF}"/>
-    <hyperlink ref="C27" r:id="rId85" xr:uid="{D3838068-BA75-4BF3-8EEF-773233102280}"/>
-    <hyperlink ref="C7" r:id="rId86" xr:uid="{D04B27E3-F568-469C-B42E-2B61B4066585}"/>
-    <hyperlink ref="C131" r:id="rId87" xr:uid="{D4070502-49B8-441A-8214-2FC3E287FBDD}"/>
-    <hyperlink ref="C132" r:id="rId88" xr:uid="{A3C66069-98F9-4AB9-B5E9-619DA48CEA31}"/>
-    <hyperlink ref="C133" r:id="rId89" xr:uid="{AFF8A0CC-3893-4D3A-B945-885B6B22C47D}"/>
-    <hyperlink ref="C134" r:id="rId90" xr:uid="{DAF41585-BB7E-4F9B-9CBA-D3E3A5488860}"/>
-    <hyperlink ref="E134" r:id="rId91" xr:uid="{98E39949-68E6-4633-ADAF-E1A7E8280175}"/>
-    <hyperlink ref="C135" r:id="rId92" xr:uid="{7DC3D85D-85A2-4CA4-81C2-BB917732217C}"/>
-    <hyperlink ref="C136" r:id="rId93" xr:uid="{88F93F0C-52AB-470A-A899-2220E09CB6E2}"/>
-    <hyperlink ref="C137" r:id="rId94" xr:uid="{CDD3BDD9-1FE5-4359-A564-7D6B58F2F971}"/>
-    <hyperlink ref="C138" r:id="rId95" xr:uid="{63FAF3ED-2222-451F-AED6-EFA70E060AA3}"/>
-    <hyperlink ref="C139" r:id="rId96" xr:uid="{30ACC8D6-4A74-45DB-8B12-BD8406DED0B2}"/>
-    <hyperlink ref="C140" r:id="rId97" xr:uid="{DF0BA91E-1971-4011-955A-DA31E77816C7}"/>
+    <hyperlink ref="C10:C17" r:id="rId66" display="CRMTest02@corp.premierinc.com" xr:uid="{5E951E68-F759-4A8B-8D5E-74E1DB8FBEB8}"/>
+    <hyperlink ref="C19" r:id="rId67" xr:uid="{3EBA7228-DE62-438A-8E68-E18EF0323C34}"/>
+    <hyperlink ref="DS19" r:id="rId68" xr:uid="{558F1011-DCFF-438E-96B8-7AA96C164068}"/>
+    <hyperlink ref="C121" r:id="rId69" xr:uid="{746EBFB2-151E-40D3-AE55-79B9BC5DED1F}"/>
+    <hyperlink ref="E122" r:id="rId70" xr:uid="{D6AB8FA4-13F3-4E22-9A66-98C0A0525051}"/>
+    <hyperlink ref="C124" r:id="rId71" xr:uid="{6BF8CAF4-B892-4CE6-8DEC-C7F39D884BD8}"/>
+    <hyperlink ref="C125" r:id="rId72" xr:uid="{EC651A7F-4A6B-4DE6-82F3-7DF9CD169926}"/>
+    <hyperlink ref="C126" r:id="rId73" xr:uid="{FB833FFD-8613-4E39-A26D-7E4ACB703464}"/>
+    <hyperlink ref="C127" r:id="rId74" xr:uid="{C5FB9522-A7BF-4171-8F5F-C89826D19296}"/>
+    <hyperlink ref="C128" r:id="rId75" xr:uid="{5DDE73DC-D5AB-45C0-8623-5068DC3782F5}"/>
+    <hyperlink ref="C129" r:id="rId76" xr:uid="{2C3B9E27-09F0-4E99-8879-178C6E517CFE}"/>
+    <hyperlink ref="C130" r:id="rId77" xr:uid="{E15EF213-4A2E-454C-AEC4-2BB9C4F7BD9E}"/>
+    <hyperlink ref="C21" r:id="rId78" xr:uid="{41BDBFA1-19C7-40CF-BE8E-AE28E7384D20}"/>
+    <hyperlink ref="C22" r:id="rId79" xr:uid="{AE8E882E-CD4E-4A8D-8543-E09F9F2CFBDF}"/>
+    <hyperlink ref="C23" r:id="rId80" xr:uid="{DB4B16BD-1CF1-47E3-80FA-4DED7FA29FBA}"/>
+    <hyperlink ref="C24" r:id="rId81" xr:uid="{B6FB9A83-C9BF-4397-87DB-8D77092B7F0F}"/>
+    <hyperlink ref="C25" r:id="rId82" xr:uid="{217128AA-03A3-4F1B-8F80-A4FFCEC825EF}"/>
+    <hyperlink ref="C26" r:id="rId83" xr:uid="{EC17A159-4F9E-46A6-93B9-3EF1DC2BB1FF}"/>
+    <hyperlink ref="C27" r:id="rId84" xr:uid="{D3838068-BA75-4BF3-8EEF-773233102280}"/>
+    <hyperlink ref="C7" r:id="rId85" xr:uid="{D04B27E3-F568-469C-B42E-2B61B4066585}"/>
+    <hyperlink ref="C131" r:id="rId86" xr:uid="{D4070502-49B8-441A-8214-2FC3E287FBDD}"/>
+    <hyperlink ref="C132" r:id="rId87" xr:uid="{A3C66069-98F9-4AB9-B5E9-619DA48CEA31}"/>
+    <hyperlink ref="C133" r:id="rId88" xr:uid="{AFF8A0CC-3893-4D3A-B945-885B6B22C47D}"/>
+    <hyperlink ref="C134" r:id="rId89" xr:uid="{DAF41585-BB7E-4F9B-9CBA-D3E3A5488860}"/>
+    <hyperlink ref="E134" r:id="rId90" xr:uid="{98E39949-68E6-4633-ADAF-E1A7E8280175}"/>
+    <hyperlink ref="C135" r:id="rId91" xr:uid="{7DC3D85D-85A2-4CA4-81C2-BB917732217C}"/>
+    <hyperlink ref="C136" r:id="rId92" xr:uid="{88F93F0C-52AB-470A-A899-2220E09CB6E2}"/>
+    <hyperlink ref="C137" r:id="rId93" xr:uid="{CDD3BDD9-1FE5-4359-A564-7D6B58F2F971}"/>
+    <hyperlink ref="C138" r:id="rId94" xr:uid="{63FAF3ED-2222-451F-AED6-EFA70E060AA3}"/>
+    <hyperlink ref="C139" r:id="rId95" xr:uid="{30ACC8D6-4A74-45DB-8B12-BD8406DED0B2}"/>
+    <hyperlink ref="C140" r:id="rId96" xr:uid="{DF0BA91E-1971-4011-955A-DA31E77816C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId98"/>
+  <pageSetup orientation="portrait" r:id="rId97"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updating the Latest code
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\Dynamics-CRM-Cloud\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452D4E05-39A8-4164-AE42-0645AFFFB0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FFF47F-475E-4CE2-B9FC-30CC44F58175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" firstSheet="2" activeTab="5" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10591" uniqueCount="1525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10640" uniqueCount="1531">
   <si>
     <t>Premier1a</t>
   </si>
@@ -4622,9 +4622,6 @@
     <t>SdirectParent</t>
   </si>
   <si>
-    <t>2022_10_27_10_16_38</t>
-  </si>
-  <si>
     <t>AB9796</t>
   </si>
   <si>
@@ -4632,6 +4629,27 @@
   </si>
   <si>
     <t>2022_10_27_11_05_09</t>
+  </si>
+  <si>
+    <t>TFS ID_8802:Cloud - Verify newly added "GPO memberships" in DP should not get cascaded to the "location type children" in draft status.</t>
+  </si>
+  <si>
+    <t>8802_Shipto</t>
+  </si>
+  <si>
+    <t>2022_10_27_02_40_15</t>
+  </si>
+  <si>
+    <t>1000048435</t>
+  </si>
+  <si>
+    <t>2000331034</t>
+  </si>
+  <si>
+    <t>2022_10_28_08_11_41</t>
+  </si>
+  <si>
+    <t>TFS ID_8804:Cloud - Verify User should be able to override "CP and FSP" values and user should not allow to choose "Supplier" as CP or FSP.</t>
   </si>
 </sst>
 </file>
@@ -5609,24 +5627,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
-  <dimension ref="A1:P316"/>
+  <dimension ref="A1:P318"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="132.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="9" max="10" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="46.0" collapsed="true"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="132.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="46" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -8801,9 +8819,11 @@
         <v>39</v>
       </c>
       <c r="F120" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G120" s="104"/>
+        <v>1453</v>
+      </c>
+      <c r="G120" s="104" t="s">
+        <v>1529</v>
+      </c>
       <c r="H120" s="104"/>
       <c r="I120" s="104"/>
       <c r="J120" s="104"/>
@@ -13752,7 +13772,7 @@
         <v>1516</v>
       </c>
       <c r="C316" s="150" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D316" s="150" t="s">
         <v>2</v>
@@ -13764,10 +13784,56 @@
         <v>1453</v>
       </c>
       <c r="G316" t="s">
+        <v>1523</v>
+      </c>
+      <c r="H316" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A317" s="150">
+        <v>309</v>
+      </c>
+      <c r="B317" t="s">
         <v>1524</v>
       </c>
-      <c r="H316" t="s">
-        <v>1523</v>
+      <c r="C317" s="150" t="s">
+        <v>34</v>
+      </c>
+      <c r="D317" s="150" t="s">
+        <v>2</v>
+      </c>
+      <c r="E317" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F317" s="17" t="s">
+        <v>1455</v>
+      </c>
+      <c r="G317" t="s">
+        <v>1526</v>
+      </c>
+      <c r="H317" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A318" s="150">
+        <v>310</v>
+      </c>
+      <c r="B318" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C318" s="150" t="s">
+        <v>33</v>
+      </c>
+      <c r="D318" s="150" t="s">
+        <v>2</v>
+      </c>
+      <c r="E318" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F318" s="17" t="s">
+        <v>1455</v>
       </c>
     </row>
   </sheetData>
@@ -15975,7 +16041,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:168" x14ac:dyDescent="0.25">
@@ -18036,7 +18102,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:155" x14ac:dyDescent="0.25">
@@ -19524,7 +19590,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="136.0" collapsed="true"/>
+    <col min="2" max="2" width="136" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:141" x14ac:dyDescent="0.25">
@@ -20927,7 +20993,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" style="127" width="60.28515625" collapsed="true"/>
+    <col min="2" max="2" width="60.28515625" style="127" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:141" x14ac:dyDescent="0.25">
@@ -23591,7 +23657,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="84.140625" collapsed="true"/>
+    <col min="2" max="2" width="84.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:141" x14ac:dyDescent="0.25">
@@ -33062,69 +33128,69 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="114.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="82.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="25.85546875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="28" max="36" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="42" max="42" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="43" max="43" customWidth="true" width="54.42578125" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="46" max="47" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="49" max="49" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="51" max="51" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="55" max="56" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="68" max="68" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="69" max="69" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="70" max="70" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="71" max="71" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="74" max="75" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="114" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="82.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="28" max="36" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="34.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="54.42578125" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="47" width="29" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="56" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="74" max="75" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:77" x14ac:dyDescent="0.25">
@@ -37329,27 +37395,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="108.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="4" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="65.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="73.85546875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="108" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="7" width="29.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="65.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="73.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -38419,8 +38485,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" style="152" width="9.140625" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="2" max="2" width="9.140625" style="152" collapsed="1"/>
+    <col min="56" max="56" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:89" x14ac:dyDescent="0.25">
@@ -41376,116 +41442,116 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
-  <dimension ref="A1:FH141"/>
+  <dimension ref="A1:FH143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="ES123" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="FC141" sqref="FC141"/>
+    <sheetView topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="5.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="121.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="29.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="13.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="13.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="11.28515625" collapsed="true"/>
-    <col min="7" max="9" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="69.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="2" width="36.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="73.5703125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="2" width="73.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="20.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="15.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
-    <col min="19" max="20" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="21" max="24" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="21.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="2" width="4.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="2" width="8.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="2" width="24.140625" collapsed="true"/>
-    <col min="38" max="38" customWidth="true" style="2" width="24.140625" collapsed="true"/>
-    <col min="39" max="39" customWidth="true" style="2" width="15.0" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="2" width="9.85546875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="2" width="9.5703125" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="2" width="22.28515625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="2" width="24.5703125" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
-    <col min="50" max="50" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" style="2" width="20.5703125" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" style="2" width="26.42578125" collapsed="true"/>
-    <col min="54" max="56" customWidth="true" style="2" width="26.42578125" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
-    <col min="58" max="58" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" style="2" width="25.0" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" style="2" width="15.140625" collapsed="true"/>
-    <col min="61" max="61" customWidth="true" style="2" width="15.140625" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" style="2" width="15.7109375" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
-    <col min="65" max="65" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" style="2" width="30.42578125" collapsed="true"/>
-    <col min="68" max="68" bestFit="true" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
-    <col min="69" max="80" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
-    <col min="81" max="81" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="82" max="82" bestFit="true" customWidth="true" style="2" width="26.140625" collapsed="true"/>
-    <col min="83" max="83" bestFit="true" customWidth="true" style="2" width="18.140625" collapsed="true"/>
-    <col min="84" max="84" customWidth="true" style="2" width="18.140625" collapsed="true"/>
-    <col min="85" max="91" customWidth="true" style="2" width="26.140625" collapsed="true"/>
-    <col min="92" max="92" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="93" max="93" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="94" max="94" bestFit="true" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
-    <col min="95" max="95" bestFit="true" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
-    <col min="96" max="96" style="2" width="9.140625" collapsed="true"/>
-    <col min="97" max="97" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
-    <col min="98" max="98" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="99" max="99" bestFit="true" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
-    <col min="100" max="100" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="101" max="101" bestFit="true" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
-    <col min="102" max="102" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
-    <col min="103" max="103" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
-    <col min="104" max="104" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
-    <col min="105" max="105" bestFit="true" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
-    <col min="106" max="106" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
-    <col min="107" max="107" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
-    <col min="108" max="108" bestFit="true" customWidth="true" style="2" width="10.7109375" collapsed="true"/>
-    <col min="109" max="109" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
-    <col min="110" max="110" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
-    <col min="111" max="111" bestFit="true" customWidth="true" style="2" width="9.28515625" collapsed="true"/>
-    <col min="112" max="112" bestFit="true" customWidth="true" style="2" width="14.140625" collapsed="true"/>
-    <col min="113" max="113" bestFit="true" customWidth="true" style="2" width="32.0" collapsed="true"/>
-    <col min="114" max="114" bestFit="true" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
-    <col min="115" max="121" style="2" width="9.140625" collapsed="true"/>
-    <col min="122" max="122" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="123" max="130" style="2" width="9.140625" collapsed="true"/>
-    <col min="131" max="131" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="132" max="132" bestFit="true" customWidth="true" style="2" width="16.42578125" collapsed="true"/>
-    <col min="133" max="133" bestFit="true" customWidth="true" style="2" width="15.5703125" collapsed="true"/>
-    <col min="134" max="134" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="135" max="135" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="136" max="137" style="2" width="9.140625" collapsed="true"/>
-    <col min="138" max="138" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="139" max="140" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
-    <col min="141" max="141" bestFit="true" customWidth="true" style="2" width="38.5703125" collapsed="true"/>
-    <col min="142" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="121" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="69.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="73.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="73.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="20" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="24" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="21.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="27.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="18.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="4.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="8.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="24.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="24.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="15" style="2" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="9.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="17.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="9.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="22.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="24.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="16.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="10.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="10.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="20.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="20.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="26.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="56" width="26.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="24.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="25" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="15.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="15.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="15.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="17.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="26.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="30.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="23.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="80" width="23.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="81" max="81" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="82" max="82" width="26.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="83" max="83" width="18.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="84" max="84" width="18.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="85" max="91" width="26.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="92" max="92" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="93" max="93" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="94" max="94" width="22.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="95" max="95" width="18.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="96" max="96" width="9.140625" style="2" collapsed="1"/>
+    <col min="97" max="97" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="98" max="98" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="99" max="99" width="17.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="100" max="100" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="101" max="101" width="15.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="102" max="102" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="103" max="103" width="19.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="104" max="104" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="105" max="105" width="14.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="106" max="106" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="107" max="107" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="108" max="108" width="10.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="109" max="109" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="110" max="110" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="111" max="111" width="9.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="112" max="112" width="14.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="113" max="113" width="32" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="114" max="114" width="16.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="115" max="121" width="9.140625" style="2" collapsed="1"/>
+    <col min="122" max="122" width="10" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="123" max="130" width="9.140625" style="2" collapsed="1"/>
+    <col min="131" max="131" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="132" max="132" width="16.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="133" max="133" width="15.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="134" max="134" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="135" max="135" width="11.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="136" max="137" width="9.140625" style="2" collapsed="1"/>
+    <col min="138" max="138" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="139" max="140" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="141" max="141" width="38.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="142" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:159" s="59" customFormat="1" x14ac:dyDescent="0.25">
@@ -65568,7 +65634,254 @@
         <v>87</v>
       </c>
       <c r="FC141" s="163" t="s">
-        <v>1522</v>
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="142" spans="1:164" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>140</v>
+      </c>
+      <c r="B142" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C142" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="D142" s="13" t="s">
+        <v>1439</v>
+      </c>
+      <c r="F142" s="79" t="s">
+        <v>1527</v>
+      </c>
+      <c r="G142" s="79" t="s">
+        <v>1528</v>
+      </c>
+      <c r="J142" s="15" t="s">
+        <v>1525</v>
+      </c>
+      <c r="K142" s="15"/>
+      <c r="L142" s="15"/>
+      <c r="M142" s="15"/>
+      <c r="N142" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="O142" s="33"/>
+      <c r="P142" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q142" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="R142" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="S142" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="T142" s="15"/>
+      <c r="U142" s="15"/>
+      <c r="V142" s="15"/>
+      <c r="W142" s="15"/>
+      <c r="X142" s="15"/>
+      <c r="Y142" s="15"/>
+      <c r="Z142" s="15"/>
+      <c r="AA142" s="15"/>
+      <c r="AB142" s="15"/>
+      <c r="AC142" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD142" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE142" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF142" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG142" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH142" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI142" s="36" t="s">
+        <v>933</v>
+      </c>
+      <c r="AJ142" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK142" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="AL142" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="AM142" s="34"/>
+      <c r="AN142" s="15"/>
+      <c r="AO142" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="AP142" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="AQ142" s="15"/>
+      <c r="AR142" s="15"/>
+      <c r="AS142" s="15"/>
+      <c r="AT142" s="15"/>
+      <c r="AU142" s="15"/>
+      <c r="AV142" s="15"/>
+      <c r="AW142" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AX142" s="15"/>
+      <c r="AY142" s="15"/>
+      <c r="AZ142" s="15"/>
+      <c r="BA142" s="34"/>
+      <c r="BB142" s="34"/>
+      <c r="BC142" s="34"/>
+      <c r="BD142" s="34"/>
+      <c r="BE142" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="BF142" s="15"/>
+      <c r="BG142" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="BH142" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="BI142" s="15"/>
+      <c r="BJ142" s="15"/>
+      <c r="BK142" s="15" t="s">
+        <v>539</v>
+      </c>
+      <c r="BL142" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="BM142" s="15"/>
+      <c r="BN142" s="34" t="s">
+        <v>383</v>
+      </c>
+      <c r="BO142" s="34" t="s">
+        <v>384</v>
+      </c>
+      <c r="BP142" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="BQ142" s="34"/>
+      <c r="BR142" s="34"/>
+      <c r="BS142" s="34"/>
+      <c r="BT142" s="34"/>
+      <c r="BU142" s="34"/>
+      <c r="BV142" s="34"/>
+      <c r="BW142" s="34"/>
+      <c r="BX142" s="34"/>
+      <c r="BY142" s="34"/>
+      <c r="BZ142" s="34"/>
+      <c r="CA142" s="34"/>
+      <c r="CB142" s="34"/>
+      <c r="CC142" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="CD142" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="CE142" s="15" t="s">
+        <v>397</v>
+      </c>
+      <c r="CF142" s="15"/>
+      <c r="CG142" s="34"/>
+      <c r="CH142" s="34"/>
+      <c r="CI142" s="34"/>
+      <c r="CJ142" s="34"/>
+      <c r="CK142" s="34"/>
+      <c r="CL142" s="34"/>
+      <c r="CM142" s="34"/>
+      <c r="CN142" s="15"/>
+      <c r="CO142" s="15"/>
+      <c r="CP142" s="15"/>
+      <c r="CQ142" s="15"/>
+      <c r="CR142" s="15"/>
+      <c r="CS142" s="15"/>
+      <c r="CT142" s="15"/>
+      <c r="CU142" s="15"/>
+      <c r="CV142" s="15"/>
+      <c r="CW142" s="15"/>
+      <c r="CX142" s="15"/>
+      <c r="CY142" s="15"/>
+      <c r="CZ142" s="15"/>
+      <c r="DA142" s="15"/>
+      <c r="DB142" s="15"/>
+      <c r="DC142" s="15"/>
+      <c r="DD142" s="15"/>
+      <c r="DE142" s="15"/>
+      <c r="DF142" s="15"/>
+      <c r="DG142" s="15"/>
+      <c r="DH142" s="15"/>
+      <c r="DI142" s="15"/>
+      <c r="DJ142" s="15"/>
+      <c r="DK142" s="15"/>
+      <c r="DL142" s="15"/>
+      <c r="DM142" s="15"/>
+      <c r="DN142" s="15"/>
+      <c r="DO142" s="15"/>
+      <c r="DP142" s="15"/>
+      <c r="DQ142" s="15"/>
+      <c r="DR142" s="15"/>
+      <c r="DS142" s="15"/>
+      <c r="DT142" s="15"/>
+      <c r="DU142" s="15"/>
+      <c r="DV142" s="15"/>
+      <c r="DW142" s="15"/>
+      <c r="DX142" s="15"/>
+      <c r="DY142" s="15"/>
+      <c r="DZ142" s="15"/>
+      <c r="EA142" s="15"/>
+      <c r="EB142" s="15"/>
+      <c r="EC142" s="15"/>
+      <c r="ED142" s="15"/>
+      <c r="EE142" s="15"/>
+      <c r="EF142" s="15"/>
+      <c r="EG142" s="87"/>
+      <c r="EH142" s="15"/>
+      <c r="EI142" s="15"/>
+      <c r="EJ142" s="15"/>
+      <c r="EK142" s="15"/>
+      <c r="EL142" s="4"/>
+      <c r="EM142" s="4"/>
+      <c r="EN142" s="4"/>
+      <c r="EO142" s="4"/>
+      <c r="EP142" s="4"/>
+      <c r="EQ142" s="4"/>
+      <c r="ER142" s="4"/>
+      <c r="ES142" s="4"/>
+      <c r="ET142" s="4"/>
+      <c r="EU142" s="4"/>
+      <c r="EV142" s="4"/>
+      <c r="EW142" s="4"/>
+      <c r="EX142" s="4"/>
+      <c r="EY142" s="4"/>
+      <c r="EZ142" s="4"/>
+      <c r="FA142" s="4"/>
+      <c r="FB142" s="4"/>
+      <c r="FC142" s="4"/>
+    </row>
+    <row r="143" spans="1:164" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>141</v>
+      </c>
+      <c r="B143" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C143" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="D143" s="13" t="s">
+        <v>1439</v>
+      </c>
+      <c r="F143" s="79" t="s">
+        <v>1527</v>
       </c>
     </row>
   </sheetData>
@@ -66932,8 +67245,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -67085,9 +67398,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" style="127" width="53.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="2" max="2" width="53.42578125" style="127" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="59" customFormat="1" x14ac:dyDescent="0.25">
@@ -67498,15 +67811,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -67740,6 +68044,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
   <ds:schemaRefs>
@@ -67751,14 +68064,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC0974DE-324A-423C-B9D7-F4F768EFCB0A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -67776,4 +68081,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Test Data sheet update for PAM server run
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fahmed2\git\Dynamics_CRM_Cloud_After_Wave1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5852DC84-AB59-47C3-88B2-1486D606BC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA2C9B0-2BA5-44FD-BE78-10C010DCD492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -41,7 +41,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10656" uniqueCount="1540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10646" uniqueCount="1535">
   <si>
     <t>Auditorium/Museum</t>
   </si>
@@ -4686,27 +4686,9 @@
     <t>2023_02_06_12_47_10</t>
   </si>
   <si>
-    <t>2023_02_06_01_27_19</t>
-  </si>
-  <si>
-    <t>2023_02_06_01_31_15</t>
-  </si>
-  <si>
-    <t>2023_02_06_01_34_46</t>
-  </si>
-  <si>
     <t>2023_02_06_01_38_27</t>
   </si>
   <si>
-    <t>2023_02_06_01_42_22</t>
-  </si>
-  <si>
-    <t>2023_02_06_01_45_47</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
     <t>2000516692</t>
   </si>
   <si>
@@ -4735,6 +4717,9 @@
   </si>
   <si>
     <t>2023_02_07_10_24_05</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -4744,7 +4729,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4893,12 +4878,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -5720,24 +5699,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B149" sqref="B149"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B322" sqref="B322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="132.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="9" max="10" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="46.0" collapsed="true"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="132.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="46" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -5784,7 +5764,7 @@
         <v>34</v>
       </c>
       <c r="C2" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>1</v>
@@ -5804,7 +5784,7 @@
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
       <c r="K2" s="106" t="s">
-        <v>1533</v>
+        <v>1527</v>
       </c>
       <c r="L2" s="99" t="s">
         <v>529</v>
@@ -5818,7 +5798,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>1</v>
@@ -5850,7 +5830,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>1</v>
@@ -5871,7 +5851,7 @@
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
       <c r="L4" s="106" t="s">
-        <v>1533</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -5882,7 +5862,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>1</v>
@@ -5912,7 +5892,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>1</v>
@@ -5940,7 +5920,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>1</v>
@@ -5968,7 +5948,7 @@
         <v>446</v>
       </c>
       <c r="C8" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>1</v>
@@ -5998,7 +5978,7 @@
         <v>44</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>1</v>
@@ -6026,7 +6006,7 @@
         <v>445</v>
       </c>
       <c r="C10" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>1</v>
@@ -6056,7 +6036,7 @@
         <v>54</v>
       </c>
       <c r="C11" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>1</v>
@@ -6086,7 +6066,7 @@
         <v>444</v>
       </c>
       <c r="C12" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>1</v>
@@ -6115,7 +6095,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>1</v>
@@ -6141,7 +6121,7 @@
         <v>247</v>
       </c>
       <c r="C14" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>1</v>
@@ -6167,7 +6147,7 @@
         <v>51</v>
       </c>
       <c r="C15" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>1</v>
@@ -6195,7 +6175,7 @@
         <v>443</v>
       </c>
       <c r="C16" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>1</v>
@@ -6215,7 +6195,7 @@
       <c r="K16" s="17"/>
       <c r="L16" s="104"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>16</v>
       </c>
@@ -6241,7 +6221,7 @@
       <c r="K17" s="17"/>
       <c r="L17" s="104"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>17</v>
       </c>
@@ -6267,7 +6247,7 @@
       <c r="K18" s="17"/>
       <c r="L18" s="104"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>18</v>
       </c>
@@ -6293,7 +6273,7 @@
       <c r="K19" s="17"/>
       <c r="L19" s="104"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>19</v>
       </c>
@@ -6319,7 +6299,7 @@
       <c r="K20" s="23"/>
       <c r="L20" s="104"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>20</v>
       </c>
@@ -6347,7 +6327,7 @@
       <c r="K21" s="17"/>
       <c r="L21" s="104"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>21</v>
       </c>
@@ -6373,7 +6353,7 @@
       <c r="K22" s="17"/>
       <c r="L22" s="104"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>22</v>
       </c>
@@ -6399,7 +6379,7 @@
       <c r="K23" s="17"/>
       <c r="L23" s="104"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>23</v>
       </c>
@@ -6425,7 +6405,7 @@
       <c r="K24" s="17"/>
       <c r="L24" s="104"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <v>24</v>
       </c>
@@ -6451,7 +6431,7 @@
       <c r="K25" s="17"/>
       <c r="L25" s="104"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>25</v>
       </c>
@@ -6477,7 +6457,7 @@
       <c r="K26" s="17"/>
       <c r="L26" s="104"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>26</v>
       </c>
@@ -6503,7 +6483,7 @@
       <c r="K27" s="17"/>
       <c r="L27" s="104"/>
     </row>
-    <row r="28" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>27</v>
       </c>
@@ -6529,7 +6509,7 @@
       <c r="K28" s="17"/>
       <c r="L28" s="107"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>28</v>
       </c>
@@ -6555,7 +6535,7 @@
       <c r="K29" s="22"/>
       <c r="L29" s="104"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>29</v>
       </c>
@@ -6581,7 +6561,7 @@
       <c r="K30" s="22"/>
       <c r="L30" s="104"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <v>30</v>
       </c>
@@ -6607,7 +6587,7 @@
       <c r="K31" s="22"/>
       <c r="L31" s="104"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>31</v>
       </c>
@@ -6633,7 +6613,7 @@
       <c r="K32" s="22"/>
       <c r="L32" s="104"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>32</v>
       </c>
@@ -6659,7 +6639,7 @@
       <c r="K33" s="22"/>
       <c r="L33" s="104"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>33</v>
       </c>
@@ -6685,7 +6665,7 @@
       <c r="K34" s="22"/>
       <c r="L34" s="104"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>34</v>
       </c>
@@ -6711,7 +6691,7 @@
       <c r="K35" s="22"/>
       <c r="L35" s="104"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>35</v>
       </c>
@@ -6737,7 +6717,7 @@
       <c r="K36" s="22"/>
       <c r="L36" s="104"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>36</v>
       </c>
@@ -6763,7 +6743,7 @@
       <c r="K37" s="22"/>
       <c r="L37" s="104"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>37</v>
       </c>
@@ -6789,7 +6769,7 @@
       <c r="K38" s="22"/>
       <c r="L38" s="104"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>38</v>
       </c>
@@ -6815,7 +6795,7 @@
       <c r="K39" s="22"/>
       <c r="L39" s="104"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>39</v>
       </c>
@@ -6841,7 +6821,7 @@
       <c r="K40" s="22"/>
       <c r="L40" s="104"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>40</v>
       </c>
@@ -6867,7 +6847,7 @@
       <c r="K41" s="22"/>
       <c r="L41" s="104"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>41</v>
       </c>
@@ -6893,7 +6873,7 @@
       <c r="K42" s="22"/>
       <c r="L42" s="104"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>42</v>
       </c>
@@ -6919,7 +6899,7 @@
       <c r="K43" s="22"/>
       <c r="L43" s="104"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>43</v>
       </c>
@@ -6945,7 +6925,7 @@
       <c r="K44" s="22"/>
       <c r="L44" s="104"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>44</v>
       </c>
@@ -6971,7 +6951,7 @@
       <c r="K45" s="22"/>
       <c r="L45" s="104"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
         <v>45</v>
       </c>
@@ -6997,7 +6977,7 @@
       <c r="K46" s="22"/>
       <c r="L46" s="104"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>46</v>
       </c>
@@ -7023,7 +7003,7 @@
       <c r="K47" s="22"/>
       <c r="L47" s="104"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>47</v>
       </c>
@@ -7049,7 +7029,7 @@
       <c r="K48" s="22"/>
       <c r="L48" s="104"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>48</v>
       </c>
@@ -7075,7 +7055,7 @@
       <c r="K49" s="22"/>
       <c r="L49" s="104"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>49</v>
       </c>
@@ -7101,7 +7081,7 @@
       <c r="K50" s="22"/>
       <c r="L50" s="104"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>50</v>
       </c>
@@ -7127,7 +7107,7 @@
       <c r="K51" s="22"/>
       <c r="L51" s="104"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
         <v>51</v>
       </c>
@@ -7153,7 +7133,7 @@
       <c r="K52" s="22"/>
       <c r="L52" s="104"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17">
         <v>52</v>
       </c>
@@ -7179,7 +7159,7 @@
       <c r="K53" s="22"/>
       <c r="L53" s="104"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <v>53</v>
       </c>
@@ -7205,7 +7185,7 @@
       <c r="K54" s="22"/>
       <c r="L54" s="104"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="17">
         <v>54</v>
       </c>
@@ -7231,7 +7211,7 @@
       <c r="K55" s="22"/>
       <c r="L55" s="104"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>55</v>
       </c>
@@ -7257,7 +7237,7 @@
       <c r="K56" s="22"/>
       <c r="L56" s="104"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>56</v>
       </c>
@@ -7283,7 +7263,7 @@
       <c r="K57" s="22"/>
       <c r="L57" s="104"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <v>57</v>
       </c>
@@ -7309,7 +7289,7 @@
       <c r="K58" s="22"/>
       <c r="L58" s="104"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="17">
         <v>58</v>
       </c>
@@ -7335,7 +7315,7 @@
       <c r="K59" s="22"/>
       <c r="L59" s="104"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="17">
         <v>59</v>
       </c>
@@ -7361,7 +7341,7 @@
       <c r="K60" s="22"/>
       <c r="L60" s="104"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <v>60</v>
       </c>
@@ -7387,7 +7367,7 @@
       <c r="K61" s="22"/>
       <c r="L61" s="104"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="17">
         <v>61</v>
       </c>
@@ -7413,7 +7393,7 @@
       <c r="K62" s="22"/>
       <c r="L62" s="104"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
         <v>62</v>
       </c>
@@ -7439,7 +7419,7 @@
       <c r="K63" s="22"/>
       <c r="L63" s="104"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
         <v>63</v>
       </c>
@@ -7465,7 +7445,7 @@
       <c r="K64" s="22"/>
       <c r="L64" s="104"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="17">
         <v>64</v>
       </c>
@@ -7491,7 +7471,7 @@
       <c r="K65" s="22"/>
       <c r="L65" s="104"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="17">
         <v>65</v>
       </c>
@@ -7517,7 +7497,7 @@
       <c r="K66" s="22"/>
       <c r="L66" s="104"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="17">
         <v>66</v>
       </c>
@@ -7543,7 +7523,7 @@
       <c r="K67" s="22"/>
       <c r="L67" s="104"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="17">
         <v>67</v>
       </c>
@@ -7569,7 +7549,7 @@
       <c r="K68" s="22"/>
       <c r="L68" s="104"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
         <v>68</v>
       </c>
@@ -7595,7 +7575,7 @@
       <c r="K69" s="22"/>
       <c r="L69" s="104"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
         <v>69</v>
       </c>
@@ -7623,7 +7603,7 @@
       <c r="K70" s="22"/>
       <c r="L70" s="104"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
         <v>70</v>
       </c>
@@ -7649,7 +7629,7 @@
       <c r="K71" s="22"/>
       <c r="L71" s="104"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
         <v>71</v>
       </c>
@@ -7675,7 +7655,7 @@
       <c r="K72" s="22"/>
       <c r="L72" s="104"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
         <v>72</v>
       </c>
@@ -7701,7 +7681,7 @@
       <c r="K73" s="22"/>
       <c r="L73" s="104"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="17">
         <v>73</v>
       </c>
@@ -7727,7 +7707,7 @@
       <c r="K74" s="22"/>
       <c r="L74" s="104"/>
     </row>
-    <row r="75" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="17">
         <v>74</v>
       </c>
@@ -7753,7 +7733,7 @@
       <c r="K75" s="17"/>
       <c r="L75" s="107"/>
     </row>
-    <row r="76" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="17">
         <v>75</v>
       </c>
@@ -7779,7 +7759,7 @@
       <c r="K76" s="17"/>
       <c r="L76" s="107"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="17">
         <v>76</v>
       </c>
@@ -7805,7 +7785,7 @@
       <c r="K77" s="45"/>
       <c r="L77" s="108"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="17">
         <v>77</v>
       </c>
@@ -7831,7 +7811,7 @@
       <c r="K78" s="45"/>
       <c r="L78" s="108"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="17">
         <v>78</v>
       </c>
@@ -7857,7 +7837,7 @@
       <c r="K79" s="45"/>
       <c r="L79" s="108"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="17">
         <v>79</v>
       </c>
@@ -7883,7 +7863,7 @@
       <c r="K80" s="45"/>
       <c r="L80" s="108"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="17">
         <v>80</v>
       </c>
@@ -7909,7 +7889,7 @@
       <c r="K81" s="45"/>
       <c r="L81" s="108"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="17">
         <v>81</v>
       </c>
@@ -7935,7 +7915,7 @@
       <c r="K82" s="45"/>
       <c r="L82" s="108"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="17">
         <v>82</v>
       </c>
@@ -7961,7 +7941,7 @@
       <c r="K83" s="45"/>
       <c r="L83" s="108"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="17">
         <v>83</v>
       </c>
@@ -7987,7 +7967,7 @@
       <c r="K84" s="45"/>
       <c r="L84" s="108"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="17">
         <v>84</v>
       </c>
@@ -8013,7 +7993,7 @@
       <c r="K85" s="45"/>
       <c r="L85" s="108"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="17">
         <v>85</v>
       </c>
@@ -8039,7 +8019,7 @@
       <c r="K86" s="45"/>
       <c r="L86" s="108"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="17">
         <v>86</v>
       </c>
@@ -8065,7 +8045,7 @@
       <c r="K87" s="45"/>
       <c r="L87" s="108"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="17">
         <v>87</v>
       </c>
@@ -8091,7 +8071,7 @@
       <c r="K88" s="45"/>
       <c r="L88" s="108"/>
     </row>
-    <row r="89" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="17">
         <v>88</v>
       </c>
@@ -8117,7 +8097,7 @@
       <c r="K89" s="17"/>
       <c r="L89" s="107"/>
     </row>
-    <row r="90" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="17">
         <v>89</v>
       </c>
@@ -8143,7 +8123,7 @@
       <c r="K90" s="17"/>
       <c r="L90" s="107"/>
     </row>
-    <row r="91" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="17">
         <v>90</v>
       </c>
@@ -8169,7 +8149,7 @@
       <c r="K91" s="17"/>
       <c r="L91" s="107"/>
     </row>
-    <row r="92" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="17">
         <v>91</v>
       </c>
@@ -8195,7 +8175,7 @@
       <c r="K92" s="17"/>
       <c r="L92" s="107"/>
     </row>
-    <row r="93" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="17">
         <v>92</v>
       </c>
@@ -8221,7 +8201,7 @@
       <c r="K93" s="17"/>
       <c r="L93" s="107"/>
     </row>
-    <row r="94" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="17">
         <v>93</v>
       </c>
@@ -8247,7 +8227,7 @@
       <c r="K94" s="17"/>
       <c r="L94" s="107"/>
     </row>
-    <row r="95" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="17">
         <v>94</v>
       </c>
@@ -8273,7 +8253,7 @@
       <c r="K95" s="17"/>
       <c r="L95" s="107"/>
     </row>
-    <row r="96" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="17">
         <v>95</v>
       </c>
@@ -8299,7 +8279,7 @@
       <c r="K96" s="17"/>
       <c r="L96" s="107"/>
     </row>
-    <row r="97" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="17">
         <v>96</v>
       </c>
@@ -8325,7 +8305,7 @@
       <c r="K97" s="17"/>
       <c r="L97" s="107"/>
     </row>
-    <row r="98" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="17">
         <v>97</v>
       </c>
@@ -8351,7 +8331,7 @@
       <c r="K98" s="17"/>
       <c r="L98" s="107"/>
     </row>
-    <row r="99" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="17">
         <v>98</v>
       </c>
@@ -8377,7 +8357,7 @@
       <c r="K99" s="17"/>
       <c r="L99" s="107"/>
     </row>
-    <row r="100" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="17">
         <v>99</v>
       </c>
@@ -8403,7 +8383,7 @@
       <c r="K100" s="17"/>
       <c r="L100" s="107"/>
     </row>
-    <row r="101" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="17">
         <v>100</v>
       </c>
@@ -8429,7 +8409,7 @@
       <c r="K101" s="17"/>
       <c r="L101" s="107"/>
     </row>
-    <row r="102" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="17">
         <v>101</v>
       </c>
@@ -8455,7 +8435,7 @@
       <c r="K102" s="17"/>
       <c r="L102" s="107"/>
     </row>
-    <row r="103" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="17">
         <v>102</v>
       </c>
@@ -8481,7 +8461,7 @@
       <c r="K103" s="17"/>
       <c r="L103" s="107"/>
     </row>
-    <row r="104" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="17">
         <v>103</v>
       </c>
@@ -8507,7 +8487,7 @@
       <c r="K104" s="17"/>
       <c r="L104" s="107"/>
     </row>
-    <row r="105" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="17">
         <v>104</v>
       </c>
@@ -8533,7 +8513,7 @@
       <c r="K105" s="17"/>
       <c r="L105" s="107"/>
     </row>
-    <row r="106" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="17">
         <v>105</v>
       </c>
@@ -8559,7 +8539,7 @@
       <c r="K106" s="17"/>
       <c r="L106" s="107"/>
     </row>
-    <row r="107" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="17">
         <v>106</v>
       </c>
@@ -8585,7 +8565,7 @@
       <c r="K107" s="17"/>
       <c r="L107" s="107"/>
     </row>
-    <row r="108" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="17">
         <v>107</v>
       </c>
@@ -8611,7 +8591,7 @@
       <c r="K108" s="17"/>
       <c r="L108" s="107"/>
     </row>
-    <row r="109" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="17">
         <v>108</v>
       </c>
@@ -8637,7 +8617,7 @@
       <c r="K109" s="17"/>
       <c r="L109" s="107"/>
     </row>
-    <row r="110" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="17">
         <v>109</v>
       </c>
@@ -8663,7 +8643,7 @@
       <c r="K110" s="17"/>
       <c r="L110" s="107"/>
     </row>
-    <row r="111" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="17">
         <v>110</v>
       </c>
@@ -8689,7 +8669,7 @@
       <c r="K111" s="17"/>
       <c r="L111" s="107"/>
     </row>
-    <row r="112" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="17">
         <v>111</v>
       </c>
@@ -8715,7 +8695,7 @@
       <c r="K112" s="17"/>
       <c r="L112" s="107"/>
     </row>
-    <row r="113" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="17">
         <v>112</v>
       </c>
@@ -8741,7 +8721,7 @@
       <c r="K113" s="17"/>
       <c r="L113" s="107"/>
     </row>
-    <row r="114" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="17">
         <v>113</v>
       </c>
@@ -8767,7 +8747,7 @@
       <c r="K114" s="17"/>
       <c r="L114" s="107"/>
     </row>
-    <row r="115" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="17">
         <v>114</v>
       </c>
@@ -8793,7 +8773,7 @@
       <c r="K115" s="17"/>
       <c r="L115" s="107"/>
     </row>
-    <row r="116" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="17">
         <v>115</v>
       </c>
@@ -8819,7 +8799,7 @@
       <c r="K116" s="17"/>
       <c r="L116" s="107"/>
     </row>
-    <row r="117" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="17">
         <v>116</v>
       </c>
@@ -8845,7 +8825,7 @@
       <c r="K117" s="17"/>
       <c r="L117" s="107"/>
     </row>
-    <row r="118" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="17">
         <v>117</v>
       </c>
@@ -8871,7 +8851,7 @@
       <c r="K118" s="17"/>
       <c r="L118" s="107"/>
     </row>
-    <row r="119" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="17">
         <v>118</v>
       </c>
@@ -8897,7 +8877,7 @@
       <c r="K119" s="17"/>
       <c r="L119" s="107"/>
     </row>
-    <row r="120" spans="1:12" s="98" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" s="98" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="17">
         <v>119</v>
       </c>
@@ -8925,7 +8905,7 @@
       <c r="K120" s="97"/>
       <c r="L120" s="109"/>
     </row>
-    <row r="121" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="17">
         <v>120</v>
       </c>
@@ -8951,7 +8931,7 @@
       <c r="K121" s="17"/>
       <c r="L121" s="107"/>
     </row>
-    <row r="122" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="17">
         <v>121</v>
       </c>
@@ -8977,7 +8957,7 @@
       <c r="K122" s="17"/>
       <c r="L122" s="107"/>
     </row>
-    <row r="123" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="17">
         <v>122</v>
       </c>
@@ -9003,7 +8983,7 @@
       <c r="K123" s="17"/>
       <c r="L123" s="107"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="17">
         <v>123</v>
       </c>
@@ -9029,7 +9009,7 @@
       <c r="K124" s="13"/>
       <c r="L124" s="104"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="17">
         <v>124</v>
       </c>
@@ -9050,7 +9030,7 @@
       </c>
       <c r="L125" s="104"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="17">
         <v>125</v>
       </c>
@@ -9071,7 +9051,7 @@
       </c>
       <c r="L126" s="104"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="17">
         <v>126</v>
       </c>
@@ -9092,7 +9072,7 @@
       </c>
       <c r="L127" s="104"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="17">
         <v>127</v>
       </c>
@@ -9113,7 +9093,7 @@
       </c>
       <c r="L128" s="104"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="17">
         <v>128</v>
       </c>
@@ -9134,7 +9114,7 @@
       </c>
       <c r="L129" s="104"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="17">
         <v>129</v>
       </c>
@@ -9155,7 +9135,7 @@
       </c>
       <c r="L130" s="104"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="17">
         <v>130</v>
       </c>
@@ -9176,7 +9156,7 @@
       </c>
       <c r="L131" s="104"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="17">
         <v>131</v>
       </c>
@@ -9206,7 +9186,7 @@
       <c r="K132" s="20"/>
       <c r="L132" s="104"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="17">
         <v>132</v>
       </c>
@@ -9236,7 +9216,7 @@
       <c r="K133" s="20"/>
       <c r="L133" s="104"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="17">
         <v>133</v>
       </c>
@@ -9266,7 +9246,7 @@
       <c r="K134" s="20"/>
       <c r="L134" s="104"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="17">
         <v>134</v>
       </c>
@@ -9296,7 +9276,7 @@
       <c r="K135" s="20"/>
       <c r="L135" s="104"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="17">
         <v>135</v>
       </c>
@@ -9326,12 +9306,12 @@
       <c r="K136" s="20"/>
       <c r="L136" s="104"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="17">
         <v>136</v>
       </c>
-      <c r="B137" s="19" t="s">
-        <v>1529</v>
+      <c r="B137" s="37" t="s">
+        <v>94</v>
       </c>
       <c r="C137" s="134" t="s">
         <v>33</v>
@@ -9356,7 +9336,7 @@
       <c r="K137" s="20"/>
       <c r="L137" s="104"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="17">
         <v>137</v>
       </c>
@@ -9386,7 +9366,7 @@
       <c r="K138" s="20"/>
       <c r="L138" s="104"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="17">
         <v>138</v>
       </c>
@@ -9416,7 +9396,7 @@
       <c r="K139" s="20"/>
       <c r="L139" s="104"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="17">
         <v>139</v>
       </c>
@@ -9446,7 +9426,7 @@
       <c r="K140" s="20"/>
       <c r="L140" s="104"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="17">
         <v>140</v>
       </c>
@@ -9476,7 +9456,7 @@
       <c r="K141" s="20"/>
       <c r="L141" s="104"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="17">
         <v>141</v>
       </c>
@@ -9506,7 +9486,7 @@
       <c r="K142" s="20"/>
       <c r="L142" s="104"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="17">
         <v>142</v>
       </c>
@@ -9536,7 +9516,7 @@
       <c r="K143" s="20"/>
       <c r="L143" s="104"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="17">
         <v>143</v>
       </c>
@@ -9566,7 +9546,7 @@
       <c r="K144" s="20"/>
       <c r="L144" s="104"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="17">
         <v>144</v>
       </c>
@@ -9586,7 +9566,7 @@
         <v>1451</v>
       </c>
       <c r="G145" s="19" t="s">
-        <v>1534</v>
+        <v>1528</v>
       </c>
       <c r="H145" s="19"/>
       <c r="I145" s="19"/>
@@ -9594,7 +9574,7 @@
       <c r="K145" s="20"/>
       <c r="L145" s="104"/>
     </row>
-    <row r="146" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="17">
         <v>145</v>
       </c>
@@ -9624,7 +9604,7 @@
       <c r="K146" s="20"/>
       <c r="L146" s="107"/>
     </row>
-    <row r="147" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="17">
         <v>146</v>
       </c>
@@ -9644,10 +9624,10 @@
         <v>1451</v>
       </c>
       <c r="G147" s="19" t="s">
-        <v>1531</v>
+        <v>1525</v>
       </c>
       <c r="H147" s="19" t="s">
-        <v>1530</v>
+        <v>1524</v>
       </c>
       <c r="I147" s="19"/>
       <c r="J147" s="19"/>
@@ -9662,7 +9642,7 @@
         <v>449</v>
       </c>
       <c r="C148" s="141" t="s">
-        <v>32</v>
+        <v>1534</v>
       </c>
       <c r="D148" s="19" t="s">
         <v>25</v>
@@ -9674,7 +9654,7 @@
         <v>1453</v>
       </c>
       <c r="G148" s="22" t="s">
-        <v>1535</v>
+        <v>1529</v>
       </c>
       <c r="H148" s="22"/>
       <c r="I148" s="22"/>
@@ -9690,7 +9670,7 @@
         <v>456</v>
       </c>
       <c r="C149" s="141" t="s">
-        <v>32</v>
+        <v>1534</v>
       </c>
       <c r="D149" s="19" t="s">
         <v>25</v>
@@ -9702,7 +9682,7 @@
         <v>1453</v>
       </c>
       <c r="G149" s="22" t="s">
-        <v>1536</v>
+        <v>1530</v>
       </c>
       <c r="H149" s="22"/>
       <c r="I149" s="22"/>
@@ -9718,7 +9698,7 @@
         <v>461</v>
       </c>
       <c r="C150" s="141" t="s">
-        <v>32</v>
+        <v>1534</v>
       </c>
       <c r="D150" s="19" t="s">
         <v>25</v>
@@ -9730,7 +9710,7 @@
         <v>1453</v>
       </c>
       <c r="G150" s="22" t="s">
-        <v>1537</v>
+        <v>1531</v>
       </c>
       <c r="H150" s="22"/>
       <c r="I150" s="22"/>
@@ -9738,7 +9718,7 @@
       <c r="K150" s="22"/>
       <c r="L150" s="104"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="17">
         <v>150</v>
       </c>
@@ -9766,7 +9746,7 @@
       <c r="K151" s="22"/>
       <c r="L151" s="104"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="17">
         <v>151</v>
       </c>
@@ -9786,7 +9766,7 @@
         <v>1451</v>
       </c>
       <c r="G152" s="22" t="s">
-        <v>1526</v>
+        <v>1523</v>
       </c>
       <c r="H152" s="22"/>
       <c r="I152" s="22"/>
@@ -9794,7 +9774,7 @@
       <c r="K152" s="22"/>
       <c r="L152" s="104"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="17">
         <v>152</v>
       </c>
@@ -9830,7 +9810,7 @@
         <v>467</v>
       </c>
       <c r="C154" s="141" t="s">
-        <v>32</v>
+        <v>1534</v>
       </c>
       <c r="D154" s="19" t="s">
         <v>25</v>
@@ -9842,7 +9822,7 @@
         <v>1453</v>
       </c>
       <c r="G154" s="22" t="s">
-        <v>1538</v>
+        <v>1532</v>
       </c>
       <c r="H154" s="22"/>
       <c r="I154" s="22"/>
@@ -9850,7 +9830,7 @@
       <c r="K154" s="22"/>
       <c r="L154" s="104"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="17">
         <v>154</v>
       </c>
@@ -9884,7 +9864,7 @@
         <v>598</v>
       </c>
       <c r="C156" s="141" t="s">
-        <v>32</v>
+        <v>1534</v>
       </c>
       <c r="D156" s="19" t="s">
         <v>25</v>
@@ -9896,7 +9876,7 @@
         <v>1453</v>
       </c>
       <c r="G156" s="22" t="s">
-        <v>1539</v>
+        <v>1533</v>
       </c>
       <c r="H156" s="22"/>
       <c r="I156" s="22"/>
@@ -9904,7 +9884,7 @@
       <c r="K156" s="22"/>
       <c r="L156" s="104"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="17">
         <v>156</v>
       </c>
@@ -9932,7 +9912,7 @@
       <c r="K157" s="22"/>
       <c r="L157" s="104"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="17">
         <v>157</v>
       </c>
@@ -9962,7 +9942,7 @@
       <c r="K158" s="22"/>
       <c r="L158" s="104"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="17">
         <v>158</v>
       </c>
@@ -9990,7 +9970,7 @@
       <c r="K159" s="20"/>
       <c r="L159" s="104"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="17">
         <v>159</v>
       </c>
@@ -10018,7 +9998,7 @@
       <c r="K160" s="20"/>
       <c r="L160" s="104"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="17">
         <v>160</v>
       </c>
@@ -10046,7 +10026,7 @@
       <c r="K161" s="20"/>
       <c r="L161" s="104"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="17">
         <v>161</v>
       </c>
@@ -10074,7 +10054,7 @@
       <c r="K162" s="20"/>
       <c r="L162" s="104"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="17">
         <v>162</v>
       </c>
@@ -10102,7 +10082,7 @@
       <c r="K163" s="20"/>
       <c r="L163" s="104"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="17">
         <v>163</v>
       </c>
@@ -10130,7 +10110,7 @@
       <c r="K164" s="20"/>
       <c r="L164" s="104"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="17">
         <v>164</v>
       </c>
@@ -10158,7 +10138,7 @@
       <c r="K165" s="20"/>
       <c r="L165" s="104"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="17">
         <v>165</v>
       </c>
@@ -10186,7 +10166,7 @@
       <c r="K166" s="20"/>
       <c r="L166" s="104"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="17">
         <v>166</v>
       </c>
@@ -10212,7 +10192,7 @@
       <c r="K167" s="20"/>
       <c r="L167" s="104"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="17">
         <v>167</v>
       </c>
@@ -10240,7 +10220,7 @@
       <c r="K168" s="20"/>
       <c r="L168" s="104"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="17">
         <v>167</v>
       </c>
@@ -10270,7 +10250,7 @@
       <c r="K169" s="24"/>
       <c r="L169" s="104"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="17">
         <v>168</v>
       </c>
@@ -10296,7 +10276,7 @@
       <c r="K170" s="24"/>
       <c r="L170" s="104"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="17">
         <v>169</v>
       </c>
@@ -10322,7 +10302,7 @@
       <c r="K171" s="24"/>
       <c r="L171" s="104"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="17">
         <v>170</v>
       </c>
@@ -10348,7 +10328,7 @@
       <c r="K172" s="25"/>
       <c r="L172" s="104"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="17">
         <v>171</v>
       </c>
@@ -10374,7 +10354,7 @@
       <c r="K173" s="25"/>
       <c r="L173" s="104"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="17">
         <v>172</v>
       </c>
@@ -10400,7 +10380,7 @@
       <c r="K174" s="25"/>
       <c r="L174" s="104"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="17">
         <v>173</v>
       </c>
@@ -10426,7 +10406,7 @@
       <c r="K175" s="25"/>
       <c r="L175" s="104"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="17">
         <v>174</v>
       </c>
@@ -10452,7 +10432,7 @@
       <c r="K176" s="25"/>
       <c r="L176" s="104"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="17">
         <v>175</v>
       </c>
@@ -10478,7 +10458,7 @@
       <c r="K177" s="25"/>
       <c r="L177" s="104"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="17">
         <v>176</v>
       </c>
@@ -10506,7 +10486,7 @@
       <c r="K178" s="138"/>
       <c r="L178" s="104"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="17">
         <v>176</v>
       </c>
@@ -10527,7 +10507,7 @@
       </c>
       <c r="L179" s="104"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="17">
         <v>177</v>
       </c>
@@ -10554,7 +10534,7 @@
       </c>
       <c r="L180" s="104"/>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="17">
         <v>178</v>
       </c>
@@ -10581,7 +10561,7 @@
       </c>
       <c r="L181" s="104"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="17">
         <v>179</v>
       </c>
@@ -10608,7 +10588,7 @@
       </c>
       <c r="L182" s="104"/>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="17">
         <v>180</v>
       </c>
@@ -10635,7 +10615,7 @@
       </c>
       <c r="L183" s="104"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="17">
         <v>181</v>
       </c>
@@ -10662,7 +10642,7 @@
       </c>
       <c r="L184" s="104"/>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="17">
         <v>182</v>
       </c>
@@ -10689,7 +10669,7 @@
       </c>
       <c r="L185" s="104"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="17">
         <v>183</v>
       </c>
@@ -10716,7 +10696,7 @@
       </c>
       <c r="L186" s="104"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="17">
         <v>184</v>
       </c>
@@ -10743,7 +10723,7 @@
       </c>
       <c r="L187" s="104"/>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="17">
         <v>185</v>
       </c>
@@ -10770,7 +10750,7 @@
       </c>
       <c r="L188" s="104"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="17">
         <v>186</v>
       </c>
@@ -10797,7 +10777,7 @@
       </c>
       <c r="L189" s="104"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="17">
         <v>187</v>
       </c>
@@ -10818,7 +10798,7 @@
       </c>
       <c r="L190" s="104"/>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="17">
         <v>188</v>
       </c>
@@ -10839,7 +10819,7 @@
       </c>
       <c r="L191" s="104"/>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="17">
         <v>189</v>
       </c>
@@ -10860,7 +10840,7 @@
       </c>
       <c r="L192" s="104"/>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="17">
         <v>190</v>
       </c>
@@ -10881,7 +10861,7 @@
       </c>
       <c r="L193" s="104"/>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="17">
         <v>191</v>
       </c>
@@ -10902,7 +10882,7 @@
       </c>
       <c r="L194" s="104"/>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="17">
         <v>192</v>
       </c>
@@ -10923,7 +10903,7 @@
       </c>
       <c r="L195" s="104"/>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="17">
         <v>193</v>
       </c>
@@ -10944,7 +10924,7 @@
       </c>
       <c r="L196" s="104"/>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="17">
         <v>194</v>
       </c>
@@ -10965,7 +10945,7 @@
       </c>
       <c r="L197" s="104"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="17">
         <v>195</v>
       </c>
@@ -10986,7 +10966,7 @@
       </c>
       <c r="L198" s="104"/>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="17">
         <v>196</v>
       </c>
@@ -11007,7 +10987,7 @@
       </c>
       <c r="L199" s="104"/>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="17">
         <v>197</v>
       </c>
@@ -11028,7 +11008,7 @@
       </c>
       <c r="L200" s="104"/>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="17">
         <v>198</v>
       </c>
@@ -11049,7 +11029,7 @@
       </c>
       <c r="L201" s="104"/>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="17">
         <v>199</v>
       </c>
@@ -11076,7 +11056,7 @@
       </c>
       <c r="L202" s="104"/>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="17">
         <v>200</v>
       </c>
@@ -11103,7 +11083,7 @@
       </c>
       <c r="L203" s="104"/>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="17">
         <v>201</v>
       </c>
@@ -11130,7 +11110,7 @@
       </c>
       <c r="L204" s="104"/>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="17">
         <v>202</v>
       </c>
@@ -11157,7 +11137,7 @@
       </c>
       <c r="L205" s="104"/>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="17">
         <v>203</v>
       </c>
@@ -11187,7 +11167,7 @@
       <c r="K206" s="112"/>
       <c r="L206" s="113"/>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="17">
         <v>204</v>
       </c>
@@ -11213,7 +11193,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="17">
         <v>205</v>
       </c>
@@ -11236,7 +11216,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="17">
         <v>206</v>
       </c>
@@ -11262,7 +11242,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="17">
         <v>207</v>
       </c>
@@ -11288,7 +11268,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="17">
         <v>208</v>
       </c>
@@ -11314,7 +11294,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="17">
         <v>209</v>
       </c>
@@ -11340,7 +11320,7 @@
       <c r="K212" s="20"/>
       <c r="L212" s="104"/>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="17">
         <v>210</v>
       </c>
@@ -11360,7 +11340,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="17">
         <v>211</v>
       </c>
@@ -11380,7 +11360,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="17">
         <v>212</v>
       </c>
@@ -11400,7 +11380,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="17">
         <v>213</v>
       </c>
@@ -11420,7 +11400,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="17">
         <v>214</v>
       </c>
@@ -11440,7 +11420,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="17">
         <v>215</v>
       </c>
@@ -11466,7 +11446,7 @@
       <c r="K218" s="17"/>
       <c r="L218" s="104"/>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="17">
         <v>216</v>
       </c>
@@ -11489,7 +11469,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="17">
         <v>217</v>
       </c>
@@ -11512,7 +11492,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="17">
         <v>218</v>
       </c>
@@ -11535,7 +11515,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="17">
         <v>219</v>
       </c>
@@ -11558,7 +11538,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="223" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="17">
         <v>220</v>
       </c>
@@ -11581,7 +11561,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="17">
         <v>221</v>
       </c>
@@ -11604,7 +11584,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="225" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="17">
         <v>222</v>
       </c>
@@ -11624,7 +11604,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="226" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="17">
         <v>223</v>
       </c>
@@ -11644,7 +11624,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="227" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="17">
         <v>224</v>
       </c>
@@ -11664,7 +11644,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="17">
         <v>225</v>
       </c>
@@ -11684,7 +11664,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="17">
         <v>226</v>
       </c>
@@ -11707,7 +11687,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="17">
         <v>227</v>
       </c>
@@ -11730,7 +11710,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="17">
         <v>228</v>
       </c>
@@ -11753,7 +11733,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="17">
         <v>229</v>
       </c>
@@ -11773,7 +11753,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="17">
         <v>230</v>
       </c>
@@ -11793,7 +11773,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="17">
         <v>231</v>
       </c>
@@ -11813,7 +11793,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="17">
         <v>232</v>
       </c>
@@ -11833,7 +11813,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="17">
         <v>233</v>
       </c>
@@ -11853,7 +11833,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="17">
         <v>234</v>
       </c>
@@ -11873,7 +11853,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="17">
         <v>235</v>
       </c>
@@ -11893,7 +11873,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="17">
         <v>236</v>
       </c>
@@ -11913,7 +11893,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="17">
         <v>237</v>
       </c>
@@ -11939,7 +11919,7 @@
       <c r="K240" s="22"/>
       <c r="L240" s="104"/>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="17">
         <v>238</v>
       </c>
@@ -11965,7 +11945,7 @@
       <c r="K241" s="17"/>
       <c r="L241" s="104"/>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="17">
         <v>239</v>
       </c>
@@ -11986,7 +11966,7 @@
       </c>
       <c r="L242" s="104"/>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="17">
         <v>240</v>
       </c>
@@ -12012,7 +11992,7 @@
       <c r="K243" s="22"/>
       <c r="L243" s="104"/>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="17">
         <v>241</v>
       </c>
@@ -12038,7 +12018,7 @@
       <c r="K244" s="22"/>
       <c r="L244" s="104"/>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="17">
         <v>242</v>
       </c>
@@ -12058,7 +12038,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="17">
         <v>243</v>
       </c>
@@ -12078,7 +12058,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="17">
         <v>244</v>
       </c>
@@ -12098,7 +12078,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="17">
         <v>245</v>
       </c>
@@ -12118,7 +12098,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="17">
         <v>246</v>
       </c>
@@ -12146,7 +12126,7 @@
       <c r="K249" s="22"/>
       <c r="L249" s="104"/>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="17">
         <v>247</v>
       </c>
@@ -12174,7 +12154,7 @@
       <c r="K250" s="22"/>
       <c r="L250" s="104"/>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="17">
         <v>248</v>
       </c>
@@ -12197,7 +12177,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="17">
         <v>249</v>
       </c>
@@ -12220,7 +12200,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="17">
         <v>250</v>
       </c>
@@ -12243,7 +12223,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="17">
         <v>251</v>
       </c>
@@ -12266,7 +12246,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="17">
         <v>252</v>
       </c>
@@ -12286,7 +12266,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="17">
         <v>253</v>
       </c>
@@ -12309,7 +12289,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="17">
         <v>254</v>
       </c>
@@ -12332,7 +12312,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="17">
         <v>255</v>
       </c>
@@ -12355,7 +12335,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="17">
         <v>256</v>
       </c>
@@ -12378,7 +12358,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="17">
         <v>257</v>
       </c>
@@ -12404,7 +12384,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="17">
         <v>258</v>
       </c>
@@ -12430,7 +12410,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="17">
         <v>259</v>
       </c>
@@ -12456,7 +12436,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="134">
         <v>260</v>
       </c>
@@ -12482,7 +12462,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="134">
         <v>261</v>
       </c>
@@ -12508,7 +12488,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="134">
         <v>262</v>
       </c>
@@ -12534,7 +12514,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="134">
         <v>263</v>
       </c>
@@ -12560,7 +12540,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="134">
         <v>264</v>
       </c>
@@ -12583,7 +12563,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="134">
         <v>265</v>
       </c>
@@ -12606,7 +12586,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="134">
         <v>265</v>
       </c>
@@ -12629,7 +12609,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="134">
         <v>266</v>
       </c>
@@ -12652,7 +12632,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="134">
         <v>267</v>
       </c>
@@ -12675,7 +12655,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="134">
         <v>268</v>
       </c>
@@ -12698,7 +12678,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="134">
         <v>269</v>
       </c>
@@ -12721,7 +12701,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="134">
         <v>270</v>
       </c>
@@ -12744,7 +12724,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="134">
         <v>271</v>
       </c>
@@ -12767,7 +12747,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="134">
         <v>272</v>
       </c>
@@ -12790,7 +12770,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="134">
         <v>273</v>
       </c>
@@ -12813,7 +12793,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="134">
         <v>274</v>
       </c>
@@ -12836,7 +12816,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="134">
         <v>275</v>
       </c>
@@ -12859,7 +12839,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="134">
         <v>275</v>
       </c>
@@ -12882,7 +12862,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="134">
         <v>276</v>
       </c>
@@ -12905,7 +12885,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="134">
         <v>277</v>
       </c>
@@ -12928,7 +12908,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="134">
         <v>278</v>
       </c>
@@ -12951,7 +12931,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="134">
         <v>279</v>
       </c>
@@ -12974,7 +12954,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="134">
         <v>280</v>
       </c>
@@ -12997,7 +12977,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="134">
         <v>281</v>
       </c>
@@ -13020,7 +13000,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="134">
         <v>282</v>
       </c>
@@ -13043,7 +13023,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="134">
         <v>283</v>
       </c>
@@ -13066,7 +13046,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="134">
         <v>284</v>
       </c>
@@ -13089,7 +13069,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="134">
         <v>285</v>
       </c>
@@ -13112,7 +13092,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="134">
         <v>285</v>
       </c>
@@ -13135,7 +13115,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="134">
         <v>285</v>
       </c>
@@ -13158,7 +13138,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="134">
         <v>286</v>
       </c>
@@ -13184,7 +13164,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="134">
         <v>287</v>
       </c>
@@ -13210,7 +13190,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="134">
         <v>288</v>
       </c>
@@ -13233,7 +13213,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="134">
         <v>289</v>
       </c>
@@ -13253,7 +13233,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="134">
         <v>289</v>
       </c>
@@ -13276,7 +13256,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="134">
         <v>290</v>
       </c>
@@ -13299,7 +13279,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="134">
         <v>291</v>
       </c>
@@ -13322,7 +13302,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="134">
         <v>292</v>
       </c>
@@ -13345,7 +13325,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="134">
         <v>293</v>
       </c>
@@ -13365,7 +13345,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="134">
         <v>294</v>
       </c>
@@ -13388,7 +13368,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="134">
         <v>295</v>
       </c>
@@ -13411,7 +13391,7 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="134">
         <v>296</v>
       </c>
@@ -13437,7 +13417,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="134">
         <v>297</v>
       </c>
@@ -13460,7 +13440,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="134">
         <v>298</v>
       </c>
@@ -13483,7 +13463,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="134">
         <v>299</v>
       </c>
@@ -13506,7 +13486,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="134">
         <v>300</v>
       </c>
@@ -13532,7 +13512,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="134">
         <v>301</v>
       </c>
@@ -13558,7 +13538,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="134">
         <v>302</v>
       </c>
@@ -13584,7 +13564,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="134">
         <v>303</v>
       </c>
@@ -13610,7 +13590,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="134">
         <v>304</v>
       </c>
@@ -13636,7 +13616,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="134">
         <v>305</v>
       </c>
@@ -13662,7 +13642,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="134">
         <v>306</v>
       </c>
@@ -13688,7 +13668,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="134">
         <v>307</v>
       </c>
@@ -13714,7 +13694,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="134">
         <v>308</v>
       </c>
@@ -13740,7 +13720,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="134">
         <v>309</v>
       </c>
@@ -13766,7 +13746,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="134">
         <v>310</v>
       </c>
@@ -13790,6 +13770,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P318" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1" xr:uid="{C4DE44B4-9E86-4104-81E3-C93D60F64BE3}"/>
     <hyperlink ref="L2" r:id="rId2" xr:uid="{A4124D5F-F457-4A70-A072-5DFAF5EA33F8}"/>
@@ -15996,7 +15983,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="136.7109375" collapsed="true"/>
+    <col min="2" max="2" width="136.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:168" x14ac:dyDescent="0.25">
@@ -18057,8 +18044,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:155" x14ac:dyDescent="0.25">
@@ -19546,8 +19533,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="136.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="2" max="2" width="136" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:141" x14ac:dyDescent="0.25">
@@ -20955,7 +20942,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" style="115" width="60.28515625" collapsed="true"/>
+    <col min="2" max="2" width="60.28515625" style="115" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:141" x14ac:dyDescent="0.25">
@@ -23619,7 +23606,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="84.140625" collapsed="true"/>
+    <col min="2" max="2" width="84.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:141" x14ac:dyDescent="0.25">
@@ -33082,75 +33069,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D073B921-24DF-4F78-BD1E-1984D65F897D}">
   <dimension ref="A1:BZ39"/>
   <sheetViews>
-    <sheetView topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="AX13" sqref="AX13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="114.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="82.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="25.85546875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="28" max="36" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="42" max="42" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="43" max="43" customWidth="true" width="54.42578125" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="46" max="47" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="49" max="50" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="52" max="52" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="56" max="57" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="68" max="68" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="69" max="69" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="70" max="70" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="71" max="71" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="74" max="74" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="75" max="76" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="114" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="82.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="28" max="36" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="34.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="54.42578125" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="47" width="29" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="50" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="57" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="76" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:78" x14ac:dyDescent="0.25">
@@ -33302,7 +33289,7 @@
         <v>201</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>1532</v>
+        <v>1526</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>251</v>
@@ -37399,27 +37386,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="108.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="4" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="65.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="73.85546875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="108" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="7" width="29.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="65.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="73.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -38489,8 +38476,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="2" max="2" width="9.140625" collapsed="1"/>
+    <col min="56" max="56" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:89" x14ac:dyDescent="0.25">
@@ -41454,108 +41441,108 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="5.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="121.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="29.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="13.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="13.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="11.28515625" collapsed="true"/>
-    <col min="7" max="9" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="69.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="2" width="36.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="73.5703125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="2" width="73.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="20.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="15.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
-    <col min="19" max="20" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="21" max="24" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="21.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="2" width="4.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="2" width="8.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="2" width="24.140625" collapsed="true"/>
-    <col min="38" max="38" customWidth="true" style="2" width="24.140625" collapsed="true"/>
-    <col min="39" max="39" customWidth="true" style="2" width="15.0" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="2" width="9.85546875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="2" width="9.5703125" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="2" width="22.28515625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="2" width="24.5703125" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
-    <col min="50" max="50" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" style="2" width="20.5703125" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" style="2" width="26.42578125" collapsed="true"/>
-    <col min="54" max="56" customWidth="true" style="2" width="26.42578125" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
-    <col min="58" max="58" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" style="2" width="25.0" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" style="2" width="15.140625" collapsed="true"/>
-    <col min="61" max="61" customWidth="true" style="2" width="15.140625" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" style="2" width="15.7109375" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
-    <col min="65" max="65" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" style="2" width="30.42578125" collapsed="true"/>
-    <col min="68" max="68" bestFit="true" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
-    <col min="69" max="80" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
-    <col min="81" max="81" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="82" max="82" bestFit="true" customWidth="true" style="2" width="26.140625" collapsed="true"/>
-    <col min="83" max="83" bestFit="true" customWidth="true" style="2" width="18.140625" collapsed="true"/>
-    <col min="84" max="84" customWidth="true" style="2" width="18.140625" collapsed="true"/>
-    <col min="85" max="91" customWidth="true" style="2" width="26.140625" collapsed="true"/>
-    <col min="92" max="92" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="93" max="93" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="94" max="94" bestFit="true" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
-    <col min="95" max="95" bestFit="true" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
-    <col min="96" max="96" style="2" width="9.140625" collapsed="true"/>
-    <col min="97" max="97" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
-    <col min="98" max="98" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="99" max="99" bestFit="true" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
-    <col min="100" max="100" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="101" max="101" bestFit="true" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
-    <col min="102" max="102" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
-    <col min="103" max="103" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
-    <col min="104" max="104" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
-    <col min="105" max="105" bestFit="true" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
-    <col min="106" max="106" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
-    <col min="107" max="107" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
-    <col min="108" max="108" bestFit="true" customWidth="true" style="2" width="10.7109375" collapsed="true"/>
-    <col min="109" max="109" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
-    <col min="110" max="110" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
-    <col min="111" max="111" bestFit="true" customWidth="true" style="2" width="9.28515625" collapsed="true"/>
-    <col min="112" max="112" bestFit="true" customWidth="true" style="2" width="14.140625" collapsed="true"/>
-    <col min="113" max="113" bestFit="true" customWidth="true" style="2" width="32.0" collapsed="true"/>
-    <col min="114" max="114" bestFit="true" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
-    <col min="115" max="121" style="2" width="9.140625" collapsed="true"/>
-    <col min="122" max="122" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="123" max="130" style="2" width="9.140625" collapsed="true"/>
-    <col min="131" max="131" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="132" max="132" bestFit="true" customWidth="true" style="2" width="16.42578125" collapsed="true"/>
-    <col min="133" max="133" bestFit="true" customWidth="true" style="2" width="15.5703125" collapsed="true"/>
-    <col min="134" max="134" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="135" max="135" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="136" max="137" style="2" width="9.140625" collapsed="true"/>
-    <col min="138" max="138" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="139" max="140" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
-    <col min="141" max="141" bestFit="true" customWidth="true" style="2" width="38.5703125" collapsed="true"/>
-    <col min="142" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="121" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="69.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="73.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="73.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="20" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="24" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="21.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="27.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="18.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="4.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="8.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="24.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="24.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="15" style="2" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="9.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="17.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="9.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="22.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="24.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="16.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="10.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="10.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="20.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="20.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="26.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="56" width="26.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="24.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="25" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="15.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="15.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="15.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="17.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="26.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="30.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="23.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="80" width="23.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="81" max="81" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="82" max="82" width="26.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="83" max="83" width="18.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="84" max="84" width="18.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="85" max="91" width="26.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="92" max="92" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="93" max="93" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="94" max="94" width="22.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="95" max="95" width="18.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="96" max="96" width="9.140625" style="2" collapsed="1"/>
+    <col min="97" max="97" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="98" max="98" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="99" max="99" width="17.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="100" max="100" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="101" max="101" width="15.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="102" max="102" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="103" max="103" width="19.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="104" max="104" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="105" max="105" width="14.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="106" max="106" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="107" max="107" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="108" max="108" width="10.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="109" max="109" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="110" max="110" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="111" max="111" width="9.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="112" max="112" width="14.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="113" max="113" width="32" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="114" max="114" width="16.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="115" max="121" width="9.140625" style="2" collapsed="1"/>
+    <col min="122" max="122" width="10" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="123" max="130" width="9.140625" style="2" collapsed="1"/>
+    <col min="131" max="131" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="132" max="132" width="16.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="133" max="133" width="15.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="134" max="134" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="135" max="135" width="11.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="136" max="137" width="9.140625" style="2" collapsed="1"/>
+    <col min="138" max="138" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="139" max="140" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="141" max="141" width="38.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="142" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:159" s="54" customFormat="1" x14ac:dyDescent="0.25">
@@ -67249,8 +67236,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -67402,9 +67389,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" style="115" width="53.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="2" max="2" width="53.42578125" style="115" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.25">
@@ -67806,6 +67793,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -68039,25 +68044,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC0974DE-324A-423C-B9D7-F4F768EFCB0A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -68075,22 +68080,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Test Data Update for Dev1 Run
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fahmed2\git\Dynamics_CRM_Cloud_After_Wave1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3679EE-25EA-41AB-8ED1-E43624B22117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23216A1A-1C50-4702-B646-113489228DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -589,7 +589,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10693" uniqueCount="1577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10700" uniqueCount="1583">
   <si>
     <t>Auditorium/Museum</t>
   </si>
@@ -4989,9 +4989,6 @@
     <t>2023_01_25_07_20_11</t>
   </si>
   <si>
-    <t>2023_01_25_07_33_06</t>
-  </si>
-  <si>
     <t>2000516675</t>
   </si>
   <si>
@@ -5007,18 +5004,9 @@
     <t>2023_02_06_01_38_27</t>
   </si>
   <si>
-    <t>2000516692</t>
-  </si>
-  <si>
-    <t>2023_02_06_03_39_48</t>
-  </si>
-  <si>
     <t>membershipStartDate</t>
   </si>
   <si>
-    <t>2023_02_07_09_58_00</t>
-  </si>
-  <si>
     <t>7/4/1976</t>
   </si>
   <si>
@@ -5043,9 +5031,6 @@
     <t>2023_02_08_05_49_14</t>
   </si>
   <si>
-    <t>2023_02_08_07_22_59</t>
-  </si>
-  <si>
     <t>2023_02_08_08_19_35</t>
   </si>
   <si>
@@ -5067,9 +5052,6 @@
     <t>2023_02_08_10_36_36</t>
   </si>
   <si>
-    <t>2023_02_08_11_12_11</t>
-  </si>
-  <si>
     <t>2023_02_09_02_52_32</t>
   </si>
   <si>
@@ -5079,12 +5061,6 @@
     <t>2023_02_09_04_37_54</t>
   </si>
   <si>
-    <t>2023_02_09_06_02_06</t>
-  </si>
-  <si>
-    <t>2023_02_09_06_22_13</t>
-  </si>
-  <si>
     <t>2023_02_09_06_36_25</t>
   </si>
   <si>
@@ -5112,12 +5088,6 @@
     <t>12/9/2023</t>
   </si>
   <si>
-    <t>7000580167</t>
-  </si>
-  <si>
-    <t>2023_02_10_05_43_31</t>
-  </si>
-  <si>
     <t>7000580168</t>
   </si>
   <si>
@@ -5154,9 +5124,6 @@
     <t>2023_02_10_10_06_28</t>
   </si>
   <si>
-    <t>2023_02_10_10_44_00</t>
-  </si>
-  <si>
     <t>2023_02_10_10_46_14</t>
   </si>
   <si>
@@ -5211,9 +5178,6 @@
     <t>2023_03_09_10_01_57</t>
   </si>
   <si>
-    <t>2023_03_09_10_19_41</t>
-  </si>
-  <si>
     <t>2023_03_09_10_31_39</t>
   </si>
   <si>
@@ -5320,6 +5284,60 @@
   </si>
   <si>
     <t>2023_03_14_12_51_48</t>
+  </si>
+  <si>
+    <t>2023_03_15_10_06_03</t>
+  </si>
+  <si>
+    <t>2000571721</t>
+  </si>
+  <si>
+    <t>2023_03_15_10_14_00</t>
+  </si>
+  <si>
+    <t>2023_03_15_10_25_48</t>
+  </si>
+  <si>
+    <t>2023_03_15_10_35_59</t>
+  </si>
+  <si>
+    <t>2023_03_15_10_45_19</t>
+  </si>
+  <si>
+    <t>2023_03_15_10_48_38</t>
+  </si>
+  <si>
+    <t>2023_03_15_10_56_57</t>
+  </si>
+  <si>
+    <t>2000571730</t>
+  </si>
+  <si>
+    <t>2023_03_15_11_20_52</t>
+  </si>
+  <si>
+    <t>2023_03_15_11_26_44</t>
+  </si>
+  <si>
+    <t>2023_03_15_11_30_42</t>
+  </si>
+  <si>
+    <t>2023_03_15_11_34_19</t>
+  </si>
+  <si>
+    <t>2023_03_15_11_43_53</t>
+  </si>
+  <si>
+    <t>2023_03_15_11_53_29</t>
+  </si>
+  <si>
+    <t>7000583024</t>
+  </si>
+  <si>
+    <t>2023_03_15_12_02_52</t>
+  </si>
+  <si>
+    <t>2023_03_15_12_09_09</t>
   </si>
 </sst>
 </file>
@@ -6481,10 +6499,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P318"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6554,18 +6573,18 @@
         <v>38</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>1576</v>
+        <v>1564</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>1575</v>
+        <v>1563</v>
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
       <c r="K2" s="105" t="s">
-        <v>1574</v>
+        <v>1516</v>
       </c>
       <c r="L2" s="99" t="s">
         <v>523</v>
@@ -6694,15 +6713,17 @@
         <v>38</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="G7" s="17"/>
+        <v>1517</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>1565</v>
+      </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
       <c r="L7" s="105" t="s">
-        <v>1527</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -6722,14 +6743,20 @@
         <v>38</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+        <v>1519</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>1567</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>1566</v>
+      </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
-      <c r="L8" s="103"/>
+      <c r="L8" s="105" t="s">
+        <v>1562</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
@@ -6748,9 +6775,11 @@
         <v>38</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="G9" s="17"/>
+        <v>1517</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>1568</v>
+      </c>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
@@ -6879,9 +6908,11 @@
         <v>38</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="G14" s="17"/>
+        <v>1519</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>1569</v>
+      </c>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
@@ -6957,10 +6988,10 @@
         <v>38</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>1529</v>
+        <v>1518</v>
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
@@ -6985,10 +7016,10 @@
         <v>38</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>1534</v>
+        <v>1523</v>
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
@@ -6996,7 +7027,7 @@
       <c r="K18" s="17"/>
       <c r="L18" s="103"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>18</v>
       </c>
@@ -7022,7 +7053,7 @@
       <c r="K19" s="17"/>
       <c r="L19" s="103"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>19</v>
       </c>
@@ -7204,7 +7235,7 @@
       <c r="K26" s="17"/>
       <c r="L26" s="103"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>26</v>
       </c>
@@ -7212,7 +7243,7 @@
         <v>180</v>
       </c>
       <c r="C27" s="135" t="s">
-        <v>1537</v>
+        <v>1526</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>1</v>
@@ -7221,10 +7252,10 @@
         <v>38</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>1536</v>
+        <v>1525</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
@@ -7232,7 +7263,7 @@
       <c r="K27" s="17"/>
       <c r="L27" s="103"/>
     </row>
-    <row r="28" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>27</v>
       </c>
@@ -7249,10 +7280,10 @@
         <v>38</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>1538</v>
+        <v>1527</v>
       </c>
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
@@ -7329,10 +7360,10 @@
         <v>38</v>
       </c>
       <c r="F31" s="17" t="s">
+        <v>1517</v>
+      </c>
+      <c r="G31" s="22" t="s">
         <v>1528</v>
-      </c>
-      <c r="G31" s="22" t="s">
-        <v>1539</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
@@ -7357,10 +7388,10 @@
         <v>38</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>1540</v>
+        <v>1570</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
@@ -7385,10 +7416,10 @@
         <v>38</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G33" s="22" t="s">
-        <v>1541</v>
+        <v>1529</v>
       </c>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
@@ -7413,10 +7444,10 @@
         <v>38</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>1542</v>
+        <v>1530</v>
       </c>
       <c r="H34" s="22"/>
       <c r="I34" s="22"/>
@@ -7441,10 +7472,10 @@
         <v>38</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>1543</v>
+        <v>1531</v>
       </c>
       <c r="H35" s="22"/>
       <c r="I35" s="22"/>
@@ -7469,10 +7500,10 @@
         <v>38</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>1544</v>
+        <v>1532</v>
       </c>
       <c r="H36" s="22"/>
       <c r="I36" s="22"/>
@@ -7497,10 +7528,10 @@
         <v>38</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>1545</v>
+        <v>1533</v>
       </c>
       <c r="H37" s="22"/>
       <c r="I37" s="22"/>
@@ -7525,10 +7556,10 @@
         <v>38</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>1546</v>
+        <v>1534</v>
       </c>
       <c r="H38" s="22"/>
       <c r="I38" s="22"/>
@@ -7553,10 +7584,10 @@
         <v>38</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>1547</v>
+        <v>1535</v>
       </c>
       <c r="H39" s="22"/>
       <c r="I39" s="22"/>
@@ -7581,10 +7612,10 @@
         <v>38</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G40" s="22" t="s">
-        <v>1557</v>
+        <v>1545</v>
       </c>
       <c r="H40" s="22"/>
       <c r="I40" s="22"/>
@@ -7609,10 +7640,10 @@
         <v>38</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G41" s="22" t="s">
-        <v>1548</v>
+        <v>1536</v>
       </c>
       <c r="H41" s="22"/>
       <c r="I41" s="22"/>
@@ -7637,10 +7668,10 @@
         <v>38</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G42" s="22" t="s">
-        <v>1549</v>
+        <v>1537</v>
       </c>
       <c r="H42" s="22"/>
       <c r="I42" s="22"/>
@@ -7665,10 +7696,10 @@
         <v>38</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>1550</v>
+        <v>1538</v>
       </c>
       <c r="H43" s="22"/>
       <c r="I43" s="22"/>
@@ -7693,10 +7724,10 @@
         <v>38</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>1551</v>
+        <v>1539</v>
       </c>
       <c r="H44" s="22"/>
       <c r="I44" s="22"/>
@@ -7721,10 +7752,10 @@
         <v>38</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G45" s="22" t="s">
-        <v>1552</v>
+        <v>1540</v>
       </c>
       <c r="H45" s="22"/>
       <c r="I45" s="22"/>
@@ -7749,10 +7780,10 @@
         <v>38</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G46" s="22" t="s">
-        <v>1553</v>
+        <v>1541</v>
       </c>
       <c r="H46" s="22"/>
       <c r="I46" s="22"/>
@@ -7777,10 +7808,10 @@
         <v>38</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>1554</v>
+        <v>1542</v>
       </c>
       <c r="H47" s="22"/>
       <c r="I47" s="22"/>
@@ -7805,10 +7836,10 @@
         <v>38</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G48" s="22" t="s">
-        <v>1555</v>
+        <v>1543</v>
       </c>
       <c r="H48" s="22"/>
       <c r="I48" s="22"/>
@@ -7833,10 +7864,10 @@
         <v>38</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G49" s="22" t="s">
-        <v>1558</v>
+        <v>1546</v>
       </c>
       <c r="H49" s="22"/>
       <c r="I49" s="22"/>
@@ -7861,10 +7892,10 @@
         <v>38</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G50" s="22" t="s">
-        <v>1559</v>
+        <v>1547</v>
       </c>
       <c r="H50" s="22"/>
       <c r="I50" s="22"/>
@@ -7889,10 +7920,10 @@
         <v>38</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G51" s="22" t="s">
-        <v>1556</v>
+        <v>1544</v>
       </c>
       <c r="H51" s="22"/>
       <c r="I51" s="22"/>
@@ -7908,7 +7939,7 @@
         <v>544</v>
       </c>
       <c r="C52" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D52" s="17" t="s">
         <v>1</v>
@@ -7917,10 +7948,10 @@
         <v>38</v>
       </c>
       <c r="F52" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G52" s="22" t="s">
-        <v>1560</v>
+        <v>1548</v>
       </c>
       <c r="H52" s="22"/>
       <c r="I52" s="22"/>
@@ -7936,7 +7967,7 @@
         <v>546</v>
       </c>
       <c r="C53" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D53" s="17" t="s">
         <v>1</v>
@@ -7945,10 +7976,10 @@
         <v>38</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G53" s="22" t="s">
-        <v>1561</v>
+        <v>1549</v>
       </c>
       <c r="H53" s="22"/>
       <c r="I53" s="22"/>
@@ -7973,10 +8004,10 @@
         <v>38</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G54" s="22" t="s">
-        <v>1562</v>
+        <v>1550</v>
       </c>
       <c r="H54" s="22"/>
       <c r="I54" s="22"/>
@@ -7992,7 +8023,7 @@
         <v>552</v>
       </c>
       <c r="C55" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D55" s="17" t="s">
         <v>1</v>
@@ -8001,10 +8032,10 @@
         <v>38</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G55" s="22" t="s">
-        <v>1563</v>
+        <v>1551</v>
       </c>
       <c r="H55" s="22"/>
       <c r="I55" s="22"/>
@@ -8020,7 +8051,7 @@
         <v>554</v>
       </c>
       <c r="C56" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D56" s="17" t="s">
         <v>1</v>
@@ -8029,10 +8060,10 @@
         <v>38</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>1564</v>
+        <v>1552</v>
       </c>
       <c r="H56" s="22" t="s">
         <v>318</v>
@@ -8050,7 +8081,7 @@
         <v>556</v>
       </c>
       <c r="C57" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D57" s="17" t="s">
         <v>1</v>
@@ -8059,10 +8090,10 @@
         <v>38</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G57" s="22" t="s">
-        <v>1565</v>
+        <v>1553</v>
       </c>
       <c r="H57" s="22" t="s">
         <v>318</v>
@@ -8080,7 +8111,7 @@
         <v>557</v>
       </c>
       <c r="C58" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D58" s="17" t="s">
         <v>1</v>
@@ -8089,10 +8120,10 @@
         <v>38</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G58" s="22" t="s">
-        <v>1566</v>
+        <v>1554</v>
       </c>
       <c r="H58" s="22"/>
       <c r="I58" s="22"/>
@@ -8108,7 +8139,7 @@
         <v>560</v>
       </c>
       <c r="C59" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D59" s="17" t="s">
         <v>1</v>
@@ -8117,10 +8148,10 @@
         <v>38</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G59" s="22" t="s">
-        <v>1567</v>
+        <v>1555</v>
       </c>
       <c r="H59" s="22" t="s">
         <v>318</v>
@@ -8138,7 +8169,7 @@
         <v>562</v>
       </c>
       <c r="C60" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D60" s="17" t="s">
         <v>1</v>
@@ -8147,10 +8178,10 @@
         <v>38</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G60" s="22" t="s">
-        <v>1568</v>
+        <v>1556</v>
       </c>
       <c r="H60" s="22" t="s">
         <v>318</v>
@@ -8168,7 +8199,7 @@
         <v>564</v>
       </c>
       <c r="C61" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D61" s="17" t="s">
         <v>1</v>
@@ -8177,10 +8208,10 @@
         <v>38</v>
       </c>
       <c r="F61" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G61" s="22" t="s">
-        <v>1569</v>
+        <v>1557</v>
       </c>
       <c r="H61" s="22" t="s">
         <v>318</v>
@@ -8198,7 +8229,7 @@
         <v>566</v>
       </c>
       <c r="C62" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D62" s="17" t="s">
         <v>1</v>
@@ -8207,10 +8238,10 @@
         <v>38</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G62" s="22" t="s">
-        <v>1570</v>
+        <v>1558</v>
       </c>
       <c r="H62" s="22" t="s">
         <v>318</v>
@@ -8228,7 +8259,7 @@
         <v>568</v>
       </c>
       <c r="C63" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D63" s="17" t="s">
         <v>1</v>
@@ -8237,10 +8268,10 @@
         <v>38</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>1571</v>
+        <v>1559</v>
       </c>
       <c r="H63" s="22"/>
       <c r="I63" s="22"/>
@@ -8256,7 +8287,7 @@
         <v>570</v>
       </c>
       <c r="C64" s="132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>1</v>
@@ -8265,10 +8296,10 @@
         <v>38</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="G64" s="22" t="s">
-        <v>1572</v>
+        <v>1560</v>
       </c>
       <c r="H64" s="22" t="s">
         <v>318</v>
@@ -8295,10 +8326,10 @@
         <v>38</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="G65" s="22" t="s">
-        <v>1573</v>
+        <v>1561</v>
       </c>
       <c r="H65" s="22"/>
       <c r="I65" s="22"/>
@@ -8323,16 +8354,18 @@
         <v>38</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="G66" s="22"/>
+        <v>1519</v>
+      </c>
+      <c r="G66" s="22" t="s">
+        <v>1571</v>
+      </c>
       <c r="H66" s="22"/>
       <c r="I66" s="22"/>
       <c r="J66" s="22"/>
       <c r="K66" s="22"/>
       <c r="L66" s="103"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="17">
         <v>66</v>
       </c>
@@ -8358,7 +8391,7 @@
       <c r="K67" s="22"/>
       <c r="L67" s="103"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="17">
         <v>67</v>
       </c>
@@ -8384,7 +8417,7 @@
       <c r="K68" s="22"/>
       <c r="L68" s="103"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
         <v>68</v>
       </c>
@@ -8410,7 +8443,7 @@
       <c r="K69" s="22"/>
       <c r="L69" s="103"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
         <v>69</v>
       </c>
@@ -8427,10 +8460,10 @@
         <v>38</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>259</v>
+        <v>1519</v>
       </c>
       <c r="G70" s="22" t="s">
-        <v>1466</v>
+        <v>1575</v>
       </c>
       <c r="H70" s="22"/>
       <c r="I70" s="22"/>
@@ -8438,7 +8471,7 @@
       <c r="K70" s="22"/>
       <c r="L70" s="103"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
         <v>70</v>
       </c>
@@ -8464,7 +8497,7 @@
       <c r="K71" s="22"/>
       <c r="L71" s="103"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
         <v>71</v>
       </c>
@@ -8490,7 +8523,7 @@
       <c r="K72" s="22"/>
       <c r="L72" s="103"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
         <v>72</v>
       </c>
@@ -8516,7 +8549,7 @@
       <c r="K73" s="22"/>
       <c r="L73" s="103"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="17">
         <v>73</v>
       </c>
@@ -8542,7 +8575,7 @@
       <c r="K74" s="22"/>
       <c r="L74" s="103"/>
     </row>
-    <row r="75" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="17">
         <v>74</v>
       </c>
@@ -8568,7 +8601,7 @@
       <c r="K75" s="17"/>
       <c r="L75" s="106"/>
     </row>
-    <row r="76" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="17">
         <v>75</v>
       </c>
@@ -8594,7 +8627,7 @@
       <c r="K76" s="17"/>
       <c r="L76" s="106"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="17">
         <v>76</v>
       </c>
@@ -8620,7 +8653,7 @@
       <c r="K77" s="45"/>
       <c r="L77" s="107"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="17">
         <v>77</v>
       </c>
@@ -8646,7 +8679,7 @@
       <c r="K78" s="45"/>
       <c r="L78" s="107"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="17">
         <v>78</v>
       </c>
@@ -8672,7 +8705,7 @@
       <c r="K79" s="45"/>
       <c r="L79" s="107"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="17">
         <v>79</v>
       </c>
@@ -8698,7 +8731,7 @@
       <c r="K80" s="45"/>
       <c r="L80" s="107"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="17">
         <v>80</v>
       </c>
@@ -8724,7 +8757,7 @@
       <c r="K81" s="45"/>
       <c r="L81" s="107"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="17">
         <v>81</v>
       </c>
@@ -8750,7 +8783,7 @@
       <c r="K82" s="45"/>
       <c r="L82" s="107"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="17">
         <v>82</v>
       </c>
@@ -8776,7 +8809,7 @@
       <c r="K83" s="45"/>
       <c r="L83" s="107"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="17">
         <v>83</v>
       </c>
@@ -8802,7 +8835,7 @@
       <c r="K84" s="45"/>
       <c r="L84" s="107"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="17">
         <v>84</v>
       </c>
@@ -8828,7 +8861,7 @@
       <c r="K85" s="45"/>
       <c r="L85" s="107"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="17">
         <v>85</v>
       </c>
@@ -8854,7 +8887,7 @@
       <c r="K86" s="45"/>
       <c r="L86" s="107"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="17">
         <v>86</v>
       </c>
@@ -8880,7 +8913,7 @@
       <c r="K87" s="45"/>
       <c r="L87" s="107"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="17">
         <v>87</v>
       </c>
@@ -8906,7 +8939,7 @@
       <c r="K88" s="45"/>
       <c r="L88" s="107"/>
     </row>
-    <row r="89" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="17">
         <v>88</v>
       </c>
@@ -8932,7 +8965,7 @@
       <c r="K89" s="17"/>
       <c r="L89" s="106"/>
     </row>
-    <row r="90" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="17">
         <v>89</v>
       </c>
@@ -8958,7 +8991,7 @@
       <c r="K90" s="17"/>
       <c r="L90" s="106"/>
     </row>
-    <row r="91" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="17">
         <v>90</v>
       </c>
@@ -8984,7 +9017,7 @@
       <c r="K91" s="17"/>
       <c r="L91" s="106"/>
     </row>
-    <row r="92" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="17">
         <v>91</v>
       </c>
@@ -9010,7 +9043,7 @@
       <c r="K92" s="17"/>
       <c r="L92" s="106"/>
     </row>
-    <row r="93" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="17">
         <v>92</v>
       </c>
@@ -9036,7 +9069,7 @@
       <c r="K93" s="17"/>
       <c r="L93" s="106"/>
     </row>
-    <row r="94" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="17">
         <v>93</v>
       </c>
@@ -9062,7 +9095,7 @@
       <c r="K94" s="17"/>
       <c r="L94" s="106"/>
     </row>
-    <row r="95" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="17">
         <v>94</v>
       </c>
@@ -9088,7 +9121,7 @@
       <c r="K95" s="17"/>
       <c r="L95" s="106"/>
     </row>
-    <row r="96" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="17">
         <v>95</v>
       </c>
@@ -9114,7 +9147,7 @@
       <c r="K96" s="17"/>
       <c r="L96" s="106"/>
     </row>
-    <row r="97" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="17">
         <v>96</v>
       </c>
@@ -9140,7 +9173,7 @@
       <c r="K97" s="17"/>
       <c r="L97" s="106"/>
     </row>
-    <row r="98" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="17">
         <v>97</v>
       </c>
@@ -9166,7 +9199,7 @@
       <c r="K98" s="17"/>
       <c r="L98" s="106"/>
     </row>
-    <row r="99" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="17">
         <v>98</v>
       </c>
@@ -9192,7 +9225,7 @@
       <c r="K99" s="17"/>
       <c r="L99" s="106"/>
     </row>
-    <row r="100" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="17">
         <v>99</v>
       </c>
@@ -9218,7 +9251,7 @@
       <c r="K100" s="17"/>
       <c r="L100" s="106"/>
     </row>
-    <row r="101" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="17">
         <v>100</v>
       </c>
@@ -9244,7 +9277,7 @@
       <c r="K101" s="17"/>
       <c r="L101" s="106"/>
     </row>
-    <row r="102" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="17">
         <v>101</v>
       </c>
@@ -9270,7 +9303,7 @@
       <c r="K102" s="17"/>
       <c r="L102" s="106"/>
     </row>
-    <row r="103" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="17">
         <v>102</v>
       </c>
@@ -9296,7 +9329,7 @@
       <c r="K103" s="17"/>
       <c r="L103" s="106"/>
     </row>
-    <row r="104" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="17">
         <v>103</v>
       </c>
@@ -9322,7 +9355,7 @@
       <c r="K104" s="17"/>
       <c r="L104" s="106"/>
     </row>
-    <row r="105" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="17">
         <v>104</v>
       </c>
@@ -9348,7 +9381,7 @@
       <c r="K105" s="17"/>
       <c r="L105" s="106"/>
     </row>
-    <row r="106" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="17">
         <v>105</v>
       </c>
@@ -9374,7 +9407,7 @@
       <c r="K106" s="17"/>
       <c r="L106" s="106"/>
     </row>
-    <row r="107" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="17">
         <v>106</v>
       </c>
@@ -9400,7 +9433,7 @@
       <c r="K107" s="17"/>
       <c r="L107" s="106"/>
     </row>
-    <row r="108" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="17">
         <v>107</v>
       </c>
@@ -9426,7 +9459,7 @@
       <c r="K108" s="17"/>
       <c r="L108" s="106"/>
     </row>
-    <row r="109" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="17">
         <v>108</v>
       </c>
@@ -9452,7 +9485,7 @@
       <c r="K109" s="17"/>
       <c r="L109" s="106"/>
     </row>
-    <row r="110" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="17">
         <v>109</v>
       </c>
@@ -9478,7 +9511,7 @@
       <c r="K110" s="17"/>
       <c r="L110" s="106"/>
     </row>
-    <row r="111" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="17">
         <v>110</v>
       </c>
@@ -9504,7 +9537,7 @@
       <c r="K111" s="17"/>
       <c r="L111" s="106"/>
     </row>
-    <row r="112" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="17">
         <v>111</v>
       </c>
@@ -9530,7 +9563,7 @@
       <c r="K112" s="17"/>
       <c r="L112" s="106"/>
     </row>
-    <row r="113" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="17">
         <v>112</v>
       </c>
@@ -9556,7 +9589,7 @@
       <c r="K113" s="17"/>
       <c r="L113" s="106"/>
     </row>
-    <row r="114" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="17">
         <v>113</v>
       </c>
@@ -9582,7 +9615,7 @@
       <c r="K114" s="17"/>
       <c r="L114" s="106"/>
     </row>
-    <row r="115" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="17">
         <v>114</v>
       </c>
@@ -9608,7 +9641,7 @@
       <c r="K115" s="17"/>
       <c r="L115" s="106"/>
     </row>
-    <row r="116" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="17">
         <v>115</v>
       </c>
@@ -9634,7 +9667,7 @@
       <c r="K116" s="17"/>
       <c r="L116" s="106"/>
     </row>
-    <row r="117" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="17">
         <v>116</v>
       </c>
@@ -9660,7 +9693,7 @@
       <c r="K117" s="17"/>
       <c r="L117" s="106"/>
     </row>
-    <row r="118" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="17">
         <v>117</v>
       </c>
@@ -9686,7 +9719,7 @@
       <c r="K118" s="17"/>
       <c r="L118" s="106"/>
     </row>
-    <row r="119" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="17">
         <v>118</v>
       </c>
@@ -9712,7 +9745,7 @@
       <c r="K119" s="17"/>
       <c r="L119" s="106"/>
     </row>
-    <row r="120" spans="1:12" s="98" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" s="98" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="17">
         <v>119</v>
       </c>
@@ -9740,7 +9773,7 @@
       <c r="K120" s="97"/>
       <c r="L120" s="108"/>
     </row>
-    <row r="121" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="17">
         <v>120</v>
       </c>
@@ -9766,7 +9799,7 @@
       <c r="K121" s="17"/>
       <c r="L121" s="106"/>
     </row>
-    <row r="122" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="17">
         <v>121</v>
       </c>
@@ -9792,7 +9825,7 @@
       <c r="K122" s="17"/>
       <c r="L122" s="106"/>
     </row>
-    <row r="123" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="17">
         <v>122</v>
       </c>
@@ -9818,7 +9851,7 @@
       <c r="K123" s="17"/>
       <c r="L123" s="106"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="17">
         <v>123</v>
       </c>
@@ -9844,7 +9877,7 @@
       <c r="K124" s="13"/>
       <c r="L124" s="103"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="17">
         <v>124</v>
       </c>
@@ -9865,7 +9898,7 @@
       </c>
       <c r="L125" s="103"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="17">
         <v>125</v>
       </c>
@@ -9886,7 +9919,7 @@
       </c>
       <c r="L126" s="103"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="17">
         <v>126</v>
       </c>
@@ -9907,7 +9940,7 @@
       </c>
       <c r="L127" s="103"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="17">
         <v>127</v>
       </c>
@@ -9928,7 +9961,7 @@
       </c>
       <c r="L128" s="103"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="17">
         <v>128</v>
       </c>
@@ -9949,7 +9982,7 @@
       </c>
       <c r="L129" s="103"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="17">
         <v>129</v>
       </c>
@@ -9970,7 +10003,7 @@
       </c>
       <c r="L130" s="103"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="17">
         <v>130</v>
       </c>
@@ -10041,10 +10074,10 @@
         <v>259</v>
       </c>
       <c r="G133" s="19" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="H133" s="19" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="I133" s="19"/>
       <c r="J133" s="19"/>
@@ -10221,10 +10254,10 @@
         <v>259</v>
       </c>
       <c r="G139" s="19" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="H139" s="19" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="I139" s="19"/>
       <c r="J139" s="19"/>
@@ -10398,10 +10431,10 @@
         <v>38</v>
       </c>
       <c r="F145" s="17" t="s">
-        <v>259</v>
+        <v>1519</v>
       </c>
       <c r="G145" s="19" t="s">
-        <v>1475</v>
+        <v>1572</v>
       </c>
       <c r="H145" s="19"/>
       <c r="I145" s="19"/>
@@ -10456,13 +10489,13 @@
         <v>38</v>
       </c>
       <c r="F147" s="17" t="s">
-        <v>259</v>
+        <v>1517</v>
       </c>
       <c r="G147" s="19" t="s">
-        <v>1473</v>
+        <v>1574</v>
       </c>
       <c r="H147" s="19" t="s">
-        <v>1472</v>
+        <v>1573</v>
       </c>
       <c r="I147" s="19"/>
       <c r="J147" s="19"/>
@@ -10489,7 +10522,7 @@
         <v>259</v>
       </c>
       <c r="G148" s="22" t="s">
-        <v>1479</v>
+        <v>1475</v>
       </c>
       <c r="H148" s="22"/>
       <c r="I148" s="22"/>
@@ -10517,7 +10550,7 @@
         <v>259</v>
       </c>
       <c r="G149" s="22" t="s">
-        <v>1480</v>
+        <v>1476</v>
       </c>
       <c r="H149" s="22"/>
       <c r="I149" s="22"/>
@@ -10545,7 +10578,7 @@
         <v>259</v>
       </c>
       <c r="G150" s="22" t="s">
-        <v>1482</v>
+        <v>1478</v>
       </c>
       <c r="H150" s="22"/>
       <c r="I150" s="22"/>
@@ -10601,7 +10634,7 @@
         <v>259</v>
       </c>
       <c r="G152" s="22" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="H152" s="22"/>
       <c r="I152" s="22"/>
@@ -10657,7 +10690,7 @@
         <v>259</v>
       </c>
       <c r="G154" s="22" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="H154" s="22"/>
       <c r="I154" s="22"/>
@@ -10708,10 +10741,10 @@
         <v>38</v>
       </c>
       <c r="F156" s="17" t="s">
-        <v>259</v>
+        <v>1517</v>
       </c>
       <c r="G156" s="22" t="s">
-        <v>1484</v>
+        <v>1576</v>
       </c>
       <c r="H156" s="22"/>
       <c r="I156" s="22"/>
@@ -10739,7 +10772,7 @@
         <v>259</v>
       </c>
       <c r="G157" s="22" t="s">
-        <v>1485</v>
+        <v>1480</v>
       </c>
       <c r="H157" s="22"/>
       <c r="I157" s="22"/>
@@ -10767,10 +10800,10 @@
         <v>259</v>
       </c>
       <c r="G158" s="22" t="s">
-        <v>1487</v>
+        <v>1482</v>
       </c>
       <c r="H158" s="22" t="s">
-        <v>1486</v>
+        <v>1481</v>
       </c>
       <c r="I158" s="22"/>
       <c r="J158" s="22"/>
@@ -10797,7 +10830,7 @@
         <v>259</v>
       </c>
       <c r="G159" s="19" t="s">
-        <v>1490</v>
+        <v>1485</v>
       </c>
       <c r="H159" s="19"/>
       <c r="I159" s="19"/>
@@ -10822,10 +10855,10 @@
         <v>38</v>
       </c>
       <c r="F160" s="17" t="s">
-        <v>259</v>
+        <v>1519</v>
       </c>
       <c r="G160" s="19" t="s">
-        <v>1492</v>
+        <v>1577</v>
       </c>
       <c r="H160" s="19"/>
       <c r="I160" s="19"/>
@@ -10853,7 +10886,7 @@
         <v>259</v>
       </c>
       <c r="G161" s="19" t="s">
-        <v>1491</v>
+        <v>1486</v>
       </c>
       <c r="H161" s="19"/>
       <c r="I161" s="19"/>
@@ -10881,7 +10914,7 @@
         <v>259</v>
       </c>
       <c r="G162" s="19" t="s">
-        <v>1493</v>
+        <v>1487</v>
       </c>
       <c r="H162" s="19"/>
       <c r="I162" s="19"/>
@@ -10909,7 +10942,7 @@
         <v>259</v>
       </c>
       <c r="G163" s="19" t="s">
-        <v>1494</v>
+        <v>1488</v>
       </c>
       <c r="H163" s="19"/>
       <c r="I163" s="19"/>
@@ -10937,7 +10970,7 @@
         <v>259</v>
       </c>
       <c r="G164" s="19" t="s">
-        <v>1495</v>
+        <v>1489</v>
       </c>
       <c r="H164" s="19"/>
       <c r="I164" s="19"/>
@@ -10962,10 +10995,10 @@
         <v>38</v>
       </c>
       <c r="F165" s="17" t="s">
-        <v>259</v>
+        <v>1519</v>
       </c>
       <c r="G165" s="19" t="s">
-        <v>1496</v>
+        <v>1578</v>
       </c>
       <c r="H165" s="19"/>
       <c r="I165" s="19"/>
@@ -10990,10 +11023,10 @@
         <v>38</v>
       </c>
       <c r="F166" s="17" t="s">
-        <v>259</v>
+        <v>1519</v>
       </c>
       <c r="G166" s="19" t="s">
-        <v>1497</v>
+        <v>1579</v>
       </c>
       <c r="H166" s="19"/>
       <c r="I166" s="19"/>
@@ -11047,7 +11080,7 @@
         <v>259</v>
       </c>
       <c r="G168" s="19" t="s">
-        <v>1500</v>
+        <v>1492</v>
       </c>
       <c r="H168" s="19"/>
       <c r="I168" s="19"/>
@@ -11075,10 +11108,10 @@
         <v>259</v>
       </c>
       <c r="G169" s="24" t="s">
-        <v>1504</v>
+        <v>1496</v>
       </c>
       <c r="H169" s="24" t="s">
-        <v>1503</v>
+        <v>1495</v>
       </c>
       <c r="I169" s="24"/>
       <c r="J169" s="24"/>
@@ -11102,13 +11135,13 @@
         <v>38</v>
       </c>
       <c r="F170" s="17" t="s">
-        <v>259</v>
+        <v>1519</v>
       </c>
       <c r="G170" s="24" t="s">
-        <v>1508</v>
+        <v>1581</v>
       </c>
       <c r="H170" s="24" t="s">
-        <v>1507</v>
+        <v>1580</v>
       </c>
       <c r="I170" s="24"/>
       <c r="J170" s="24"/>
@@ -11135,10 +11168,10 @@
         <v>259</v>
       </c>
       <c r="G171" s="24" t="s">
-        <v>1510</v>
+        <v>1500</v>
       </c>
       <c r="H171" s="24" t="s">
-        <v>1509</v>
+        <v>1499</v>
       </c>
       <c r="I171" s="24"/>
       <c r="J171" s="24"/>
@@ -11165,10 +11198,10 @@
         <v>259</v>
       </c>
       <c r="G172" s="25" t="s">
-        <v>1512</v>
+        <v>1502</v>
       </c>
       <c r="H172" s="25" t="s">
-        <v>1511</v>
+        <v>1501</v>
       </c>
       <c r="I172" s="25"/>
       <c r="J172" s="25"/>
@@ -11195,10 +11228,10 @@
         <v>259</v>
       </c>
       <c r="G173" s="25" t="s">
-        <v>1514</v>
+        <v>1504</v>
       </c>
       <c r="H173" s="25" t="s">
-        <v>1513</v>
+        <v>1503</v>
       </c>
       <c r="I173" s="25"/>
       <c r="J173" s="25"/>
@@ -11225,7 +11258,7 @@
         <v>259</v>
       </c>
       <c r="G174" s="25" t="s">
-        <v>1515</v>
+        <v>1505</v>
       </c>
       <c r="H174" s="25"/>
       <c r="I174" s="25"/>
@@ -11253,7 +11286,7 @@
         <v>259</v>
       </c>
       <c r="G175" s="25" t="s">
-        <v>1516</v>
+        <v>1506</v>
       </c>
       <c r="H175" s="25"/>
       <c r="I175" s="25"/>
@@ -11281,10 +11314,10 @@
         <v>259</v>
       </c>
       <c r="G176" s="25" t="s">
-        <v>1520</v>
+        <v>1510</v>
       </c>
       <c r="H176" s="25" t="s">
-        <v>1519</v>
+        <v>1509</v>
       </c>
       <c r="I176" s="25"/>
       <c r="J176" s="25"/>
@@ -11311,10 +11344,10 @@
         <v>259</v>
       </c>
       <c r="G177" s="25" t="s">
-        <v>1518</v>
+        <v>1508</v>
       </c>
       <c r="H177" s="25" t="s">
-        <v>1517</v>
+        <v>1507</v>
       </c>
       <c r="I177" s="25"/>
       <c r="J177" s="25"/>
@@ -11338,10 +11371,10 @@
         <v>38</v>
       </c>
       <c r="F178" s="17" t="s">
-        <v>259</v>
+        <v>1519</v>
       </c>
       <c r="G178" s="130" t="s">
-        <v>1521</v>
+        <v>1582</v>
       </c>
       <c r="H178" s="130" t="s">
         <v>475</v>
@@ -11371,11 +11404,11 @@
         <v>259</v>
       </c>
       <c r="G179" t="s">
-        <v>1522</v>
+        <v>1511</v>
       </c>
       <c r="L179" s="103"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="17">
         <v>177</v>
       </c>
@@ -11402,7 +11435,7 @@
       </c>
       <c r="L180" s="103"/>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="17">
         <v>178</v>
       </c>
@@ -11429,7 +11462,7 @@
       </c>
       <c r="L181" s="103"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="17">
         <v>179</v>
       </c>
@@ -11456,7 +11489,7 @@
       </c>
       <c r="L182" s="103"/>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="17">
         <v>180</v>
       </c>
@@ -11483,7 +11516,7 @@
       </c>
       <c r="L183" s="103"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="17">
         <v>181</v>
       </c>
@@ -11510,7 +11543,7 @@
       </c>
       <c r="L184" s="103"/>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="17">
         <v>182</v>
       </c>
@@ -11537,7 +11570,7 @@
       </c>
       <c r="L185" s="103"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="17">
         <v>183</v>
       </c>
@@ -11564,7 +11597,7 @@
       </c>
       <c r="L186" s="103"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="17">
         <v>184</v>
       </c>
@@ -11591,7 +11624,7 @@
       </c>
       <c r="L187" s="103"/>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="17">
         <v>185</v>
       </c>
@@ -11618,7 +11651,7 @@
       </c>
       <c r="L188" s="103"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="17">
         <v>186</v>
       </c>
@@ -11645,7 +11678,7 @@
       </c>
       <c r="L189" s="103"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="17">
         <v>187</v>
       </c>
@@ -11666,7 +11699,7 @@
       </c>
       <c r="L190" s="103"/>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="17">
         <v>188</v>
       </c>
@@ -11687,7 +11720,7 @@
       </c>
       <c r="L191" s="103"/>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="17">
         <v>189</v>
       </c>
@@ -11708,7 +11741,7 @@
       </c>
       <c r="L192" s="103"/>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="17">
         <v>190</v>
       </c>
@@ -11729,7 +11762,7 @@
       </c>
       <c r="L193" s="103"/>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="17">
         <v>191</v>
       </c>
@@ -11750,7 +11783,7 @@
       </c>
       <c r="L194" s="103"/>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="17">
         <v>192</v>
       </c>
@@ -11771,7 +11804,7 @@
       </c>
       <c r="L195" s="103"/>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="17">
         <v>193</v>
       </c>
@@ -11792,7 +11825,7 @@
       </c>
       <c r="L196" s="103"/>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="17">
         <v>194</v>
       </c>
@@ -11813,7 +11846,7 @@
       </c>
       <c r="L197" s="103"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="17">
         <v>195</v>
       </c>
@@ -11834,7 +11867,7 @@
       </c>
       <c r="L198" s="103"/>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="17">
         <v>196</v>
       </c>
@@ -11855,7 +11888,7 @@
       </c>
       <c r="L199" s="103"/>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="17">
         <v>197</v>
       </c>
@@ -11876,7 +11909,7 @@
       </c>
       <c r="L200" s="103"/>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="17">
         <v>198</v>
       </c>
@@ -11897,7 +11930,7 @@
       </c>
       <c r="L201" s="103"/>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="17">
         <v>199</v>
       </c>
@@ -11924,7 +11957,7 @@
       </c>
       <c r="L202" s="103"/>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="17">
         <v>200</v>
       </c>
@@ -11951,7 +11984,7 @@
       </c>
       <c r="L203" s="103"/>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="17">
         <v>201</v>
       </c>
@@ -11978,7 +12011,7 @@
       </c>
       <c r="L204" s="103"/>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="17">
         <v>202</v>
       </c>
@@ -12005,7 +12038,7 @@
       </c>
       <c r="L205" s="103"/>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="17">
         <v>203</v>
       </c>
@@ -12035,7 +12068,7 @@
       <c r="K206" s="110"/>
       <c r="L206" s="111"/>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="17">
         <v>204</v>
       </c>
@@ -12061,7 +12094,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="17">
         <v>205</v>
       </c>
@@ -12084,7 +12117,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="17">
         <v>206</v>
       </c>
@@ -12110,7 +12143,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="17">
         <v>207</v>
       </c>
@@ -12136,7 +12169,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="17">
         <v>208</v>
       </c>
@@ -12162,7 +12195,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="17">
         <v>209</v>
       </c>
@@ -12188,7 +12221,7 @@
       <c r="K212" s="20"/>
       <c r="L212" s="103"/>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="17">
         <v>210</v>
       </c>
@@ -12208,7 +12241,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="17">
         <v>211</v>
       </c>
@@ -12228,7 +12261,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="17">
         <v>212</v>
       </c>
@@ -12248,7 +12281,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="17">
         <v>213</v>
       </c>
@@ -12268,7 +12301,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="17">
         <v>214</v>
       </c>
@@ -12288,7 +12321,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="17">
         <v>215</v>
       </c>
@@ -12314,7 +12347,7 @@
       <c r="K218" s="17"/>
       <c r="L218" s="103"/>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="17">
         <v>216</v>
       </c>
@@ -12337,7 +12370,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="17">
         <v>217</v>
       </c>
@@ -12360,7 +12393,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="17">
         <v>218</v>
       </c>
@@ -12383,7 +12416,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="17">
         <v>219</v>
       </c>
@@ -12406,7 +12439,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="223" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="17">
         <v>220</v>
       </c>
@@ -12429,7 +12462,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="17">
         <v>221</v>
       </c>
@@ -12452,7 +12485,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="225" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="17">
         <v>222</v>
       </c>
@@ -12472,7 +12505,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="226" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="17">
         <v>223</v>
       </c>
@@ -12492,7 +12525,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="227" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="17">
         <v>224</v>
       </c>
@@ -12512,7 +12545,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="17">
         <v>225</v>
       </c>
@@ -12532,7 +12565,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="17">
         <v>226</v>
       </c>
@@ -12555,7 +12588,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="17">
         <v>227</v>
       </c>
@@ -12578,7 +12611,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="17">
         <v>228</v>
       </c>
@@ -12601,7 +12634,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="17">
         <v>229</v>
       </c>
@@ -12621,7 +12654,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="17">
         <v>230</v>
       </c>
@@ -12641,7 +12674,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="17">
         <v>231</v>
       </c>
@@ -12661,7 +12694,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="17">
         <v>232</v>
       </c>
@@ -12681,7 +12714,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="17">
         <v>233</v>
       </c>
@@ -12701,7 +12734,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="17">
         <v>234</v>
       </c>
@@ -12721,7 +12754,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="17">
         <v>235</v>
       </c>
@@ -12741,7 +12774,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="17">
         <v>236</v>
       </c>
@@ -12761,7 +12794,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="17">
         <v>237</v>
       </c>
@@ -12787,7 +12820,7 @@
       <c r="K240" s="22"/>
       <c r="L240" s="103"/>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="17">
         <v>238</v>
       </c>
@@ -12813,7 +12846,7 @@
       <c r="K241" s="17"/>
       <c r="L241" s="103"/>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="17">
         <v>239</v>
       </c>
@@ -12834,7 +12867,7 @@
       </c>
       <c r="L242" s="103"/>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="17">
         <v>240</v>
       </c>
@@ -12860,7 +12893,7 @@
       <c r="K243" s="22"/>
       <c r="L243" s="103"/>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="17">
         <v>241</v>
       </c>
@@ -12886,7 +12919,7 @@
       <c r="K244" s="22"/>
       <c r="L244" s="103"/>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="17">
         <v>242</v>
       </c>
@@ -12906,7 +12939,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="17">
         <v>243</v>
       </c>
@@ -12926,7 +12959,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="17">
         <v>244</v>
       </c>
@@ -12946,7 +12979,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="17">
         <v>245</v>
       </c>
@@ -12966,7 +12999,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="17">
         <v>246</v>
       </c>
@@ -12994,7 +13027,7 @@
       <c r="K249" s="22"/>
       <c r="L249" s="103"/>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="17">
         <v>247</v>
       </c>
@@ -13022,7 +13055,7 @@
       <c r="K250" s="22"/>
       <c r="L250" s="103"/>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="17">
         <v>248</v>
       </c>
@@ -13045,7 +13078,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="17">
         <v>249</v>
       </c>
@@ -13068,7 +13101,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="17">
         <v>250</v>
       </c>
@@ -13091,7 +13124,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="17">
         <v>251</v>
       </c>
@@ -13114,7 +13147,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="17">
         <v>252</v>
       </c>
@@ -13134,7 +13167,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="17">
         <v>253</v>
       </c>
@@ -13157,7 +13190,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="17">
         <v>254</v>
       </c>
@@ -13180,7 +13213,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="17">
         <v>255</v>
       </c>
@@ -13203,7 +13236,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="17">
         <v>256</v>
       </c>
@@ -13226,7 +13259,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="17">
         <v>257</v>
       </c>
@@ -13252,7 +13285,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="17">
         <v>258</v>
       </c>
@@ -13278,7 +13311,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="17">
         <v>259</v>
       </c>
@@ -13304,7 +13337,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="126">
         <v>260</v>
       </c>
@@ -13330,7 +13363,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="126">
         <v>261</v>
       </c>
@@ -13356,7 +13389,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="126">
         <v>262</v>
       </c>
@@ -13382,7 +13415,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="126">
         <v>263</v>
       </c>
@@ -13408,7 +13441,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="126">
         <v>264</v>
       </c>
@@ -13431,7 +13464,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="126">
         <v>265</v>
       </c>
@@ -13454,7 +13487,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="126">
         <v>265</v>
       </c>
@@ -13477,7 +13510,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="126">
         <v>266</v>
       </c>
@@ -13500,7 +13533,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="126">
         <v>267</v>
       </c>
@@ -13523,7 +13556,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="126">
         <v>268</v>
       </c>
@@ -13546,7 +13579,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="126">
         <v>269</v>
       </c>
@@ -13569,7 +13602,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="126">
         <v>270</v>
       </c>
@@ -13592,7 +13625,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="126">
         <v>271</v>
       </c>
@@ -13615,7 +13648,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="126">
         <v>272</v>
       </c>
@@ -13638,7 +13671,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="126">
         <v>273</v>
       </c>
@@ -13661,7 +13694,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="126">
         <v>274</v>
       </c>
@@ -13684,7 +13717,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="126">
         <v>275</v>
       </c>
@@ -13707,7 +13740,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="126">
         <v>275</v>
       </c>
@@ -13730,7 +13763,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="126">
         <v>276</v>
       </c>
@@ -13753,7 +13786,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="126">
         <v>277</v>
       </c>
@@ -13776,7 +13809,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="126">
         <v>278</v>
       </c>
@@ -13799,7 +13832,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="126">
         <v>279</v>
       </c>
@@ -13822,7 +13855,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="126">
         <v>280</v>
       </c>
@@ -13845,7 +13878,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="126">
         <v>281</v>
       </c>
@@ -13868,7 +13901,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="126">
         <v>282</v>
       </c>
@@ -13891,7 +13924,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="126">
         <v>283</v>
       </c>
@@ -13914,7 +13947,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="126">
         <v>284</v>
       </c>
@@ -13937,7 +13970,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="126">
         <v>285</v>
       </c>
@@ -13960,7 +13993,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="126">
         <v>285</v>
       </c>
@@ -13983,7 +14016,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="126">
         <v>285</v>
       </c>
@@ -14006,7 +14039,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="126">
         <v>286</v>
       </c>
@@ -14032,7 +14065,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="126">
         <v>287</v>
       </c>
@@ -14058,7 +14091,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="126">
         <v>288</v>
       </c>
@@ -14078,10 +14111,10 @@
         <v>259</v>
       </c>
       <c r="G295" t="s">
-        <v>1501</v>
+        <v>1493</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="126">
         <v>289</v>
       </c>
@@ -14101,7 +14134,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="126">
         <v>289</v>
       </c>
@@ -14124,7 +14157,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="126">
         <v>290</v>
       </c>
@@ -14147,7 +14180,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="126">
         <v>291</v>
       </c>
@@ -14170,7 +14203,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="126">
         <v>292</v>
       </c>
@@ -14193,7 +14226,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="126">
         <v>293</v>
       </c>
@@ -14213,7 +14246,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="126">
         <v>294</v>
       </c>
@@ -14236,7 +14269,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="126">
         <v>295</v>
       </c>
@@ -14256,10 +14289,10 @@
         <v>259</v>
       </c>
       <c r="G303" t="s">
-        <v>1498</v>
+        <v>1490</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="126">
         <v>296</v>
       </c>
@@ -14285,7 +14318,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="126">
         <v>297</v>
       </c>
@@ -14308,7 +14341,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="126">
         <v>298</v>
       </c>
@@ -14331,7 +14364,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="126">
         <v>299</v>
       </c>
@@ -14354,7 +14387,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="126">
         <v>300</v>
       </c>
@@ -14380,7 +14413,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="126">
         <v>301</v>
       </c>
@@ -14406,7 +14439,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="126">
         <v>302</v>
       </c>
@@ -14432,7 +14465,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="126">
         <v>303</v>
       </c>
@@ -14458,7 +14491,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="126">
         <v>304</v>
       </c>
@@ -14484,7 +14517,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="126">
         <v>305</v>
       </c>
@@ -14510,7 +14543,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="126">
         <v>306</v>
       </c>
@@ -14536,7 +14569,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="126">
         <v>307</v>
       </c>
@@ -14562,7 +14595,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="126">
         <v>308</v>
       </c>
@@ -14588,7 +14621,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="126">
         <v>309</v>
       </c>
@@ -14614,7 +14647,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="126">
         <v>310</v>
       </c>
@@ -14638,16 +14671,23 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P318" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}"/>
+  <autoFilter ref="A1:P318" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1" xr:uid="{C4DE44B4-9E86-4104-81E3-C93D60F64BE3}"/>
     <hyperlink ref="L2" r:id="rId2" xr:uid="{A4124D5F-F457-4A70-A072-5DFAF5EA33F8}"/>
     <hyperlink ref="L7" r:id="rId3" xr:uid="{25B2C645-4F48-40EF-B244-993C9919EC53}"/>
-    <hyperlink ref="K2" r:id="rId4" xr:uid="{83E02DC1-316B-4DED-B81F-931FDB0A7FBA}"/>
+    <hyperlink ref="L8" r:id="rId4" xr:uid="{7232C0DB-4105-4970-9DC9-351E323A6B9A}"/>
+    <hyperlink ref="K2" r:id="rId5" xr:uid="{D769CF7F-3B55-42B5-B5B8-D367817C08E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -34153,7 +34193,7 @@
         <v>200</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>1474</v>
+        <v>1471</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>250</v>
@@ -34168,7 +34208,7 @@
         <v>257</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>1478</v>
+        <v>1474</v>
       </c>
       <c r="BD1" s="1" t="s">
         <v>184</v>
@@ -36088,7 +36128,7 @@
       <c r="AR18" s="13"/>
       <c r="AS18" s="13"/>
       <c r="AT18" s="13" t="s">
-        <v>1477</v>
+        <v>1473</v>
       </c>
       <c r="AU18" s="13" t="s">
         <v>453</v>
@@ -36096,7 +36136,7 @@
       <c r="AV18" s="13"/>
       <c r="AW18" s="13"/>
       <c r="AX18" s="96" t="s">
-        <v>1476</v>
+        <v>1472</v>
       </c>
       <c r="AY18" s="31" t="s">
         <v>450</v>
@@ -36106,7 +36146,7 @@
         <v>232</v>
       </c>
       <c r="BB18" s="96" t="s">
-        <v>1476</v>
+        <v>1472</v>
       </c>
       <c r="BC18" s="61" t="s">
         <v>254</v>
@@ -36198,13 +36238,13 @@
       <c r="AR19" s="13"/>
       <c r="AS19" s="13"/>
       <c r="AT19" s="13" t="s">
-        <v>1477</v>
+        <v>1473</v>
       </c>
       <c r="AU19" s="13"/>
       <c r="AV19" s="13"/>
       <c r="AW19" s="13"/>
       <c r="AX19" s="96" t="s">
-        <v>1476</v>
+        <v>1472</v>
       </c>
       <c r="AY19" s="31" t="s">
         <v>450</v>
@@ -36216,7 +36256,7 @@
         <v>232</v>
       </c>
       <c r="BB19" s="96" t="s">
-        <v>1476</v>
+        <v>1472</v>
       </c>
       <c r="BC19" s="61" t="s">
         <v>254</v>
@@ -36286,7 +36326,7 @@
       <c r="X20" s="13"/>
       <c r="Y20" s="13"/>
       <c r="Z20" s="44" t="s">
-        <v>1481</v>
+        <v>1477</v>
       </c>
       <c r="AA20" s="44"/>
       <c r="AB20" s="44"/>
@@ -36308,13 +36348,13 @@
       <c r="AR20" s="13"/>
       <c r="AS20" s="13"/>
       <c r="AT20" s="13" t="s">
-        <v>1477</v>
+        <v>1473</v>
       </c>
       <c r="AU20" s="13"/>
       <c r="AV20" s="13"/>
       <c r="AW20" s="13"/>
       <c r="AX20" s="96" t="s">
-        <v>1476</v>
+        <v>1472</v>
       </c>
       <c r="AY20" s="31" t="s">
         <v>450</v>
@@ -36326,7 +36366,7 @@
         <v>232</v>
       </c>
       <c r="BB20" s="96" t="s">
-        <v>1476</v>
+        <v>1472</v>
       </c>
       <c r="BC20" s="61" t="s">
         <v>254</v>
@@ -37246,7 +37286,7 @@
       <c r="S29" s="13"/>
       <c r="T29" s="55"/>
       <c r="U29" s="47" t="s">
-        <v>1488</v>
+        <v>1483</v>
       </c>
       <c r="V29" s="47" t="s">
         <v>675</v>
@@ -37274,7 +37314,7 @@
       <c r="AM29" s="55"/>
       <c r="AN29" s="55"/>
       <c r="AO29" s="47" t="s">
-        <v>1489</v>
+        <v>1484</v>
       </c>
       <c r="AP29" s="55" t="s">
         <v>686</v>
@@ -38045,7 +38085,7 @@
         <v>1331</v>
       </c>
       <c r="Z37" s="136" t="s">
-        <v>1499</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="38" spans="1:78" x14ac:dyDescent="0.25">
@@ -38184,7 +38224,7 @@
         <v>1369</v>
       </c>
       <c r="P39" s="47" t="s">
-        <v>1502</v>
+        <v>1494</v>
       </c>
       <c r="S39" s="13" t="s">
         <v>5</v>
@@ -38445,7 +38485,7 @@
         <v>227</v>
       </c>
       <c r="Q3" s="67" t="s">
-        <v>1506</v>
+        <v>1498</v>
       </c>
       <c r="R3" s="21" t="s">
         <v>24</v>
@@ -38457,7 +38497,7 @@
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
       <c r="W3" s="67" t="s">
-        <v>1505</v>
+        <v>1497</v>
       </c>
       <c r="X3" s="11"/>
       <c r="Y3" s="8"/>
@@ -46675,10 +46715,10 @@
       </c>
       <c r="AK18" s="15"/>
       <c r="AL18" s="31" t="s">
-        <v>1532</v>
+        <v>1521</v>
       </c>
       <c r="AM18" s="31" t="s">
-        <v>1532</v>
+        <v>1521</v>
       </c>
       <c r="AN18" s="31"/>
       <c r="AO18" s="41"/>
@@ -46686,7 +46726,7 @@
         <v>275</v>
       </c>
       <c r="AQ18" s="31" t="s">
-        <v>1532</v>
+        <v>1521</v>
       </c>
       <c r="AR18" s="41"/>
       <c r="AS18" s="41"/>
@@ -46726,7 +46766,7 @@
         <v>14</v>
       </c>
       <c r="BQ18" s="31" t="s">
-        <v>1533</v>
+        <v>1522</v>
       </c>
       <c r="BR18" s="31" t="s">
         <v>45</v>
@@ -46735,7 +46775,7 @@
         <v>45</v>
       </c>
       <c r="BT18" s="31" t="s">
-        <v>1532</v>
+        <v>1521</v>
       </c>
       <c r="BU18" s="31"/>
       <c r="BV18" s="31"/>
@@ -46750,7 +46790,7 @@
         <v>231</v>
       </c>
       <c r="CE18" s="31" t="s">
-        <v>1532</v>
+        <v>1521</v>
       </c>
       <c r="CF18" s="15" t="s">
         <v>232</v>
@@ -46759,7 +46799,7 @@
         <v>45</v>
       </c>
       <c r="CH18" s="31" t="s">
-        <v>1532</v>
+        <v>1521</v>
       </c>
       <c r="CI18" s="31"/>
       <c r="CJ18" s="31"/>
@@ -46832,7 +46872,7 @@
       <c r="EQ18" s="41"/>
       <c r="ER18" s="41"/>
       <c r="ES18" s="46" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="ET18" s="41"/>
       <c r="EU18" s="41"/>
@@ -46968,7 +47008,7 @@
       </c>
       <c r="BA19" s="41"/>
       <c r="BB19" s="43" t="s">
-        <v>1525</v>
+        <v>1514</v>
       </c>
       <c r="BC19" s="43"/>
       <c r="BD19" s="43"/>
@@ -47088,7 +47128,7 @@
         <v>154</v>
       </c>
       <c r="DL19" s="31" t="s">
-        <v>1525</v>
+        <v>1514</v>
       </c>
       <c r="DM19" s="13" t="s">
         <v>155</v>
@@ -48570,7 +48610,7 @@
         <v>6</v>
       </c>
       <c r="AJ27" s="46" t="s">
-        <v>1535</v>
+        <v>1524</v>
       </c>
       <c r="AK27" s="46"/>
       <c r="AL27" s="31" t="s">
@@ -48723,7 +48763,7 @@
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="47" t="s">
-        <v>1531</v>
+        <v>1520</v>
       </c>
       <c r="G28" s="41"/>
       <c r="H28" s="41"/>
@@ -49403,7 +49443,7 @@
         <v>276</v>
       </c>
       <c r="AQ31" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR31" s="14"/>
       <c r="AS31" s="14"/>
@@ -49620,7 +49660,7 @@
         <v>276</v>
       </c>
       <c r="AQ32" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR32" s="14"/>
       <c r="AS32" s="14"/>
@@ -49837,7 +49877,7 @@
         <v>276</v>
       </c>
       <c r="AQ33" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR33" s="14"/>
       <c r="AS33" s="14"/>
@@ -50054,7 +50094,7 @@
         <v>276</v>
       </c>
       <c r="AQ34" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR34" s="14"/>
       <c r="AS34" s="14"/>
@@ -50271,7 +50311,7 @@
         <v>276</v>
       </c>
       <c r="AQ35" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR35" s="14"/>
       <c r="AS35" s="14"/>
@@ -50488,7 +50528,7 @@
         <v>276</v>
       </c>
       <c r="AQ36" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR36" s="14"/>
       <c r="AS36" s="14"/>
@@ -50699,7 +50739,7 @@
         <v>1236</v>
       </c>
       <c r="AM37" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AN37" s="34"/>
       <c r="AO37" s="14"/>
@@ -50707,7 +50747,7 @@
         <v>276</v>
       </c>
       <c r="AQ37" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR37" s="14"/>
       <c r="AS37" s="14"/>
@@ -50918,7 +50958,7 @@
         <v>1236</v>
       </c>
       <c r="AM38" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AN38" s="34"/>
       <c r="AO38" s="14"/>
@@ -50926,7 +50966,7 @@
         <v>276</v>
       </c>
       <c r="AQ38" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR38" s="14"/>
       <c r="AS38" s="14"/>
@@ -51137,7 +51177,7 @@
         <v>1236</v>
       </c>
       <c r="AM39" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AN39" s="34"/>
       <c r="AO39" s="14"/>
@@ -51145,7 +51185,7 @@
         <v>276</v>
       </c>
       <c r="AQ39" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR39" s="14"/>
       <c r="AS39" s="14"/>
@@ -51362,7 +51402,7 @@
         <v>276</v>
       </c>
       <c r="AQ40" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR40" s="14"/>
       <c r="AS40" s="14"/>
@@ -51585,7 +51625,7 @@
         <v>276</v>
       </c>
       <c r="AQ41" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR41" s="14"/>
       <c r="AS41" s="14"/>
@@ -51808,7 +51848,7 @@
         <v>276</v>
       </c>
       <c r="AQ42" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR42" s="14"/>
       <c r="AS42" s="14"/>
@@ -52031,7 +52071,7 @@
         <v>276</v>
       </c>
       <c r="AQ43" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR43" s="14"/>
       <c r="AS43" s="14"/>
@@ -52254,7 +52294,7 @@
         <v>276</v>
       </c>
       <c r="AQ44" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR44" s="14"/>
       <c r="AS44" s="14"/>
@@ -52477,7 +52517,7 @@
         <v>276</v>
       </c>
       <c r="AQ45" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR45" s="14"/>
       <c r="AS45" s="14"/>
@@ -52694,7 +52734,7 @@
         <v>1236</v>
       </c>
       <c r="AM46" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AN46" s="34"/>
       <c r="AO46" s="14"/>
@@ -52702,7 +52742,7 @@
         <v>276</v>
       </c>
       <c r="AQ46" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR46" s="14"/>
       <c r="AS46" s="14"/>
@@ -52919,7 +52959,7 @@
         <v>1236</v>
       </c>
       <c r="AM47" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AN47" s="34"/>
       <c r="AO47" s="14"/>
@@ -52927,7 +52967,7 @@
         <v>276</v>
       </c>
       <c r="AQ47" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR47" s="14"/>
       <c r="AS47" s="14"/>
@@ -53144,7 +53184,7 @@
         <v>1236</v>
       </c>
       <c r="AM48" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AN48" s="34"/>
       <c r="AO48" s="14"/>
@@ -53152,7 +53192,7 @@
         <v>276</v>
       </c>
       <c r="AQ48" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR48" s="14"/>
       <c r="AS48" s="14"/>
@@ -53375,7 +53415,7 @@
         <v>276</v>
       </c>
       <c r="AQ49" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR49" s="14"/>
       <c r="AS49" s="14"/>
@@ -53592,7 +53632,7 @@
         <v>276</v>
       </c>
       <c r="AQ50" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR50" s="14"/>
       <c r="AS50" s="14"/>
@@ -53811,7 +53851,7 @@
         <v>275</v>
       </c>
       <c r="AQ51" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR51" s="14"/>
       <c r="AS51" s="14"/>
@@ -53957,7 +53997,7 @@
         <v>275</v>
       </c>
       <c r="AQ52" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR52" s="14"/>
       <c r="AY52" s="15"/>
@@ -53973,7 +54013,7 @@
         <v>14</v>
       </c>
       <c r="BQ52" s="31" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="BR52" s="31" t="s">
         <v>45</v>
@@ -53982,7 +54022,7 @@
         <v>45</v>
       </c>
       <c r="BT52" s="31" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="CD52" s="15" t="s">
         <v>231</v>
@@ -53997,7 +54037,7 @@
         <v>45</v>
       </c>
       <c r="CH52" s="31" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="CR52" s="31" t="s">
         <v>407</v>
@@ -54107,7 +54147,7 @@
         <v>276</v>
       </c>
       <c r="AQ53" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR53" s="2" t="s">
         <v>55</v>
@@ -54125,7 +54165,7 @@
         <v>14</v>
       </c>
       <c r="BQ53" s="31" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="CD53" s="15" t="s">
         <v>231</v>
@@ -54297,7 +54337,7 @@
         <v>275</v>
       </c>
       <c r="AQ55" s="34" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="AR55" s="14"/>
       <c r="AS55" s="14"/>
@@ -54915,17 +54955,17 @@
       </c>
       <c r="AK58" s="15"/>
       <c r="AL58" s="31" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="AM58" s="31" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="AO58" s="41"/>
       <c r="AP58" s="15" t="s">
         <v>275</v>
       </c>
       <c r="AQ58" s="31" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="AR58" s="41"/>
       <c r="AS58" s="41"/>
@@ -54959,7 +54999,7 @@
         <v>14</v>
       </c>
       <c r="BQ58" s="31" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="BR58" s="31" t="s">
         <v>45</v>
@@ -54968,7 +55008,7 @@
         <v>45</v>
       </c>
       <c r="BT58" s="31" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="BU58" s="31"/>
       <c r="BV58" s="31"/>
@@ -54983,7 +55023,7 @@
         <v>231</v>
       </c>
       <c r="CE58" s="31" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="CF58" s="15" t="s">
         <v>232</v>
@@ -54992,7 +55032,7 @@
         <v>45</v>
       </c>
       <c r="CH58" s="31" t="s">
-        <v>1524</v>
+        <v>1513</v>
       </c>
       <c r="CI58" s="31"/>
       <c r="CJ58" s="31"/>
@@ -55829,7 +55869,7 @@
         <v>14</v>
       </c>
       <c r="BQ62" s="34" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="BR62" s="34" t="s">
         <v>45</v>
@@ -55838,7 +55878,7 @@
         <v>45</v>
       </c>
       <c r="BT62" s="34" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="CD62" s="14" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
Final Commit before Wave1 2023 fix
</commit_message>
<xml_diff>
--- a/data/CRMCloud_Testdata.xlsx
+++ b/data/CRMCloud_Testdata.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fahmed2\git\Dynamics_CRM_Cloud_After_Wave1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23216A1A-1C50-4702-B646-113489228DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCF8ADD-6F29-4B49-B3BD-877ED00A4C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -41,7 +41,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -589,7 +589,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10700" uniqueCount="1583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10711" uniqueCount="1589">
   <si>
     <t>Auditorium/Museum</t>
   </si>
@@ -5280,12 +5280,6 @@
     <t>https://premierstage.crm.dynamics.com/main.aspx?appid=3dc0808e-d6b3-ed11-9885-0022481d602d</t>
   </si>
   <si>
-    <t>2000571642</t>
-  </si>
-  <si>
-    <t>2023_03_14_12_51_48</t>
-  </si>
-  <si>
     <t>2023_03_15_10_06_03</t>
   </si>
   <si>
@@ -5338,6 +5332,30 @@
   </si>
   <si>
     <t>2023_03_15_12_09_09</t>
+  </si>
+  <si>
+    <t>2023_03_16_03_06_17</t>
+  </si>
+  <si>
+    <t>2000571745</t>
+  </si>
+  <si>
+    <t>2023_03_16_05_45_06</t>
+  </si>
+  <si>
+    <t>2023_03_16_06_15_44</t>
+  </si>
+  <si>
+    <t>2023_03_16_06_20_14</t>
+  </si>
+  <si>
+    <t>2023_03_16_06_25_55</t>
+  </si>
+  <si>
+    <t>2023_03_16_06_36_28</t>
+  </si>
+  <si>
+    <t>2023_03_17_12_38_37</t>
   </si>
 </sst>
 </file>
@@ -6502,22 +6520,22 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="120.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="46" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="120.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="9" max="10" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="46.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -6573,13 +6591,13 @@
         <v>38</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>1517</v>
+        <v>1519</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>1564</v>
+        <v>1588</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>1563</v>
+        <v>1582</v>
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
@@ -6598,7 +6616,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>1</v>
@@ -6607,9 +6625,11 @@
         <v>38</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="G3" s="17"/>
+        <v>1519</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>1581</v>
+      </c>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -6626,7 +6646,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>1</v>
@@ -6652,7 +6672,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>1</v>
@@ -6678,7 +6698,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>1</v>
@@ -6704,7 +6724,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>1</v>
@@ -6716,7 +6736,7 @@
         <v>1517</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
@@ -6734,7 +6754,7 @@
         <v>445</v>
       </c>
       <c r="C8" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>1</v>
@@ -6746,10 +6766,10 @@
         <v>1519</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
@@ -6766,7 +6786,7 @@
         <v>44</v>
       </c>
       <c r="C9" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>1</v>
@@ -6778,7 +6798,7 @@
         <v>1517</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
@@ -6794,7 +6814,7 @@
         <v>444</v>
       </c>
       <c r="C10" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>1</v>
@@ -6820,7 +6840,7 @@
         <v>54</v>
       </c>
       <c r="C11" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>1</v>
@@ -6846,7 +6866,7 @@
         <v>443</v>
       </c>
       <c r="C12" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>1</v>
@@ -6873,7 +6893,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>1</v>
@@ -6899,7 +6919,7 @@
         <v>246</v>
       </c>
       <c r="C14" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>1</v>
@@ -6911,7 +6931,7 @@
         <v>1519</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
@@ -6927,7 +6947,7 @@
         <v>51</v>
       </c>
       <c r="C15" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>1</v>
@@ -6953,7 +6973,7 @@
         <v>442</v>
       </c>
       <c r="C16" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>1</v>
@@ -6979,7 +6999,7 @@
         <v>440</v>
       </c>
       <c r="C17" s="133" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>1</v>
@@ -7007,7 +7027,7 @@
         <v>439</v>
       </c>
       <c r="C18" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>1</v>
@@ -7087,7 +7107,7 @@
         <v>174</v>
       </c>
       <c r="C21" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>1</v>
@@ -7113,7 +7133,7 @@
         <v>173</v>
       </c>
       <c r="C22" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>1</v>
@@ -7139,7 +7159,7 @@
         <v>165</v>
       </c>
       <c r="C23" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>1</v>
@@ -7165,7 +7185,7 @@
         <v>175</v>
       </c>
       <c r="C24" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>1</v>
@@ -7191,7 +7211,7 @@
         <v>176</v>
       </c>
       <c r="C25" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>1</v>
@@ -7217,7 +7237,7 @@
         <v>177</v>
       </c>
       <c r="C26" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>1</v>
@@ -7299,7 +7319,7 @@
         <v>352</v>
       </c>
       <c r="C29" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>1</v>
@@ -7325,7 +7345,7 @@
         <v>355</v>
       </c>
       <c r="C30" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>1</v>
@@ -7351,7 +7371,7 @@
         <v>438</v>
       </c>
       <c r="C31" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>1</v>
@@ -7379,7 +7399,7 @@
         <v>447</v>
       </c>
       <c r="C32" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>1</v>
@@ -7391,7 +7411,7 @@
         <v>1517</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
@@ -7407,7 +7427,7 @@
         <v>437</v>
       </c>
       <c r="C33" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>1</v>
@@ -7435,7 +7455,7 @@
         <v>436</v>
       </c>
       <c r="C34" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>1</v>
@@ -7463,7 +7483,7 @@
         <v>435</v>
       </c>
       <c r="C35" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>1</v>
@@ -7491,7 +7511,7 @@
         <v>434</v>
       </c>
       <c r="C36" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>1</v>
@@ -7519,7 +7539,7 @@
         <v>433</v>
       </c>
       <c r="C37" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>1</v>
@@ -7547,7 +7567,7 @@
         <v>432</v>
       </c>
       <c r="C38" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D38" s="17" t="s">
         <v>1</v>
@@ -7575,7 +7595,7 @@
         <v>431</v>
       </c>
       <c r="C39" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D39" s="17" t="s">
         <v>1</v>
@@ -7603,7 +7623,7 @@
         <v>430</v>
       </c>
       <c r="C40" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>1</v>
@@ -7631,7 +7651,7 @@
         <v>429</v>
       </c>
       <c r="C41" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D41" s="17" t="s">
         <v>1</v>
@@ -7659,7 +7679,7 @@
         <v>428</v>
       </c>
       <c r="C42" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>1</v>
@@ -7687,7 +7707,7 @@
         <v>427</v>
       </c>
       <c r="C43" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>1</v>
@@ -7715,7 +7735,7 @@
         <v>426</v>
       </c>
       <c r="C44" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>1</v>
@@ -7743,7 +7763,7 @@
         <v>425</v>
       </c>
       <c r="C45" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>1</v>
@@ -7771,7 +7791,7 @@
         <v>424</v>
       </c>
       <c r="C46" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D46" s="17" t="s">
         <v>1</v>
@@ -7799,7 +7819,7 @@
         <v>423</v>
       </c>
       <c r="C47" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>1</v>
@@ -7827,7 +7847,7 @@
         <v>422</v>
       </c>
       <c r="C48" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>1</v>
@@ -7855,7 +7875,7 @@
         <v>421</v>
       </c>
       <c r="C49" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D49" s="17" t="s">
         <v>1</v>
@@ -7883,7 +7903,7 @@
         <v>420</v>
       </c>
       <c r="C50" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D50" s="17" t="s">
         <v>1</v>
@@ -7911,7 +7931,7 @@
         <v>543</v>
       </c>
       <c r="C51" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D51" s="17" t="s">
         <v>1</v>
@@ -7939,7 +7959,7 @@
         <v>544</v>
       </c>
       <c r="C52" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D52" s="17" t="s">
         <v>1</v>
@@ -7967,7 +7987,7 @@
         <v>546</v>
       </c>
       <c r="C53" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D53" s="17" t="s">
         <v>1</v>
@@ -7995,7 +8015,7 @@
         <v>548</v>
       </c>
       <c r="C54" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D54" s="17" t="s">
         <v>1</v>
@@ -8023,7 +8043,7 @@
         <v>552</v>
       </c>
       <c r="C55" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D55" s="17" t="s">
         <v>1</v>
@@ -8051,7 +8071,7 @@
         <v>554</v>
       </c>
       <c r="C56" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D56" s="17" t="s">
         <v>1</v>
@@ -8081,7 +8101,7 @@
         <v>556</v>
       </c>
       <c r="C57" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D57" s="17" t="s">
         <v>1</v>
@@ -8111,7 +8131,7 @@
         <v>557</v>
       </c>
       <c r="C58" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D58" s="17" t="s">
         <v>1</v>
@@ -8139,7 +8159,7 @@
         <v>560</v>
       </c>
       <c r="C59" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D59" s="17" t="s">
         <v>1</v>
@@ -8169,7 +8189,7 @@
         <v>562</v>
       </c>
       <c r="C60" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D60" s="17" t="s">
         <v>1</v>
@@ -8199,7 +8219,7 @@
         <v>564</v>
       </c>
       <c r="C61" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D61" s="17" t="s">
         <v>1</v>
@@ -8229,7 +8249,7 @@
         <v>566</v>
       </c>
       <c r="C62" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D62" s="17" t="s">
         <v>1</v>
@@ -8259,7 +8279,7 @@
         <v>568</v>
       </c>
       <c r="C63" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D63" s="17" t="s">
         <v>1</v>
@@ -8287,7 +8307,7 @@
         <v>570</v>
       </c>
       <c r="C64" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>1</v>
@@ -8317,7 +8337,7 @@
         <v>573</v>
       </c>
       <c r="C65" s="145" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D65" s="17" t="s">
         <v>1</v>
@@ -8345,7 +8365,7 @@
         <v>575</v>
       </c>
       <c r="C66" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D66" s="17" t="s">
         <v>1</v>
@@ -8357,7 +8377,7 @@
         <v>1519</v>
       </c>
       <c r="G66" s="22" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="H66" s="22"/>
       <c r="I66" s="22"/>
@@ -8463,7 +8483,7 @@
         <v>1519</v>
       </c>
       <c r="G70" s="22" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="H70" s="22"/>
       <c r="I70" s="22"/>
@@ -10032,7 +10052,7 @@
         <v>28</v>
       </c>
       <c r="C132" s="145" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D132" s="19" t="s">
         <v>25</v>
@@ -10062,7 +10082,7 @@
         <v>457</v>
       </c>
       <c r="C133" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D133" s="19" t="s">
         <v>25</v>
@@ -10092,7 +10112,7 @@
         <v>461</v>
       </c>
       <c r="C134" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D134" s="19" t="s">
         <v>25</v>
@@ -10122,7 +10142,7 @@
         <v>446</v>
       </c>
       <c r="C135" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D135" s="19" t="s">
         <v>25</v>
@@ -10152,7 +10172,7 @@
         <v>89</v>
       </c>
       <c r="C136" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D136" s="19" t="s">
         <v>25</v>
@@ -10182,7 +10202,7 @@
         <v>94</v>
       </c>
       <c r="C137" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D137" s="19" t="s">
         <v>25</v>
@@ -10212,7 +10232,7 @@
         <v>98</v>
       </c>
       <c r="C138" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D138" s="19" t="s">
         <v>25</v>
@@ -10242,7 +10262,7 @@
         <v>103</v>
       </c>
       <c r="C139" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D139" s="19" t="s">
         <v>25</v>
@@ -10272,7 +10292,7 @@
         <v>106</v>
       </c>
       <c r="C140" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D140" s="19" t="s">
         <v>25</v>
@@ -10302,7 +10322,7 @@
         <v>109</v>
       </c>
       <c r="C141" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D141" s="19" t="s">
         <v>25</v>
@@ -10332,7 +10352,7 @@
         <v>112</v>
       </c>
       <c r="C142" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D142" s="19" t="s">
         <v>25</v>
@@ -10362,7 +10382,7 @@
         <v>119</v>
       </c>
       <c r="C143" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D143" s="19" t="s">
         <v>25</v>
@@ -10392,7 +10412,7 @@
         <v>126</v>
       </c>
       <c r="C144" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D144" s="19" t="s">
         <v>25</v>
@@ -10422,7 +10442,7 @@
         <v>251</v>
       </c>
       <c r="C145" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D145" s="19" t="s">
         <v>25</v>
@@ -10434,7 +10454,7 @@
         <v>1519</v>
       </c>
       <c r="G145" s="19" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="H145" s="19"/>
       <c r="I145" s="19"/>
@@ -10450,7 +10470,7 @@
         <v>182</v>
       </c>
       <c r="C146" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D146" s="19" t="s">
         <v>25</v>
@@ -10480,7 +10500,7 @@
         <v>411</v>
       </c>
       <c r="C147" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D147" s="19" t="s">
         <v>25</v>
@@ -10492,10 +10512,10 @@
         <v>1517</v>
       </c>
       <c r="G147" s="19" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="H147" s="19" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="I147" s="19"/>
       <c r="J147" s="19"/>
@@ -10510,7 +10530,7 @@
         <v>448</v>
       </c>
       <c r="C148" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D148" s="19" t="s">
         <v>25</v>
@@ -10538,7 +10558,7 @@
         <v>454</v>
       </c>
       <c r="C149" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D149" s="19" t="s">
         <v>25</v>
@@ -10566,7 +10586,7 @@
         <v>458</v>
       </c>
       <c r="C150" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D150" s="19" t="s">
         <v>25</v>
@@ -10594,7 +10614,7 @@
         <v>463</v>
       </c>
       <c r="C151" s="133" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D151" s="19" t="s">
         <v>25</v>
@@ -10622,7 +10642,7 @@
         <v>466</v>
       </c>
       <c r="C152" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D152" s="19" t="s">
         <v>25</v>
@@ -10650,7 +10670,7 @@
         <v>469</v>
       </c>
       <c r="C153" s="133" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D153" s="19" t="s">
         <v>25</v>
@@ -10678,7 +10698,7 @@
         <v>464</v>
       </c>
       <c r="C154" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D154" s="19" t="s">
         <v>25</v>
@@ -10706,7 +10726,7 @@
         <v>584</v>
       </c>
       <c r="C155" s="133" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D155" s="17" t="s">
         <v>25</v>
@@ -10732,7 +10752,7 @@
         <v>589</v>
       </c>
       <c r="C156" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D156" s="19" t="s">
         <v>25</v>
@@ -10744,7 +10764,7 @@
         <v>1517</v>
       </c>
       <c r="G156" s="22" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="H156" s="22"/>
       <c r="I156" s="22"/>
@@ -10760,7 +10780,7 @@
         <v>590</v>
       </c>
       <c r="C157" s="133" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D157" s="19" t="s">
         <v>25</v>
@@ -10788,7 +10808,7 @@
         <v>591</v>
       </c>
       <c r="C158" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D158" s="19" t="s">
         <v>25</v>
@@ -10818,7 +10838,7 @@
         <v>592</v>
       </c>
       <c r="C159" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D159" s="19" t="s">
         <v>25</v>
@@ -10846,7 +10866,7 @@
         <v>593</v>
       </c>
       <c r="C160" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D160" s="19" t="s">
         <v>25</v>
@@ -10858,7 +10878,7 @@
         <v>1519</v>
       </c>
       <c r="G160" s="19" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="H160" s="19"/>
       <c r="I160" s="19"/>
@@ -10874,7 +10894,7 @@
         <v>594</v>
       </c>
       <c r="C161" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D161" s="19" t="s">
         <v>25</v>
@@ -10902,7 +10922,7 @@
         <v>595</v>
       </c>
       <c r="C162" s="133" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D162" s="19" t="s">
         <v>25</v>
@@ -10930,7 +10950,7 @@
         <v>596</v>
       </c>
       <c r="C163" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D163" s="19" t="s">
         <v>25</v>
@@ -10958,7 +10978,7 @@
         <v>597</v>
       </c>
       <c r="C164" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D164" s="19" t="s">
         <v>25</v>
@@ -10986,7 +11006,7 @@
         <v>740</v>
       </c>
       <c r="C165" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D165" s="19" t="s">
         <v>25</v>
@@ -10998,7 +11018,7 @@
         <v>1519</v>
       </c>
       <c r="G165" s="19" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="H165" s="19"/>
       <c r="I165" s="19"/>
@@ -11014,7 +11034,7 @@
         <v>888</v>
       </c>
       <c r="C166" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D166" s="19" t="s">
         <v>25</v>
@@ -11026,7 +11046,7 @@
         <v>1519</v>
       </c>
       <c r="G166" s="19" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="H166" s="19"/>
       <c r="I166" s="19"/>
@@ -11042,7 +11062,7 @@
         <v>888</v>
       </c>
       <c r="C167" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D167" s="19" t="s">
         <v>25</v>
@@ -11068,7 +11088,7 @@
         <v>1330</v>
       </c>
       <c r="C168" s="135" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D168" s="19" t="s">
         <v>25</v>
@@ -11096,7 +11116,7 @@
         <v>217</v>
       </c>
       <c r="C169" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D169" s="27" t="s">
         <v>216</v>
@@ -11126,7 +11146,7 @@
         <v>413</v>
       </c>
       <c r="C170" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D170" s="27" t="s">
         <v>216</v>
@@ -11138,10 +11158,10 @@
         <v>1519</v>
       </c>
       <c r="G170" s="24" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="H170" s="24" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="I170" s="24"/>
       <c r="J170" s="24"/>
@@ -11156,7 +11176,7 @@
         <v>414</v>
       </c>
       <c r="C171" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D171" s="27" t="s">
         <v>216</v>
@@ -11186,7 +11206,7 @@
         <v>415</v>
       </c>
       <c r="C172" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D172" s="26" t="s">
         <v>216</v>
@@ -11216,7 +11236,7 @@
         <v>416</v>
       </c>
       <c r="C173" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D173" s="26" t="s">
         <v>216</v>
@@ -11246,7 +11266,7 @@
         <v>412</v>
       </c>
       <c r="C174" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D174" s="26" t="s">
         <v>216</v>
@@ -11274,7 +11294,7 @@
         <v>417</v>
       </c>
       <c r="C175" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D175" s="26" t="s">
         <v>216</v>
@@ -11302,7 +11322,7 @@
         <v>418</v>
       </c>
       <c r="C176" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D176" s="26" t="s">
         <v>216</v>
@@ -11332,7 +11352,7 @@
         <v>419</v>
       </c>
       <c r="C177" s="126" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D177" s="26" t="s">
         <v>216</v>
@@ -11362,7 +11382,7 @@
         <v>1326</v>
       </c>
       <c r="C178" s="132" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D178" s="26" t="s">
         <v>216</v>
@@ -11374,7 +11394,7 @@
         <v>1519</v>
       </c>
       <c r="G178" s="130" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="H178" s="130" t="s">
         <v>475</v>
@@ -11392,7 +11412,7 @@
         <v>950</v>
       </c>
       <c r="C179" s="145" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D179" s="26" t="s">
         <v>216</v>
@@ -14683,7 +14703,7 @@
     <hyperlink ref="L2" r:id="rId2" xr:uid="{A4124D5F-F457-4A70-A072-5DFAF5EA33F8}"/>
     <hyperlink ref="L7" r:id="rId3" xr:uid="{25B2C645-4F48-40EF-B244-993C9919EC53}"/>
     <hyperlink ref="L8" r:id="rId4" xr:uid="{7232C0DB-4105-4970-9DC9-351E323A6B9A}"/>
-    <hyperlink ref="K2" r:id="rId5" xr:uid="{D769CF7F-3B55-42B5-B5B8-D367817C08E1}"/>
+    <hyperlink ref="K2" r:id="rId5" xr:uid="{AD47B4D5-663C-4C80-B0BF-772B1E0F633A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
@@ -16885,7 +16905,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="136.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="136.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:168" x14ac:dyDescent="0.25">
@@ -18946,8 +18966,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:155" x14ac:dyDescent="0.25">
@@ -20435,8 +20455,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="136" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="136.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:141" x14ac:dyDescent="0.25">
@@ -21844,7 +21864,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="60.28515625" style="112" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" style="112" width="60.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:141" x14ac:dyDescent="0.25">
@@ -24508,7 +24528,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="84.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="84.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:141" x14ac:dyDescent="0.25">
@@ -33979,69 +33999,69 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="114" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="82.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="28" max="36" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="34.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="54.42578125" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="47" width="29" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="50" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="57" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="73" max="73" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="74" max="74" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="76" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="114.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="82.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="28" max="36" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" width="54.42578125" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="46" max="47" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="49" max="50" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="52" max="52" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="56" max="57" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="61" max="61" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="62" max="62" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="63" max="63" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="64" max="64" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
+    <col min="65" max="65" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="66" max="66" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="67" max="67" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="68" max="68" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="69" max="69" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="70" max="70" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="71" max="71" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="72" max="72" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="73" max="73" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="74" max="74" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="75" max="76" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:78" x14ac:dyDescent="0.25">
@@ -38295,27 +38315,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="108" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="7" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="65.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="73.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="108.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="4" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="65.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="73.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -39385,8 +39405,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" collapsed="1"/>
-    <col min="56" max="56" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.140625" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:89" x14ac:dyDescent="0.25">
@@ -42342,7 +42362,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
-  <dimension ref="A1:FI143"/>
+  <dimension ref="A1:FH143"/>
   <sheetViews>
     <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B69" sqref="B69"/>
@@ -42350,113 +42370,111 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="121" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="69.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="36.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="73.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="73.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="20" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="21" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="25" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="21.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="27.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="10.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="4.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="8.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="24.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="24.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="15" style="2" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="9.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="17.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="9.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="24.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="16.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="10.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="20.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="20.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="26.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="57" width="26.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="24.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="25" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="15.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="15.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="15.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="17.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="26.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="30.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="23.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="81" width="23.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="82" max="82" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="83" max="83" width="26.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="84" max="84" width="18.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="85" max="85" width="18.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="86" max="92" width="26.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="93" max="93" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="94" max="94" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="95" max="95" width="22.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="96" max="96" width="18.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="97" max="97" width="9.140625" style="2" collapsed="1"/>
-    <col min="98" max="98" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="99" max="99" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="100" max="100" width="17.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="101" max="101" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="102" max="102" width="15.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="103" max="103" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="104" max="104" width="19.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="105" max="105" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="106" max="106" width="14.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="107" max="107" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="108" max="108" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="109" max="109" width="10.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="110" max="110" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="111" max="111" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="112" max="112" width="9.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="113" max="113" width="14.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="114" max="114" width="32" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="115" max="115" width="16.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="116" max="122" width="9.140625" style="2" collapsed="1"/>
-    <col min="123" max="123" width="10" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="124" max="131" width="9.140625" style="2" collapsed="1"/>
-    <col min="132" max="132" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="133" max="133" width="16.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="134" max="134" width="15.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="135" max="135" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="136" max="136" width="11.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="137" max="138" width="9.140625" style="2" collapsed="1"/>
-    <col min="139" max="139" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="140" max="141" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="142" max="142" width="38.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="143" max="148" width="9.140625" style="2" collapsed="1"/>
-    <col min="149" max="149" width="19.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="150" max="164" width="9.140625" style="2" collapsed="1"/>
-    <col min="165" max="165" width="9.140625" style="2"/>
-    <col min="166" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="5.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="121.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="29.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="11.28515625" collapsed="true"/>
+    <col min="7" max="9" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="69.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="2" width="36.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="73.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="2" width="73.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="20.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="15.42578125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
+    <col min="20" max="21" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="22" max="25" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="2" width="21.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="4.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="2" width="8.28515625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" style="2" width="24.140625" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" style="2" width="24.140625" collapsed="true"/>
+    <col min="40" max="40" customWidth="true" style="2" width="15.0" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" style="2" width="9.85546875" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="2" width="9.5703125" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" style="2" width="22.28515625" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" style="2" width="24.5703125" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
+    <col min="51" max="51" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" style="2" width="20.5703125" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" style="2" width="26.42578125" collapsed="true"/>
+    <col min="55" max="57" customWidth="true" style="2" width="26.42578125" collapsed="true"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
+    <col min="59" max="59" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="61" max="61" bestFit="true" customWidth="true" style="2" width="15.140625" collapsed="true"/>
+    <col min="62" max="62" customWidth="true" style="2" width="15.140625" collapsed="true"/>
+    <col min="63" max="63" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
+    <col min="64" max="64" bestFit="true" customWidth="true" style="2" width="15.7109375" collapsed="true"/>
+    <col min="65" max="65" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
+    <col min="66" max="66" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
+    <col min="67" max="67" bestFit="true" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
+    <col min="68" max="68" bestFit="true" customWidth="true" style="2" width="30.42578125" collapsed="true"/>
+    <col min="69" max="69" bestFit="true" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
+    <col min="70" max="81" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
+    <col min="82" max="82" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="83" max="83" bestFit="true" customWidth="true" style="2" width="26.140625" collapsed="true"/>
+    <col min="84" max="84" bestFit="true" customWidth="true" style="2" width="18.140625" collapsed="true"/>
+    <col min="85" max="85" customWidth="true" style="2" width="18.140625" collapsed="true"/>
+    <col min="86" max="92" customWidth="true" style="2" width="26.140625" collapsed="true"/>
+    <col min="93" max="93" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="94" max="94" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="95" max="95" bestFit="true" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
+    <col min="96" max="96" bestFit="true" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
+    <col min="97" max="97" style="2" width="9.140625" collapsed="true"/>
+    <col min="98" max="98" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
+    <col min="99" max="99" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="100" max="100" bestFit="true" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
+    <col min="101" max="101" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="102" max="102" bestFit="true" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
+    <col min="103" max="103" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
+    <col min="104" max="104" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
+    <col min="105" max="105" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
+    <col min="106" max="106" bestFit="true" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
+    <col min="107" max="107" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
+    <col min="108" max="108" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
+    <col min="109" max="109" bestFit="true" customWidth="true" style="2" width="10.7109375" collapsed="true"/>
+    <col min="110" max="110" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
+    <col min="111" max="111" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
+    <col min="112" max="112" bestFit="true" customWidth="true" style="2" width="9.28515625" collapsed="true"/>
+    <col min="113" max="113" bestFit="true" customWidth="true" style="2" width="14.140625" collapsed="true"/>
+    <col min="114" max="114" bestFit="true" customWidth="true" style="2" width="32.0" collapsed="true"/>
+    <col min="115" max="115" bestFit="true" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
+    <col min="116" max="122" style="2" width="9.140625" collapsed="true"/>
+    <col min="123" max="123" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
+    <col min="124" max="131" style="2" width="9.140625" collapsed="true"/>
+    <col min="132" max="132" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="133" max="133" bestFit="true" customWidth="true" style="2" width="16.42578125" collapsed="true"/>
+    <col min="134" max="134" bestFit="true" customWidth="true" style="2" width="15.5703125" collapsed="true"/>
+    <col min="135" max="135" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="136" max="136" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="137" max="138" style="2" width="9.140625" collapsed="true"/>
+    <col min="139" max="139" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="140" max="141" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
+    <col min="142" max="142" bestFit="true" customWidth="true" style="2" width="38.5703125" collapsed="true"/>
+    <col min="143" max="148" style="2" width="9.140625" collapsed="true"/>
+    <col min="149" max="149" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
+    <col min="150" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:161" s="54" customFormat="1" x14ac:dyDescent="0.25">
@@ -70895,8 +70913,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -71048,9 +71066,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="53.42578125" style="112" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" style="112" width="53.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="24.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.25">
@@ -71452,12 +71470,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -71695,20 +71713,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -71734,9 +71750,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD45B30-098E-4D79-A294-CA56938A6C1B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BF8EFB6-861E-4E07-8FE0-B0C68FAC562F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>